<commit_message>
Actualización de prueba en Excel
</commit_message>
<xml_diff>
--- a/excel/CLIENTES_PERMISOS.xlsx
+++ b/excel/CLIENTES_PERMISOS.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
   <si>
     <t>CUENTA</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>00958</t>
+  </si>
+  <si>
+    <t>FABIAN FERRETERIA</t>
   </si>
 </sst>
 </file>
@@ -312,10 +315,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -366,6 +369,20 @@
         <v>6</v>
       </c>
     </row>
+    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>946</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Normalización de códigos de producto en ProductManagerPROBLEMA:- Inconsistencia en el formato de códigos de productos
</commit_message>
<xml_diff>
--- a/excel/CLIENTES_PERMISOS.xlsx
+++ b/excel/CLIENTES_PERMISOS.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
   <si>
     <t>CUENTA</t>
   </si>
@@ -45,17 +45,17 @@
     <t>FORRAJERIA MARTIN</t>
   </si>
   <si>
-    <t>00958</t>
-  </si>
-  <si>
     <t>FABIAN FERRETERIA</t>
+  </si>
+  <si>
+    <t>MARIANO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -66,6 +66,14 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -76,7 +84,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -84,18 +92,38 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -315,10 +343,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -327,7 +355,7 @@
     <col min="3" max="3" width="66.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -341,7 +369,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>20246</v>
       </c>
@@ -355,12 +383,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>946</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>5</v>
@@ -369,21 +397,36 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>946</v>
-      </c>
-      <c r="B4" s="1" t="s">
+    <row r="4" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>950</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>958</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
cambios en excel, probar diferentes grupos de clientes, y diferentes listas
</commit_message>
<xml_diff>
--- a/excel/CLIENTES_PERMISOS.xlsx
+++ b/excel/CLIENTES_PERMISOS.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>CUENTA</t>
   </si>
@@ -49,6 +49,12 @@
   </si>
   <si>
     <t>MARIANO</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
   </si>
 </sst>
 </file>
@@ -346,7 +352,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -394,7 +400,7 @@
         <v>5</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -408,7 +414,7 @@
         <v>5</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -422,7 +428,7 @@
         <v>5</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
subi nuevas imagenes, cambie la lista de acuario,tambien agregue todos los crupos de clientees al excel y les puse articulos para mostrar, por ahora todos iguales
</commit_message>
<xml_diff>
--- a/excel/CLIENTES_PERMISOS.xlsx
+++ b/excel/CLIENTES_PERMISOS.xlsx
@@ -1080,15 +1080,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1315,8 +1307,8 @@
   </sheetPr>
   <dimension ref="A1:D319"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A298" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D319"/>
+    <sheetView tabSelected="1" topLeftCell="A62" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D71" sqref="D71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2302,7 +2294,7 @@
         <v>4</v>
       </c>
       <c r="D70" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5794,7 +5786,7 @@
   </sheetData>
   <autoFilter ref="A1:D319"/>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
actialice precios, lista de los clientes
</commit_message>
<xml_diff>
--- a/excel/CLIENTES_PERMISOS.xlsx
+++ b/excel/CLIENTES_PERMISOS.xlsx
@@ -1062,20 +1062,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1307,14 +1309,15 @@
   </sheetPr>
   <dimension ref="A1:D319"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D71" sqref="D71"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="34" customWidth="1"/>
     <col min="3" max="3" width="66.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1332,7 +1335,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
+      <c r="A2" s="4">
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1346,7 +1349,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3">
+      <c r="A3" s="5">
         <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1356,39 +1359,39 @@
         <v>4</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3">
+      <c r="A4" s="5">
         <v>12</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="2" t="s">
         <v>211</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3">
+      <c r="A5" s="5">
         <v>20</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="2" t="s">
         <v>203</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="A6" s="6">
         <v>27</v>
       </c>
       <c r="B6" t="s">
@@ -1397,12 +1400,12 @@
       <c r="C6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7">
+      <c r="A7" s="6">
         <v>33</v>
       </c>
       <c r="B7" t="s">
@@ -1411,12 +1414,12 @@
       <c r="C7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8">
+      <c r="A8" s="6">
         <v>233</v>
       </c>
       <c r="B8" t="s">
@@ -1425,12 +1428,12 @@
       <c r="C8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9">
+      <c r="A9" s="6">
         <v>237</v>
       </c>
       <c r="B9" t="s">
@@ -1439,12 +1442,12 @@
       <c r="C9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10">
+      <c r="A10" s="6">
         <v>246</v>
       </c>
       <c r="B10" t="s">
@@ -1453,12 +1456,12 @@
       <c r="C10" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11">
+      <c r="A11" s="6">
         <v>251</v>
       </c>
       <c r="B11" t="s">
@@ -1467,12 +1470,12 @@
       <c r="C11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12">
+      <c r="A12" s="6">
         <v>265</v>
       </c>
       <c r="B12" t="s">
@@ -1481,12 +1484,12 @@
       <c r="C12" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13">
+      <c r="A13" s="6">
         <v>308</v>
       </c>
       <c r="B13" t="s">
@@ -1495,12 +1498,12 @@
       <c r="C13" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D13" t="s">
-        <v>5</v>
+      <c r="D13" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14">
+      <c r="A14" s="6">
         <v>920</v>
       </c>
       <c r="B14" t="s">
@@ -1509,12 +1512,12 @@
       <c r="C14" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15">
+      <c r="A15" s="6">
         <v>936</v>
       </c>
       <c r="B15" t="s">
@@ -1523,12 +1526,12 @@
       <c r="C15" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16">
+      <c r="A16" s="6">
         <v>938</v>
       </c>
       <c r="B16" t="s">
@@ -1537,12 +1540,12 @@
       <c r="C16" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D16" t="s">
-        <v>8</v>
+      <c r="D16" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17">
+      <c r="A17" s="6">
         <v>939</v>
       </c>
       <c r="B17" t="s">
@@ -1551,12 +1554,12 @@
       <c r="C17" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D17" t="s">
-        <v>5</v>
+      <c r="D17" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18">
+      <c r="A18" s="6">
         <v>940</v>
       </c>
       <c r="B18" t="s">
@@ -1565,12 +1568,12 @@
       <c r="C18" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19">
+      <c r="A19" s="6">
         <v>946</v>
       </c>
       <c r="B19" t="s">
@@ -1580,11 +1583,11 @@
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20">
+      <c r="A20" s="6">
         <v>947</v>
       </c>
       <c r="B20" t="s">
@@ -1593,12 +1596,12 @@
       <c r="C20" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21">
+      <c r="A21" s="6">
         <v>949</v>
       </c>
       <c r="B21" t="s">
@@ -1607,12 +1610,12 @@
       <c r="C21" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22">
+      <c r="A22" s="6">
         <v>950</v>
       </c>
       <c r="B22" t="s">
@@ -1621,12 +1624,12 @@
       <c r="C22" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23">
+      <c r="A23" s="6">
         <v>951</v>
       </c>
       <c r="B23" t="s">
@@ -1635,12 +1638,12 @@
       <c r="C23" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D23" t="s">
-        <v>5</v>
+      <c r="D23" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24">
+      <c r="A24" s="6">
         <v>952</v>
       </c>
       <c r="B24" t="s">
@@ -1650,11 +1653,11 @@
         <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25">
+      <c r="A25" s="6">
         <v>954</v>
       </c>
       <c r="B25" t="s">
@@ -1663,12 +1666,12 @@
       <c r="C25" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26">
+      <c r="A26" s="6">
         <v>955</v>
       </c>
       <c r="B26" t="s">
@@ -1677,12 +1680,12 @@
       <c r="C26" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27">
+      <c r="A27" s="6">
         <v>956</v>
       </c>
       <c r="B27" t="s">
@@ -1691,12 +1694,12 @@
       <c r="C27" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28">
+      <c r="A28" s="6">
         <v>958</v>
       </c>
       <c r="B28" t="s">
@@ -1705,12 +1708,12 @@
       <c r="C28" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D28" t="s">
-        <v>8</v>
+      <c r="D28" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29">
+      <c r="A29" s="6">
         <v>961</v>
       </c>
       <c r="B29" t="s">
@@ -1719,12 +1722,12 @@
       <c r="C29" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30">
+      <c r="A30" s="6">
         <v>962</v>
       </c>
       <c r="B30" t="s">
@@ -1733,12 +1736,12 @@
       <c r="C30" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31">
+      <c r="A31" s="6">
         <v>963</v>
       </c>
       <c r="B31" t="s">
@@ -1747,12 +1750,12 @@
       <c r="C31" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32">
+      <c r="A32" s="6">
         <v>965</v>
       </c>
       <c r="B32" t="s">
@@ -1761,12 +1764,12 @@
       <c r="C32" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D32" t="s">
-        <v>8</v>
+      <c r="D32" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33">
+      <c r="A33" s="6">
         <v>969</v>
       </c>
       <c r="B33" t="s">
@@ -1775,12 +1778,12 @@
       <c r="C33" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D33" t="s">
-        <v>5</v>
+      <c r="D33" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34">
+      <c r="A34" s="6">
         <v>970</v>
       </c>
       <c r="B34" t="s">
@@ -1790,11 +1793,11 @@
         <v>4</v>
       </c>
       <c r="D34" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35">
+      <c r="A35" s="6">
         <v>972</v>
       </c>
       <c r="B35" t="s">
@@ -1803,12 +1806,12 @@
       <c r="C35" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D35" t="s">
-        <v>8</v>
+      <c r="D35" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36">
+      <c r="A36" s="6">
         <v>973</v>
       </c>
       <c r="B36" t="s">
@@ -1817,12 +1820,12 @@
       <c r="C36" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37">
+      <c r="A37" s="6">
         <v>974</v>
       </c>
       <c r="B37" t="s">
@@ -1831,12 +1834,12 @@
       <c r="C37" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D37" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38">
+      <c r="A38" s="6">
         <v>980</v>
       </c>
       <c r="B38" t="s">
@@ -1845,12 +1848,12 @@
       <c r="C38" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39">
+      <c r="A39" s="6">
         <v>982</v>
       </c>
       <c r="B39" t="s">
@@ -1859,12 +1862,12 @@
       <c r="C39" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D39" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40">
+      <c r="A40" s="6">
         <v>987</v>
       </c>
       <c r="B40" t="s">
@@ -1873,12 +1876,12 @@
       <c r="C40" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D40" t="s">
-        <v>8</v>
+      <c r="D40" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41">
+      <c r="A41" s="6">
         <v>989</v>
       </c>
       <c r="B41" t="s">
@@ -1887,12 +1890,12 @@
       <c r="C41" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42">
+      <c r="A42" s="6">
         <v>992</v>
       </c>
       <c r="B42" t="s">
@@ -1901,12 +1904,12 @@
       <c r="C42" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43">
+      <c r="A43" s="6">
         <v>993</v>
       </c>
       <c r="B43" t="s">
@@ -1915,12 +1918,12 @@
       <c r="C43" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D43" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44">
+      <c r="A44" s="6">
         <v>994</v>
       </c>
       <c r="B44" t="s">
@@ -1929,12 +1932,12 @@
       <c r="C44" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D44" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45">
+      <c r="A45" s="6">
         <v>997</v>
       </c>
       <c r="B45" t="s">
@@ -1943,12 +1946,12 @@
       <c r="C45" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D45" t="s">
-        <v>5</v>
+      <c r="D45" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46">
+      <c r="A46" s="6">
         <v>998</v>
       </c>
       <c r="B46" t="s">
@@ -1957,12 +1960,12 @@
       <c r="C46" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D46" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47">
+      <c r="A47" s="6">
         <v>999</v>
       </c>
       <c r="B47" t="s">
@@ -1972,11 +1975,11 @@
         <v>4</v>
       </c>
       <c r="D47" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48">
+      <c r="A48" s="6">
         <v>1000</v>
       </c>
       <c r="B48" t="s">
@@ -1985,12 +1988,12 @@
       <c r="C48" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D48" t="s">
-        <v>5</v>
+      <c r="D48" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49">
+      <c r="A49" s="6">
         <v>1001</v>
       </c>
       <c r="B49" t="s">
@@ -1999,12 +2002,12 @@
       <c r="C49" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D49" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50">
+      <c r="A50" s="6">
         <v>1002</v>
       </c>
       <c r="B50" t="s">
@@ -2013,12 +2016,12 @@
       <c r="C50" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D50" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51">
+      <c r="A51" s="6">
         <v>1005</v>
       </c>
       <c r="B51" t="s">
@@ -2027,12 +2030,12 @@
       <c r="C51" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D51" t="s">
-        <v>5</v>
+      <c r="D51" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52">
+      <c r="A52" s="6">
         <v>1006</v>
       </c>
       <c r="B52" t="s">
@@ -2041,12 +2044,12 @@
       <c r="C52" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D52" t="s">
-        <v>8</v>
+      <c r="D52" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53">
+      <c r="A53" s="6">
         <v>1007</v>
       </c>
       <c r="B53" t="s">
@@ -2055,12 +2058,12 @@
       <c r="C53" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D53" t="s">
-        <v>5</v>
+      <c r="D53" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54">
+      <c r="A54" s="6">
         <v>1009</v>
       </c>
       <c r="B54" t="s">
@@ -2069,12 +2072,12 @@
       <c r="C54" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D54" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55">
+      <c r="A55" s="6">
         <v>1010</v>
       </c>
       <c r="B55" t="s">
@@ -2084,11 +2087,11 @@
         <v>4</v>
       </c>
       <c r="D55" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56">
+      <c r="A56" s="6">
         <v>1012</v>
       </c>
       <c r="B56" t="s">
@@ -2098,11 +2101,11 @@
         <v>4</v>
       </c>
       <c r="D56" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57">
+      <c r="A57" s="6">
         <v>1013</v>
       </c>
       <c r="B57" t="s">
@@ -2111,12 +2114,12 @@
       <c r="C57" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D57" t="s">
+      <c r="D57" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58">
+      <c r="A58" s="6">
         <v>1015</v>
       </c>
       <c r="B58" t="s">
@@ -2125,12 +2128,12 @@
       <c r="C58" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D58" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59">
+      <c r="A59" s="6">
         <v>1416</v>
       </c>
       <c r="B59" t="s">
@@ -2139,12 +2142,12 @@
       <c r="C59" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D59" t="s">
-        <v>5</v>
+      <c r="D59" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60">
+      <c r="A60" s="6">
         <v>10107</v>
       </c>
       <c r="B60" t="s">
@@ -2154,11 +2157,11 @@
         <v>4</v>
       </c>
       <c r="D60" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61">
+      <c r="A61" s="6">
         <v>10137</v>
       </c>
       <c r="B61" t="s">
@@ -2167,12 +2170,12 @@
       <c r="C61" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D61" t="s">
-        <v>5</v>
+      <c r="D61" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62">
+      <c r="A62" s="6">
         <v>10157</v>
       </c>
       <c r="B62" t="s">
@@ -2181,12 +2184,12 @@
       <c r="C62" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D62" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63">
+      <c r="A63" s="6">
         <v>10158</v>
       </c>
       <c r="B63" t="s">
@@ -2195,12 +2198,12 @@
       <c r="C63" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D63" t="s">
+      <c r="D63" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64">
+      <c r="A64" s="6">
         <v>10160</v>
       </c>
       <c r="B64" t="s">
@@ -2209,12 +2212,12 @@
       <c r="C64" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D64" t="s">
+      <c r="D64" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65">
+      <c r="A65" s="6">
         <v>10162</v>
       </c>
       <c r="B65" t="s">
@@ -2223,12 +2226,12 @@
       <c r="C65" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D65" t="s">
+      <c r="D65" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66">
+      <c r="A66" s="6">
         <v>10163</v>
       </c>
       <c r="B66" t="s">
@@ -2237,12 +2240,12 @@
       <c r="C66" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D66" t="s">
-        <v>8</v>
+      <c r="D66" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67">
+      <c r="A67" s="6">
         <v>10165</v>
       </c>
       <c r="B67" t="s">
@@ -2251,12 +2254,12 @@
       <c r="C67" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D67" t="s">
+      <c r="D67" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68">
+      <c r="A68" s="6">
         <v>10167</v>
       </c>
       <c r="B68" t="s">
@@ -2265,12 +2268,12 @@
       <c r="C68" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D68" t="s">
-        <v>8</v>
+      <c r="D68" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69">
+      <c r="A69" s="6">
         <v>10424</v>
       </c>
       <c r="B69" t="s">
@@ -2280,11 +2283,11 @@
         <v>4</v>
       </c>
       <c r="D69" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70">
+      <c r="A70" s="6">
         <v>10425</v>
       </c>
       <c r="B70" t="s">
@@ -2298,7 +2301,7 @@
       </c>
     </row>
     <row r="71" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71">
+      <c r="A71" s="6">
         <v>20094</v>
       </c>
       <c r="B71" t="s">
@@ -2307,12 +2310,12 @@
       <c r="C71" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D71" t="s">
-        <v>5</v>
+      <c r="D71" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72">
+      <c r="A72" s="6">
         <v>20095</v>
       </c>
       <c r="B72" t="s">
@@ -2321,12 +2324,12 @@
       <c r="C72" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D72" t="s">
+      <c r="D72" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73">
+      <c r="A73" s="6">
         <v>20096</v>
       </c>
       <c r="B73" t="s">
@@ -2335,12 +2338,12 @@
       <c r="C73" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D73" t="s">
-        <v>5</v>
+      <c r="D73" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A74">
+      <c r="A74" s="6">
         <v>20100</v>
       </c>
       <c r="B74" t="s">
@@ -2349,12 +2352,12 @@
       <c r="C74" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D74" t="s">
-        <v>5</v>
+      <c r="D74" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A75">
+      <c r="A75" s="6">
         <v>20101</v>
       </c>
       <c r="B75" t="s">
@@ -2363,12 +2366,12 @@
       <c r="C75" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D75" t="s">
+      <c r="D75" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A76">
+      <c r="A76" s="6">
         <v>20103</v>
       </c>
       <c r="B76" t="s">
@@ -2377,12 +2380,12 @@
       <c r="C76" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D76" t="s">
+      <c r="D76" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77">
+      <c r="A77" s="6">
         <v>20106</v>
       </c>
       <c r="B77" t="s">
@@ -2391,12 +2394,12 @@
       <c r="C77" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D77" t="s">
+      <c r="D77" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78">
+      <c r="A78" s="6">
         <v>20108</v>
       </c>
       <c r="B78" t="s">
@@ -2405,12 +2408,12 @@
       <c r="C78" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D78" t="s">
+      <c r="D78" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A79">
+      <c r="A79" s="6">
         <v>20109</v>
       </c>
       <c r="B79" t="s">
@@ -2419,12 +2422,12 @@
       <c r="C79" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D79" t="s">
+      <c r="D79" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A80">
+      <c r="A80" s="6">
         <v>20110</v>
       </c>
       <c r="B80" t="s">
@@ -2433,12 +2436,12 @@
       <c r="C80" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D80" t="s">
-        <v>8</v>
+      <c r="D80" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A81">
+      <c r="A81" s="6">
         <v>20113</v>
       </c>
       <c r="B81" t="s">
@@ -2447,12 +2450,12 @@
       <c r="C81" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D81" t="s">
+      <c r="D81" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A82">
+      <c r="A82" s="6">
         <v>20114</v>
       </c>
       <c r="B82" t="s">
@@ -2461,12 +2464,12 @@
       <c r="C82" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D82" t="s">
-        <v>5</v>
+      <c r="D82" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A83">
+      <c r="A83" s="6">
         <v>20116</v>
       </c>
       <c r="B83" t="s">
@@ -2475,12 +2478,12 @@
       <c r="C83" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D83" t="s">
-        <v>5</v>
+      <c r="D83" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A84">
+      <c r="A84" s="6">
         <v>20117</v>
       </c>
       <c r="B84" t="s">
@@ -2489,12 +2492,12 @@
       <c r="C84" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D84" t="s">
+      <c r="D84" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85">
+      <c r="A85" s="6">
         <v>20118</v>
       </c>
       <c r="B85" t="s">
@@ -2503,12 +2506,12 @@
       <c r="C85" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D85" t="s">
+      <c r="D85" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A86">
+      <c r="A86" s="6">
         <v>20120</v>
       </c>
       <c r="B86" t="s">
@@ -2517,12 +2520,12 @@
       <c r="C86" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D86" t="s">
-        <v>5</v>
+      <c r="D86" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A87">
+      <c r="A87" s="6">
         <v>20121</v>
       </c>
       <c r="B87" t="s">
@@ -2531,12 +2534,12 @@
       <c r="C87" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D87" t="s">
+      <c r="D87" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A88">
+      <c r="A88" s="6">
         <v>20125</v>
       </c>
       <c r="B88" t="s">
@@ -2545,12 +2548,12 @@
       <c r="C88" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D88" t="s">
-        <v>5</v>
+      <c r="D88" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A89">
+      <c r="A89" s="6">
         <v>20127</v>
       </c>
       <c r="B89" t="s">
@@ -2559,12 +2562,12 @@
       <c r="C89" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D89" t="s">
-        <v>5</v>
+      <c r="D89" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A90">
+      <c r="A90" s="6">
         <v>20128</v>
       </c>
       <c r="B90" t="s">
@@ -2573,12 +2576,12 @@
       <c r="C90" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D90" t="s">
-        <v>5</v>
+      <c r="D90" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A91">
+      <c r="A91" s="6">
         <v>20137</v>
       </c>
       <c r="B91" t="s">
@@ -2587,12 +2590,12 @@
       <c r="C91" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D91" t="s">
-        <v>8</v>
+      <c r="D91" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A92">
+      <c r="A92" s="6">
         <v>20138</v>
       </c>
       <c r="B92" t="s">
@@ -2601,12 +2604,12 @@
       <c r="C92" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D92" t="s">
+      <c r="D92" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A93">
+      <c r="A93" s="6">
         <v>20140</v>
       </c>
       <c r="B93" t="s">
@@ -2615,12 +2618,12 @@
       <c r="C93" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D93" t="s">
+      <c r="D93" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="94" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A94">
+      <c r="A94" s="6">
         <v>20142</v>
       </c>
       <c r="B94" t="s">
@@ -2629,12 +2632,12 @@
       <c r="C94" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D94" t="s">
+      <c r="D94" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A95">
+      <c r="A95" s="6">
         <v>20146</v>
       </c>
       <c r="B95" t="s">
@@ -2643,12 +2646,12 @@
       <c r="C95" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D95" t="s">
-        <v>5</v>
+      <c r="D95" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A96">
+      <c r="A96" s="6">
         <v>20148</v>
       </c>
       <c r="B96" t="s">
@@ -2657,12 +2660,12 @@
       <c r="C96" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D96" t="s">
+      <c r="D96" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A97">
+      <c r="A97" s="6">
         <v>20156</v>
       </c>
       <c r="B97" t="s">
@@ -2671,12 +2674,12 @@
       <c r="C97" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D97" t="s">
-        <v>5</v>
+      <c r="D97" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="98" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A98">
+      <c r="A98" s="6">
         <v>20159</v>
       </c>
       <c r="B98" t="s">
@@ -2686,11 +2689,11 @@
         <v>4</v>
       </c>
       <c r="D98" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A99">
+      <c r="A99" s="6">
         <v>20160</v>
       </c>
       <c r="B99" t="s">
@@ -2699,12 +2702,12 @@
       <c r="C99" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D99" t="s">
-        <v>5</v>
+      <c r="D99" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A100">
+      <c r="A100" s="6">
         <v>20163</v>
       </c>
       <c r="B100" t="s">
@@ -2713,12 +2716,12 @@
       <c r="C100" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D100" t="s">
-        <v>5</v>
+      <c r="D100" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="101" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A101">
+      <c r="A101" s="6">
         <v>20164</v>
       </c>
       <c r="B101" t="s">
@@ -2728,11 +2731,11 @@
         <v>4</v>
       </c>
       <c r="D101" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="102" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A102">
+      <c r="A102" s="6">
         <v>20165</v>
       </c>
       <c r="B102" t="s">
@@ -2741,12 +2744,12 @@
       <c r="C102" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D102" t="s">
+      <c r="D102" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="103" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A103">
+      <c r="A103" s="6">
         <v>20166</v>
       </c>
       <c r="B103" t="s">
@@ -2755,12 +2758,12 @@
       <c r="C103" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D103" t="s">
+      <c r="D103" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="104" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A104">
+      <c r="A104" s="6">
         <v>20169</v>
       </c>
       <c r="B104" t="s">
@@ -2769,12 +2772,12 @@
       <c r="C104" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D104" t="s">
-        <v>5</v>
+      <c r="D104" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="105" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A105">
+      <c r="A105" s="6">
         <v>20173</v>
       </c>
       <c r="B105" t="s">
@@ -2783,12 +2786,12 @@
       <c r="C105" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D105" t="s">
-        <v>5</v>
+      <c r="D105" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="106" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A106">
+      <c r="A106" s="6">
         <v>20174</v>
       </c>
       <c r="B106" t="s">
@@ -2797,12 +2800,12 @@
       <c r="C106" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D106" t="s">
+      <c r="D106" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="107" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A107">
+      <c r="A107" s="6">
         <v>20178</v>
       </c>
       <c r="B107" t="s">
@@ -2811,12 +2814,12 @@
       <c r="C107" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D107" t="s">
+      <c r="D107" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="108" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A108">
+      <c r="A108" s="6">
         <v>20179</v>
       </c>
       <c r="B108" t="s">
@@ -2826,11 +2829,11 @@
         <v>4</v>
       </c>
       <c r="D108" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="109" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A109">
+      <c r="A109" s="6">
         <v>20180</v>
       </c>
       <c r="B109" t="s">
@@ -2839,12 +2842,12 @@
       <c r="C109" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D109" t="s">
-        <v>5</v>
+      <c r="D109" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="110" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A110">
+      <c r="A110" s="6">
         <v>20200</v>
       </c>
       <c r="B110" t="s">
@@ -2853,12 +2856,12 @@
       <c r="C110" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D110" t="s">
+      <c r="D110" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="111" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A111">
+      <c r="A111" s="6">
         <v>20201</v>
       </c>
       <c r="B111" t="s">
@@ -2867,12 +2870,12 @@
       <c r="C111" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D111" t="s">
+      <c r="D111" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="112" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A112">
+      <c r="A112" s="6">
         <v>20204</v>
       </c>
       <c r="B112" t="s">
@@ -2881,12 +2884,12 @@
       <c r="C112" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D112" t="s">
+      <c r="D112" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="113" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A113">
+      <c r="A113" s="6">
         <v>20205</v>
       </c>
       <c r="B113" t="s">
@@ -2895,12 +2898,12 @@
       <c r="C113" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D113" t="s">
+      <c r="D113" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="114" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A114">
+      <c r="A114" s="6">
         <v>20211</v>
       </c>
       <c r="B114" t="s">
@@ -2909,12 +2912,12 @@
       <c r="C114" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D114" t="s">
+      <c r="D114" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="115" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A115">
+      <c r="A115" s="6">
         <v>20224</v>
       </c>
       <c r="B115" t="s">
@@ -2923,12 +2926,12 @@
       <c r="C115" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D115" t="s">
-        <v>5</v>
+      <c r="D115" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="116" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A116">
+      <c r="A116" s="6">
         <v>20227</v>
       </c>
       <c r="B116" t="s">
@@ -2937,12 +2940,12 @@
       <c r="C116" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D116" t="s">
+      <c r="D116" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="117" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A117">
+      <c r="A117" s="6">
         <v>20228</v>
       </c>
       <c r="B117" t="s">
@@ -2951,12 +2954,12 @@
       <c r="C117" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D117" t="s">
-        <v>8</v>
+      <c r="D117" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="118" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A118">
+      <c r="A118" s="6">
         <v>20230</v>
       </c>
       <c r="B118" t="s">
@@ -2965,12 +2968,12 @@
       <c r="C118" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D118" t="s">
+      <c r="D118" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="119" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A119">
+      <c r="A119" s="6">
         <v>20234</v>
       </c>
       <c r="B119" t="s">
@@ -2979,12 +2982,12 @@
       <c r="C119" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D119" t="s">
-        <v>8</v>
+      <c r="D119" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="120" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A120">
+      <c r="A120" s="6">
         <v>20236</v>
       </c>
       <c r="B120" t="s">
@@ -2993,12 +2996,12 @@
       <c r="C120" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D120" t="s">
-        <v>8</v>
+      <c r="D120" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="121" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A121">
+      <c r="A121" s="6">
         <v>20238</v>
       </c>
       <c r="B121" t="s">
@@ -3007,12 +3010,12 @@
       <c r="C121" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D121" t="s">
-        <v>8</v>
+      <c r="D121" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="122" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A122">
+      <c r="A122" s="6">
         <v>20241</v>
       </c>
       <c r="B122" t="s">
@@ -3021,12 +3024,12 @@
       <c r="C122" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D122" t="s">
+      <c r="D122" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="123" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A123">
+      <c r="A123" s="6">
         <v>20242</v>
       </c>
       <c r="B123" t="s">
@@ -3035,12 +3038,12 @@
       <c r="C123" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D123" t="s">
-        <v>5</v>
+      <c r="D123" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="124" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A124">
+      <c r="A124" s="6">
         <v>20244</v>
       </c>
       <c r="B124" t="s">
@@ -3049,12 +3052,12 @@
       <c r="C124" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D124" t="s">
-        <v>5</v>
+      <c r="D124" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="125" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A125">
+      <c r="A125" s="6">
         <v>20246</v>
       </c>
       <c r="B125" t="s">
@@ -3063,12 +3066,12 @@
       <c r="C125" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D125" t="s">
-        <v>8</v>
+      <c r="D125" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="126" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A126">
+      <c r="A126" s="6">
         <v>20249</v>
       </c>
       <c r="B126" t="s">
@@ -3077,12 +3080,12 @@
       <c r="C126" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D126" t="s">
-        <v>5</v>
+      <c r="D126" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="127" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A127">
+      <c r="A127" s="6">
         <v>20256</v>
       </c>
       <c r="B127" t="s">
@@ -3091,12 +3094,12 @@
       <c r="C127" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D127" t="s">
-        <v>5</v>
+      <c r="D127" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="128" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A128">
+      <c r="A128" s="6">
         <v>20257</v>
       </c>
       <c r="B128" t="s">
@@ -3106,11 +3109,11 @@
         <v>4</v>
       </c>
       <c r="D128" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="129" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A129">
+      <c r="A129" s="6">
         <v>20258</v>
       </c>
       <c r="B129" t="s">
@@ -3119,12 +3122,12 @@
       <c r="C129" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D129" t="s">
+      <c r="D129" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="130" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A130">
+      <c r="A130" s="6">
         <v>20260</v>
       </c>
       <c r="B130" t="s">
@@ -3133,12 +3136,12 @@
       <c r="C130" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D130" t="s">
+      <c r="D130" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="131" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A131">
+      <c r="A131" s="6">
         <v>20261</v>
       </c>
       <c r="B131" t="s">
@@ -3147,12 +3150,12 @@
       <c r="C131" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D131" t="s">
+      <c r="D131" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="132" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A132">
+      <c r="A132" s="6">
         <v>20262</v>
       </c>
       <c r="B132" t="s">
@@ -3161,12 +3164,12 @@
       <c r="C132" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D132" t="s">
+      <c r="D132" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="133" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A133">
+      <c r="A133" s="6">
         <v>20268</v>
       </c>
       <c r="B133" t="s">
@@ -3175,12 +3178,12 @@
       <c r="C133" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D133" t="s">
+      <c r="D133" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="134" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A134">
+      <c r="A134" s="6">
         <v>20271</v>
       </c>
       <c r="B134" t="s">
@@ -3189,12 +3192,12 @@
       <c r="C134" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D134" t="s">
-        <v>8</v>
+      <c r="D134" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="135" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A135">
+      <c r="A135" s="6">
         <v>20272</v>
       </c>
       <c r="B135" t="s">
@@ -3203,12 +3206,12 @@
       <c r="C135" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D135" t="s">
-        <v>5</v>
+      <c r="D135" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="136" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A136">
+      <c r="A136" s="6">
         <v>20275</v>
       </c>
       <c r="B136" t="s">
@@ -3217,12 +3220,12 @@
       <c r="C136" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D136" t="s">
+      <c r="D136" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="137" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A137">
+      <c r="A137" s="6">
         <v>20277</v>
       </c>
       <c r="B137" t="s">
@@ -3231,12 +3234,12 @@
       <c r="C137" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D137" t="s">
+      <c r="D137" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="138" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A138">
+      <c r="A138" s="6">
         <v>20281</v>
       </c>
       <c r="B138" t="s">
@@ -3245,12 +3248,12 @@
       <c r="C138" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D138" t="s">
-        <v>8</v>
+      <c r="D138" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="139" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A139">
+      <c r="A139" s="6">
         <v>20282</v>
       </c>
       <c r="B139" t="s">
@@ -3259,12 +3262,12 @@
       <c r="C139" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D139" t="s">
+      <c r="D139" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="140" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A140">
+      <c r="A140" s="6">
         <v>20284</v>
       </c>
       <c r="B140" t="s">
@@ -3274,11 +3277,11 @@
         <v>4</v>
       </c>
       <c r="D140" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="141" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A141">
+      <c r="A141" s="6">
         <v>20285</v>
       </c>
       <c r="B141" t="s">
@@ -3287,12 +3290,12 @@
       <c r="C141" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D141" t="s">
-        <v>5</v>
+      <c r="D141" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="142" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A142">
+      <c r="A142" s="6">
         <v>20289</v>
       </c>
       <c r="B142" t="s">
@@ -3301,12 +3304,12 @@
       <c r="C142" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D142" t="s">
+      <c r="D142" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="143" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A143">
+      <c r="A143" s="6">
         <v>20290</v>
       </c>
       <c r="B143" t="s">
@@ -3315,12 +3318,12 @@
       <c r="C143" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D143" t="s">
+      <c r="D143" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="144" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A144">
+      <c r="A144" s="6">
         <v>20291</v>
       </c>
       <c r="B144" t="s">
@@ -3329,12 +3332,12 @@
       <c r="C144" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D144" t="s">
+      <c r="D144" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="145" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A145">
+      <c r="A145" s="6">
         <v>20292</v>
       </c>
       <c r="B145" t="s">
@@ -3343,12 +3346,12 @@
       <c r="C145" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D145" t="s">
-        <v>8</v>
+      <c r="D145" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="146" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A146">
+      <c r="A146" s="6">
         <v>20293</v>
       </c>
       <c r="B146" t="s">
@@ -3357,12 +3360,12 @@
       <c r="C146" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D146" t="s">
-        <v>8</v>
+      <c r="D146" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="147" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A147">
+      <c r="A147" s="6">
         <v>20294</v>
       </c>
       <c r="B147" t="s">
@@ -3371,12 +3374,12 @@
       <c r="C147" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D147" t="s">
+      <c r="D147" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="148" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A148">
+      <c r="A148" s="6">
         <v>20296</v>
       </c>
       <c r="B148" t="s">
@@ -3385,12 +3388,12 @@
       <c r="C148" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D148" t="s">
-        <v>8</v>
+      <c r="D148" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="149" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A149">
+      <c r="A149" s="6">
         <v>20298</v>
       </c>
       <c r="B149" t="s">
@@ -3399,12 +3402,12 @@
       <c r="C149" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D149" t="s">
-        <v>5</v>
+      <c r="D149" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="150" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A150">
+      <c r="A150" s="6">
         <v>20299</v>
       </c>
       <c r="B150" t="s">
@@ -3413,12 +3416,12 @@
       <c r="C150" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D150" t="s">
+      <c r="D150" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="151" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A151">
+      <c r="A151" s="6">
         <v>20301</v>
       </c>
       <c r="B151" t="s">
@@ -3427,12 +3430,12 @@
       <c r="C151" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D151" t="s">
+      <c r="D151" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="152" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A152">
+      <c r="A152" s="6">
         <v>20303</v>
       </c>
       <c r="B152" t="s">
@@ -3441,12 +3444,12 @@
       <c r="C152" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D152" t="s">
+      <c r="D152" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="153" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A153">
+      <c r="A153" s="6">
         <v>20309</v>
       </c>
       <c r="B153" t="s">
@@ -3455,12 +3458,12 @@
       <c r="C153" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D153" t="s">
-        <v>8</v>
+      <c r="D153" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="154" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A154">
+      <c r="A154" s="6">
         <v>20310</v>
       </c>
       <c r="B154" t="s">
@@ -3469,12 +3472,12 @@
       <c r="C154" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D154" t="s">
-        <v>8</v>
+      <c r="D154" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="155" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A155">
+      <c r="A155" s="6">
         <v>20318</v>
       </c>
       <c r="B155" t="s">
@@ -3483,12 +3486,12 @@
       <c r="C155" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D155" t="s">
-        <v>5</v>
+      <c r="D155" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="156" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A156">
+      <c r="A156" s="6">
         <v>20319</v>
       </c>
       <c r="B156" t="s">
@@ -3497,12 +3500,12 @@
       <c r="C156" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D156" t="s">
+      <c r="D156" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="157" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A157">
+      <c r="A157" s="6">
         <v>20320</v>
       </c>
       <c r="B157" t="s">
@@ -3511,12 +3514,12 @@
       <c r="C157" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D157" t="s">
+      <c r="D157" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="158" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A158">
+      <c r="A158" s="6">
         <v>20324</v>
       </c>
       <c r="B158" t="s">
@@ -3525,12 +3528,12 @@
       <c r="C158" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D158" t="s">
+      <c r="D158" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="159" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A159">
+      <c r="A159" s="6">
         <v>20331</v>
       </c>
       <c r="B159" t="s">
@@ -3539,12 +3542,12 @@
       <c r="C159" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D159" t="s">
+      <c r="D159" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="160" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A160">
+      <c r="A160" s="6">
         <v>20333</v>
       </c>
       <c r="B160" t="s">
@@ -3553,12 +3556,12 @@
       <c r="C160" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D160" t="s">
-        <v>8</v>
+      <c r="D160" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="161" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A161">
+      <c r="A161" s="6">
         <v>20337</v>
       </c>
       <c r="B161" t="s">
@@ -3567,12 +3570,12 @@
       <c r="C161" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D161" t="s">
+      <c r="D161" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="162" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A162">
+      <c r="A162" s="6">
         <v>20343</v>
       </c>
       <c r="B162" t="s">
@@ -3581,12 +3584,12 @@
       <c r="C162" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D162" t="s">
+      <c r="D162" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="163" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A163">
+      <c r="A163" s="6">
         <v>20344</v>
       </c>
       <c r="B163" t="s">
@@ -3595,12 +3598,12 @@
       <c r="C163" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D163" t="s">
+      <c r="D163" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="164" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A164">
+      <c r="A164" s="6">
         <v>20351</v>
       </c>
       <c r="B164" t="s">
@@ -3609,12 +3612,12 @@
       <c r="C164" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D164" t="s">
-        <v>8</v>
+      <c r="D164" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="165" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A165">
+      <c r="A165" s="6">
         <v>20357</v>
       </c>
       <c r="B165" t="s">
@@ -3623,12 +3626,12 @@
       <c r="C165" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D165" t="s">
+      <c r="D165" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="166" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A166">
+      <c r="A166" s="6">
         <v>20361</v>
       </c>
       <c r="B166" t="s">
@@ -3637,12 +3640,12 @@
       <c r="C166" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D166" t="s">
+      <c r="D166" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="167" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A167">
+      <c r="A167" s="6">
         <v>20362</v>
       </c>
       <c r="B167" t="s">
@@ -3651,12 +3654,12 @@
       <c r="C167" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D167" t="s">
+      <c r="D167" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="168" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A168">
+      <c r="A168" s="6">
         <v>20363</v>
       </c>
       <c r="B168" t="s">
@@ -3665,12 +3668,12 @@
       <c r="C168" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D168" t="s">
-        <v>5</v>
+      <c r="D168" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="169" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A169">
+      <c r="A169" s="6">
         <v>20364</v>
       </c>
       <c r="B169" t="s">
@@ -3679,12 +3682,12 @@
       <c r="C169" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D169" t="s">
-        <v>8</v>
+      <c r="D169" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="170" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A170">
+      <c r="A170" s="6">
         <v>20366</v>
       </c>
       <c r="B170" t="s">
@@ -3693,12 +3696,12 @@
       <c r="C170" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D170" t="s">
+      <c r="D170" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="171" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A171">
+      <c r="A171" s="6">
         <v>20367</v>
       </c>
       <c r="B171" t="s">
@@ -3707,12 +3710,12 @@
       <c r="C171" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D171" t="s">
+      <c r="D171" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="172" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A172">
+      <c r="A172" s="6">
         <v>20369</v>
       </c>
       <c r="B172" t="s">
@@ -3721,12 +3724,12 @@
       <c r="C172" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D172" t="s">
+      <c r="D172" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="173" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A173">
+      <c r="A173" s="6">
         <v>20371</v>
       </c>
       <c r="B173" t="s">
@@ -3735,12 +3738,12 @@
       <c r="C173" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D173" t="s">
-        <v>5</v>
+      <c r="D173" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="174" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A174">
+      <c r="A174" s="6">
         <v>20372</v>
       </c>
       <c r="B174" t="s">
@@ -3749,12 +3752,12 @@
       <c r="C174" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D174" t="s">
+      <c r="D174" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="175" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A175">
+      <c r="A175" s="6">
         <v>20374</v>
       </c>
       <c r="B175" t="s">
@@ -3763,12 +3766,12 @@
       <c r="C175" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D175" t="s">
+      <c r="D175" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="176" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A176">
+      <c r="A176" s="6">
         <v>20377</v>
       </c>
       <c r="B176" t="s">
@@ -3777,12 +3780,12 @@
       <c r="C176" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D176" t="s">
-        <v>5</v>
+      <c r="D176" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="177" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A177">
+      <c r="A177" s="6">
         <v>20379</v>
       </c>
       <c r="B177" t="s">
@@ -3791,12 +3794,12 @@
       <c r="C177" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D177" t="s">
+      <c r="D177" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="178" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A178">
+      <c r="A178" s="6">
         <v>20380</v>
       </c>
       <c r="B178" t="s">
@@ -3805,12 +3808,12 @@
       <c r="C178" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D178" t="s">
+      <c r="D178" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="179" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A179">
+      <c r="A179" s="6">
         <v>20381</v>
       </c>
       <c r="B179" t="s">
@@ -3819,12 +3822,12 @@
       <c r="C179" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D179" t="s">
+      <c r="D179" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="180" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A180">
+      <c r="A180" s="6">
         <v>20384</v>
       </c>
       <c r="B180" t="s">
@@ -3833,12 +3836,12 @@
       <c r="C180" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D180" t="s">
-        <v>5</v>
+      <c r="D180" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="181" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A181">
+      <c r="A181" s="6">
         <v>20385</v>
       </c>
       <c r="B181" t="s">
@@ -3847,12 +3850,12 @@
       <c r="C181" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D181" t="s">
+      <c r="D181" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="182" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A182">
+      <c r="A182" s="6">
         <v>20386</v>
       </c>
       <c r="B182" t="s">
@@ -3861,12 +3864,12 @@
       <c r="C182" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D182" t="s">
-        <v>5</v>
+      <c r="D182" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="183" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A183">
+      <c r="A183" s="6">
         <v>20388</v>
       </c>
       <c r="B183" t="s">
@@ -3875,12 +3878,12 @@
       <c r="C183" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D183" t="s">
+      <c r="D183" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="184" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A184">
+      <c r="A184" s="6">
         <v>20391</v>
       </c>
       <c r="B184" t="s">
@@ -3889,12 +3892,12 @@
       <c r="C184" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D184" t="s">
+      <c r="D184" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="185" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A185">
+      <c r="A185" s="6">
         <v>20394</v>
       </c>
       <c r="B185" t="s">
@@ -3903,12 +3906,12 @@
       <c r="C185" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D185" t="s">
+      <c r="D185" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="186" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A186">
+      <c r="A186" s="6">
         <v>20395</v>
       </c>
       <c r="B186" t="s">
@@ -3917,12 +3920,12 @@
       <c r="C186" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D186" t="s">
+      <c r="D186" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="187" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A187">
+      <c r="A187" s="6">
         <v>30101</v>
       </c>
       <c r="B187" t="s">
@@ -3931,12 +3934,12 @@
       <c r="C187" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D187" t="s">
-        <v>5</v>
+      <c r="D187" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="188" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A188">
+      <c r="A188" s="6">
         <v>40124</v>
       </c>
       <c r="B188" t="s">
@@ -3945,12 +3948,12 @@
       <c r="C188" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D188" t="s">
-        <v>9</v>
+      <c r="D188" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="189" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A189">
+      <c r="A189" s="6">
         <v>40125</v>
       </c>
       <c r="B189" t="s">
@@ -3959,12 +3962,12 @@
       <c r="C189" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D189" t="s">
-        <v>8</v>
+      <c r="D189" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="190" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A190">
+      <c r="A190" s="6">
         <v>40127</v>
       </c>
       <c r="B190" t="s">
@@ -3973,12 +3976,12 @@
       <c r="C190" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D190" t="s">
-        <v>5</v>
+      <c r="D190" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="191" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A191">
+      <c r="A191" s="6">
         <v>40129</v>
       </c>
       <c r="B191" t="s">
@@ -3987,12 +3990,12 @@
       <c r="C191" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D191" t="s">
+      <c r="D191" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="192" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A192">
+      <c r="A192" s="6">
         <v>40137</v>
       </c>
       <c r="B192" t="s">
@@ -4001,12 +4004,12 @@
       <c r="C192" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D192" t="s">
+      <c r="D192" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="193" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A193">
+      <c r="A193" s="6">
         <v>40140</v>
       </c>
       <c r="B193" t="s">
@@ -4015,12 +4018,12 @@
       <c r="C193" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D193" t="s">
+      <c r="D193" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="194" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A194">
+      <c r="A194" s="6">
         <v>40141</v>
       </c>
       <c r="B194" t="s">
@@ -4029,12 +4032,12 @@
       <c r="C194" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D194" t="s">
+      <c r="D194" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="195" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A195">
+      <c r="A195" s="6">
         <v>40143</v>
       </c>
       <c r="B195" t="s">
@@ -4043,12 +4046,12 @@
       <c r="C195" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D195" t="s">
+      <c r="D195" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="196" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A196">
+      <c r="A196" s="6">
         <v>40144</v>
       </c>
       <c r="B196" t="s">
@@ -4057,12 +4060,12 @@
       <c r="C196" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D196" t="s">
-        <v>8</v>
+      <c r="D196" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="197" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A197">
+      <c r="A197" s="6">
         <v>40145</v>
       </c>
       <c r="B197" t="s">
@@ -4071,12 +4074,12 @@
       <c r="C197" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D197" t="s">
+      <c r="D197" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="198" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A198">
+      <c r="A198" s="6">
         <v>40150</v>
       </c>
       <c r="B198" t="s">
@@ -4085,12 +4088,12 @@
       <c r="C198" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D198" t="s">
-        <v>5</v>
+      <c r="D198" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="199" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A199">
+      <c r="A199" s="6">
         <v>40151</v>
       </c>
       <c r="B199" t="s">
@@ -4099,12 +4102,12 @@
       <c r="C199" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D199" t="s">
+      <c r="D199" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="200" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A200">
+      <c r="A200" s="6">
         <v>50102</v>
       </c>
       <c r="B200" t="s">
@@ -4113,12 +4116,12 @@
       <c r="C200" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D200" t="s">
-        <v>8</v>
+      <c r="D200" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="201" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A201">
+      <c r="A201" s="6">
         <v>50222</v>
       </c>
       <c r="B201" t="s">
@@ -4127,12 +4130,12 @@
       <c r="C201" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D201" t="s">
-        <v>5</v>
+      <c r="D201" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="202" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A202">
+      <c r="A202" s="6">
         <v>50223</v>
       </c>
       <c r="B202" t="s">
@@ -4141,12 +4144,12 @@
       <c r="C202" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D202" t="s">
+      <c r="D202" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="203" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A203">
+      <c r="A203" s="6">
         <v>50224</v>
       </c>
       <c r="B203" t="s">
@@ -4155,12 +4158,12 @@
       <c r="C203" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D203" t="s">
+      <c r="D203" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="204" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A204">
+      <c r="A204" s="6">
         <v>50444</v>
       </c>
       <c r="B204" t="s">
@@ -4169,12 +4172,12 @@
       <c r="C204" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D204" t="s">
+      <c r="D204" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="205" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A205">
+      <c r="A205" s="6">
         <v>50607</v>
       </c>
       <c r="B205" t="s">
@@ -4183,12 +4186,12 @@
       <c r="C205" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D205" t="s">
-        <v>8</v>
+      <c r="D205" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="206" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A206">
+      <c r="A206" s="6">
         <v>50608</v>
       </c>
       <c r="B206" t="s">
@@ -4197,12 +4200,12 @@
       <c r="C206" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D206" t="s">
-        <v>5</v>
+      <c r="D206" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="207" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A207">
+      <c r="A207" s="6">
         <v>50622</v>
       </c>
       <c r="B207" t="s">
@@ -4211,12 +4214,12 @@
       <c r="C207" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D207" t="s">
+      <c r="D207" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="208" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A208">
+      <c r="A208" s="6">
         <v>50623</v>
       </c>
       <c r="B208" t="s">
@@ -4225,12 +4228,12 @@
       <c r="C208" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D208" t="s">
+      <c r="D208" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="209" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A209">
+      <c r="A209" s="6">
         <v>50625</v>
       </c>
       <c r="B209" t="s">
@@ -4239,12 +4242,12 @@
       <c r="C209" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D209" t="s">
+      <c r="D209" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="210" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A210">
+      <c r="A210" s="6">
         <v>50629</v>
       </c>
       <c r="B210" t="s">
@@ -4253,12 +4256,12 @@
       <c r="C210" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D210" t="s">
+      <c r="D210" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="211" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A211">
+      <c r="A211" s="6">
         <v>50803</v>
       </c>
       <c r="B211" t="s">
@@ -4267,12 +4270,12 @@
       <c r="C211" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D211" t="s">
+      <c r="D211" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="212" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A212">
+      <c r="A212" s="6">
         <v>50805</v>
       </c>
       <c r="B212" t="s">
@@ -4281,12 +4284,12 @@
       <c r="C212" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D212" t="s">
+      <c r="D212" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="213" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A213">
+      <c r="A213" s="6">
         <v>50806</v>
       </c>
       <c r="B213" t="s">
@@ -4295,12 +4298,12 @@
       <c r="C213" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D213" t="s">
+      <c r="D213" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="214" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A214">
+      <c r="A214" s="6">
         <v>50808</v>
       </c>
       <c r="B214" t="s">
@@ -4309,12 +4312,12 @@
       <c r="C214" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D214" t="s">
-        <v>8</v>
+      <c r="D214" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="215" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A215">
+      <c r="A215" s="6">
         <v>50809</v>
       </c>
       <c r="B215" t="s">
@@ -4323,12 +4326,12 @@
       <c r="C215" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D215" t="s">
-        <v>8</v>
+      <c r="D215" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="216" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A216">
+      <c r="A216" s="6">
         <v>50810</v>
       </c>
       <c r="B216" t="s">
@@ -4337,12 +4340,12 @@
       <c r="C216" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D216" t="s">
-        <v>5</v>
+      <c r="D216" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="217" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A217">
+      <c r="A217" s="6">
         <v>50812</v>
       </c>
       <c r="B217" t="s">
@@ -4351,12 +4354,12 @@
       <c r="C217" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D217" t="s">
+      <c r="D217" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="218" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A218">
+      <c r="A218" s="6">
         <v>50813</v>
       </c>
       <c r="B218" t="s">
@@ -4366,11 +4369,11 @@
         <v>4</v>
       </c>
       <c r="D218" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="219" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A219">
+      <c r="A219" s="6">
         <v>50815</v>
       </c>
       <c r="B219" t="s">
@@ -4379,12 +4382,12 @@
       <c r="C219" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D219" t="s">
+      <c r="D219" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="220" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A220">
+      <c r="A220" s="6">
         <v>50816</v>
       </c>
       <c r="B220" t="s">
@@ -4393,12 +4396,12 @@
       <c r="C220" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D220" t="s">
+      <c r="D220" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="221" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A221">
+      <c r="A221" s="6">
         <v>50818</v>
       </c>
       <c r="B221" t="s">
@@ -4407,12 +4410,12 @@
       <c r="C221" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D221" t="s">
+      <c r="D221" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="222" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A222">
+      <c r="A222" s="6">
         <v>50819</v>
       </c>
       <c r="B222" t="s">
@@ -4421,12 +4424,12 @@
       <c r="C222" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D222" t="s">
+      <c r="D222" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="223" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A223">
+      <c r="A223" s="6">
         <v>50820</v>
       </c>
       <c r="B223" t="s">
@@ -4435,12 +4438,12 @@
       <c r="C223" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D223" t="s">
+      <c r="D223" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="224" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A224">
+      <c r="A224" s="6">
         <v>50821</v>
       </c>
       <c r="B224" t="s">
@@ -4449,12 +4452,12 @@
       <c r="C224" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D224" t="s">
+      <c r="D224" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="225" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A225">
+      <c r="A225" s="6">
         <v>50823</v>
       </c>
       <c r="B225" t="s">
@@ -4464,11 +4467,11 @@
         <v>4</v>
       </c>
       <c r="D225" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="226" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A226">
+      <c r="A226" s="6">
         <v>50824</v>
       </c>
       <c r="B226" t="s">
@@ -4477,12 +4480,12 @@
       <c r="C226" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D226" t="s">
-        <v>8</v>
+      <c r="D226" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="227" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A227">
+      <c r="A227" s="6">
         <v>50825</v>
       </c>
       <c r="B227" t="s">
@@ -4491,12 +4494,12 @@
       <c r="C227" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D227" t="s">
+      <c r="D227" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="228" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A228">
+      <c r="A228" s="6">
         <v>50826</v>
       </c>
       <c r="B228" t="s">
@@ -4505,12 +4508,12 @@
       <c r="C228" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D228" t="s">
+      <c r="D228" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="229" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A229">
+      <c r="A229" s="6">
         <v>50827</v>
       </c>
       <c r="B229" t="s">
@@ -4519,12 +4522,12 @@
       <c r="C229" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D229" t="s">
+      <c r="D229" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="230" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A230">
+      <c r="A230" s="6">
         <v>50829</v>
       </c>
       <c r="B230" t="s">
@@ -4533,12 +4536,12 @@
       <c r="C230" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D230" t="s">
+      <c r="D230" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="231" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A231">
+      <c r="A231" s="6">
         <v>60103</v>
       </c>
       <c r="B231" t="s">
@@ -4547,12 +4550,12 @@
       <c r="C231" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D231" t="s">
+      <c r="D231" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="232" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A232">
+      <c r="A232" s="6">
         <v>60124</v>
       </c>
       <c r="B232" t="s">
@@ -4561,12 +4564,12 @@
       <c r="C232" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D232" t="s">
-        <v>8</v>
+      <c r="D232" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="233" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A233">
+      <c r="A233" s="6">
         <v>60125</v>
       </c>
       <c r="B233" t="s">
@@ -4575,12 +4578,12 @@
       <c r="C233" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D233" t="s">
-        <v>8</v>
+      <c r="D233" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="234" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A234">
+      <c r="A234" s="6">
         <v>60126</v>
       </c>
       <c r="B234" t="s">
@@ -4589,12 +4592,12 @@
       <c r="C234" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D234" t="s">
-        <v>5</v>
+      <c r="D234" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="235" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A235">
+      <c r="A235" s="6">
         <v>60128</v>
       </c>
       <c r="B235" t="s">
@@ -4603,12 +4606,12 @@
       <c r="C235" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D235" t="s">
-        <v>8</v>
+      <c r="D235" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="236" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A236">
+      <c r="A236" s="6">
         <v>60130</v>
       </c>
       <c r="B236" t="s">
@@ -4617,12 +4620,12 @@
       <c r="C236" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D236" t="s">
+      <c r="D236" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="237" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A237">
+      <c r="A237" s="6">
         <v>60133</v>
       </c>
       <c r="B237" t="s">
@@ -4631,12 +4634,12 @@
       <c r="C237" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D237" t="s">
+      <c r="D237" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="238" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A238">
+      <c r="A238" s="6">
         <v>60134</v>
       </c>
       <c r="B238" t="s">
@@ -4645,12 +4648,12 @@
       <c r="C238" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D238" t="s">
+      <c r="D238" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="239" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A239">
+      <c r="A239" s="6">
         <v>60137</v>
       </c>
       <c r="B239" t="s">
@@ -4659,12 +4662,12 @@
       <c r="C239" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D239" t="s">
+      <c r="D239" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="240" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A240">
+      <c r="A240" s="6">
         <v>60139</v>
       </c>
       <c r="B240" t="s">
@@ -4673,12 +4676,12 @@
       <c r="C240" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D240" t="s">
-        <v>5</v>
+      <c r="D240" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="241" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A241">
+      <c r="A241" s="6">
         <v>60142</v>
       </c>
       <c r="B241" t="s">
@@ -4687,12 +4690,12 @@
       <c r="C241" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D241" t="s">
-        <v>5</v>
+      <c r="D241" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="242" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A242">
+      <c r="A242" s="6">
         <v>60148</v>
       </c>
       <c r="B242" t="s">
@@ -4701,12 +4704,12 @@
       <c r="C242" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D242" t="s">
+      <c r="D242" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="243" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A243">
+      <c r="A243" s="6">
         <v>60149</v>
       </c>
       <c r="B243" t="s">
@@ -4715,12 +4718,12 @@
       <c r="C243" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D243" t="s">
+      <c r="D243" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="244" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A244">
+      <c r="A244" s="6">
         <v>60158</v>
       </c>
       <c r="B244" t="s">
@@ -4729,12 +4732,12 @@
       <c r="C244" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D244" t="s">
-        <v>5</v>
+      <c r="D244" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="245" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A245">
+      <c r="A245" s="6">
         <v>60159</v>
       </c>
       <c r="B245" t="s">
@@ -4743,12 +4746,12 @@
       <c r="C245" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D245" t="s">
+      <c r="D245" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="246" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A246">
+      <c r="A246" s="6">
         <v>60162</v>
       </c>
       <c r="B246" t="s">
@@ -4757,12 +4760,12 @@
       <c r="C246" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D246" t="s">
-        <v>8</v>
+      <c r="D246" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="247" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A247">
+      <c r="A247" s="6">
         <v>60163</v>
       </c>
       <c r="B247" t="s">
@@ -4771,12 +4774,12 @@
       <c r="C247" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D247" t="s">
+      <c r="D247" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="248" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A248">
+      <c r="A248" s="6">
         <v>60165</v>
       </c>
       <c r="B248" t="s">
@@ -4785,12 +4788,12 @@
       <c r="C248" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D248" t="s">
+      <c r="D248" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="249" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A249">
+      <c r="A249" s="6">
         <v>60169</v>
       </c>
       <c r="B249" t="s">
@@ -4799,12 +4802,12 @@
       <c r="C249" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D249" t="s">
+      <c r="D249" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="250" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A250">
+      <c r="A250" s="6">
         <v>60172</v>
       </c>
       <c r="B250" t="s">
@@ -4813,12 +4816,12 @@
       <c r="C250" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D250" t="s">
+      <c r="D250" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="251" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A251">
+      <c r="A251" s="6">
         <v>60174</v>
       </c>
       <c r="B251" t="s">
@@ -4827,12 +4830,12 @@
       <c r="C251" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D251" t="s">
-        <v>8</v>
+      <c r="D251" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="252" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A252">
+      <c r="A252" s="6">
         <v>60176</v>
       </c>
       <c r="B252" t="s">
@@ -4841,12 +4844,12 @@
       <c r="C252" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D252" t="s">
-        <v>8</v>
+      <c r="D252" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="253" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A253">
+      <c r="A253" s="6">
         <v>60178</v>
       </c>
       <c r="B253" t="s">
@@ -4855,12 +4858,12 @@
       <c r="C253" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D253" t="s">
-        <v>5</v>
+      <c r="D253" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="254" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A254">
+      <c r="A254" s="6">
         <v>60180</v>
       </c>
       <c r="B254" t="s">
@@ -4869,12 +4872,12 @@
       <c r="C254" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D254" t="s">
+      <c r="D254" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="255" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A255">
+      <c r="A255" s="6">
         <v>60184</v>
       </c>
       <c r="B255" t="s">
@@ -4883,12 +4886,12 @@
       <c r="C255" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D255" t="s">
+      <c r="D255" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="256" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A256">
+      <c r="A256" s="6">
         <v>60190</v>
       </c>
       <c r="B256" t="s">
@@ -4897,12 +4900,12 @@
       <c r="C256" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D256" t="s">
+      <c r="D256" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="257" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A257">
+      <c r="A257" s="6">
         <v>60191</v>
       </c>
       <c r="B257" t="s">
@@ -4911,12 +4914,12 @@
       <c r="C257" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D257" t="s">
+      <c r="D257" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="258" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A258">
+      <c r="A258" s="6">
         <v>60192</v>
       </c>
       <c r="B258" t="s">
@@ -4925,12 +4928,12 @@
       <c r="C258" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D258" t="s">
+      <c r="D258" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="259" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A259">
+      <c r="A259" s="6">
         <v>60195</v>
       </c>
       <c r="B259" t="s">
@@ -4939,12 +4942,12 @@
       <c r="C259" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D259" t="s">
+      <c r="D259" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="260" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A260">
+      <c r="A260" s="6">
         <v>60196</v>
       </c>
       <c r="B260" t="s">
@@ -4953,12 +4956,12 @@
       <c r="C260" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D260" t="s">
-        <v>5</v>
+      <c r="D260" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="261" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A261">
+      <c r="A261" s="6">
         <v>60198</v>
       </c>
       <c r="B261" t="s">
@@ -4967,12 +4970,12 @@
       <c r="C261" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D261" t="s">
+      <c r="D261" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="262" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A262">
+      <c r="A262" s="6">
         <v>60200</v>
       </c>
       <c r="B262" t="s">
@@ -4981,12 +4984,12 @@
       <c r="C262" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D262" t="s">
+      <c r="D262" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="263" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A263">
+      <c r="A263" s="6">
         <v>60201</v>
       </c>
       <c r="B263" t="s">
@@ -4996,11 +4999,11 @@
         <v>4</v>
       </c>
       <c r="D263" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="264" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A264">
+      <c r="A264" s="6">
         <v>60202</v>
       </c>
       <c r="B264" t="s">
@@ -5009,12 +5012,12 @@
       <c r="C264" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D264" t="s">
-        <v>8</v>
+      <c r="D264" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="265" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A265">
+      <c r="A265" s="6">
         <v>60204</v>
       </c>
       <c r="B265" t="s">
@@ -5023,12 +5026,12 @@
       <c r="C265" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D265" t="s">
-        <v>5</v>
+      <c r="D265" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="266" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A266">
+      <c r="A266" s="6">
         <v>60205</v>
       </c>
       <c r="B266" t="s">
@@ -5037,12 +5040,12 @@
       <c r="C266" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D266" t="s">
+      <c r="D266" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="267" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A267">
+      <c r="A267" s="6">
         <v>60206</v>
       </c>
       <c r="B267" t="s">
@@ -5051,12 +5054,12 @@
       <c r="C267" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D267" t="s">
-        <v>5</v>
+      <c r="D267" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="268" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A268">
+      <c r="A268" s="6">
         <v>60209</v>
       </c>
       <c r="B268" t="s">
@@ -5065,12 +5068,12 @@
       <c r="C268" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D268" t="s">
+      <c r="D268" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="269" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A269">
+      <c r="A269" s="6">
         <v>60211</v>
       </c>
       <c r="B269" t="s">
@@ -5079,12 +5082,12 @@
       <c r="C269" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D269" t="s">
+      <c r="D269" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="270" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A270">
+      <c r="A270" s="6">
         <v>60215</v>
       </c>
       <c r="B270" t="s">
@@ -5093,12 +5096,12 @@
       <c r="C270" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D270" t="s">
+      <c r="D270" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="271" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A271">
+      <c r="A271" s="6">
         <v>60217</v>
       </c>
       <c r="B271" t="s">
@@ -5107,12 +5110,12 @@
       <c r="C271" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D271" t="s">
-        <v>5</v>
+      <c r="D271" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="272" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A272">
+      <c r="A272" s="6">
         <v>60219</v>
       </c>
       <c r="B272" t="s">
@@ -5121,12 +5124,12 @@
       <c r="C272" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D272" t="s">
+      <c r="D272" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="273" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A273">
+      <c r="A273" s="6">
         <v>60222</v>
       </c>
       <c r="B273" t="s">
@@ -5135,12 +5138,12 @@
       <c r="C273" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D273" t="s">
+      <c r="D273" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="274" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A274">
+      <c r="A274" s="6">
         <v>60225</v>
       </c>
       <c r="B274" t="s">
@@ -5150,11 +5153,11 @@
         <v>4</v>
       </c>
       <c r="D274" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="275" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A275">
+      <c r="A275" s="6">
         <v>60230</v>
       </c>
       <c r="B275" t="s">
@@ -5163,12 +5166,12 @@
       <c r="C275" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D275" t="s">
+      <c r="D275" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="276" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A276">
+      <c r="A276" s="6">
         <v>60234</v>
       </c>
       <c r="B276" t="s">
@@ -5177,12 +5180,12 @@
       <c r="C276" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D276" t="s">
+      <c r="D276" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="277" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A277">
+      <c r="A277" s="6">
         <v>60253</v>
       </c>
       <c r="B277" t="s">
@@ -5191,12 +5194,12 @@
       <c r="C277" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D277" t="s">
-        <v>5</v>
+      <c r="D277" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="278" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A278">
+      <c r="A278" s="6">
         <v>60254</v>
       </c>
       <c r="B278" t="s">
@@ -5205,12 +5208,12 @@
       <c r="C278" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D278" t="s">
+      <c r="D278" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="279" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A279">
+      <c r="A279" s="6">
         <v>60257</v>
       </c>
       <c r="B279" t="s">
@@ -5219,12 +5222,12 @@
       <c r="C279" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D279" t="s">
-        <v>5</v>
+      <c r="D279" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="280" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A280">
+      <c r="A280" s="6">
         <v>60258</v>
       </c>
       <c r="B280" t="s">
@@ -5233,12 +5236,12 @@
       <c r="C280" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D280" t="s">
+      <c r="D280" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="281" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A281">
+      <c r="A281" s="6">
         <v>60269</v>
       </c>
       <c r="B281" t="s">
@@ -5247,12 +5250,12 @@
       <c r="C281" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D281" t="s">
-        <v>5</v>
+      <c r="D281" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="282" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A282">
+      <c r="A282" s="6">
         <v>60270</v>
       </c>
       <c r="B282" t="s">
@@ -5261,12 +5264,12 @@
       <c r="C282" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D282" t="s">
+      <c r="D282" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="283" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A283">
+      <c r="A283" s="6">
         <v>60272</v>
       </c>
       <c r="B283" t="s">
@@ -5275,12 +5278,12 @@
       <c r="C283" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D283" t="s">
+      <c r="D283" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="284" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A284">
+      <c r="A284" s="6">
         <v>60275</v>
       </c>
       <c r="B284" t="s">
@@ -5289,12 +5292,12 @@
       <c r="C284" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D284" t="s">
-        <v>5</v>
+      <c r="D284" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="285" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A285">
+      <c r="A285" s="6">
         <v>60276</v>
       </c>
       <c r="B285" t="s">
@@ -5303,12 +5306,12 @@
       <c r="C285" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D285" t="s">
-        <v>5</v>
+      <c r="D285" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="286" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A286">
+      <c r="A286" s="6">
         <v>60278</v>
       </c>
       <c r="B286" t="s">
@@ -5317,12 +5320,12 @@
       <c r="C286" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D286" t="s">
-        <v>8</v>
+      <c r="D286" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="287" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A287">
+      <c r="A287" s="6">
         <v>60279</v>
       </c>
       <c r="B287" t="s">
@@ -5331,12 +5334,12 @@
       <c r="C287" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D287" t="s">
+      <c r="D287" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="288" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A288">
+      <c r="A288" s="6">
         <v>60280</v>
       </c>
       <c r="B288" t="s">
@@ -5345,12 +5348,12 @@
       <c r="C288" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D288" t="s">
+      <c r="D288" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="289" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A289">
+      <c r="A289" s="6">
         <v>61004</v>
       </c>
       <c r="B289" t="s">
@@ -5359,12 +5362,12 @@
       <c r="C289" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D289" t="s">
-        <v>8</v>
+      <c r="D289" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="290" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A290">
+      <c r="A290" s="6">
         <v>61009</v>
       </c>
       <c r="B290" t="s">
@@ -5373,12 +5376,12 @@
       <c r="C290" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D290" t="s">
-        <v>5</v>
+      <c r="D290" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="291" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A291">
+      <c r="A291" s="6">
         <v>61012</v>
       </c>
       <c r="B291" t="s">
@@ -5387,12 +5390,12 @@
       <c r="C291" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D291" t="s">
+      <c r="D291" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="292" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A292">
+      <c r="A292" s="6">
         <v>61018</v>
       </c>
       <c r="B292" t="s">
@@ -5401,12 +5404,12 @@
       <c r="C292" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D292" t="s">
+      <c r="D292" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="293" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A293">
+      <c r="A293" s="6">
         <v>61102</v>
       </c>
       <c r="B293" t="s">
@@ -5415,12 +5418,12 @@
       <c r="C293" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D293" t="s">
+      <c r="D293" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="294" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A294">
+      <c r="A294" s="6">
         <v>61205</v>
       </c>
       <c r="B294" t="s">
@@ -5429,12 +5432,12 @@
       <c r="C294" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D294" t="s">
+      <c r="D294" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="295" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A295">
+      <c r="A295" s="6">
         <v>70100</v>
       </c>
       <c r="B295" t="s">
@@ -5443,12 +5446,12 @@
       <c r="C295" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D295" t="s">
+      <c r="D295" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="296" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A296">
+      <c r="A296" s="6">
         <v>70101</v>
       </c>
       <c r="B296" t="s">
@@ -5457,12 +5460,12 @@
       <c r="C296" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D296" t="s">
-        <v>8</v>
+      <c r="D296" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="297" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A297">
+      <c r="A297" s="6">
         <v>70102</v>
       </c>
       <c r="B297" t="s">
@@ -5471,12 +5474,12 @@
       <c r="C297" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D297" t="s">
-        <v>8</v>
+      <c r="D297" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="298" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A298">
+      <c r="A298" s="6">
         <v>70103</v>
       </c>
       <c r="B298" t="s">
@@ -5485,12 +5488,12 @@
       <c r="C298" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D298" t="s">
+      <c r="D298" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="299" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A299">
+      <c r="A299" s="6">
         <v>70106</v>
       </c>
       <c r="B299" t="s">
@@ -5499,12 +5502,12 @@
       <c r="C299" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D299" t="s">
+      <c r="D299" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="300" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A300">
+      <c r="A300" s="6">
         <v>70109</v>
       </c>
       <c r="B300" t="s">
@@ -5513,12 +5516,12 @@
       <c r="C300" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D300" t="s">
-        <v>5</v>
+      <c r="D300" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="301" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A301">
+      <c r="A301" s="6">
         <v>70113</v>
       </c>
       <c r="B301" t="s">
@@ -5527,12 +5530,12 @@
       <c r="C301" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D301" t="s">
-        <v>8</v>
+      <c r="D301" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="302" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A302">
+      <c r="A302" s="6">
         <v>70638</v>
       </c>
       <c r="B302" t="s">
@@ -5541,12 +5544,12 @@
       <c r="C302" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D302" t="s">
+      <c r="D302" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="303" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A303">
+      <c r="A303" s="6">
         <v>70639</v>
       </c>
       <c r="B303" t="s">
@@ -5555,12 +5558,12 @@
       <c r="C303" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D303" t="s">
+      <c r="D303" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="304" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A304">
+      <c r="A304" s="6">
         <v>70640</v>
       </c>
       <c r="B304" t="s">
@@ -5569,12 +5572,12 @@
       <c r="C304" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D304" t="s">
+      <c r="D304" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="305" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A305">
+      <c r="A305" s="6">
         <v>70642</v>
       </c>
       <c r="B305" t="s">
@@ -5583,12 +5586,12 @@
       <c r="C305" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D305" t="s">
+      <c r="D305" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="306" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A306">
+      <c r="A306" s="6">
         <v>90504</v>
       </c>
       <c r="B306" t="s">
@@ -5597,12 +5600,12 @@
       <c r="C306" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D306" t="s">
-        <v>5</v>
+      <c r="D306" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="307" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A307">
+      <c r="A307" s="6">
         <v>90509</v>
       </c>
       <c r="B307" t="s">
@@ -5611,12 +5614,12 @@
       <c r="C307" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D307" t="s">
+      <c r="D307" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="308" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A308">
+      <c r="A308" s="6">
         <v>90602</v>
       </c>
       <c r="B308" t="s">
@@ -5625,12 +5628,12 @@
       <c r="C308" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D308" t="s">
-        <v>8</v>
+      <c r="D308" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="309" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A309">
+      <c r="A309" s="6">
         <v>90621</v>
       </c>
       <c r="B309" t="s">
@@ -5639,12 +5642,12 @@
       <c r="C309" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D309" t="s">
+      <c r="D309" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="310" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A310">
+      <c r="A310" s="6">
         <v>90658</v>
       </c>
       <c r="B310" t="s">
@@ -5653,12 +5656,12 @@
       <c r="C310" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D310" t="s">
+      <c r="D310" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="311" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A311">
+      <c r="A311" s="6">
         <v>90660</v>
       </c>
       <c r="B311" t="s">
@@ -5667,12 +5670,12 @@
       <c r="C311" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D311" t="s">
-        <v>5</v>
+      <c r="D311" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="312" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A312">
+      <c r="A312" s="6">
         <v>90668</v>
       </c>
       <c r="B312" t="s">
@@ -5681,12 +5684,12 @@
       <c r="C312" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D312" t="s">
+      <c r="D312" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="313" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A313">
+      <c r="A313" s="6">
         <v>90671</v>
       </c>
       <c r="B313" t="s">
@@ -5695,12 +5698,12 @@
       <c r="C313" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D313" t="s">
+      <c r="D313" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="314" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A314">
+      <c r="A314" s="6">
         <v>90679</v>
       </c>
       <c r="B314" t="s">
@@ -5709,12 +5712,12 @@
       <c r="C314" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D314" t="s">
-        <v>5</v>
+      <c r="D314" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="315" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A315">
+      <c r="A315" s="6">
         <v>90683</v>
       </c>
       <c r="B315" t="s">
@@ -5723,12 +5726,12 @@
       <c r="C315" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D315" t="s">
-        <v>5</v>
+      <c r="D315" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="316" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A316">
+      <c r="A316" s="6">
         <v>90705</v>
       </c>
       <c r="B316" t="s">
@@ -5737,12 +5740,12 @@
       <c r="C316" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D316" t="s">
+      <c r="D316" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="317" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A317">
+      <c r="A317" s="6">
         <v>90706</v>
       </c>
       <c r="B317" t="s">
@@ -5751,12 +5754,12 @@
       <c r="C317" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D317" t="s">
+      <c r="D317" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="318" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A318">
+      <c r="A318" s="6">
         <v>90708</v>
       </c>
       <c r="B318" t="s">
@@ -5765,12 +5768,12 @@
       <c r="C318" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D318" t="s">
-        <v>5</v>
+      <c r="D318" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="319" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A319">
+      <c r="A319" s="6">
         <v>90709</v>
       </c>
       <c r="B319" t="s">
@@ -5779,8 +5782,8 @@
       <c r="C319" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D319" t="s">
-        <v>5</v>
+      <c r="D319" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -5789,6 +5792,6 @@
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
agregue cliente consumidor final
</commit_message>
<xml_diff>
--- a/excel/CLIENTES_PERMISOS.xlsx
+++ b/excel/CLIENTES_PERMISOS.xlsx
@@ -15,14 +15,14 @@
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Hoja 1'!$A$1:$D$319</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Hoja 1'!$A$1:$D$320</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="958" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="961" uniqueCount="327">
   <si>
     <t>CUENTA</t>
   </si>
@@ -1000,6 +1000,9 @@
   </si>
   <si>
     <t>OMAR OLIVERA</t>
+  </si>
+  <si>
+    <t>CONSUMIDOR FINAL</t>
   </si>
 </sst>
 </file>
@@ -1307,10 +1310,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D319"/>
+  <dimension ref="A1:D320"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1335,25 +1338,25 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4">
-        <v>5</v>
+      <c r="A2" s="1">
+        <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>162</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="5">
-        <v>11</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>4</v>
@@ -1364,10 +1367,10 @@
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
-        <v>12</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>211</v>
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>69</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>4</v>
@@ -1378,24 +1381,24 @@
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
+        <v>12</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="5">
         <v>20</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B6" s="2" t="s">
         <v>203</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="6">
-        <v>27</v>
-      </c>
-      <c r="B6" t="s">
-        <v>142</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>4</v>
@@ -1406,10 +1409,10 @@
     </row>
     <row r="7" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>142</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>4</v>
@@ -1420,10 +1423,10 @@
     </row>
     <row r="8" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
-        <v>233</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>4</v>
@@ -1434,10 +1437,10 @@
     </row>
     <row r="9" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="B9" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>4</v>
@@ -1448,10 +1451,10 @@
     </row>
     <row r="10" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
-        <v>246</v>
+        <v>237</v>
       </c>
       <c r="B10" t="s">
-        <v>157</v>
+        <v>62</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>4</v>
@@ -1462,10 +1465,10 @@
     </row>
     <row r="11" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>157</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>4</v>
@@ -1476,10 +1479,10 @@
     </row>
     <row r="12" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
-        <v>265</v>
+        <v>251</v>
       </c>
       <c r="B12" t="s">
-        <v>212</v>
+        <v>25</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>4</v>
@@ -1490,10 +1493,10 @@
     </row>
     <row r="13" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
-        <v>308</v>
+        <v>265</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>212</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>4</v>
@@ -1504,10 +1507,10 @@
     </row>
     <row r="14" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
-        <v>920</v>
+        <v>308</v>
       </c>
       <c r="B14" t="s">
-        <v>195</v>
+        <v>27</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>4</v>
@@ -1518,10 +1521,10 @@
     </row>
     <row r="15" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
-        <v>936</v>
+        <v>920</v>
       </c>
       <c r="B15" t="s">
-        <v>86</v>
+        <v>195</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>4</v>
@@ -1532,38 +1535,38 @@
     </row>
     <row r="16" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6">
-        <v>938</v>
+        <v>936</v>
       </c>
       <c r="B16" t="s">
-        <v>185</v>
+        <v>86</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>5</v>
+      <c r="D16" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="B17" t="s">
-        <v>41</v>
+        <v>185</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>8</v>
+      <c r="D17" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="B18" t="s">
-        <v>128</v>
+        <v>41</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>4</v>
@@ -1574,38 +1577,38 @@
     </row>
     <row r="19" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6">
-        <v>946</v>
+        <v>940</v>
       </c>
       <c r="B19" t="s">
-        <v>7</v>
+        <v>128</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D19" t="s">
-        <v>9</v>
+      <c r="D19" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="6">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="B20" t="s">
-        <v>200</v>
+        <v>7</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>8</v>
+      <c r="D20" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6">
-        <v>949</v>
+        <v>947</v>
       </c>
       <c r="B21" t="s">
-        <v>10</v>
+        <v>200</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>4</v>
@@ -1616,10 +1619,10 @@
     </row>
     <row r="22" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="6">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="B22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>4</v>
@@ -1630,10 +1633,10 @@
     </row>
     <row r="23" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="6">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="B23" t="s">
-        <v>147</v>
+        <v>11</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>4</v>
@@ -1644,38 +1647,38 @@
     </row>
     <row r="24" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="6">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="B24" t="s">
-        <v>64</v>
+        <v>147</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D24" t="s">
-        <v>9</v>
+      <c r="D24" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="6">
-        <v>954</v>
+        <v>952</v>
       </c>
       <c r="B25" t="s">
-        <v>129</v>
+        <v>64</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>8</v>
+      <c r="D25" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="6">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="B26" t="s">
-        <v>102</v>
+        <v>129</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>4</v>
@@ -1686,10 +1689,10 @@
     </row>
     <row r="27" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="6">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="B27" t="s">
-        <v>158</v>
+        <v>102</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>4</v>
@@ -1700,38 +1703,38 @@
     </row>
     <row r="28" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="6">
-        <v>958</v>
+        <v>956</v>
       </c>
       <c r="B28" t="s">
-        <v>6</v>
+        <v>158</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D28" s="3" t="s">
-        <v>5</v>
+      <c r="D28" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="6">
-        <v>961</v>
+        <v>958</v>
       </c>
       <c r="B29" t="s">
-        <v>55</v>
+        <v>6</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D29" s="1" t="s">
-        <v>8</v>
+      <c r="D29" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="6">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="B30" t="s">
-        <v>140</v>
+        <v>55</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>4</v>
@@ -1742,24 +1745,24 @@
     </row>
     <row r="31" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="6">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="B31" t="s">
-        <v>21</v>
+        <v>140</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D31" s="3" t="s">
-        <v>5</v>
+      <c r="D31" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="6">
-        <v>965</v>
+        <v>963</v>
       </c>
       <c r="B32" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>4</v>
@@ -1770,66 +1773,66 @@
     </row>
     <row r="33" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="6">
-        <v>969</v>
+        <v>965</v>
       </c>
       <c r="B33" t="s">
-        <v>87</v>
+        <v>30</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D33" s="1" t="s">
-        <v>8</v>
+      <c r="D33" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="6">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="B34" t="s">
-        <v>226</v>
+        <v>87</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D34" t="s">
-        <v>9</v>
+      <c r="D34" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="6">
-        <v>972</v>
+        <v>970</v>
       </c>
       <c r="B35" t="s">
-        <v>174</v>
+        <v>226</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D35" s="3" t="s">
-        <v>5</v>
+      <c r="D35" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="6">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="B36" t="s">
-        <v>137</v>
+        <v>174</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D36" s="1" t="s">
-        <v>8</v>
+      <c r="D36" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="6">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="B37" t="s">
-        <v>172</v>
+        <v>137</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>4</v>
@@ -1840,10 +1843,10 @@
     </row>
     <row r="38" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="6">
-        <v>980</v>
+        <v>974</v>
       </c>
       <c r="B38" t="s">
-        <v>133</v>
+        <v>172</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>4</v>
@@ -1854,24 +1857,24 @@
     </row>
     <row r="39" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="6">
-        <v>982</v>
+        <v>980</v>
       </c>
       <c r="B39" t="s">
-        <v>197</v>
+        <v>133</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D39" s="3" t="s">
-        <v>5</v>
+      <c r="D39" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="6">
-        <v>987</v>
+        <v>982</v>
       </c>
       <c r="B40" t="s">
-        <v>80</v>
+        <v>197</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>4</v>
@@ -1882,24 +1885,24 @@
     </row>
     <row r="41" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="6">
-        <v>989</v>
+        <v>987</v>
       </c>
       <c r="B41" t="s">
-        <v>191</v>
+        <v>80</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D41" s="1" t="s">
-        <v>8</v>
+      <c r="D41" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="6">
-        <v>992</v>
+        <v>989</v>
       </c>
       <c r="B42" t="s">
-        <v>66</v>
+        <v>191</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>4</v>
@@ -1910,10 +1913,10 @@
     </row>
     <row r="43" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="6">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="B43" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>4</v>
@@ -1924,10 +1927,10 @@
     </row>
     <row r="44" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="6">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="B44" t="s">
-        <v>97</v>
+        <v>78</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>4</v>
@@ -1938,10 +1941,10 @@
     </row>
     <row r="45" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="6">
-        <v>997</v>
+        <v>994</v>
       </c>
       <c r="B45" t="s">
-        <v>44</v>
+        <v>97</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>4</v>
@@ -1952,10 +1955,10 @@
     </row>
     <row r="46" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="6">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="B46" t="s">
-        <v>99</v>
+        <v>44</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>4</v>
@@ -1966,38 +1969,38 @@
     </row>
     <row r="47" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="6">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="B47" t="s">
-        <v>180</v>
+        <v>99</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D47" t="s">
-        <v>9</v>
+      <c r="D47" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="6">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="B48" t="s">
-        <v>222</v>
+        <v>180</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D48" s="1" t="s">
-        <v>8</v>
+      <c r="D48" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="6">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="B49" t="s">
-        <v>75</v>
+        <v>222</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>4</v>
@@ -2008,10 +2011,10 @@
     </row>
     <row r="50" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="6">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="B50" t="s">
-        <v>46</v>
+        <v>75</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>4</v>
@@ -2022,10 +2025,10 @@
     </row>
     <row r="51" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="6">
-        <v>1005</v>
+        <v>1002</v>
       </c>
       <c r="B51" t="s">
-        <v>182</v>
+        <v>46</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>4</v>
@@ -2036,38 +2039,38 @@
     </row>
     <row r="52" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="6">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="B52" t="s">
-        <v>115</v>
+        <v>182</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D52" s="3" t="s">
-        <v>5</v>
+      <c r="D52" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="6">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="B53" t="s">
-        <v>214</v>
+        <v>115</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D53" s="1" t="s">
-        <v>8</v>
+      <c r="D53" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="6">
-        <v>1009</v>
+        <v>1007</v>
       </c>
       <c r="B54" t="s">
-        <v>74</v>
+        <v>214</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>4</v>
@@ -2078,24 +2081,24 @@
     </row>
     <row r="55" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="6">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="B55" t="s">
-        <v>109</v>
+        <v>74</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D55" t="s">
-        <v>9</v>
+      <c r="D55" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="6">
-        <v>1012</v>
+        <v>1010</v>
       </c>
       <c r="B56" t="s">
-        <v>189</v>
+        <v>109</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>4</v>
@@ -2106,24 +2109,24 @@
     </row>
     <row r="57" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="6">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B57" t="s">
-        <v>152</v>
+        <v>189</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D57" s="1" t="s">
-        <v>8</v>
+      <c r="D57" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="6">
-        <v>1015</v>
+        <v>1013</v>
       </c>
       <c r="B58" t="s">
-        <v>35</v>
+        <v>152</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>4</v>
@@ -2134,10 +2137,10 @@
     </row>
     <row r="59" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="6">
-        <v>1416</v>
+        <v>1015</v>
       </c>
       <c r="B59" t="s">
-        <v>217</v>
+        <v>35</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>4</v>
@@ -2148,38 +2151,38 @@
     </row>
     <row r="60" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="6">
-        <v>10107</v>
+        <v>1416</v>
       </c>
       <c r="B60" t="s">
-        <v>96</v>
+        <v>217</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D60" t="s">
-        <v>9</v>
+      <c r="D60" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="6">
-        <v>10137</v>
+        <v>10107</v>
       </c>
       <c r="B61" t="s">
-        <v>123</v>
+        <v>96</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D61" s="1" t="s">
-        <v>8</v>
+      <c r="D61" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="6">
-        <v>10157</v>
+        <v>10137</v>
       </c>
       <c r="B62" t="s">
-        <v>183</v>
+        <v>123</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>4</v>
@@ -2190,10 +2193,10 @@
     </row>
     <row r="63" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="6">
-        <v>10158</v>
+        <v>10157</v>
       </c>
       <c r="B63" t="s">
-        <v>65</v>
+        <v>183</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>4</v>
@@ -2204,94 +2207,94 @@
     </row>
     <row r="64" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="6">
-        <v>10160</v>
+        <v>10158</v>
       </c>
       <c r="B64" t="s">
-        <v>125</v>
+        <v>65</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D64" s="3" t="s">
-        <v>5</v>
+      <c r="D64" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="6">
-        <v>10162</v>
+        <v>10160</v>
       </c>
       <c r="B65" t="s">
-        <v>108</v>
+        <v>125</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D65" s="1" t="s">
-        <v>8</v>
+      <c r="D65" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="6">
-        <v>10163</v>
+        <v>10162</v>
       </c>
       <c r="B66" t="s">
-        <v>90</v>
+        <v>108</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D66" s="3" t="s">
-        <v>5</v>
+      <c r="D66" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="6">
-        <v>10165</v>
+        <v>10163</v>
       </c>
       <c r="B67" t="s">
-        <v>19</v>
+        <v>90</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D67" s="1" t="s">
-        <v>8</v>
+      <c r="D67" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="6">
-        <v>10167</v>
+        <v>10165</v>
       </c>
       <c r="B68" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D68" s="3" t="s">
-        <v>5</v>
+      <c r="D68" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="6">
-        <v>10424</v>
+        <v>10167</v>
       </c>
       <c r="B69" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D69" t="s">
-        <v>9</v>
+      <c r="D69" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="6">
-        <v>10425</v>
+        <v>10424</v>
       </c>
       <c r="B70" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>4</v>
@@ -2302,24 +2305,24 @@
     </row>
     <row r="71" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="6">
-        <v>20094</v>
+        <v>10425</v>
       </c>
       <c r="B71" t="s">
-        <v>198</v>
+        <v>15</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D71" s="1" t="s">
-        <v>8</v>
+      <c r="D71" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="6">
-        <v>20095</v>
+        <v>20094</v>
       </c>
       <c r="B72" t="s">
-        <v>153</v>
+        <v>198</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>4</v>
@@ -2330,10 +2333,10 @@
     </row>
     <row r="73" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="6">
-        <v>20096</v>
+        <v>20095</v>
       </c>
       <c r="B73" t="s">
-        <v>122</v>
+        <v>153</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>4</v>
@@ -2344,10 +2347,10 @@
     </row>
     <row r="74" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="6">
-        <v>20100</v>
+        <v>20096</v>
       </c>
       <c r="B74" t="s">
-        <v>84</v>
+        <v>122</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>4</v>
@@ -2358,10 +2361,10 @@
     </row>
     <row r="75" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="6">
-        <v>20101</v>
+        <v>20100</v>
       </c>
       <c r="B75" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>4</v>
@@ -2372,10 +2375,10 @@
     </row>
     <row r="76" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="6">
-        <v>20103</v>
+        <v>20101</v>
       </c>
       <c r="B76" t="s">
-        <v>81</v>
+        <v>40</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>4</v>
@@ -2386,10 +2389,10 @@
     </row>
     <row r="77" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="6">
-        <v>20106</v>
+        <v>20103</v>
       </c>
       <c r="B77" t="s">
-        <v>155</v>
+        <v>81</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>4</v>
@@ -2400,10 +2403,10 @@
     </row>
     <row r="78" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="6">
-        <v>20108</v>
+        <v>20106</v>
       </c>
       <c r="B78" t="s">
-        <v>219</v>
+        <v>155</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>4</v>
@@ -2414,10 +2417,10 @@
     </row>
     <row r="79" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="6">
-        <v>20109</v>
+        <v>20108</v>
       </c>
       <c r="B79" t="s">
-        <v>53</v>
+        <v>219</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>4</v>
@@ -2428,38 +2431,38 @@
     </row>
     <row r="80" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="6">
-        <v>20110</v>
+        <v>20109</v>
       </c>
       <c r="B80" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D80" s="3" t="s">
-        <v>5</v>
+      <c r="D80" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="6">
-        <v>20113</v>
+        <v>20110</v>
       </c>
       <c r="B81" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D81" s="1" t="s">
-        <v>8</v>
+      <c r="D81" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="6">
-        <v>20114</v>
+        <v>20113</v>
       </c>
       <c r="B82" t="s">
-        <v>126</v>
+        <v>93</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>4</v>
@@ -2470,10 +2473,10 @@
     </row>
     <row r="83" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="6">
-        <v>20116</v>
+        <v>20114</v>
       </c>
       <c r="B83" t="s">
-        <v>73</v>
+        <v>126</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>4</v>
@@ -2484,10 +2487,10 @@
     </row>
     <row r="84" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="6">
-        <v>20117</v>
+        <v>20116</v>
       </c>
       <c r="B84" t="s">
-        <v>186</v>
+        <v>73</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>4</v>
@@ -2498,10 +2501,10 @@
     </row>
     <row r="85" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="6">
-        <v>20118</v>
+        <v>20117</v>
       </c>
       <c r="B85" t="s">
-        <v>160</v>
+        <v>186</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>4</v>
@@ -2512,10 +2515,10 @@
     </row>
     <row r="86" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="6">
-        <v>20120</v>
+        <v>20118</v>
       </c>
       <c r="B86" t="s">
-        <v>176</v>
+        <v>160</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>4</v>
@@ -2526,10 +2529,10 @@
     </row>
     <row r="87" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="6">
-        <v>20121</v>
+        <v>20120</v>
       </c>
       <c r="B87" t="s">
-        <v>159</v>
+        <v>176</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>4</v>
@@ -2540,10 +2543,10 @@
     </row>
     <row r="88" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="6">
-        <v>20125</v>
+        <v>20121</v>
       </c>
       <c r="B88" t="s">
-        <v>88</v>
+        <v>159</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>4</v>
@@ -2554,10 +2557,10 @@
     </row>
     <row r="89" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="6">
-        <v>20127</v>
+        <v>20125</v>
       </c>
       <c r="B89" t="s">
-        <v>168</v>
+        <v>88</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>4</v>
@@ -2568,10 +2571,10 @@
     </row>
     <row r="90" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="6">
-        <v>20128</v>
+        <v>20127</v>
       </c>
       <c r="B90" t="s">
-        <v>208</v>
+        <v>168</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>4</v>
@@ -2582,24 +2585,24 @@
     </row>
     <row r="91" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="6">
-        <v>20137</v>
+        <v>20128</v>
       </c>
       <c r="B91" t="s">
-        <v>79</v>
+        <v>208</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D91" s="3" t="s">
-        <v>5</v>
+      <c r="D91" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="6">
-        <v>20138</v>
+        <v>20137</v>
       </c>
       <c r="B92" t="s">
-        <v>113</v>
+        <v>79</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>4</v>
@@ -2610,10 +2613,10 @@
     </row>
     <row r="93" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="6">
-        <v>20140</v>
+        <v>20138</v>
       </c>
       <c r="B93" t="s">
-        <v>218</v>
+        <v>113</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>4</v>
@@ -2624,24 +2627,24 @@
     </row>
     <row r="94" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="6">
-        <v>20142</v>
+        <v>20140</v>
       </c>
       <c r="B94" t="s">
-        <v>193</v>
+        <v>218</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D94" s="1" t="s">
-        <v>8</v>
+      <c r="D94" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="6">
-        <v>20146</v>
+        <v>20142</v>
       </c>
       <c r="B95" t="s">
-        <v>148</v>
+        <v>193</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>4</v>
@@ -2652,10 +2655,10 @@
     </row>
     <row r="96" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="6">
-        <v>20148</v>
+        <v>20146</v>
       </c>
       <c r="B96" t="s">
-        <v>38</v>
+        <v>148</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>4</v>
@@ -2666,10 +2669,10 @@
     </row>
     <row r="97" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="6">
-        <v>20156</v>
+        <v>20148</v>
       </c>
       <c r="B97" t="s">
-        <v>179</v>
+        <v>38</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>4</v>
@@ -2680,38 +2683,38 @@
     </row>
     <row r="98" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="6">
-        <v>20159</v>
+        <v>20156</v>
       </c>
       <c r="B98" t="s">
-        <v>120</v>
+        <v>179</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D98" t="s">
-        <v>9</v>
+      <c r="D98" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="6">
-        <v>20160</v>
+        <v>20159</v>
       </c>
       <c r="B99" t="s">
-        <v>224</v>
+        <v>120</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D99" s="1" t="s">
-        <v>8</v>
+      <c r="D99" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" s="6">
-        <v>20163</v>
+        <v>20160</v>
       </c>
       <c r="B100" t="s">
-        <v>23</v>
+        <v>224</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>4</v>
@@ -2722,38 +2725,38 @@
     </row>
     <row r="101" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="6">
-        <v>20164</v>
+        <v>20163</v>
       </c>
       <c r="B101" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D101" t="s">
-        <v>9</v>
+      <c r="D101" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="102" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" s="6">
-        <v>20165</v>
+        <v>20164</v>
       </c>
       <c r="B102" t="s">
-        <v>131</v>
+        <v>18</v>
       </c>
       <c r="C102" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D102" s="1" t="s">
-        <v>8</v>
+      <c r="D102" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="103" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="6">
-        <v>20166</v>
+        <v>20165</v>
       </c>
       <c r="B103" t="s">
-        <v>77</v>
+        <v>131</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>4</v>
@@ -2764,10 +2767,10 @@
     </row>
     <row r="104" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="6">
-        <v>20169</v>
+        <v>20166</v>
       </c>
       <c r="B104" t="s">
-        <v>151</v>
+        <v>77</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>4</v>
@@ -2778,10 +2781,10 @@
     </row>
     <row r="105" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" s="6">
-        <v>20173</v>
+        <v>20169</v>
       </c>
       <c r="B105" t="s">
-        <v>112</v>
+        <v>151</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>4</v>
@@ -2792,10 +2795,10 @@
     </row>
     <row r="106" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="6">
-        <v>20174</v>
+        <v>20173</v>
       </c>
       <c r="B106" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>4</v>
@@ -2806,10 +2809,10 @@
     </row>
     <row r="107" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="6">
-        <v>20178</v>
+        <v>20174</v>
       </c>
       <c r="B107" t="s">
-        <v>117</v>
+        <v>132</v>
       </c>
       <c r="C107" s="1" t="s">
         <v>4</v>
@@ -2820,52 +2823,52 @@
     </row>
     <row r="108" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="6">
-        <v>20179</v>
+        <v>20178</v>
       </c>
       <c r="B108" t="s">
-        <v>171</v>
+        <v>117</v>
       </c>
       <c r="C108" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D108" t="s">
-        <v>9</v>
+      <c r="D108" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="109" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A109" s="6">
-        <v>20180</v>
+        <v>20179</v>
       </c>
       <c r="B109" t="s">
-        <v>149</v>
+        <v>171</v>
       </c>
       <c r="C109" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D109" s="1" t="s">
-        <v>8</v>
+      <c r="D109" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="110" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" s="6">
-        <v>20200</v>
+        <v>20180</v>
       </c>
       <c r="B110" t="s">
-        <v>83</v>
+        <v>149</v>
       </c>
       <c r="C110" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D110" s="3" t="s">
-        <v>5</v>
+      <c r="D110" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="111" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="6">
-        <v>20201</v>
+        <v>20200</v>
       </c>
       <c r="B111" t="s">
-        <v>145</v>
+        <v>83</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>4</v>
@@ -2876,24 +2879,24 @@
     </row>
     <row r="112" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="6">
-        <v>20204</v>
+        <v>20201</v>
       </c>
       <c r="B112" t="s">
-        <v>57</v>
+        <v>145</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D112" s="1" t="s">
-        <v>8</v>
+      <c r="D112" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="113" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A113" s="6">
-        <v>20205</v>
+        <v>20204</v>
       </c>
       <c r="B113" t="s">
-        <v>206</v>
+        <v>57</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>4</v>
@@ -2904,10 +2907,10 @@
     </row>
     <row r="114" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A114" s="6">
-        <v>20211</v>
+        <v>20205</v>
       </c>
       <c r="B114" t="s">
-        <v>190</v>
+        <v>206</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>4</v>
@@ -2918,10 +2921,10 @@
     </row>
     <row r="115" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" s="6">
-        <v>20224</v>
+        <v>20211</v>
       </c>
       <c r="B115" t="s">
-        <v>85</v>
+        <v>190</v>
       </c>
       <c r="C115" s="1" t="s">
         <v>4</v>
@@ -2932,10 +2935,10 @@
     </row>
     <row r="116" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" s="6">
-        <v>20227</v>
+        <v>20224</v>
       </c>
       <c r="B116" t="s">
-        <v>192</v>
+        <v>85</v>
       </c>
       <c r="C116" s="1" t="s">
         <v>4</v>
@@ -2946,52 +2949,52 @@
     </row>
     <row r="117" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A117" s="6">
-        <v>20228</v>
+        <v>20227</v>
       </c>
       <c r="B117" t="s">
-        <v>91</v>
+        <v>192</v>
       </c>
       <c r="C117" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D117" s="3" t="s">
-        <v>5</v>
+      <c r="D117" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="118" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A118" s="6">
-        <v>20230</v>
+        <v>20228</v>
       </c>
       <c r="B118" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C118" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D118" s="1" t="s">
-        <v>8</v>
+      <c r="D118" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="119" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A119" s="6">
-        <v>20234</v>
+        <v>20230</v>
       </c>
       <c r="B119" t="s">
-        <v>29</v>
+        <v>89</v>
       </c>
       <c r="C119" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D119" s="3" t="s">
-        <v>5</v>
+      <c r="D119" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="120" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A120" s="6">
-        <v>20236</v>
+        <v>20234</v>
       </c>
       <c r="B120" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C120" s="1" t="s">
         <v>4</v>
@@ -3002,10 +3005,10 @@
     </row>
     <row r="121" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A121" s="6">
-        <v>20238</v>
+        <v>20236</v>
       </c>
       <c r="B121" t="s">
-        <v>139</v>
+        <v>31</v>
       </c>
       <c r="C121" s="1" t="s">
         <v>4</v>
@@ -3016,10 +3019,10 @@
     </row>
     <row r="122" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A122" s="6">
-        <v>20241</v>
+        <v>20238</v>
       </c>
       <c r="B122" t="s">
-        <v>22</v>
+        <v>139</v>
       </c>
       <c r="C122" s="1" t="s">
         <v>4</v>
@@ -3030,24 +3033,24 @@
     </row>
     <row r="123" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A123" s="6">
-        <v>20242</v>
+        <v>20241</v>
       </c>
       <c r="B123" t="s">
-        <v>216</v>
+        <v>22</v>
       </c>
       <c r="C123" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D123" s="1" t="s">
-        <v>8</v>
+      <c r="D123" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="124" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" s="6">
-        <v>20244</v>
+        <v>20242</v>
       </c>
       <c r="B124" t="s">
-        <v>124</v>
+        <v>216</v>
       </c>
       <c r="C124" s="1" t="s">
         <v>4</v>
@@ -3058,38 +3061,38 @@
     </row>
     <row r="125" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A125" s="6">
-        <v>20246</v>
+        <v>20244</v>
       </c>
       <c r="B125" t="s">
-        <v>14</v>
+        <v>124</v>
       </c>
       <c r="C125" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D125" s="3" t="s">
-        <v>5</v>
+      <c r="D125" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="126" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A126" s="6">
-        <v>20249</v>
+        <v>20246</v>
       </c>
       <c r="B126" t="s">
-        <v>72</v>
+        <v>14</v>
       </c>
       <c r="C126" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D126" s="1" t="s">
-        <v>8</v>
+      <c r="D126" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="127" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A127" s="6">
-        <v>20256</v>
+        <v>20249</v>
       </c>
       <c r="B127" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="C127" s="1" t="s">
         <v>4</v>
@@ -3100,66 +3103,66 @@
     </row>
     <row r="128" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A128" s="6">
-        <v>20257</v>
+        <v>20256</v>
       </c>
       <c r="B128" t="s">
-        <v>150</v>
+        <v>50</v>
       </c>
       <c r="C128" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D128" t="s">
-        <v>9</v>
+      <c r="D128" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="129" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A129" s="6">
-        <v>20258</v>
+        <v>20257</v>
       </c>
       <c r="B129" t="s">
-        <v>199</v>
+        <v>150</v>
       </c>
       <c r="C129" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D129" s="1" t="s">
-        <v>8</v>
+      <c r="D129" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="130" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A130" s="6">
-        <v>20260</v>
+        <v>20258</v>
       </c>
       <c r="B130" t="s">
-        <v>68</v>
+        <v>199</v>
       </c>
       <c r="C130" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D130" s="3" t="s">
-        <v>5</v>
+      <c r="D130" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="131" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A131" s="6">
-        <v>20261</v>
+        <v>20260</v>
       </c>
       <c r="B131" t="s">
-        <v>207</v>
+        <v>68</v>
       </c>
       <c r="C131" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D131" s="1" t="s">
-        <v>8</v>
+      <c r="D131" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="132" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A132" s="6">
-        <v>20262</v>
+        <v>20261</v>
       </c>
       <c r="B132" t="s">
-        <v>92</v>
+        <v>207</v>
       </c>
       <c r="C132" s="1" t="s">
         <v>4</v>
@@ -3170,10 +3173,10 @@
     </row>
     <row r="133" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A133" s="6">
-        <v>20268</v>
+        <v>20262</v>
       </c>
       <c r="B133" t="s">
-        <v>201</v>
+        <v>92</v>
       </c>
       <c r="C133" s="1" t="s">
         <v>4</v>
@@ -3184,150 +3187,150 @@
     </row>
     <row r="134" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A134" s="6">
-        <v>20271</v>
+        <v>20268</v>
       </c>
       <c r="B134" t="s">
-        <v>34</v>
+        <v>201</v>
       </c>
       <c r="C134" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D134" s="3" t="s">
-        <v>5</v>
+      <c r="D134" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="135" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A135" s="6">
-        <v>20272</v>
+        <v>20271</v>
       </c>
       <c r="B135" t="s">
-        <v>178</v>
+        <v>34</v>
       </c>
       <c r="C135" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D135" s="1" t="s">
-        <v>8</v>
+      <c r="D135" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="136" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A136" s="6">
-        <v>20275</v>
+        <v>20272</v>
       </c>
       <c r="B136" t="s">
-        <v>166</v>
+        <v>178</v>
       </c>
       <c r="C136" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D136" s="3" t="s">
-        <v>5</v>
+      <c r="D136" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="137" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A137" s="6">
-        <v>20277</v>
+        <v>20275</v>
       </c>
       <c r="B137" t="s">
-        <v>154</v>
+        <v>166</v>
       </c>
       <c r="C137" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D137" s="1" t="s">
-        <v>8</v>
+      <c r="D137" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="138" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A138" s="6">
-        <v>20281</v>
+        <v>20277</v>
       </c>
       <c r="B138" t="s">
-        <v>105</v>
+        <v>154</v>
       </c>
       <c r="C138" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D138" s="3" t="s">
-        <v>5</v>
+      <c r="D138" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="139" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A139" s="6">
-        <v>20282</v>
+        <v>20281</v>
       </c>
       <c r="B139" t="s">
-        <v>141</v>
+        <v>105</v>
       </c>
       <c r="C139" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D139" s="1" t="s">
-        <v>8</v>
+      <c r="D139" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="140" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A140" s="6">
-        <v>20284</v>
+        <v>20282</v>
       </c>
       <c r="B140" t="s">
-        <v>17</v>
+        <v>141</v>
       </c>
       <c r="C140" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D140" t="s">
-        <v>9</v>
+      <c r="D140" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="141" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A141" s="6">
-        <v>20285</v>
+        <v>20284</v>
       </c>
       <c r="B141" t="s">
-        <v>146</v>
+        <v>17</v>
       </c>
       <c r="C141" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D141" s="1" t="s">
-        <v>8</v>
+      <c r="D141" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="142" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A142" s="6">
-        <v>20289</v>
+        <v>20285</v>
       </c>
       <c r="B142" t="s">
-        <v>52</v>
+        <v>146</v>
       </c>
       <c r="C142" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D142" s="3" t="s">
-        <v>5</v>
+      <c r="D142" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="143" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A143" s="6">
-        <v>20290</v>
+        <v>20289</v>
       </c>
       <c r="B143" t="s">
-        <v>103</v>
+        <v>52</v>
       </c>
       <c r="C143" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D143" s="1" t="s">
-        <v>8</v>
+      <c r="D143" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="144" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A144" s="6">
-        <v>20291</v>
+        <v>20290</v>
       </c>
       <c r="B144" t="s">
-        <v>187</v>
+        <v>103</v>
       </c>
       <c r="C144" s="1" t="s">
         <v>4</v>
@@ -3338,24 +3341,24 @@
     </row>
     <row r="145" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A145" s="6">
-        <v>20292</v>
+        <v>20291</v>
       </c>
       <c r="B145" t="s">
-        <v>32</v>
+        <v>187</v>
       </c>
       <c r="C145" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D145" s="3" t="s">
-        <v>5</v>
+      <c r="D145" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="146" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A146" s="6">
-        <v>20293</v>
+        <v>20292</v>
       </c>
       <c r="B146" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="C146" s="1" t="s">
         <v>4</v>
@@ -3366,52 +3369,52 @@
     </row>
     <row r="147" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A147" s="6">
-        <v>20294</v>
+        <v>20293</v>
       </c>
       <c r="B147" t="s">
-        <v>202</v>
+        <v>43</v>
       </c>
       <c r="C147" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D147" s="1" t="s">
-        <v>8</v>
+      <c r="D147" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="148" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A148" s="6">
-        <v>20296</v>
+        <v>20294</v>
       </c>
       <c r="B148" t="s">
-        <v>144</v>
+        <v>202</v>
       </c>
       <c r="C148" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D148" s="3" t="s">
-        <v>5</v>
+      <c r="D148" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="149" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A149" s="6">
-        <v>20298</v>
+        <v>20296</v>
       </c>
       <c r="B149" t="s">
-        <v>169</v>
+        <v>144</v>
       </c>
       <c r="C149" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D149" s="1" t="s">
-        <v>8</v>
+      <c r="D149" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="150" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A150" s="6">
-        <v>20299</v>
+        <v>20298</v>
       </c>
       <c r="B150" t="s">
-        <v>58</v>
+        <v>169</v>
       </c>
       <c r="C150" s="1" t="s">
         <v>4</v>
@@ -3422,10 +3425,10 @@
     </row>
     <row r="151" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A151" s="6">
-        <v>20301</v>
+        <v>20299</v>
       </c>
       <c r="B151" t="s">
-        <v>134</v>
+        <v>58</v>
       </c>
       <c r="C151" s="1" t="s">
         <v>4</v>
@@ -3436,10 +3439,10 @@
     </row>
     <row r="152" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A152" s="6">
-        <v>20303</v>
+        <v>20301</v>
       </c>
       <c r="B152" t="s">
-        <v>37</v>
+        <v>134</v>
       </c>
       <c r="C152" s="1" t="s">
         <v>4</v>
@@ -3450,24 +3453,24 @@
     </row>
     <row r="153" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A153" s="6">
-        <v>20309</v>
+        <v>20303</v>
       </c>
       <c r="B153" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="C153" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D153" s="3" t="s">
-        <v>5</v>
+      <c r="D153" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="154" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A154" s="6">
-        <v>20310</v>
+        <v>20309</v>
       </c>
       <c r="B154" t="s">
-        <v>59</v>
+        <v>28</v>
       </c>
       <c r="C154" s="1" t="s">
         <v>4</v>
@@ -3478,24 +3481,24 @@
     </row>
     <row r="155" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A155" s="6">
-        <v>20318</v>
+        <v>20310</v>
       </c>
       <c r="B155" t="s">
-        <v>209</v>
+        <v>59</v>
       </c>
       <c r="C155" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D155" s="1" t="s">
-        <v>8</v>
+      <c r="D155" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="156" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A156" s="6">
-        <v>20319</v>
+        <v>20318</v>
       </c>
       <c r="B156" t="s">
-        <v>101</v>
+        <v>209</v>
       </c>
       <c r="C156" s="1" t="s">
         <v>4</v>
@@ -3506,10 +3509,10 @@
     </row>
     <row r="157" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A157" s="6">
-        <v>20320</v>
+        <v>20319</v>
       </c>
       <c r="B157" t="s">
-        <v>130</v>
+        <v>101</v>
       </c>
       <c r="C157" s="1" t="s">
         <v>4</v>
@@ -3520,10 +3523,10 @@
     </row>
     <row r="158" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A158" s="6">
-        <v>20324</v>
+        <v>20320</v>
       </c>
       <c r="B158" t="s">
-        <v>210</v>
+        <v>130</v>
       </c>
       <c r="C158" s="1" t="s">
         <v>4</v>
@@ -3534,10 +3537,10 @@
     </row>
     <row r="159" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A159" s="6">
-        <v>20331</v>
+        <v>20324</v>
       </c>
       <c r="B159" t="s">
-        <v>51</v>
+        <v>210</v>
       </c>
       <c r="C159" s="1" t="s">
         <v>4</v>
@@ -3548,38 +3551,38 @@
     </row>
     <row r="160" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A160" s="6">
-        <v>20333</v>
+        <v>20331</v>
       </c>
       <c r="B160" t="s">
-        <v>136</v>
+        <v>51</v>
       </c>
       <c r="C160" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D160" s="3" t="s">
-        <v>5</v>
+      <c r="D160" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="161" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A161" s="6">
-        <v>20337</v>
+        <v>20333</v>
       </c>
       <c r="B161" t="s">
-        <v>104</v>
+        <v>136</v>
       </c>
       <c r="C161" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D161" s="1" t="s">
-        <v>8</v>
+      <c r="D161" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="162" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A162" s="6">
-        <v>20343</v>
+        <v>20337</v>
       </c>
       <c r="B162" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="C162" s="1" t="s">
         <v>4</v>
@@ -3590,10 +3593,10 @@
     </row>
     <row r="163" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A163" s="6">
-        <v>20344</v>
+        <v>20343</v>
       </c>
       <c r="B163" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="C163" s="1" t="s">
         <v>4</v>
@@ -3604,66 +3607,66 @@
     </row>
     <row r="164" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A164" s="6">
-        <v>20351</v>
+        <v>20344</v>
       </c>
       <c r="B164" t="s">
-        <v>26</v>
+        <v>127</v>
       </c>
       <c r="C164" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D164" s="3" t="s">
-        <v>5</v>
+      <c r="D164" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="165" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A165" s="6">
-        <v>20357</v>
+        <v>20351</v>
       </c>
       <c r="B165" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="C165" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D165" s="1" t="s">
-        <v>8</v>
+      <c r="D165" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="166" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A166" s="6">
-        <v>20361</v>
+        <v>20357</v>
       </c>
       <c r="B166" t="s">
-        <v>164</v>
+        <v>56</v>
       </c>
       <c r="C166" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D166" s="3" t="s">
-        <v>5</v>
+      <c r="D166" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="167" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A167" s="6">
-        <v>20362</v>
+        <v>20361</v>
       </c>
       <c r="B167" t="s">
-        <v>45</v>
+        <v>164</v>
       </c>
       <c r="C167" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D167" s="1" t="s">
-        <v>8</v>
+      <c r="D167" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="168" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A168" s="6">
-        <v>20363</v>
+        <v>20362</v>
       </c>
       <c r="B168" t="s">
-        <v>213</v>
+        <v>45</v>
       </c>
       <c r="C168" s="1" t="s">
         <v>4</v>
@@ -3674,38 +3677,38 @@
     </row>
     <row r="169" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A169" s="6">
-        <v>20364</v>
+        <v>20363</v>
       </c>
       <c r="B169" t="s">
-        <v>196</v>
+        <v>213</v>
       </c>
       <c r="C169" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D169" s="3" t="s">
-        <v>5</v>
+      <c r="D169" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="170" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A170" s="6">
-        <v>20366</v>
+        <v>20364</v>
       </c>
       <c r="B170" t="s">
-        <v>220</v>
+        <v>196</v>
       </c>
       <c r="C170" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D170" s="1" t="s">
-        <v>8</v>
+      <c r="D170" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="171" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A171" s="6">
-        <v>20367</v>
+        <v>20366</v>
       </c>
       <c r="B171" t="s">
-        <v>47</v>
+        <v>220</v>
       </c>
       <c r="C171" s="1" t="s">
         <v>4</v>
@@ -3716,10 +3719,10 @@
     </row>
     <row r="172" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A172" s="6">
-        <v>20369</v>
+        <v>20367</v>
       </c>
       <c r="B172" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="C172" s="1" t="s">
         <v>4</v>
@@ -3730,10 +3733,10 @@
     </row>
     <row r="173" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A173" s="6">
-        <v>20371</v>
+        <v>20369</v>
       </c>
       <c r="B173" t="s">
-        <v>223</v>
+        <v>63</v>
       </c>
       <c r="C173" s="1" t="s">
         <v>4</v>
@@ -3744,10 +3747,10 @@
     </row>
     <row r="174" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A174" s="6">
-        <v>20372</v>
+        <v>20371</v>
       </c>
       <c r="B174" t="s">
-        <v>70</v>
+        <v>223</v>
       </c>
       <c r="C174" s="1" t="s">
         <v>4</v>
@@ -3758,10 +3761,10 @@
     </row>
     <row r="175" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A175" s="6">
-        <v>20374</v>
+        <v>20372</v>
       </c>
       <c r="B175" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="C175" s="1" t="s">
         <v>4</v>
@@ -3772,10 +3775,10 @@
     </row>
     <row r="176" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A176" s="6">
-        <v>20377</v>
+        <v>20374</v>
       </c>
       <c r="B176" t="s">
-        <v>225</v>
+        <v>61</v>
       </c>
       <c r="C176" s="1" t="s">
         <v>4</v>
@@ -3786,10 +3789,10 @@
     </row>
     <row r="177" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A177" s="6">
-        <v>20379</v>
+        <v>20377</v>
       </c>
       <c r="B177" t="s">
-        <v>49</v>
+        <v>225</v>
       </c>
       <c r="C177" s="1" t="s">
         <v>4</v>
@@ -3800,38 +3803,38 @@
     </row>
     <row r="178" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A178" s="6">
-        <v>20380</v>
+        <v>20379</v>
       </c>
       <c r="B178" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="C178" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D178" s="3" t="s">
-        <v>5</v>
+      <c r="D178" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="179" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A179" s="6">
-        <v>20381</v>
+        <v>20380</v>
       </c>
       <c r="B179" t="s">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="C179" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D179" s="1" t="s">
-        <v>8</v>
+      <c r="D179" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="180" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A180" s="6">
-        <v>20384</v>
+        <v>20381</v>
       </c>
       <c r="B180" t="s">
-        <v>181</v>
+        <v>60</v>
       </c>
       <c r="C180" s="1" t="s">
         <v>4</v>
@@ -3842,10 +3845,10 @@
     </row>
     <row r="181" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A181" s="6">
-        <v>20385</v>
+        <v>20384</v>
       </c>
       <c r="B181" t="s">
-        <v>36</v>
+        <v>181</v>
       </c>
       <c r="C181" s="1" t="s">
         <v>4</v>
@@ -3856,10 +3859,10 @@
     </row>
     <row r="182" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A182" s="6">
-        <v>20386</v>
+        <v>20385</v>
       </c>
       <c r="B182" t="s">
-        <v>119</v>
+        <v>36</v>
       </c>
       <c r="C182" s="1" t="s">
         <v>4</v>
@@ -3870,10 +3873,10 @@
     </row>
     <row r="183" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A183" s="6">
-        <v>20388</v>
+        <v>20386</v>
       </c>
       <c r="B183" t="s">
-        <v>100</v>
+        <v>119</v>
       </c>
       <c r="C183" s="1" t="s">
         <v>4</v>
@@ -3884,10 +3887,10 @@
     </row>
     <row r="184" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A184" s="6">
-        <v>20391</v>
+        <v>20388</v>
       </c>
       <c r="B184" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C184" s="1" t="s">
         <v>4</v>
@@ -3898,10 +3901,10 @@
     </row>
     <row r="185" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A185" s="6">
-        <v>20394</v>
+        <v>20391</v>
       </c>
       <c r="B185" t="s">
-        <v>173</v>
+        <v>106</v>
       </c>
       <c r="C185" s="1" t="s">
         <v>4</v>
@@ -3912,10 +3915,10 @@
     </row>
     <row r="186" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A186" s="6">
-        <v>20395</v>
+        <v>20394</v>
       </c>
       <c r="B186" t="s">
-        <v>161</v>
+        <v>173</v>
       </c>
       <c r="C186" s="1" t="s">
         <v>4</v>
@@ -3926,10 +3929,10 @@
     </row>
     <row r="187" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A187" s="6">
-        <v>30101</v>
+        <v>20395</v>
       </c>
       <c r="B187" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="C187" s="1" t="s">
         <v>4</v>
@@ -3940,24 +3943,24 @@
     </row>
     <row r="188" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A188" s="6">
-        <v>40124</v>
+        <v>30101</v>
       </c>
       <c r="B188" t="s">
-        <v>24</v>
+        <v>167</v>
       </c>
       <c r="C188" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D188" s="3" t="s">
-        <v>5</v>
+      <c r="D188" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="189" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A189" s="6">
-        <v>40125</v>
+        <v>40124</v>
       </c>
       <c r="B189" t="s">
-        <v>143</v>
+        <v>24</v>
       </c>
       <c r="C189" s="1" t="s">
         <v>4</v>
@@ -3968,24 +3971,24 @@
     </row>
     <row r="190" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A190" s="6">
-        <v>40127</v>
+        <v>40125</v>
       </c>
       <c r="B190" t="s">
-        <v>163</v>
+        <v>143</v>
       </c>
       <c r="C190" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D190" s="1" t="s">
-        <v>8</v>
+      <c r="D190" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="191" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A191" s="6">
-        <v>40129</v>
+        <v>40127</v>
       </c>
       <c r="B191" t="s">
-        <v>138</v>
+        <v>163</v>
       </c>
       <c r="C191" s="1" t="s">
         <v>4</v>
@@ -3996,10 +3999,10 @@
     </row>
     <row r="192" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A192" s="6">
-        <v>40137</v>
+        <v>40129</v>
       </c>
       <c r="B192" t="s">
-        <v>121</v>
+        <v>138</v>
       </c>
       <c r="C192" s="1" t="s">
         <v>4</v>
@@ -4010,10 +4013,10 @@
     </row>
     <row r="193" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A193" s="6">
-        <v>40140</v>
+        <v>40137</v>
       </c>
       <c r="B193" t="s">
-        <v>170</v>
+        <v>121</v>
       </c>
       <c r="C193" s="1" t="s">
         <v>4</v>
@@ -4024,52 +4027,52 @@
     </row>
     <row r="194" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A194" s="6">
-        <v>40141</v>
+        <v>40140</v>
       </c>
       <c r="B194" t="s">
-        <v>111</v>
+        <v>170</v>
       </c>
       <c r="C194" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D194" s="3" t="s">
-        <v>5</v>
+      <c r="D194" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="195" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A195" s="6">
-        <v>40143</v>
+        <v>40141</v>
       </c>
       <c r="B195" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
       <c r="C195" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D195" s="1" t="s">
-        <v>8</v>
+      <c r="D195" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="196" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A196" s="6">
-        <v>40144</v>
+        <v>40143</v>
       </c>
       <c r="B196" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="C196" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D196" s="3" t="s">
-        <v>5</v>
+      <c r="D196" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="197" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A197" s="6">
-        <v>40145</v>
+        <v>40144</v>
       </c>
       <c r="B197" t="s">
-        <v>165</v>
+        <v>107</v>
       </c>
       <c r="C197" s="1" t="s">
         <v>4</v>
@@ -4080,24 +4083,24 @@
     </row>
     <row r="198" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A198" s="6">
-        <v>40150</v>
+        <v>40145</v>
       </c>
       <c r="B198" t="s">
-        <v>221</v>
+        <v>165</v>
       </c>
       <c r="C198" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D198" s="1" t="s">
-        <v>8</v>
+      <c r="D198" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="199" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A199" s="6">
-        <v>40151</v>
+        <v>40150</v>
       </c>
       <c r="B199" t="s">
-        <v>54</v>
+        <v>221</v>
       </c>
       <c r="C199" s="1" t="s">
         <v>4</v>
@@ -4108,38 +4111,38 @@
     </row>
     <row r="200" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A200" s="6">
-        <v>50102</v>
+        <v>40151</v>
       </c>
       <c r="B200" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="C200" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D200" s="3" t="s">
-        <v>5</v>
+      <c r="D200" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="201" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A201" s="6">
-        <v>50222</v>
+        <v>50102</v>
       </c>
       <c r="B201" t="s">
-        <v>215</v>
+        <v>67</v>
       </c>
       <c r="C201" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D201" s="1" t="s">
-        <v>8</v>
+      <c r="D201" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="202" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A202" s="6">
-        <v>50223</v>
+        <v>50222</v>
       </c>
       <c r="B202" t="s">
-        <v>194</v>
+        <v>215</v>
       </c>
       <c r="C202" s="1" t="s">
         <v>4</v>
@@ -4150,66 +4153,66 @@
     </row>
     <row r="203" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A203" s="6">
-        <v>50224</v>
+        <v>50223</v>
       </c>
       <c r="B203" t="s">
-        <v>42</v>
+        <v>194</v>
       </c>
       <c r="C203" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D203" s="3" t="s">
-        <v>5</v>
+      <c r="D203" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="204" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A204" s="6">
-        <v>50444</v>
+        <v>50224</v>
       </c>
       <c r="B204" t="s">
-        <v>116</v>
+        <v>42</v>
       </c>
       <c r="C204" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D204" s="1" t="s">
-        <v>8</v>
+      <c r="D204" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="205" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A205" s="6">
-        <v>50607</v>
+        <v>50444</v>
       </c>
       <c r="B205" t="s">
-        <v>76</v>
+        <v>116</v>
       </c>
       <c r="C205" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D205" s="3" t="s">
-        <v>5</v>
+      <c r="D205" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="206" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A206" s="6">
-        <v>50608</v>
+        <v>50607</v>
       </c>
       <c r="B206" t="s">
-        <v>177</v>
+        <v>76</v>
       </c>
       <c r="C206" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D206" s="1" t="s">
-        <v>8</v>
+      <c r="D206" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="207" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A207" s="6">
-        <v>50622</v>
+        <v>50608</v>
       </c>
       <c r="B207" t="s">
-        <v>95</v>
+        <v>177</v>
       </c>
       <c r="C207" s="1" t="s">
         <v>4</v>
@@ -4220,10 +4223,10 @@
     </row>
     <row r="208" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A208" s="6">
-        <v>50623</v>
+        <v>50622</v>
       </c>
       <c r="B208" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="C208" s="1" t="s">
         <v>4</v>
@@ -4234,10 +4237,10 @@
     </row>
     <row r="209" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A209" s="6">
-        <v>50625</v>
+        <v>50623</v>
       </c>
       <c r="B209" t="s">
-        <v>204</v>
+        <v>110</v>
       </c>
       <c r="C209" s="1" t="s">
         <v>4</v>
@@ -4248,10 +4251,10 @@
     </row>
     <row r="210" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A210" s="6">
-        <v>50629</v>
+        <v>50625</v>
       </c>
       <c r="B210" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="C210" s="1" t="s">
         <v>4</v>
@@ -4262,10 +4265,10 @@
     </row>
     <row r="211" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A211" s="6">
-        <v>50803</v>
+        <v>50629</v>
       </c>
       <c r="B211" t="s">
-        <v>82</v>
+        <v>188</v>
       </c>
       <c r="C211" s="1" t="s">
         <v>4</v>
@@ -4276,10 +4279,10 @@
     </row>
     <row r="212" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A212" s="6">
-        <v>50805</v>
+        <v>50803</v>
       </c>
       <c r="B212" t="s">
-        <v>135</v>
+        <v>82</v>
       </c>
       <c r="C212" s="1" t="s">
         <v>4</v>
@@ -4290,10 +4293,10 @@
     </row>
     <row r="213" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A213" s="6">
-        <v>50806</v>
+        <v>50805</v>
       </c>
       <c r="B213" t="s">
-        <v>156</v>
+        <v>135</v>
       </c>
       <c r="C213" s="1" t="s">
         <v>4</v>
@@ -4304,24 +4307,24 @@
     </row>
     <row r="214" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A214" s="6">
-        <v>50808</v>
+        <v>50806</v>
       </c>
       <c r="B214" t="s">
-        <v>16</v>
+        <v>156</v>
       </c>
       <c r="C214" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D214" s="3" t="s">
-        <v>5</v>
+      <c r="D214" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="215" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A215" s="6">
-        <v>50809</v>
+        <v>50808</v>
       </c>
       <c r="B215" t="s">
-        <v>98</v>
+        <v>16</v>
       </c>
       <c r="C215" s="1" t="s">
         <v>4</v>
@@ -4332,24 +4335,24 @@
     </row>
     <row r="216" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A216" s="6">
-        <v>50810</v>
+        <v>50809</v>
       </c>
       <c r="B216" t="s">
-        <v>175</v>
+        <v>98</v>
       </c>
       <c r="C216" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D216" s="1" t="s">
-        <v>8</v>
+      <c r="D216" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="217" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A217" s="6">
-        <v>50812</v>
+        <v>50810</v>
       </c>
       <c r="B217" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="C217" s="1" t="s">
         <v>4</v>
@@ -4360,38 +4363,38 @@
     </row>
     <row r="218" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A218" s="6">
-        <v>50813</v>
+        <v>50812</v>
       </c>
       <c r="B218" t="s">
-        <v>71</v>
+        <v>184</v>
       </c>
       <c r="C218" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D218" t="s">
-        <v>9</v>
+      <c r="D218" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="219" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A219" s="6">
-        <v>50815</v>
+        <v>50813</v>
       </c>
       <c r="B219" t="s">
-        <v>114</v>
+        <v>71</v>
       </c>
       <c r="C219" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D219" s="1" t="s">
-        <v>8</v>
+      <c r="D219" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="220" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A220" s="6">
-        <v>50816</v>
+        <v>50815</v>
       </c>
       <c r="B220" t="s">
-        <v>205</v>
+        <v>114</v>
       </c>
       <c r="C220" s="1" t="s">
         <v>4</v>
@@ -4402,38 +4405,38 @@
     </row>
     <row r="221" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A221" s="6">
-        <v>50818</v>
+        <v>50816</v>
       </c>
       <c r="B221" t="s">
-        <v>227</v>
+        <v>205</v>
       </c>
       <c r="C221" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D221" s="3" t="s">
-        <v>5</v>
+      <c r="D221" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="222" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A222" s="6">
-        <v>50819</v>
+        <v>50818</v>
       </c>
       <c r="B222" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C222" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D222" s="1" t="s">
-        <v>8</v>
+      <c r="D222" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="223" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A223" s="6">
-        <v>50820</v>
+        <v>50819</v>
       </c>
       <c r="B223" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C223" s="1" t="s">
         <v>4</v>
@@ -4444,10 +4447,10 @@
     </row>
     <row r="224" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A224" s="6">
-        <v>50821</v>
+        <v>50820</v>
       </c>
       <c r="B224" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C224" s="1" t="s">
         <v>4</v>
@@ -4458,52 +4461,52 @@
     </row>
     <row r="225" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A225" s="6">
-        <v>50823</v>
+        <v>50821</v>
       </c>
       <c r="B225" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C225" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D225" t="s">
-        <v>9</v>
+      <c r="D225" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="226" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A226" s="6">
-        <v>50824</v>
+        <v>50823</v>
       </c>
       <c r="B226" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C226" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D226" s="3" t="s">
-        <v>5</v>
+      <c r="D226" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="227" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A227" s="6">
-        <v>50825</v>
+        <v>50824</v>
       </c>
       <c r="B227" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C227" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D227" s="1" t="s">
-        <v>8</v>
+      <c r="D227" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="228" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A228" s="6">
-        <v>50826</v>
+        <v>50825</v>
       </c>
       <c r="B228" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C228" s="1" t="s">
         <v>4</v>
@@ -4514,10 +4517,10 @@
     </row>
     <row r="229" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A229" s="6">
-        <v>50827</v>
+        <v>50826</v>
       </c>
       <c r="B229" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C229" s="1" t="s">
         <v>4</v>
@@ -4528,10 +4531,10 @@
     </row>
     <row r="230" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A230" s="6">
-        <v>50829</v>
+        <v>50827</v>
       </c>
       <c r="B230" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C230" s="1" t="s">
         <v>4</v>
@@ -4542,24 +4545,24 @@
     </row>
     <row r="231" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A231" s="6">
-        <v>60103</v>
+        <v>50829</v>
       </c>
       <c r="B231" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C231" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D231" s="3" t="s">
-        <v>5</v>
+      <c r="D231" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="232" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A232" s="6">
-        <v>60124</v>
+        <v>60103</v>
       </c>
       <c r="B232" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C232" s="1" t="s">
         <v>4</v>
@@ -4570,10 +4573,10 @@
     </row>
     <row r="233" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A233" s="6">
-        <v>60125</v>
+        <v>60124</v>
       </c>
       <c r="B233" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C233" s="1" t="s">
         <v>4</v>
@@ -4584,80 +4587,80 @@
     </row>
     <row r="234" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A234" s="6">
-        <v>60126</v>
+        <v>60125</v>
       </c>
       <c r="B234" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C234" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D234" s="1" t="s">
-        <v>8</v>
+      <c r="D234" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="235" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A235" s="6">
-        <v>60128</v>
+        <v>60126</v>
       </c>
       <c r="B235" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C235" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D235" s="3" t="s">
-        <v>5</v>
+      <c r="D235" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="236" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A236" s="6">
-        <v>60130</v>
+        <v>60128</v>
       </c>
       <c r="B236" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C236" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D236" s="1" t="s">
-        <v>8</v>
+      <c r="D236" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="237" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A237" s="6">
-        <v>60133</v>
+        <v>60130</v>
       </c>
       <c r="B237" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C237" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D237" s="3" t="s">
-        <v>5</v>
+      <c r="D237" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="238" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A238" s="6">
-        <v>60134</v>
+        <v>60133</v>
       </c>
       <c r="B238" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C238" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D238" s="1" t="s">
-        <v>8</v>
+      <c r="D238" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="239" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A239" s="6">
-        <v>60137</v>
+        <v>60134</v>
       </c>
       <c r="B239" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C239" s="1" t="s">
         <v>4</v>
@@ -4668,10 +4671,10 @@
     </row>
     <row r="240" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A240" s="6">
-        <v>60139</v>
+        <v>60137</v>
       </c>
       <c r="B240" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C240" s="1" t="s">
         <v>4</v>
@@ -4682,10 +4685,10 @@
     </row>
     <row r="241" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A241" s="6">
-        <v>60142</v>
+        <v>60139</v>
       </c>
       <c r="B241" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C241" s="1" t="s">
         <v>4</v>
@@ -4696,10 +4699,10 @@
     </row>
     <row r="242" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A242" s="6">
-        <v>60148</v>
+        <v>60142</v>
       </c>
       <c r="B242" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C242" s="1" t="s">
         <v>4</v>
@@ -4710,10 +4713,10 @@
     </row>
     <row r="243" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A243" s="6">
-        <v>60149</v>
+        <v>60148</v>
       </c>
       <c r="B243" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C243" s="1" t="s">
         <v>4</v>
@@ -4724,10 +4727,10 @@
     </row>
     <row r="244" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A244" s="6">
-        <v>60158</v>
+        <v>60149</v>
       </c>
       <c r="B244" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C244" s="1" t="s">
         <v>4</v>
@@ -4738,10 +4741,10 @@
     </row>
     <row r="245" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A245" s="6">
-        <v>60159</v>
+        <v>60158</v>
       </c>
       <c r="B245" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C245" s="1" t="s">
         <v>4</v>
@@ -4752,24 +4755,24 @@
     </row>
     <row r="246" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A246" s="6">
-        <v>60162</v>
+        <v>60159</v>
       </c>
       <c r="B246" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C246" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D246" s="3" t="s">
-        <v>5</v>
+      <c r="D246" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="247" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A247" s="6">
-        <v>60163</v>
+        <v>60162</v>
       </c>
       <c r="B247" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C247" s="1" t="s">
         <v>4</v>
@@ -4780,24 +4783,24 @@
     </row>
     <row r="248" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A248" s="6">
-        <v>60165</v>
+        <v>60163</v>
       </c>
       <c r="B248" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C248" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D248" s="1" t="s">
-        <v>8</v>
+      <c r="D248" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="249" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A249" s="6">
-        <v>60169</v>
+        <v>60165</v>
       </c>
       <c r="B249" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C249" s="1" t="s">
         <v>4</v>
@@ -4808,10 +4811,10 @@
     </row>
     <row r="250" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A250" s="6">
-        <v>60172</v>
+        <v>60169</v>
       </c>
       <c r="B250" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C250" s="1" t="s">
         <v>4</v>
@@ -4822,24 +4825,24 @@
     </row>
     <row r="251" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A251" s="6">
-        <v>60174</v>
+        <v>60172</v>
       </c>
       <c r="B251" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C251" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D251" s="3" t="s">
-        <v>5</v>
+      <c r="D251" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="252" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A252" s="6">
-        <v>60176</v>
+        <v>60174</v>
       </c>
       <c r="B252" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C252" s="1" t="s">
         <v>4</v>
@@ -4850,24 +4853,24 @@
     </row>
     <row r="253" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A253" s="6">
-        <v>60178</v>
+        <v>60176</v>
       </c>
       <c r="B253" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C253" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D253" s="1" t="s">
-        <v>8</v>
+      <c r="D253" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="254" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A254" s="6">
-        <v>60180</v>
+        <v>60178</v>
       </c>
       <c r="B254" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C254" s="1" t="s">
         <v>4</v>
@@ -4878,10 +4881,10 @@
     </row>
     <row r="255" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A255" s="6">
-        <v>60184</v>
+        <v>60180</v>
       </c>
       <c r="B255" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C255" s="1" t="s">
         <v>4</v>
@@ -4892,10 +4895,10 @@
     </row>
     <row r="256" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A256" s="6">
-        <v>60190</v>
+        <v>60184</v>
       </c>
       <c r="B256" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C256" s="1" t="s">
         <v>4</v>
@@ -4906,10 +4909,10 @@
     </row>
     <row r="257" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A257" s="6">
-        <v>60191</v>
+        <v>60190</v>
       </c>
       <c r="B257" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C257" s="1" t="s">
         <v>4</v>
@@ -4920,10 +4923,10 @@
     </row>
     <row r="258" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A258" s="6">
-        <v>60192</v>
+        <v>60191</v>
       </c>
       <c r="B258" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C258" s="1" t="s">
         <v>4</v>
@@ -4934,10 +4937,10 @@
     </row>
     <row r="259" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A259" s="6">
-        <v>60195</v>
+        <v>60192</v>
       </c>
       <c r="B259" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C259" s="1" t="s">
         <v>4</v>
@@ -4948,10 +4951,10 @@
     </row>
     <row r="260" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A260" s="6">
-        <v>60196</v>
+        <v>60195</v>
       </c>
       <c r="B260" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C260" s="1" t="s">
         <v>4</v>
@@ -4962,10 +4965,10 @@
     </row>
     <row r="261" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A261" s="6">
-        <v>60198</v>
+        <v>60196</v>
       </c>
       <c r="B261" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C261" s="1" t="s">
         <v>4</v>
@@ -4976,10 +4979,10 @@
     </row>
     <row r="262" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A262" s="6">
-        <v>60200</v>
+        <v>60198</v>
       </c>
       <c r="B262" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C262" s="1" t="s">
         <v>4</v>
@@ -4990,52 +4993,52 @@
     </row>
     <row r="263" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A263" s="6">
-        <v>60201</v>
+        <v>60200</v>
       </c>
       <c r="B263" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C263" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D263" t="s">
-        <v>9</v>
+      <c r="D263" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="264" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A264" s="6">
-        <v>60202</v>
+        <v>60201</v>
       </c>
       <c r="B264" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C264" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D264" s="3" t="s">
-        <v>5</v>
+      <c r="D264" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="265" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A265" s="6">
-        <v>60204</v>
+        <v>60202</v>
       </c>
       <c r="B265" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C265" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D265" s="1" t="s">
-        <v>8</v>
+      <c r="D265" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="266" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A266" s="6">
-        <v>60205</v>
+        <v>60204</v>
       </c>
       <c r="B266" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C266" s="1" t="s">
         <v>4</v>
@@ -5046,10 +5049,10 @@
     </row>
     <row r="267" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A267" s="6">
-        <v>60206</v>
+        <v>60205</v>
       </c>
       <c r="B267" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C267" s="1" t="s">
         <v>4</v>
@@ -5060,10 +5063,10 @@
     </row>
     <row r="268" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A268" s="6">
-        <v>60209</v>
+        <v>60206</v>
       </c>
       <c r="B268" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C268" s="1" t="s">
         <v>4</v>
@@ -5074,10 +5077,10 @@
     </row>
     <row r="269" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A269" s="6">
-        <v>60211</v>
+        <v>60209</v>
       </c>
       <c r="B269" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C269" s="1" t="s">
         <v>4</v>
@@ -5088,10 +5091,10 @@
     </row>
     <row r="270" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A270" s="6">
-        <v>60215</v>
+        <v>60211</v>
       </c>
       <c r="B270" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C270" s="1" t="s">
         <v>4</v>
@@ -5102,10 +5105,10 @@
     </row>
     <row r="271" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A271" s="6">
-        <v>60217</v>
+        <v>60215</v>
       </c>
       <c r="B271" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C271" s="1" t="s">
         <v>4</v>
@@ -5116,10 +5119,10 @@
     </row>
     <row r="272" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A272" s="6">
-        <v>60219</v>
+        <v>60217</v>
       </c>
       <c r="B272" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C272" s="1" t="s">
         <v>4</v>
@@ -5130,10 +5133,10 @@
     </row>
     <row r="273" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A273" s="6">
-        <v>60222</v>
+        <v>60219</v>
       </c>
       <c r="B273" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C273" s="1" t="s">
         <v>4</v>
@@ -5144,38 +5147,38 @@
     </row>
     <row r="274" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A274" s="6">
-        <v>60225</v>
+        <v>60222</v>
       </c>
       <c r="B274" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C274" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D274" t="s">
-        <v>9</v>
+      <c r="D274" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="275" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A275" s="6">
-        <v>60230</v>
+        <v>60225</v>
       </c>
       <c r="B275" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C275" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D275" s="1" t="s">
-        <v>8</v>
+      <c r="D275" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="276" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A276" s="6">
-        <v>60234</v>
+        <v>60230</v>
       </c>
       <c r="B276" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C276" s="1" t="s">
         <v>4</v>
@@ -5186,10 +5189,10 @@
     </row>
     <row r="277" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A277" s="6">
-        <v>60253</v>
+        <v>60234</v>
       </c>
       <c r="B277" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C277" s="1" t="s">
         <v>4</v>
@@ -5200,10 +5203,10 @@
     </row>
     <row r="278" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A278" s="6">
-        <v>60254</v>
+        <v>60253</v>
       </c>
       <c r="B278" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C278" s="1" t="s">
         <v>4</v>
@@ -5214,10 +5217,10 @@
     </row>
     <row r="279" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A279" s="6">
-        <v>60257</v>
+        <v>60254</v>
       </c>
       <c r="B279" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C279" s="1" t="s">
         <v>4</v>
@@ -5228,10 +5231,10 @@
     </row>
     <row r="280" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A280" s="6">
-        <v>60258</v>
+        <v>60257</v>
       </c>
       <c r="B280" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C280" s="1" t="s">
         <v>4</v>
@@ -5242,10 +5245,10 @@
     </row>
     <row r="281" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A281" s="6">
-        <v>60269</v>
+        <v>60258</v>
       </c>
       <c r="B281" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C281" s="1" t="s">
         <v>4</v>
@@ -5256,10 +5259,10 @@
     </row>
     <row r="282" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A282" s="6">
-        <v>60270</v>
+        <v>60269</v>
       </c>
       <c r="B282" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C282" s="1" t="s">
         <v>4</v>
@@ -5270,10 +5273,10 @@
     </row>
     <row r="283" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A283" s="6">
-        <v>60272</v>
+        <v>60270</v>
       </c>
       <c r="B283" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C283" s="1" t="s">
         <v>4</v>
@@ -5284,10 +5287,10 @@
     </row>
     <row r="284" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A284" s="6">
-        <v>60275</v>
+        <v>60272</v>
       </c>
       <c r="B284" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C284" s="1" t="s">
         <v>4</v>
@@ -5298,10 +5301,10 @@
     </row>
     <row r="285" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A285" s="6">
-        <v>60276</v>
+        <v>60275</v>
       </c>
       <c r="B285" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C285" s="1" t="s">
         <v>4</v>
@@ -5312,38 +5315,38 @@
     </row>
     <row r="286" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A286" s="6">
-        <v>60278</v>
+        <v>60276</v>
       </c>
       <c r="B286" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C286" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D286" s="3" t="s">
-        <v>5</v>
+      <c r="D286" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="287" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A287" s="6">
-        <v>60279</v>
+        <v>60278</v>
       </c>
       <c r="B287" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C287" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D287" s="1" t="s">
-        <v>8</v>
+      <c r="D287" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="288" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A288" s="6">
-        <v>60280</v>
+        <v>60279</v>
       </c>
       <c r="B288" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C288" s="1" t="s">
         <v>4</v>
@@ -5354,38 +5357,38 @@
     </row>
     <row r="289" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A289" s="6">
-        <v>61004</v>
+        <v>60280</v>
       </c>
       <c r="B289" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C289" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D289" s="3" t="s">
-        <v>5</v>
+      <c r="D289" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="290" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A290" s="6">
-        <v>61009</v>
+        <v>61004</v>
       </c>
       <c r="B290" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C290" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D290" s="1" t="s">
-        <v>8</v>
+      <c r="D290" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="291" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A291" s="6">
-        <v>61012</v>
+        <v>61009</v>
       </c>
       <c r="B291" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C291" s="1" t="s">
         <v>4</v>
@@ -5396,10 +5399,10 @@
     </row>
     <row r="292" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A292" s="6">
-        <v>61018</v>
+        <v>61012</v>
       </c>
       <c r="B292" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C292" s="1" t="s">
         <v>4</v>
@@ -5410,10 +5413,10 @@
     </row>
     <row r="293" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A293" s="6">
-        <v>61102</v>
+        <v>61018</v>
       </c>
       <c r="B293" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C293" s="1" t="s">
         <v>4</v>
@@ -5424,52 +5427,52 @@
     </row>
     <row r="294" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A294" s="6">
-        <v>61205</v>
+        <v>61102</v>
       </c>
       <c r="B294" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C294" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D294" s="3" t="s">
-        <v>5</v>
+      <c r="D294" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="295" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A295" s="6">
-        <v>70100</v>
+        <v>61205</v>
       </c>
       <c r="B295" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C295" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D295" s="1" t="s">
-        <v>8</v>
+      <c r="D295" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="296" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A296" s="6">
-        <v>70101</v>
+        <v>70100</v>
       </c>
       <c r="B296" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C296" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D296" s="3" t="s">
-        <v>5</v>
+      <c r="D296" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="297" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A297" s="6">
-        <v>70102</v>
+        <v>70101</v>
       </c>
       <c r="B297" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C297" s="1" t="s">
         <v>4</v>
@@ -5480,80 +5483,80 @@
     </row>
     <row r="298" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A298" s="6">
-        <v>70103</v>
+        <v>70102</v>
       </c>
       <c r="B298" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C298" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D298" s="1" t="s">
-        <v>8</v>
+      <c r="D298" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="299" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A299" s="6">
-        <v>70106</v>
+        <v>70103</v>
       </c>
       <c r="B299" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C299" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D299" s="3" t="s">
-        <v>5</v>
+      <c r="D299" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="300" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A300" s="6">
-        <v>70109</v>
+        <v>70106</v>
       </c>
       <c r="B300" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C300" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D300" s="1" t="s">
-        <v>8</v>
+      <c r="D300" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="301" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A301" s="6">
-        <v>70113</v>
+        <v>70109</v>
       </c>
       <c r="B301" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C301" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D301" s="3" t="s">
-        <v>5</v>
+      <c r="D301" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="302" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A302" s="6">
-        <v>70638</v>
+        <v>70113</v>
       </c>
       <c r="B302" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C302" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D302" s="1" t="s">
-        <v>8</v>
+      <c r="D302" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="303" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A303" s="6">
-        <v>70639</v>
+        <v>70638</v>
       </c>
       <c r="B303" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C303" s="1" t="s">
         <v>4</v>
@@ -5564,10 +5567,10 @@
     </row>
     <row r="304" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A304" s="6">
-        <v>70640</v>
+        <v>70639</v>
       </c>
       <c r="B304" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C304" s="1" t="s">
         <v>4</v>
@@ -5578,10 +5581,10 @@
     </row>
     <row r="305" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A305" s="6">
-        <v>70642</v>
+        <v>70640</v>
       </c>
       <c r="B305" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C305" s="1" t="s">
         <v>4</v>
@@ -5592,10 +5595,10 @@
     </row>
     <row r="306" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A306" s="6">
-        <v>90504</v>
+        <v>70642</v>
       </c>
       <c r="B306" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C306" s="1" t="s">
         <v>4</v>
@@ -5606,10 +5609,10 @@
     </row>
     <row r="307" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A307" s="6">
-        <v>90509</v>
+        <v>90504</v>
       </c>
       <c r="B307" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C307" s="1" t="s">
         <v>4</v>
@@ -5620,38 +5623,38 @@
     </row>
     <row r="308" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A308" s="6">
-        <v>90602</v>
+        <v>90509</v>
       </c>
       <c r="B308" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C308" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D308" s="3" t="s">
-        <v>5</v>
+      <c r="D308" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="309" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A309" s="6">
-        <v>90621</v>
+        <v>90602</v>
       </c>
       <c r="B309" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C309" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D309" s="1" t="s">
-        <v>8</v>
+      <c r="D309" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="310" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A310" s="6">
-        <v>90658</v>
+        <v>90621</v>
       </c>
       <c r="B310" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C310" s="1" t="s">
         <v>4</v>
@@ -5662,10 +5665,10 @@
     </row>
     <row r="311" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A311" s="6">
-        <v>90660</v>
+        <v>90658</v>
       </c>
       <c r="B311" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C311" s="1" t="s">
         <v>4</v>
@@ -5676,10 +5679,10 @@
     </row>
     <row r="312" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A312" s="6">
-        <v>90668</v>
+        <v>90660</v>
       </c>
       <c r="B312" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C312" s="1" t="s">
         <v>4</v>
@@ -5690,10 +5693,10 @@
     </row>
     <row r="313" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A313" s="6">
-        <v>90671</v>
+        <v>90668</v>
       </c>
       <c r="B313" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C313" s="1" t="s">
         <v>4</v>
@@ -5704,10 +5707,10 @@
     </row>
     <row r="314" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A314" s="6">
-        <v>90679</v>
+        <v>90671</v>
       </c>
       <c r="B314" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C314" s="1" t="s">
         <v>4</v>
@@ -5718,10 +5721,10 @@
     </row>
     <row r="315" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A315" s="6">
-        <v>90683</v>
+        <v>90679</v>
       </c>
       <c r="B315" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C315" s="1" t="s">
         <v>4</v>
@@ -5732,10 +5735,10 @@
     </row>
     <row r="316" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A316" s="6">
-        <v>90705</v>
+        <v>90683</v>
       </c>
       <c r="B316" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C316" s="1" t="s">
         <v>4</v>
@@ -5746,10 +5749,10 @@
     </row>
     <row r="317" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A317" s="6">
-        <v>90706</v>
+        <v>90705</v>
       </c>
       <c r="B317" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C317" s="1" t="s">
         <v>4</v>
@@ -5760,10 +5763,10 @@
     </row>
     <row r="318" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A318" s="6">
-        <v>90708</v>
+        <v>90706</v>
       </c>
       <c r="B318" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C318" s="1" t="s">
         <v>4</v>
@@ -5774,20 +5777,34 @@
     </row>
     <row r="319" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A319" s="6">
+        <v>90708</v>
+      </c>
+      <c r="B319" t="s">
+        <v>324</v>
+      </c>
+      <c r="C319" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D319" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="320" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A320" s="6">
         <v>90709</v>
       </c>
-      <c r="B319" t="s">
+      <c r="B320" t="s">
         <v>325</v>
       </c>
-      <c r="C319" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D319" s="1" t="s">
+      <c r="C320" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D320" s="1" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D319"/>
+  <autoFilter ref="A1:D320"/>
   <conditionalFormatting sqref="B1:B1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>

</xml_diff>

<commit_message>
subi imagenes de egopreg9710,15,20. y subi datos cta 70114
</commit_message>
<xml_diff>
--- a/excel/CLIENTES_PERMISOS.xlsx
+++ b/excel/CLIENTES_PERMISOS.xlsx
@@ -15,14 +15,14 @@
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Hoja 1'!$A$1:$D$320</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Hoja 1'!$A$1:$D$321</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="961" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="964" uniqueCount="328">
   <si>
     <t>CUENTA</t>
   </si>
@@ -1003,6 +1003,9 @@
   </si>
   <si>
     <t>CONSUMIDOR FINAL</t>
+  </si>
+  <si>
+    <t>FERRETERIA FERRECAS</t>
   </si>
 </sst>
 </file>
@@ -1038,7 +1041,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1061,11 +1064,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1081,6 +1093,9 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1310,10 +1325,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D320"/>
+  <dimension ref="A1:D321"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A289" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C303" sqref="C303"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5553,24 +5568,24 @@
     </row>
     <row r="303" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A303" s="6">
-        <v>70638</v>
+        <v>70114</v>
       </c>
       <c r="B303" t="s">
-        <v>308</v>
+        <v>327</v>
       </c>
       <c r="C303" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D303" s="1" t="s">
-        <v>8</v>
+      <c r="D303" s="7" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="304" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A304" s="6">
-        <v>70639</v>
+        <v>70638</v>
       </c>
       <c r="B304" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C304" s="1" t="s">
         <v>4</v>
@@ -5581,10 +5596,10 @@
     </row>
     <row r="305" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A305" s="6">
-        <v>70640</v>
+        <v>70639</v>
       </c>
       <c r="B305" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C305" s="1" t="s">
         <v>4</v>
@@ -5595,10 +5610,10 @@
     </row>
     <row r="306" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A306" s="6">
-        <v>70642</v>
+        <v>70640</v>
       </c>
       <c r="B306" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C306" s="1" t="s">
         <v>4</v>
@@ -5609,10 +5624,10 @@
     </row>
     <row r="307" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A307" s="6">
-        <v>90504</v>
+        <v>70642</v>
       </c>
       <c r="B307" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C307" s="1" t="s">
         <v>4</v>
@@ -5623,10 +5638,10 @@
     </row>
     <row r="308" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A308" s="6">
-        <v>90509</v>
+        <v>90504</v>
       </c>
       <c r="B308" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C308" s="1" t="s">
         <v>4</v>
@@ -5637,38 +5652,38 @@
     </row>
     <row r="309" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A309" s="6">
-        <v>90602</v>
+        <v>90509</v>
       </c>
       <c r="B309" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C309" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D309" s="3" t="s">
-        <v>5</v>
+      <c r="D309" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="310" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A310" s="6">
-        <v>90621</v>
+        <v>90602</v>
       </c>
       <c r="B310" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C310" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D310" s="1" t="s">
-        <v>8</v>
+      <c r="D310" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="311" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A311" s="6">
-        <v>90658</v>
+        <v>90621</v>
       </c>
       <c r="B311" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C311" s="1" t="s">
         <v>4</v>
@@ -5679,10 +5694,10 @@
     </row>
     <row r="312" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A312" s="6">
-        <v>90660</v>
+        <v>90658</v>
       </c>
       <c r="B312" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C312" s="1" t="s">
         <v>4</v>
@@ -5693,10 +5708,10 @@
     </row>
     <row r="313" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A313" s="6">
-        <v>90668</v>
+        <v>90660</v>
       </c>
       <c r="B313" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C313" s="1" t="s">
         <v>4</v>
@@ -5707,10 +5722,10 @@
     </row>
     <row r="314" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A314" s="6">
-        <v>90671</v>
+        <v>90668</v>
       </c>
       <c r="B314" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C314" s="1" t="s">
         <v>4</v>
@@ -5721,10 +5736,10 @@
     </row>
     <row r="315" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A315" s="6">
-        <v>90679</v>
+        <v>90671</v>
       </c>
       <c r="B315" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C315" s="1" t="s">
         <v>4</v>
@@ -5735,10 +5750,10 @@
     </row>
     <row r="316" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A316" s="6">
-        <v>90683</v>
+        <v>90679</v>
       </c>
       <c r="B316" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C316" s="1" t="s">
         <v>4</v>
@@ -5749,10 +5764,10 @@
     </row>
     <row r="317" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A317" s="6">
-        <v>90705</v>
+        <v>90683</v>
       </c>
       <c r="B317" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C317" s="1" t="s">
         <v>4</v>
@@ -5763,10 +5778,10 @@
     </row>
     <row r="318" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A318" s="6">
-        <v>90706</v>
+        <v>90705</v>
       </c>
       <c r="B318" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C318" s="1" t="s">
         <v>4</v>
@@ -5777,10 +5792,10 @@
     </row>
     <row r="319" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A319" s="6">
-        <v>90708</v>
+        <v>90706</v>
       </c>
       <c r="B319" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C319" s="1" t="s">
         <v>4</v>
@@ -5791,20 +5806,34 @@
     </row>
     <row r="320" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A320" s="6">
+        <v>90708</v>
+      </c>
+      <c r="B320" t="s">
+        <v>324</v>
+      </c>
+      <c r="C320" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D320" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="321" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A321" s="6">
         <v>90709</v>
       </c>
-      <c r="B320" t="s">
+      <c r="B321" t="s">
         <v>325</v>
       </c>
-      <c r="C320" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D320" s="1" t="s">
+      <c r="C321" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D321" s="1" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D320"/>
+  <autoFilter ref="A1:D321"/>
   <conditionalFormatting sqref="B1:B1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>

</xml_diff>

<commit_message>
agregue imagenes de crecchio, agregue dtos cta 20129
</commit_message>
<xml_diff>
--- a/excel/CLIENTES_PERMISOS.xlsx
+++ b/excel/CLIENTES_PERMISOS.xlsx
@@ -15,14 +15,14 @@
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Hoja 1'!$A$1:$D$321</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Hoja 1'!$A$1:$D$322</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="964" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="967" uniqueCount="329">
   <si>
     <t>CUENTA</t>
   </si>
@@ -1006,6 +1006,9 @@
   </si>
   <si>
     <t>FERRETERIA FERRECAS</t>
+  </si>
+  <si>
+    <t>LUCIA FERRETERIA</t>
   </si>
 </sst>
 </file>
@@ -1325,10 +1328,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D321"/>
+  <dimension ref="A1:D322"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A289" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C303" sqref="C303"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D91" sqref="D91:D92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2614,24 +2617,24 @@
     </row>
     <row r="92" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="6">
-        <v>20137</v>
+        <v>20129</v>
       </c>
       <c r="B92" t="s">
-        <v>79</v>
+        <v>328</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D92" s="3" t="s">
-        <v>5</v>
+      <c r="D92" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="6">
-        <v>20138</v>
+        <v>20137</v>
       </c>
       <c r="B93" t="s">
-        <v>113</v>
+        <v>79</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>4</v>
@@ -2642,10 +2645,10 @@
     </row>
     <row r="94" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="6">
-        <v>20140</v>
+        <v>20138</v>
       </c>
       <c r="B94" t="s">
-        <v>218</v>
+        <v>113</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>4</v>
@@ -2656,24 +2659,24 @@
     </row>
     <row r="95" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="6">
-        <v>20142</v>
+        <v>20140</v>
       </c>
       <c r="B95" t="s">
-        <v>193</v>
+        <v>218</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D95" s="1" t="s">
-        <v>8</v>
+      <c r="D95" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="6">
-        <v>20146</v>
+        <v>20142</v>
       </c>
       <c r="B96" t="s">
-        <v>148</v>
+        <v>193</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>4</v>
@@ -2684,10 +2687,10 @@
     </row>
     <row r="97" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="6">
-        <v>20148</v>
+        <v>20146</v>
       </c>
       <c r="B97" t="s">
-        <v>38</v>
+        <v>148</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>4</v>
@@ -2698,10 +2701,10 @@
     </row>
     <row r="98" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="6">
-        <v>20156</v>
+        <v>20148</v>
       </c>
       <c r="B98" t="s">
-        <v>179</v>
+        <v>38</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>4</v>
@@ -2712,38 +2715,38 @@
     </row>
     <row r="99" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="6">
-        <v>20159</v>
+        <v>20156</v>
       </c>
       <c r="B99" t="s">
-        <v>120</v>
+        <v>179</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D99" t="s">
-        <v>9</v>
+      <c r="D99" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" s="6">
-        <v>20160</v>
+        <v>20159</v>
       </c>
       <c r="B100" t="s">
-        <v>224</v>
+        <v>120</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D100" s="1" t="s">
-        <v>8</v>
+      <c r="D100" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="101" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="6">
-        <v>20163</v>
+        <v>20160</v>
       </c>
       <c r="B101" t="s">
-        <v>23</v>
+        <v>224</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>4</v>
@@ -2754,38 +2757,38 @@
     </row>
     <row r="102" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" s="6">
-        <v>20164</v>
+        <v>20163</v>
       </c>
       <c r="B102" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C102" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D102" t="s">
-        <v>9</v>
+      <c r="D102" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="103" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="6">
-        <v>20165</v>
+        <v>20164</v>
       </c>
       <c r="B103" t="s">
-        <v>131</v>
+        <v>18</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D103" s="1" t="s">
-        <v>8</v>
+      <c r="D103" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="104" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="6">
-        <v>20166</v>
+        <v>20165</v>
       </c>
       <c r="B104" t="s">
-        <v>77</v>
+        <v>131</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>4</v>
@@ -2796,10 +2799,10 @@
     </row>
     <row r="105" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" s="6">
-        <v>20169</v>
+        <v>20166</v>
       </c>
       <c r="B105" t="s">
-        <v>151</v>
+        <v>77</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>4</v>
@@ -2810,10 +2813,10 @@
     </row>
     <row r="106" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="6">
-        <v>20173</v>
+        <v>20169</v>
       </c>
       <c r="B106" t="s">
-        <v>112</v>
+        <v>151</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>4</v>
@@ -2824,10 +2827,10 @@
     </row>
     <row r="107" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="6">
-        <v>20174</v>
+        <v>20173</v>
       </c>
       <c r="B107" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="C107" s="1" t="s">
         <v>4</v>
@@ -2838,10 +2841,10 @@
     </row>
     <row r="108" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="6">
-        <v>20178</v>
+        <v>20174</v>
       </c>
       <c r="B108" t="s">
-        <v>117</v>
+        <v>132</v>
       </c>
       <c r="C108" s="1" t="s">
         <v>4</v>
@@ -2852,52 +2855,52 @@
     </row>
     <row r="109" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A109" s="6">
-        <v>20179</v>
+        <v>20178</v>
       </c>
       <c r="B109" t="s">
-        <v>171</v>
+        <v>117</v>
       </c>
       <c r="C109" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D109" t="s">
-        <v>9</v>
+      <c r="D109" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="110" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" s="6">
-        <v>20180</v>
+        <v>20179</v>
       </c>
       <c r="B110" t="s">
-        <v>149</v>
+        <v>171</v>
       </c>
       <c r="C110" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D110" s="1" t="s">
-        <v>8</v>
+      <c r="D110" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="111" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="6">
-        <v>20200</v>
+        <v>20180</v>
       </c>
       <c r="B111" t="s">
-        <v>83</v>
+        <v>149</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D111" s="3" t="s">
-        <v>5</v>
+      <c r="D111" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="112" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="6">
-        <v>20201</v>
+        <v>20200</v>
       </c>
       <c r="B112" t="s">
-        <v>145</v>
+        <v>83</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>4</v>
@@ -2908,24 +2911,24 @@
     </row>
     <row r="113" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A113" s="6">
-        <v>20204</v>
+        <v>20201</v>
       </c>
       <c r="B113" t="s">
-        <v>57</v>
+        <v>145</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D113" s="1" t="s">
-        <v>8</v>
+      <c r="D113" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="114" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A114" s="6">
-        <v>20205</v>
+        <v>20204</v>
       </c>
       <c r="B114" t="s">
-        <v>206</v>
+        <v>57</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>4</v>
@@ -2936,10 +2939,10 @@
     </row>
     <row r="115" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" s="6">
-        <v>20211</v>
+        <v>20205</v>
       </c>
       <c r="B115" t="s">
-        <v>190</v>
+        <v>206</v>
       </c>
       <c r="C115" s="1" t="s">
         <v>4</v>
@@ -2950,10 +2953,10 @@
     </row>
     <row r="116" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" s="6">
-        <v>20224</v>
+        <v>20211</v>
       </c>
       <c r="B116" t="s">
-        <v>85</v>
+        <v>190</v>
       </c>
       <c r="C116" s="1" t="s">
         <v>4</v>
@@ -2964,10 +2967,10 @@
     </row>
     <row r="117" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A117" s="6">
-        <v>20227</v>
+        <v>20224</v>
       </c>
       <c r="B117" t="s">
-        <v>192</v>
+        <v>85</v>
       </c>
       <c r="C117" s="1" t="s">
         <v>4</v>
@@ -2978,52 +2981,52 @@
     </row>
     <row r="118" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A118" s="6">
-        <v>20228</v>
+        <v>20227</v>
       </c>
       <c r="B118" t="s">
-        <v>91</v>
+        <v>192</v>
       </c>
       <c r="C118" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D118" s="3" t="s">
-        <v>5</v>
+      <c r="D118" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="119" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A119" s="6">
-        <v>20230</v>
+        <v>20228</v>
       </c>
       <c r="B119" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C119" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D119" s="1" t="s">
-        <v>8</v>
+      <c r="D119" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="120" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A120" s="6">
-        <v>20234</v>
+        <v>20230</v>
       </c>
       <c r="B120" t="s">
-        <v>29</v>
+        <v>89</v>
       </c>
       <c r="C120" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D120" s="3" t="s">
-        <v>5</v>
+      <c r="D120" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="121" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A121" s="6">
-        <v>20236</v>
+        <v>20234</v>
       </c>
       <c r="B121" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C121" s="1" t="s">
         <v>4</v>
@@ -3034,10 +3037,10 @@
     </row>
     <row r="122" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A122" s="6">
-        <v>20238</v>
+        <v>20236</v>
       </c>
       <c r="B122" t="s">
-        <v>139</v>
+        <v>31</v>
       </c>
       <c r="C122" s="1" t="s">
         <v>4</v>
@@ -3048,10 +3051,10 @@
     </row>
     <row r="123" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A123" s="6">
-        <v>20241</v>
+        <v>20238</v>
       </c>
       <c r="B123" t="s">
-        <v>22</v>
+        <v>139</v>
       </c>
       <c r="C123" s="1" t="s">
         <v>4</v>
@@ -3062,24 +3065,24 @@
     </row>
     <row r="124" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" s="6">
-        <v>20242</v>
+        <v>20241</v>
       </c>
       <c r="B124" t="s">
-        <v>216</v>
+        <v>22</v>
       </c>
       <c r="C124" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D124" s="1" t="s">
-        <v>8</v>
+      <c r="D124" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="125" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A125" s="6">
-        <v>20244</v>
+        <v>20242</v>
       </c>
       <c r="B125" t="s">
-        <v>124</v>
+        <v>216</v>
       </c>
       <c r="C125" s="1" t="s">
         <v>4</v>
@@ -3090,38 +3093,38 @@
     </row>
     <row r="126" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A126" s="6">
-        <v>20246</v>
+        <v>20244</v>
       </c>
       <c r="B126" t="s">
-        <v>14</v>
+        <v>124</v>
       </c>
       <c r="C126" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D126" s="3" t="s">
-        <v>5</v>
+      <c r="D126" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="127" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A127" s="6">
-        <v>20249</v>
+        <v>20246</v>
       </c>
       <c r="B127" t="s">
-        <v>72</v>
+        <v>14</v>
       </c>
       <c r="C127" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D127" s="1" t="s">
-        <v>8</v>
+      <c r="D127" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="128" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A128" s="6">
-        <v>20256</v>
+        <v>20249</v>
       </c>
       <c r="B128" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="C128" s="1" t="s">
         <v>4</v>
@@ -3132,66 +3135,66 @@
     </row>
     <row r="129" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A129" s="6">
-        <v>20257</v>
+        <v>20256</v>
       </c>
       <c r="B129" t="s">
-        <v>150</v>
+        <v>50</v>
       </c>
       <c r="C129" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D129" t="s">
-        <v>9</v>
+      <c r="D129" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="130" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A130" s="6">
-        <v>20258</v>
+        <v>20257</v>
       </c>
       <c r="B130" t="s">
-        <v>199</v>
+        <v>150</v>
       </c>
       <c r="C130" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D130" s="1" t="s">
-        <v>8</v>
+      <c r="D130" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="131" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A131" s="6">
-        <v>20260</v>
+        <v>20258</v>
       </c>
       <c r="B131" t="s">
-        <v>68</v>
+        <v>199</v>
       </c>
       <c r="C131" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D131" s="3" t="s">
-        <v>5</v>
+      <c r="D131" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="132" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A132" s="6">
-        <v>20261</v>
+        <v>20260</v>
       </c>
       <c r="B132" t="s">
-        <v>207</v>
+        <v>68</v>
       </c>
       <c r="C132" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D132" s="1" t="s">
-        <v>8</v>
+      <c r="D132" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="133" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A133" s="6">
-        <v>20262</v>
+        <v>20261</v>
       </c>
       <c r="B133" t="s">
-        <v>92</v>
+        <v>207</v>
       </c>
       <c r="C133" s="1" t="s">
         <v>4</v>
@@ -3202,10 +3205,10 @@
     </row>
     <row r="134" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A134" s="6">
-        <v>20268</v>
+        <v>20262</v>
       </c>
       <c r="B134" t="s">
-        <v>201</v>
+        <v>92</v>
       </c>
       <c r="C134" s="1" t="s">
         <v>4</v>
@@ -3216,150 +3219,150 @@
     </row>
     <row r="135" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A135" s="6">
-        <v>20271</v>
+        <v>20268</v>
       </c>
       <c r="B135" t="s">
-        <v>34</v>
+        <v>201</v>
       </c>
       <c r="C135" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D135" s="3" t="s">
-        <v>5</v>
+      <c r="D135" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="136" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A136" s="6">
-        <v>20272</v>
+        <v>20271</v>
       </c>
       <c r="B136" t="s">
-        <v>178</v>
+        <v>34</v>
       </c>
       <c r="C136" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D136" s="1" t="s">
-        <v>8</v>
+      <c r="D136" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="137" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A137" s="6">
-        <v>20275</v>
+        <v>20272</v>
       </c>
       <c r="B137" t="s">
-        <v>166</v>
+        <v>178</v>
       </c>
       <c r="C137" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D137" s="3" t="s">
-        <v>5</v>
+      <c r="D137" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="138" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A138" s="6">
-        <v>20277</v>
+        <v>20275</v>
       </c>
       <c r="B138" t="s">
-        <v>154</v>
+        <v>166</v>
       </c>
       <c r="C138" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D138" s="1" t="s">
-        <v>8</v>
+      <c r="D138" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="139" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A139" s="6">
-        <v>20281</v>
+        <v>20277</v>
       </c>
       <c r="B139" t="s">
-        <v>105</v>
+        <v>154</v>
       </c>
       <c r="C139" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D139" s="3" t="s">
-        <v>5</v>
+      <c r="D139" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="140" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A140" s="6">
-        <v>20282</v>
+        <v>20281</v>
       </c>
       <c r="B140" t="s">
-        <v>141</v>
+        <v>105</v>
       </c>
       <c r="C140" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D140" s="1" t="s">
-        <v>8</v>
+      <c r="D140" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="141" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A141" s="6">
-        <v>20284</v>
+        <v>20282</v>
       </c>
       <c r="B141" t="s">
-        <v>17</v>
+        <v>141</v>
       </c>
       <c r="C141" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D141" t="s">
-        <v>9</v>
+      <c r="D141" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="142" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A142" s="6">
-        <v>20285</v>
+        <v>20284</v>
       </c>
       <c r="B142" t="s">
-        <v>146</v>
+        <v>17</v>
       </c>
       <c r="C142" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D142" s="1" t="s">
-        <v>8</v>
+      <c r="D142" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="143" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A143" s="6">
-        <v>20289</v>
+        <v>20285</v>
       </c>
       <c r="B143" t="s">
-        <v>52</v>
+        <v>146</v>
       </c>
       <c r="C143" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D143" s="3" t="s">
-        <v>5</v>
+      <c r="D143" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="144" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A144" s="6">
-        <v>20290</v>
+        <v>20289</v>
       </c>
       <c r="B144" t="s">
-        <v>103</v>
+        <v>52</v>
       </c>
       <c r="C144" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D144" s="1" t="s">
-        <v>8</v>
+      <c r="D144" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="145" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A145" s="6">
-        <v>20291</v>
+        <v>20290</v>
       </c>
       <c r="B145" t="s">
-        <v>187</v>
+        <v>103</v>
       </c>
       <c r="C145" s="1" t="s">
         <v>4</v>
@@ -3370,24 +3373,24 @@
     </row>
     <row r="146" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A146" s="6">
-        <v>20292</v>
+        <v>20291</v>
       </c>
       <c r="B146" t="s">
-        <v>32</v>
+        <v>187</v>
       </c>
       <c r="C146" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D146" s="3" t="s">
-        <v>5</v>
+      <c r="D146" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="147" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A147" s="6">
-        <v>20293</v>
+        <v>20292</v>
       </c>
       <c r="B147" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="C147" s="1" t="s">
         <v>4</v>
@@ -3398,52 +3401,52 @@
     </row>
     <row r="148" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A148" s="6">
-        <v>20294</v>
+        <v>20293</v>
       </c>
       <c r="B148" t="s">
-        <v>202</v>
+        <v>43</v>
       </c>
       <c r="C148" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D148" s="1" t="s">
-        <v>8</v>
+      <c r="D148" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="149" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A149" s="6">
-        <v>20296</v>
+        <v>20294</v>
       </c>
       <c r="B149" t="s">
-        <v>144</v>
+        <v>202</v>
       </c>
       <c r="C149" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D149" s="3" t="s">
-        <v>5</v>
+      <c r="D149" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="150" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A150" s="6">
-        <v>20298</v>
+        <v>20296</v>
       </c>
       <c r="B150" t="s">
-        <v>169</v>
+        <v>144</v>
       </c>
       <c r="C150" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D150" s="1" t="s">
-        <v>8</v>
+      <c r="D150" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="151" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A151" s="6">
-        <v>20299</v>
+        <v>20298</v>
       </c>
       <c r="B151" t="s">
-        <v>58</v>
+        <v>169</v>
       </c>
       <c r="C151" s="1" t="s">
         <v>4</v>
@@ -3454,10 +3457,10 @@
     </row>
     <row r="152" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A152" s="6">
-        <v>20301</v>
+        <v>20299</v>
       </c>
       <c r="B152" t="s">
-        <v>134</v>
+        <v>58</v>
       </c>
       <c r="C152" s="1" t="s">
         <v>4</v>
@@ -3468,10 +3471,10 @@
     </row>
     <row r="153" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A153" s="6">
-        <v>20303</v>
+        <v>20301</v>
       </c>
       <c r="B153" t="s">
-        <v>37</v>
+        <v>134</v>
       </c>
       <c r="C153" s="1" t="s">
         <v>4</v>
@@ -3482,24 +3485,24 @@
     </row>
     <row r="154" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A154" s="6">
-        <v>20309</v>
+        <v>20303</v>
       </c>
       <c r="B154" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="C154" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D154" s="3" t="s">
-        <v>5</v>
+      <c r="D154" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="155" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A155" s="6">
-        <v>20310</v>
+        <v>20309</v>
       </c>
       <c r="B155" t="s">
-        <v>59</v>
+        <v>28</v>
       </c>
       <c r="C155" s="1" t="s">
         <v>4</v>
@@ -3510,24 +3513,24 @@
     </row>
     <row r="156" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A156" s="6">
-        <v>20318</v>
+        <v>20310</v>
       </c>
       <c r="B156" t="s">
-        <v>209</v>
+        <v>59</v>
       </c>
       <c r="C156" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D156" s="1" t="s">
-        <v>8</v>
+      <c r="D156" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="157" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A157" s="6">
-        <v>20319</v>
+        <v>20318</v>
       </c>
       <c r="B157" t="s">
-        <v>101</v>
+        <v>209</v>
       </c>
       <c r="C157" s="1" t="s">
         <v>4</v>
@@ -3538,10 +3541,10 @@
     </row>
     <row r="158" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A158" s="6">
-        <v>20320</v>
+        <v>20319</v>
       </c>
       <c r="B158" t="s">
-        <v>130</v>
+        <v>101</v>
       </c>
       <c r="C158" s="1" t="s">
         <v>4</v>
@@ -3552,10 +3555,10 @@
     </row>
     <row r="159" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A159" s="6">
-        <v>20324</v>
+        <v>20320</v>
       </c>
       <c r="B159" t="s">
-        <v>210</v>
+        <v>130</v>
       </c>
       <c r="C159" s="1" t="s">
         <v>4</v>
@@ -3566,10 +3569,10 @@
     </row>
     <row r="160" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A160" s="6">
-        <v>20331</v>
+        <v>20324</v>
       </c>
       <c r="B160" t="s">
-        <v>51</v>
+        <v>210</v>
       </c>
       <c r="C160" s="1" t="s">
         <v>4</v>
@@ -3580,38 +3583,38 @@
     </row>
     <row r="161" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A161" s="6">
-        <v>20333</v>
+        <v>20331</v>
       </c>
       <c r="B161" t="s">
-        <v>136</v>
+        <v>51</v>
       </c>
       <c r="C161" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D161" s="3" t="s">
-        <v>5</v>
+      <c r="D161" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="162" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A162" s="6">
-        <v>20337</v>
+        <v>20333</v>
       </c>
       <c r="B162" t="s">
-        <v>104</v>
+        <v>136</v>
       </c>
       <c r="C162" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D162" s="1" t="s">
-        <v>8</v>
+      <c r="D162" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="163" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A163" s="6">
-        <v>20343</v>
+        <v>20337</v>
       </c>
       <c r="B163" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="C163" s="1" t="s">
         <v>4</v>
@@ -3622,10 +3625,10 @@
     </row>
     <row r="164" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A164" s="6">
-        <v>20344</v>
+        <v>20343</v>
       </c>
       <c r="B164" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="C164" s="1" t="s">
         <v>4</v>
@@ -3636,66 +3639,66 @@
     </row>
     <row r="165" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A165" s="6">
-        <v>20351</v>
+        <v>20344</v>
       </c>
       <c r="B165" t="s">
-        <v>26</v>
+        <v>127</v>
       </c>
       <c r="C165" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D165" s="3" t="s">
-        <v>5</v>
+      <c r="D165" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="166" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A166" s="6">
-        <v>20357</v>
+        <v>20351</v>
       </c>
       <c r="B166" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="C166" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D166" s="1" t="s">
-        <v>8</v>
+      <c r="D166" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="167" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A167" s="6">
-        <v>20361</v>
+        <v>20357</v>
       </c>
       <c r="B167" t="s">
-        <v>164</v>
+        <v>56</v>
       </c>
       <c r="C167" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D167" s="3" t="s">
-        <v>5</v>
+      <c r="D167" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="168" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A168" s="6">
-        <v>20362</v>
+        <v>20361</v>
       </c>
       <c r="B168" t="s">
-        <v>45</v>
+        <v>164</v>
       </c>
       <c r="C168" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D168" s="1" t="s">
-        <v>8</v>
+      <c r="D168" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="169" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A169" s="6">
-        <v>20363</v>
+        <v>20362</v>
       </c>
       <c r="B169" t="s">
-        <v>213</v>
+        <v>45</v>
       </c>
       <c r="C169" s="1" t="s">
         <v>4</v>
@@ -3706,38 +3709,38 @@
     </row>
     <row r="170" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A170" s="6">
-        <v>20364</v>
+        <v>20363</v>
       </c>
       <c r="B170" t="s">
-        <v>196</v>
+        <v>213</v>
       </c>
       <c r="C170" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D170" s="3" t="s">
-        <v>5</v>
+      <c r="D170" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="171" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A171" s="6">
-        <v>20366</v>
+        <v>20364</v>
       </c>
       <c r="B171" t="s">
-        <v>220</v>
+        <v>196</v>
       </c>
       <c r="C171" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D171" s="1" t="s">
-        <v>8</v>
+      <c r="D171" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="172" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A172" s="6">
-        <v>20367</v>
+        <v>20366</v>
       </c>
       <c r="B172" t="s">
-        <v>47</v>
+        <v>220</v>
       </c>
       <c r="C172" s="1" t="s">
         <v>4</v>
@@ -3748,10 +3751,10 @@
     </row>
     <row r="173" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A173" s="6">
-        <v>20369</v>
+        <v>20367</v>
       </c>
       <c r="B173" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="C173" s="1" t="s">
         <v>4</v>
@@ -3762,10 +3765,10 @@
     </row>
     <row r="174" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A174" s="6">
-        <v>20371</v>
+        <v>20369</v>
       </c>
       <c r="B174" t="s">
-        <v>223</v>
+        <v>63</v>
       </c>
       <c r="C174" s="1" t="s">
         <v>4</v>
@@ -3776,10 +3779,10 @@
     </row>
     <row r="175" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A175" s="6">
-        <v>20372</v>
+        <v>20371</v>
       </c>
       <c r="B175" t="s">
-        <v>70</v>
+        <v>223</v>
       </c>
       <c r="C175" s="1" t="s">
         <v>4</v>
@@ -3790,10 +3793,10 @@
     </row>
     <row r="176" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A176" s="6">
-        <v>20374</v>
+        <v>20372</v>
       </c>
       <c r="B176" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="C176" s="1" t="s">
         <v>4</v>
@@ -3804,10 +3807,10 @@
     </row>
     <row r="177" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A177" s="6">
-        <v>20377</v>
+        <v>20374</v>
       </c>
       <c r="B177" t="s">
-        <v>225</v>
+        <v>61</v>
       </c>
       <c r="C177" s="1" t="s">
         <v>4</v>
@@ -3818,10 +3821,10 @@
     </row>
     <row r="178" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A178" s="6">
-        <v>20379</v>
+        <v>20377</v>
       </c>
       <c r="B178" t="s">
-        <v>49</v>
+        <v>225</v>
       </c>
       <c r="C178" s="1" t="s">
         <v>4</v>
@@ -3832,38 +3835,38 @@
     </row>
     <row r="179" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A179" s="6">
-        <v>20380</v>
+        <v>20379</v>
       </c>
       <c r="B179" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="C179" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D179" s="3" t="s">
-        <v>5</v>
+      <c r="D179" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="180" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A180" s="6">
-        <v>20381</v>
+        <v>20380</v>
       </c>
       <c r="B180" t="s">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="C180" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D180" s="1" t="s">
-        <v>8</v>
+      <c r="D180" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="181" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A181" s="6">
-        <v>20384</v>
+        <v>20381</v>
       </c>
       <c r="B181" t="s">
-        <v>181</v>
+        <v>60</v>
       </c>
       <c r="C181" s="1" t="s">
         <v>4</v>
@@ -3874,10 +3877,10 @@
     </row>
     <row r="182" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A182" s="6">
-        <v>20385</v>
+        <v>20384</v>
       </c>
       <c r="B182" t="s">
-        <v>36</v>
+        <v>181</v>
       </c>
       <c r="C182" s="1" t="s">
         <v>4</v>
@@ -3888,10 +3891,10 @@
     </row>
     <row r="183" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A183" s="6">
-        <v>20386</v>
+        <v>20385</v>
       </c>
       <c r="B183" t="s">
-        <v>119</v>
+        <v>36</v>
       </c>
       <c r="C183" s="1" t="s">
         <v>4</v>
@@ -3902,10 +3905,10 @@
     </row>
     <row r="184" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A184" s="6">
-        <v>20388</v>
+        <v>20386</v>
       </c>
       <c r="B184" t="s">
-        <v>100</v>
+        <v>119</v>
       </c>
       <c r="C184" s="1" t="s">
         <v>4</v>
@@ -3916,10 +3919,10 @@
     </row>
     <row r="185" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A185" s="6">
-        <v>20391</v>
+        <v>20388</v>
       </c>
       <c r="B185" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C185" s="1" t="s">
         <v>4</v>
@@ -3930,10 +3933,10 @@
     </row>
     <row r="186" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A186" s="6">
-        <v>20394</v>
+        <v>20391</v>
       </c>
       <c r="B186" t="s">
-        <v>173</v>
+        <v>106</v>
       </c>
       <c r="C186" s="1" t="s">
         <v>4</v>
@@ -3944,10 +3947,10 @@
     </row>
     <row r="187" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A187" s="6">
-        <v>20395</v>
+        <v>20394</v>
       </c>
       <c r="B187" t="s">
-        <v>161</v>
+        <v>173</v>
       </c>
       <c r="C187" s="1" t="s">
         <v>4</v>
@@ -3958,10 +3961,10 @@
     </row>
     <row r="188" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A188" s="6">
-        <v>30101</v>
+        <v>20395</v>
       </c>
       <c r="B188" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="C188" s="1" t="s">
         <v>4</v>
@@ -3972,24 +3975,24 @@
     </row>
     <row r="189" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A189" s="6">
-        <v>40124</v>
+        <v>30101</v>
       </c>
       <c r="B189" t="s">
-        <v>24</v>
+        <v>167</v>
       </c>
       <c r="C189" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D189" s="3" t="s">
-        <v>5</v>
+      <c r="D189" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="190" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A190" s="6">
-        <v>40125</v>
+        <v>40124</v>
       </c>
       <c r="B190" t="s">
-        <v>143</v>
+        <v>24</v>
       </c>
       <c r="C190" s="1" t="s">
         <v>4</v>
@@ -4000,24 +4003,24 @@
     </row>
     <row r="191" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A191" s="6">
-        <v>40127</v>
+        <v>40125</v>
       </c>
       <c r="B191" t="s">
-        <v>163</v>
+        <v>143</v>
       </c>
       <c r="C191" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D191" s="1" t="s">
-        <v>8</v>
+      <c r="D191" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="192" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A192" s="6">
-        <v>40129</v>
+        <v>40127</v>
       </c>
       <c r="B192" t="s">
-        <v>138</v>
+        <v>163</v>
       </c>
       <c r="C192" s="1" t="s">
         <v>4</v>
@@ -4028,10 +4031,10 @@
     </row>
     <row r="193" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A193" s="6">
-        <v>40137</v>
+        <v>40129</v>
       </c>
       <c r="B193" t="s">
-        <v>121</v>
+        <v>138</v>
       </c>
       <c r="C193" s="1" t="s">
         <v>4</v>
@@ -4042,10 +4045,10 @@
     </row>
     <row r="194" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A194" s="6">
-        <v>40140</v>
+        <v>40137</v>
       </c>
       <c r="B194" t="s">
-        <v>170</v>
+        <v>121</v>
       </c>
       <c r="C194" s="1" t="s">
         <v>4</v>
@@ -4056,52 +4059,52 @@
     </row>
     <row r="195" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A195" s="6">
-        <v>40141</v>
+        <v>40140</v>
       </c>
       <c r="B195" t="s">
-        <v>111</v>
+        <v>170</v>
       </c>
       <c r="C195" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D195" s="3" t="s">
-        <v>5</v>
+      <c r="D195" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="196" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A196" s="6">
-        <v>40143</v>
+        <v>40141</v>
       </c>
       <c r="B196" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
       <c r="C196" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D196" s="1" t="s">
-        <v>8</v>
+      <c r="D196" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="197" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A197" s="6">
-        <v>40144</v>
+        <v>40143</v>
       </c>
       <c r="B197" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="C197" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D197" s="3" t="s">
-        <v>5</v>
+      <c r="D197" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="198" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A198" s="6">
-        <v>40145</v>
+        <v>40144</v>
       </c>
       <c r="B198" t="s">
-        <v>165</v>
+        <v>107</v>
       </c>
       <c r="C198" s="1" t="s">
         <v>4</v>
@@ -4112,24 +4115,24 @@
     </row>
     <row r="199" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A199" s="6">
-        <v>40150</v>
+        <v>40145</v>
       </c>
       <c r="B199" t="s">
-        <v>221</v>
+        <v>165</v>
       </c>
       <c r="C199" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D199" s="1" t="s">
-        <v>8</v>
+      <c r="D199" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="200" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A200" s="6">
-        <v>40151</v>
+        <v>40150</v>
       </c>
       <c r="B200" t="s">
-        <v>54</v>
+        <v>221</v>
       </c>
       <c r="C200" s="1" t="s">
         <v>4</v>
@@ -4140,38 +4143,38 @@
     </row>
     <row r="201" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A201" s="6">
-        <v>50102</v>
+        <v>40151</v>
       </c>
       <c r="B201" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="C201" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D201" s="3" t="s">
-        <v>5</v>
+      <c r="D201" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="202" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A202" s="6">
-        <v>50222</v>
+        <v>50102</v>
       </c>
       <c r="B202" t="s">
-        <v>215</v>
+        <v>67</v>
       </c>
       <c r="C202" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D202" s="1" t="s">
-        <v>8</v>
+      <c r="D202" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="203" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A203" s="6">
-        <v>50223</v>
+        <v>50222</v>
       </c>
       <c r="B203" t="s">
-        <v>194</v>
+        <v>215</v>
       </c>
       <c r="C203" s="1" t="s">
         <v>4</v>
@@ -4182,66 +4185,66 @@
     </row>
     <row r="204" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A204" s="6">
-        <v>50224</v>
+        <v>50223</v>
       </c>
       <c r="B204" t="s">
-        <v>42</v>
+        <v>194</v>
       </c>
       <c r="C204" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D204" s="3" t="s">
-        <v>5</v>
+      <c r="D204" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="205" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A205" s="6">
-        <v>50444</v>
+        <v>50224</v>
       </c>
       <c r="B205" t="s">
-        <v>116</v>
+        <v>42</v>
       </c>
       <c r="C205" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D205" s="1" t="s">
-        <v>8</v>
+      <c r="D205" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="206" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A206" s="6">
-        <v>50607</v>
+        <v>50444</v>
       </c>
       <c r="B206" t="s">
-        <v>76</v>
+        <v>116</v>
       </c>
       <c r="C206" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D206" s="3" t="s">
-        <v>5</v>
+      <c r="D206" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="207" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A207" s="6">
-        <v>50608</v>
+        <v>50607</v>
       </c>
       <c r="B207" t="s">
-        <v>177</v>
+        <v>76</v>
       </c>
       <c r="C207" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D207" s="1" t="s">
-        <v>8</v>
+      <c r="D207" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="208" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A208" s="6">
-        <v>50622</v>
+        <v>50608</v>
       </c>
       <c r="B208" t="s">
-        <v>95</v>
+        <v>177</v>
       </c>
       <c r="C208" s="1" t="s">
         <v>4</v>
@@ -4252,10 +4255,10 @@
     </row>
     <row r="209" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A209" s="6">
-        <v>50623</v>
+        <v>50622</v>
       </c>
       <c r="B209" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="C209" s="1" t="s">
         <v>4</v>
@@ -4266,10 +4269,10 @@
     </row>
     <row r="210" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A210" s="6">
-        <v>50625</v>
+        <v>50623</v>
       </c>
       <c r="B210" t="s">
-        <v>204</v>
+        <v>110</v>
       </c>
       <c r="C210" s="1" t="s">
         <v>4</v>
@@ -4280,10 +4283,10 @@
     </row>
     <row r="211" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A211" s="6">
-        <v>50629</v>
+        <v>50625</v>
       </c>
       <c r="B211" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="C211" s="1" t="s">
         <v>4</v>
@@ -4294,10 +4297,10 @@
     </row>
     <row r="212" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A212" s="6">
-        <v>50803</v>
+        <v>50629</v>
       </c>
       <c r="B212" t="s">
-        <v>82</v>
+        <v>188</v>
       </c>
       <c r="C212" s="1" t="s">
         <v>4</v>
@@ -4308,10 +4311,10 @@
     </row>
     <row r="213" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A213" s="6">
-        <v>50805</v>
+        <v>50803</v>
       </c>
       <c r="B213" t="s">
-        <v>135</v>
+        <v>82</v>
       </c>
       <c r="C213" s="1" t="s">
         <v>4</v>
@@ -4322,10 +4325,10 @@
     </row>
     <row r="214" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A214" s="6">
-        <v>50806</v>
+        <v>50805</v>
       </c>
       <c r="B214" t="s">
-        <v>156</v>
+        <v>135</v>
       </c>
       <c r="C214" s="1" t="s">
         <v>4</v>
@@ -4336,24 +4339,24 @@
     </row>
     <row r="215" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A215" s="6">
-        <v>50808</v>
+        <v>50806</v>
       </c>
       <c r="B215" t="s">
-        <v>16</v>
+        <v>156</v>
       </c>
       <c r="C215" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D215" s="3" t="s">
-        <v>5</v>
+      <c r="D215" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="216" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A216" s="6">
-        <v>50809</v>
+        <v>50808</v>
       </c>
       <c r="B216" t="s">
-        <v>98</v>
+        <v>16</v>
       </c>
       <c r="C216" s="1" t="s">
         <v>4</v>
@@ -4364,24 +4367,24 @@
     </row>
     <row r="217" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A217" s="6">
-        <v>50810</v>
+        <v>50809</v>
       </c>
       <c r="B217" t="s">
-        <v>175</v>
+        <v>98</v>
       </c>
       <c r="C217" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D217" s="1" t="s">
-        <v>8</v>
+      <c r="D217" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="218" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A218" s="6">
-        <v>50812</v>
+        <v>50810</v>
       </c>
       <c r="B218" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="C218" s="1" t="s">
         <v>4</v>
@@ -4392,38 +4395,38 @@
     </row>
     <row r="219" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A219" s="6">
-        <v>50813</v>
+        <v>50812</v>
       </c>
       <c r="B219" t="s">
-        <v>71</v>
+        <v>184</v>
       </c>
       <c r="C219" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D219" t="s">
-        <v>9</v>
+      <c r="D219" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="220" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A220" s="6">
-        <v>50815</v>
+        <v>50813</v>
       </c>
       <c r="B220" t="s">
-        <v>114</v>
+        <v>71</v>
       </c>
       <c r="C220" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D220" s="1" t="s">
-        <v>8</v>
+      <c r="D220" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="221" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A221" s="6">
-        <v>50816</v>
+        <v>50815</v>
       </c>
       <c r="B221" t="s">
-        <v>205</v>
+        <v>114</v>
       </c>
       <c r="C221" s="1" t="s">
         <v>4</v>
@@ -4434,38 +4437,38 @@
     </row>
     <row r="222" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A222" s="6">
-        <v>50818</v>
+        <v>50816</v>
       </c>
       <c r="B222" t="s">
-        <v>227</v>
+        <v>205</v>
       </c>
       <c r="C222" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D222" s="3" t="s">
-        <v>5</v>
+      <c r="D222" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="223" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A223" s="6">
-        <v>50819</v>
+        <v>50818</v>
       </c>
       <c r="B223" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C223" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D223" s="1" t="s">
-        <v>8</v>
+      <c r="D223" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="224" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A224" s="6">
-        <v>50820</v>
+        <v>50819</v>
       </c>
       <c r="B224" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C224" s="1" t="s">
         <v>4</v>
@@ -4476,10 +4479,10 @@
     </row>
     <row r="225" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A225" s="6">
-        <v>50821</v>
+        <v>50820</v>
       </c>
       <c r="B225" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C225" s="1" t="s">
         <v>4</v>
@@ -4490,52 +4493,52 @@
     </row>
     <row r="226" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A226" s="6">
-        <v>50823</v>
+        <v>50821</v>
       </c>
       <c r="B226" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C226" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D226" t="s">
-        <v>9</v>
+      <c r="D226" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="227" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A227" s="6">
-        <v>50824</v>
+        <v>50823</v>
       </c>
       <c r="B227" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C227" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D227" s="3" t="s">
-        <v>5</v>
+      <c r="D227" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="228" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A228" s="6">
-        <v>50825</v>
+        <v>50824</v>
       </c>
       <c r="B228" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C228" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D228" s="1" t="s">
-        <v>8</v>
+      <c r="D228" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="229" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A229" s="6">
-        <v>50826</v>
+        <v>50825</v>
       </c>
       <c r="B229" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C229" s="1" t="s">
         <v>4</v>
@@ -4546,10 +4549,10 @@
     </row>
     <row r="230" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A230" s="6">
-        <v>50827</v>
+        <v>50826</v>
       </c>
       <c r="B230" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C230" s="1" t="s">
         <v>4</v>
@@ -4560,10 +4563,10 @@
     </row>
     <row r="231" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A231" s="6">
-        <v>50829</v>
+        <v>50827</v>
       </c>
       <c r="B231" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C231" s="1" t="s">
         <v>4</v>
@@ -4574,24 +4577,24 @@
     </row>
     <row r="232" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A232" s="6">
-        <v>60103</v>
+        <v>50829</v>
       </c>
       <c r="B232" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C232" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D232" s="3" t="s">
-        <v>5</v>
+      <c r="D232" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="233" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A233" s="6">
-        <v>60124</v>
+        <v>60103</v>
       </c>
       <c r="B233" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C233" s="1" t="s">
         <v>4</v>
@@ -4602,10 +4605,10 @@
     </row>
     <row r="234" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A234" s="6">
-        <v>60125</v>
+        <v>60124</v>
       </c>
       <c r="B234" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C234" s="1" t="s">
         <v>4</v>
@@ -4616,80 +4619,80 @@
     </row>
     <row r="235" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A235" s="6">
-        <v>60126</v>
+        <v>60125</v>
       </c>
       <c r="B235" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C235" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D235" s="1" t="s">
-        <v>8</v>
+      <c r="D235" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="236" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A236" s="6">
-        <v>60128</v>
+        <v>60126</v>
       </c>
       <c r="B236" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C236" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D236" s="3" t="s">
-        <v>5</v>
+      <c r="D236" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="237" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A237" s="6">
-        <v>60130</v>
+        <v>60128</v>
       </c>
       <c r="B237" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C237" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D237" s="1" t="s">
-        <v>8</v>
+      <c r="D237" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="238" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A238" s="6">
-        <v>60133</v>
+        <v>60130</v>
       </c>
       <c r="B238" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C238" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D238" s="3" t="s">
-        <v>5</v>
+      <c r="D238" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="239" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A239" s="6">
-        <v>60134</v>
+        <v>60133</v>
       </c>
       <c r="B239" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C239" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D239" s="1" t="s">
-        <v>8</v>
+      <c r="D239" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="240" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A240" s="6">
-        <v>60137</v>
+        <v>60134</v>
       </c>
       <c r="B240" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C240" s="1" t="s">
         <v>4</v>
@@ -4700,10 +4703,10 @@
     </row>
     <row r="241" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A241" s="6">
-        <v>60139</v>
+        <v>60137</v>
       </c>
       <c r="B241" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C241" s="1" t="s">
         <v>4</v>
@@ -4714,10 +4717,10 @@
     </row>
     <row r="242" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A242" s="6">
-        <v>60142</v>
+        <v>60139</v>
       </c>
       <c r="B242" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C242" s="1" t="s">
         <v>4</v>
@@ -4728,10 +4731,10 @@
     </row>
     <row r="243" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A243" s="6">
-        <v>60148</v>
+        <v>60142</v>
       </c>
       <c r="B243" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C243" s="1" t="s">
         <v>4</v>
@@ -4742,10 +4745,10 @@
     </row>
     <row r="244" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A244" s="6">
-        <v>60149</v>
+        <v>60148</v>
       </c>
       <c r="B244" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C244" s="1" t="s">
         <v>4</v>
@@ -4756,10 +4759,10 @@
     </row>
     <row r="245" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A245" s="6">
-        <v>60158</v>
+        <v>60149</v>
       </c>
       <c r="B245" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C245" s="1" t="s">
         <v>4</v>
@@ -4770,10 +4773,10 @@
     </row>
     <row r="246" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A246" s="6">
-        <v>60159</v>
+        <v>60158</v>
       </c>
       <c r="B246" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C246" s="1" t="s">
         <v>4</v>
@@ -4784,24 +4787,24 @@
     </row>
     <row r="247" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A247" s="6">
-        <v>60162</v>
+        <v>60159</v>
       </c>
       <c r="B247" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C247" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D247" s="3" t="s">
-        <v>5</v>
+      <c r="D247" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="248" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A248" s="6">
-        <v>60163</v>
+        <v>60162</v>
       </c>
       <c r="B248" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C248" s="1" t="s">
         <v>4</v>
@@ -4812,24 +4815,24 @@
     </row>
     <row r="249" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A249" s="6">
-        <v>60165</v>
+        <v>60163</v>
       </c>
       <c r="B249" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C249" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D249" s="1" t="s">
-        <v>8</v>
+      <c r="D249" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="250" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A250" s="6">
-        <v>60169</v>
+        <v>60165</v>
       </c>
       <c r="B250" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C250" s="1" t="s">
         <v>4</v>
@@ -4840,10 +4843,10 @@
     </row>
     <row r="251" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A251" s="6">
-        <v>60172</v>
+        <v>60169</v>
       </c>
       <c r="B251" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C251" s="1" t="s">
         <v>4</v>
@@ -4854,24 +4857,24 @@
     </row>
     <row r="252" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A252" s="6">
-        <v>60174</v>
+        <v>60172</v>
       </c>
       <c r="B252" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C252" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D252" s="3" t="s">
-        <v>5</v>
+      <c r="D252" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="253" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A253" s="6">
-        <v>60176</v>
+        <v>60174</v>
       </c>
       <c r="B253" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C253" s="1" t="s">
         <v>4</v>
@@ -4882,24 +4885,24 @@
     </row>
     <row r="254" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A254" s="6">
-        <v>60178</v>
+        <v>60176</v>
       </c>
       <c r="B254" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C254" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D254" s="1" t="s">
-        <v>8</v>
+      <c r="D254" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="255" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A255" s="6">
-        <v>60180</v>
+        <v>60178</v>
       </c>
       <c r="B255" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C255" s="1" t="s">
         <v>4</v>
@@ -4910,10 +4913,10 @@
     </row>
     <row r="256" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A256" s="6">
-        <v>60184</v>
+        <v>60180</v>
       </c>
       <c r="B256" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C256" s="1" t="s">
         <v>4</v>
@@ -4924,10 +4927,10 @@
     </row>
     <row r="257" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A257" s="6">
-        <v>60190</v>
+        <v>60184</v>
       </c>
       <c r="B257" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C257" s="1" t="s">
         <v>4</v>
@@ -4938,10 +4941,10 @@
     </row>
     <row r="258" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A258" s="6">
-        <v>60191</v>
+        <v>60190</v>
       </c>
       <c r="B258" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C258" s="1" t="s">
         <v>4</v>
@@ -4952,10 +4955,10 @@
     </row>
     <row r="259" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A259" s="6">
-        <v>60192</v>
+        <v>60191</v>
       </c>
       <c r="B259" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C259" s="1" t="s">
         <v>4</v>
@@ -4966,10 +4969,10 @@
     </row>
     <row r="260" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A260" s="6">
-        <v>60195</v>
+        <v>60192</v>
       </c>
       <c r="B260" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C260" s="1" t="s">
         <v>4</v>
@@ -4980,10 +4983,10 @@
     </row>
     <row r="261" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A261" s="6">
-        <v>60196</v>
+        <v>60195</v>
       </c>
       <c r="B261" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C261" s="1" t="s">
         <v>4</v>
@@ -4994,10 +4997,10 @@
     </row>
     <row r="262" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A262" s="6">
-        <v>60198</v>
+        <v>60196</v>
       </c>
       <c r="B262" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C262" s="1" t="s">
         <v>4</v>
@@ -5008,10 +5011,10 @@
     </row>
     <row r="263" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A263" s="6">
-        <v>60200</v>
+        <v>60198</v>
       </c>
       <c r="B263" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C263" s="1" t="s">
         <v>4</v>
@@ -5022,52 +5025,52 @@
     </row>
     <row r="264" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A264" s="6">
-        <v>60201</v>
+        <v>60200</v>
       </c>
       <c r="B264" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C264" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D264" t="s">
-        <v>9</v>
+      <c r="D264" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="265" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A265" s="6">
-        <v>60202</v>
+        <v>60201</v>
       </c>
       <c r="B265" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C265" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D265" s="3" t="s">
-        <v>5</v>
+      <c r="D265" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="266" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A266" s="6">
-        <v>60204</v>
+        <v>60202</v>
       </c>
       <c r="B266" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C266" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D266" s="1" t="s">
-        <v>8</v>
+      <c r="D266" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="267" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A267" s="6">
-        <v>60205</v>
+        <v>60204</v>
       </c>
       <c r="B267" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C267" s="1" t="s">
         <v>4</v>
@@ -5078,10 +5081,10 @@
     </row>
     <row r="268" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A268" s="6">
-        <v>60206</v>
+        <v>60205</v>
       </c>
       <c r="B268" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C268" s="1" t="s">
         <v>4</v>
@@ -5092,10 +5095,10 @@
     </row>
     <row r="269" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A269" s="6">
-        <v>60209</v>
+        <v>60206</v>
       </c>
       <c r="B269" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C269" s="1" t="s">
         <v>4</v>
@@ -5106,10 +5109,10 @@
     </row>
     <row r="270" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A270" s="6">
-        <v>60211</v>
+        <v>60209</v>
       </c>
       <c r="B270" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C270" s="1" t="s">
         <v>4</v>
@@ -5120,10 +5123,10 @@
     </row>
     <row r="271" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A271" s="6">
-        <v>60215</v>
+        <v>60211</v>
       </c>
       <c r="B271" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C271" s="1" t="s">
         <v>4</v>
@@ -5134,10 +5137,10 @@
     </row>
     <row r="272" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A272" s="6">
-        <v>60217</v>
+        <v>60215</v>
       </c>
       <c r="B272" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C272" s="1" t="s">
         <v>4</v>
@@ -5148,10 +5151,10 @@
     </row>
     <row r="273" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A273" s="6">
-        <v>60219</v>
+        <v>60217</v>
       </c>
       <c r="B273" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C273" s="1" t="s">
         <v>4</v>
@@ -5162,10 +5165,10 @@
     </row>
     <row r="274" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A274" s="6">
-        <v>60222</v>
+        <v>60219</v>
       </c>
       <c r="B274" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C274" s="1" t="s">
         <v>4</v>
@@ -5176,38 +5179,38 @@
     </row>
     <row r="275" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A275" s="6">
-        <v>60225</v>
+        <v>60222</v>
       </c>
       <c r="B275" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C275" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D275" t="s">
-        <v>9</v>
+      <c r="D275" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="276" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A276" s="6">
-        <v>60230</v>
+        <v>60225</v>
       </c>
       <c r="B276" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C276" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D276" s="1" t="s">
-        <v>8</v>
+      <c r="D276" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="277" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A277" s="6">
-        <v>60234</v>
+        <v>60230</v>
       </c>
       <c r="B277" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C277" s="1" t="s">
         <v>4</v>
@@ -5218,10 +5221,10 @@
     </row>
     <row r="278" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A278" s="6">
-        <v>60253</v>
+        <v>60234</v>
       </c>
       <c r="B278" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C278" s="1" t="s">
         <v>4</v>
@@ -5232,10 +5235,10 @@
     </row>
     <row r="279" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A279" s="6">
-        <v>60254</v>
+        <v>60253</v>
       </c>
       <c r="B279" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C279" s="1" t="s">
         <v>4</v>
@@ -5246,10 +5249,10 @@
     </row>
     <row r="280" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A280" s="6">
-        <v>60257</v>
+        <v>60254</v>
       </c>
       <c r="B280" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C280" s="1" t="s">
         <v>4</v>
@@ -5260,10 +5263,10 @@
     </row>
     <row r="281" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A281" s="6">
-        <v>60258</v>
+        <v>60257</v>
       </c>
       <c r="B281" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C281" s="1" t="s">
         <v>4</v>
@@ -5274,10 +5277,10 @@
     </row>
     <row r="282" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A282" s="6">
-        <v>60269</v>
+        <v>60258</v>
       </c>
       <c r="B282" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C282" s="1" t="s">
         <v>4</v>
@@ -5288,10 +5291,10 @@
     </row>
     <row r="283" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A283" s="6">
-        <v>60270</v>
+        <v>60269</v>
       </c>
       <c r="B283" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C283" s="1" t="s">
         <v>4</v>
@@ -5302,10 +5305,10 @@
     </row>
     <row r="284" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A284" s="6">
-        <v>60272</v>
+        <v>60270</v>
       </c>
       <c r="B284" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C284" s="1" t="s">
         <v>4</v>
@@ -5316,10 +5319,10 @@
     </row>
     <row r="285" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A285" s="6">
-        <v>60275</v>
+        <v>60272</v>
       </c>
       <c r="B285" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C285" s="1" t="s">
         <v>4</v>
@@ -5330,10 +5333,10 @@
     </row>
     <row r="286" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A286" s="6">
-        <v>60276</v>
+        <v>60275</v>
       </c>
       <c r="B286" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C286" s="1" t="s">
         <v>4</v>
@@ -5344,38 +5347,38 @@
     </row>
     <row r="287" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A287" s="6">
-        <v>60278</v>
+        <v>60276</v>
       </c>
       <c r="B287" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C287" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D287" s="3" t="s">
-        <v>5</v>
+      <c r="D287" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="288" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A288" s="6">
-        <v>60279</v>
+        <v>60278</v>
       </c>
       <c r="B288" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C288" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D288" s="1" t="s">
-        <v>8</v>
+      <c r="D288" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="289" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A289" s="6">
-        <v>60280</v>
+        <v>60279</v>
       </c>
       <c r="B289" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C289" s="1" t="s">
         <v>4</v>
@@ -5386,38 +5389,38 @@
     </row>
     <row r="290" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A290" s="6">
-        <v>61004</v>
+        <v>60280</v>
       </c>
       <c r="B290" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C290" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D290" s="3" t="s">
-        <v>5</v>
+      <c r="D290" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="291" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A291" s="6">
-        <v>61009</v>
+        <v>61004</v>
       </c>
       <c r="B291" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C291" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D291" s="1" t="s">
-        <v>8</v>
+      <c r="D291" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="292" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A292" s="6">
-        <v>61012</v>
+        <v>61009</v>
       </c>
       <c r="B292" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C292" s="1" t="s">
         <v>4</v>
@@ -5428,10 +5431,10 @@
     </row>
     <row r="293" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A293" s="6">
-        <v>61018</v>
+        <v>61012</v>
       </c>
       <c r="B293" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C293" s="1" t="s">
         <v>4</v>
@@ -5442,10 +5445,10 @@
     </row>
     <row r="294" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A294" s="6">
-        <v>61102</v>
+        <v>61018</v>
       </c>
       <c r="B294" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C294" s="1" t="s">
         <v>4</v>
@@ -5456,52 +5459,52 @@
     </row>
     <row r="295" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A295" s="6">
-        <v>61205</v>
+        <v>61102</v>
       </c>
       <c r="B295" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C295" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D295" s="3" t="s">
-        <v>5</v>
+      <c r="D295" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="296" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A296" s="6">
-        <v>70100</v>
+        <v>61205</v>
       </c>
       <c r="B296" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C296" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D296" s="1" t="s">
-        <v>8</v>
+      <c r="D296" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="297" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A297" s="6">
-        <v>70101</v>
+        <v>70100</v>
       </c>
       <c r="B297" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C297" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D297" s="3" t="s">
-        <v>5</v>
+      <c r="D297" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="298" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A298" s="6">
-        <v>70102</v>
+        <v>70101</v>
       </c>
       <c r="B298" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C298" s="1" t="s">
         <v>4</v>
@@ -5512,94 +5515,94 @@
     </row>
     <row r="299" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A299" s="6">
-        <v>70103</v>
+        <v>70102</v>
       </c>
       <c r="B299" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C299" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D299" s="1" t="s">
-        <v>8</v>
+      <c r="D299" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="300" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A300" s="6">
-        <v>70106</v>
+        <v>70103</v>
       </c>
       <c r="B300" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C300" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D300" s="3" t="s">
-        <v>5</v>
+      <c r="D300" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="301" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A301" s="6">
-        <v>70109</v>
+        <v>70106</v>
       </c>
       <c r="B301" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C301" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D301" s="1" t="s">
-        <v>8</v>
+      <c r="D301" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="302" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A302" s="6">
-        <v>70113</v>
+        <v>70109</v>
       </c>
       <c r="B302" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C302" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D302" s="3" t="s">
-        <v>5</v>
+      <c r="D302" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="303" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A303" s="6">
-        <v>70114</v>
+        <v>70113</v>
       </c>
       <c r="B303" t="s">
-        <v>327</v>
+        <v>307</v>
       </c>
       <c r="C303" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D303" s="7" t="s">
-        <v>9</v>
+      <c r="D303" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="304" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A304" s="6">
-        <v>70638</v>
+        <v>70114</v>
       </c>
       <c r="B304" t="s">
-        <v>308</v>
+        <v>327</v>
       </c>
       <c r="C304" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D304" s="1" t="s">
-        <v>8</v>
+      <c r="D304" s="7" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="305" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A305" s="6">
-        <v>70639</v>
+        <v>70638</v>
       </c>
       <c r="B305" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C305" s="1" t="s">
         <v>4</v>
@@ -5610,10 +5613,10 @@
     </row>
     <row r="306" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A306" s="6">
-        <v>70640</v>
+        <v>70639</v>
       </c>
       <c r="B306" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C306" s="1" t="s">
         <v>4</v>
@@ -5624,10 +5627,10 @@
     </row>
     <row r="307" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A307" s="6">
-        <v>70642</v>
+        <v>70640</v>
       </c>
       <c r="B307" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C307" s="1" t="s">
         <v>4</v>
@@ -5638,10 +5641,10 @@
     </row>
     <row r="308" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A308" s="6">
-        <v>90504</v>
+        <v>70642</v>
       </c>
       <c r="B308" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C308" s="1" t="s">
         <v>4</v>
@@ -5652,10 +5655,10 @@
     </row>
     <row r="309" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A309" s="6">
-        <v>90509</v>
+        <v>90504</v>
       </c>
       <c r="B309" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C309" s="1" t="s">
         <v>4</v>
@@ -5666,38 +5669,38 @@
     </row>
     <row r="310" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A310" s="6">
-        <v>90602</v>
+        <v>90509</v>
       </c>
       <c r="B310" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C310" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D310" s="3" t="s">
-        <v>5</v>
+      <c r="D310" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="311" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A311" s="6">
-        <v>90621</v>
+        <v>90602</v>
       </c>
       <c r="B311" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C311" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D311" s="1" t="s">
-        <v>8</v>
+      <c r="D311" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="312" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A312" s="6">
-        <v>90658</v>
+        <v>90621</v>
       </c>
       <c r="B312" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C312" s="1" t="s">
         <v>4</v>
@@ -5708,10 +5711,10 @@
     </row>
     <row r="313" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A313" s="6">
-        <v>90660</v>
+        <v>90658</v>
       </c>
       <c r="B313" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C313" s="1" t="s">
         <v>4</v>
@@ -5722,10 +5725,10 @@
     </row>
     <row r="314" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A314" s="6">
-        <v>90668</v>
+        <v>90660</v>
       </c>
       <c r="B314" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C314" s="1" t="s">
         <v>4</v>
@@ -5736,10 +5739,10 @@
     </row>
     <row r="315" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A315" s="6">
-        <v>90671</v>
+        <v>90668</v>
       </c>
       <c r="B315" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C315" s="1" t="s">
         <v>4</v>
@@ -5750,10 +5753,10 @@
     </row>
     <row r="316" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A316" s="6">
-        <v>90679</v>
+        <v>90671</v>
       </c>
       <c r="B316" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C316" s="1" t="s">
         <v>4</v>
@@ -5764,10 +5767,10 @@
     </row>
     <row r="317" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A317" s="6">
-        <v>90683</v>
+        <v>90679</v>
       </c>
       <c r="B317" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C317" s="1" t="s">
         <v>4</v>
@@ -5778,10 +5781,10 @@
     </row>
     <row r="318" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A318" s="6">
-        <v>90705</v>
+        <v>90683</v>
       </c>
       <c r="B318" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C318" s="1" t="s">
         <v>4</v>
@@ -5792,10 +5795,10 @@
     </row>
     <row r="319" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A319" s="6">
-        <v>90706</v>
+        <v>90705</v>
       </c>
       <c r="B319" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C319" s="1" t="s">
         <v>4</v>
@@ -5806,10 +5809,10 @@
     </row>
     <row r="320" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A320" s="6">
-        <v>90708</v>
+        <v>90706</v>
       </c>
       <c r="B320" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C320" s="1" t="s">
         <v>4</v>
@@ -5820,20 +5823,34 @@
     </row>
     <row r="321" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A321" s="6">
+        <v>90708</v>
+      </c>
+      <c r="B321" t="s">
+        <v>324</v>
+      </c>
+      <c r="C321" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D321" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="322" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A322" s="6">
         <v>90709</v>
       </c>
-      <c r="B321" t="s">
+      <c r="B322" t="s">
         <v>325</v>
       </c>
-      <c r="C321" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D321" s="1" t="s">
+      <c r="C322" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D322" s="1" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D321"/>
+  <autoFilter ref="A1:D322"/>
   <conditionalFormatting sqref="B1:B1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>

</xml_diff>

<commit_message>
agregue cta 40139, ENCINA FERRETERIA
</commit_message>
<xml_diff>
--- a/excel/CLIENTES_PERMISOS.xlsx
+++ b/excel/CLIENTES_PERMISOS.xlsx
@@ -15,14 +15,14 @@
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Hoja 1'!$A$1:$D$322</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Hoja 1'!$A$1:$D$323</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="967" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="970" uniqueCount="330">
   <si>
     <t>CUENTA</t>
   </si>
@@ -1009,6 +1009,9 @@
   </si>
   <si>
     <t>LUCIA FERRETERIA</t>
+  </si>
+  <si>
+    <t>ENCINA FERRETERIA</t>
   </si>
 </sst>
 </file>
@@ -1328,10 +1331,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D322"/>
+  <dimension ref="A1:D323"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D91" sqref="D91:D92"/>
+    <sheetView tabSelected="1" topLeftCell="A178" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C195" sqref="C195:D195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4059,10 +4062,10 @@
     </row>
     <row r="195" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A195" s="6">
-        <v>40140</v>
+        <v>40139</v>
       </c>
       <c r="B195" t="s">
-        <v>170</v>
+        <v>329</v>
       </c>
       <c r="C195" s="1" t="s">
         <v>4</v>
@@ -4073,52 +4076,52 @@
     </row>
     <row r="196" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A196" s="6">
-        <v>40141</v>
+        <v>40140</v>
       </c>
       <c r="B196" t="s">
-        <v>111</v>
+        <v>170</v>
       </c>
       <c r="C196" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D196" s="3" t="s">
-        <v>5</v>
+      <c r="D196" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="197" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A197" s="6">
-        <v>40143</v>
+        <v>40141</v>
       </c>
       <c r="B197" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
       <c r="C197" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D197" s="1" t="s">
-        <v>8</v>
+      <c r="D197" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="198" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A198" s="6">
-        <v>40144</v>
+        <v>40143</v>
       </c>
       <c r="B198" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="C198" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D198" s="3" t="s">
-        <v>5</v>
+      <c r="D198" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="199" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A199" s="6">
-        <v>40145</v>
+        <v>40144</v>
       </c>
       <c r="B199" t="s">
-        <v>165</v>
+        <v>107</v>
       </c>
       <c r="C199" s="1" t="s">
         <v>4</v>
@@ -4129,24 +4132,24 @@
     </row>
     <row r="200" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A200" s="6">
-        <v>40150</v>
+        <v>40145</v>
       </c>
       <c r="B200" t="s">
-        <v>221</v>
+        <v>165</v>
       </c>
       <c r="C200" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D200" s="1" t="s">
-        <v>8</v>
+      <c r="D200" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="201" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A201" s="6">
-        <v>40151</v>
+        <v>40150</v>
       </c>
       <c r="B201" t="s">
-        <v>54</v>
+        <v>221</v>
       </c>
       <c r="C201" s="1" t="s">
         <v>4</v>
@@ -4157,38 +4160,38 @@
     </row>
     <row r="202" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A202" s="6">
-        <v>50102</v>
+        <v>40151</v>
       </c>
       <c r="B202" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="C202" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D202" s="3" t="s">
-        <v>5</v>
+      <c r="D202" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="203" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A203" s="6">
-        <v>50222</v>
+        <v>50102</v>
       </c>
       <c r="B203" t="s">
-        <v>215</v>
+        <v>67</v>
       </c>
       <c r="C203" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D203" s="1" t="s">
-        <v>8</v>
+      <c r="D203" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="204" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A204" s="6">
-        <v>50223</v>
+        <v>50222</v>
       </c>
       <c r="B204" t="s">
-        <v>194</v>
+        <v>215</v>
       </c>
       <c r="C204" s="1" t="s">
         <v>4</v>
@@ -4199,66 +4202,66 @@
     </row>
     <row r="205" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A205" s="6">
-        <v>50224</v>
+        <v>50223</v>
       </c>
       <c r="B205" t="s">
-        <v>42</v>
+        <v>194</v>
       </c>
       <c r="C205" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D205" s="3" t="s">
-        <v>5</v>
+      <c r="D205" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="206" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A206" s="6">
-        <v>50444</v>
+        <v>50224</v>
       </c>
       <c r="B206" t="s">
-        <v>116</v>
+        <v>42</v>
       </c>
       <c r="C206" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D206" s="1" t="s">
-        <v>8</v>
+      <c r="D206" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="207" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A207" s="6">
-        <v>50607</v>
+        <v>50444</v>
       </c>
       <c r="B207" t="s">
-        <v>76</v>
+        <v>116</v>
       </c>
       <c r="C207" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D207" s="3" t="s">
-        <v>5</v>
+      <c r="D207" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="208" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A208" s="6">
-        <v>50608</v>
+        <v>50607</v>
       </c>
       <c r="B208" t="s">
-        <v>177</v>
+        <v>76</v>
       </c>
       <c r="C208" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D208" s="1" t="s">
-        <v>8</v>
+      <c r="D208" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="209" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A209" s="6">
-        <v>50622</v>
+        <v>50608</v>
       </c>
       <c r="B209" t="s">
-        <v>95</v>
+        <v>177</v>
       </c>
       <c r="C209" s="1" t="s">
         <v>4</v>
@@ -4269,10 +4272,10 @@
     </row>
     <row r="210" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A210" s="6">
-        <v>50623</v>
+        <v>50622</v>
       </c>
       <c r="B210" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="C210" s="1" t="s">
         <v>4</v>
@@ -4283,10 +4286,10 @@
     </row>
     <row r="211" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A211" s="6">
-        <v>50625</v>
+        <v>50623</v>
       </c>
       <c r="B211" t="s">
-        <v>204</v>
+        <v>110</v>
       </c>
       <c r="C211" s="1" t="s">
         <v>4</v>
@@ -4297,10 +4300,10 @@
     </row>
     <row r="212" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A212" s="6">
-        <v>50629</v>
+        <v>50625</v>
       </c>
       <c r="B212" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="C212" s="1" t="s">
         <v>4</v>
@@ -4311,10 +4314,10 @@
     </row>
     <row r="213" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A213" s="6">
-        <v>50803</v>
+        <v>50629</v>
       </c>
       <c r="B213" t="s">
-        <v>82</v>
+        <v>188</v>
       </c>
       <c r="C213" s="1" t="s">
         <v>4</v>
@@ -4325,10 +4328,10 @@
     </row>
     <row r="214" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A214" s="6">
-        <v>50805</v>
+        <v>50803</v>
       </c>
       <c r="B214" t="s">
-        <v>135</v>
+        <v>82</v>
       </c>
       <c r="C214" s="1" t="s">
         <v>4</v>
@@ -4339,10 +4342,10 @@
     </row>
     <row r="215" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A215" s="6">
-        <v>50806</v>
+        <v>50805</v>
       </c>
       <c r="B215" t="s">
-        <v>156</v>
+        <v>135</v>
       </c>
       <c r="C215" s="1" t="s">
         <v>4</v>
@@ -4353,24 +4356,24 @@
     </row>
     <row r="216" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A216" s="6">
-        <v>50808</v>
+        <v>50806</v>
       </c>
       <c r="B216" t="s">
-        <v>16</v>
+        <v>156</v>
       </c>
       <c r="C216" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D216" s="3" t="s">
-        <v>5</v>
+      <c r="D216" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="217" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A217" s="6">
-        <v>50809</v>
+        <v>50808</v>
       </c>
       <c r="B217" t="s">
-        <v>98</v>
+        <v>16</v>
       </c>
       <c r="C217" s="1" t="s">
         <v>4</v>
@@ -4381,24 +4384,24 @@
     </row>
     <row r="218" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A218" s="6">
-        <v>50810</v>
+        <v>50809</v>
       </c>
       <c r="B218" t="s">
-        <v>175</v>
+        <v>98</v>
       </c>
       <c r="C218" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D218" s="1" t="s">
-        <v>8</v>
+      <c r="D218" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="219" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A219" s="6">
-        <v>50812</v>
+        <v>50810</v>
       </c>
       <c r="B219" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="C219" s="1" t="s">
         <v>4</v>
@@ -4409,38 +4412,38 @@
     </row>
     <row r="220" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A220" s="6">
-        <v>50813</v>
+        <v>50812</v>
       </c>
       <c r="B220" t="s">
-        <v>71</v>
+        <v>184</v>
       </c>
       <c r="C220" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D220" t="s">
-        <v>9</v>
+      <c r="D220" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="221" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A221" s="6">
-        <v>50815</v>
+        <v>50813</v>
       </c>
       <c r="B221" t="s">
-        <v>114</v>
+        <v>71</v>
       </c>
       <c r="C221" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D221" s="1" t="s">
-        <v>8</v>
+      <c r="D221" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="222" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A222" s="6">
-        <v>50816</v>
+        <v>50815</v>
       </c>
       <c r="B222" t="s">
-        <v>205</v>
+        <v>114</v>
       </c>
       <c r="C222" s="1" t="s">
         <v>4</v>
@@ -4451,38 +4454,38 @@
     </row>
     <row r="223" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A223" s="6">
-        <v>50818</v>
+        <v>50816</v>
       </c>
       <c r="B223" t="s">
-        <v>227</v>
+        <v>205</v>
       </c>
       <c r="C223" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D223" s="3" t="s">
-        <v>5</v>
+      <c r="D223" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="224" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A224" s="6">
-        <v>50819</v>
+        <v>50818</v>
       </c>
       <c r="B224" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C224" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D224" s="1" t="s">
-        <v>8</v>
+      <c r="D224" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="225" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A225" s="6">
-        <v>50820</v>
+        <v>50819</v>
       </c>
       <c r="B225" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C225" s="1" t="s">
         <v>4</v>
@@ -4493,10 +4496,10 @@
     </row>
     <row r="226" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A226" s="6">
-        <v>50821</v>
+        <v>50820</v>
       </c>
       <c r="B226" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C226" s="1" t="s">
         <v>4</v>
@@ -4507,52 +4510,52 @@
     </row>
     <row r="227" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A227" s="6">
-        <v>50823</v>
+        <v>50821</v>
       </c>
       <c r="B227" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C227" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D227" t="s">
-        <v>9</v>
+      <c r="D227" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="228" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A228" s="6">
-        <v>50824</v>
+        <v>50823</v>
       </c>
       <c r="B228" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C228" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D228" s="3" t="s">
-        <v>5</v>
+      <c r="D228" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="229" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A229" s="6">
-        <v>50825</v>
+        <v>50824</v>
       </c>
       <c r="B229" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C229" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D229" s="1" t="s">
-        <v>8</v>
+      <c r="D229" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="230" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A230" s="6">
-        <v>50826</v>
+        <v>50825</v>
       </c>
       <c r="B230" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C230" s="1" t="s">
         <v>4</v>
@@ -4563,10 +4566,10 @@
     </row>
     <row r="231" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A231" s="6">
-        <v>50827</v>
+        <v>50826</v>
       </c>
       <c r="B231" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C231" s="1" t="s">
         <v>4</v>
@@ -4577,10 +4580,10 @@
     </row>
     <row r="232" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A232" s="6">
-        <v>50829</v>
+        <v>50827</v>
       </c>
       <c r="B232" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C232" s="1" t="s">
         <v>4</v>
@@ -4591,24 +4594,24 @@
     </row>
     <row r="233" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A233" s="6">
-        <v>60103</v>
+        <v>50829</v>
       </c>
       <c r="B233" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C233" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D233" s="3" t="s">
-        <v>5</v>
+      <c r="D233" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="234" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A234" s="6">
-        <v>60124</v>
+        <v>60103</v>
       </c>
       <c r="B234" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C234" s="1" t="s">
         <v>4</v>
@@ -4619,10 +4622,10 @@
     </row>
     <row r="235" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A235" s="6">
-        <v>60125</v>
+        <v>60124</v>
       </c>
       <c r="B235" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C235" s="1" t="s">
         <v>4</v>
@@ -4633,80 +4636,80 @@
     </row>
     <row r="236" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A236" s="6">
-        <v>60126</v>
+        <v>60125</v>
       </c>
       <c r="B236" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C236" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D236" s="1" t="s">
-        <v>8</v>
+      <c r="D236" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="237" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A237" s="6">
-        <v>60128</v>
+        <v>60126</v>
       </c>
       <c r="B237" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C237" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D237" s="3" t="s">
-        <v>5</v>
+      <c r="D237" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="238" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A238" s="6">
-        <v>60130</v>
+        <v>60128</v>
       </c>
       <c r="B238" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C238" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D238" s="1" t="s">
-        <v>8</v>
+      <c r="D238" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="239" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A239" s="6">
-        <v>60133</v>
+        <v>60130</v>
       </c>
       <c r="B239" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C239" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D239" s="3" t="s">
-        <v>5</v>
+      <c r="D239" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="240" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A240" s="6">
-        <v>60134</v>
+        <v>60133</v>
       </c>
       <c r="B240" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C240" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D240" s="1" t="s">
-        <v>8</v>
+      <c r="D240" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="241" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A241" s="6">
-        <v>60137</v>
+        <v>60134</v>
       </c>
       <c r="B241" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C241" s="1" t="s">
         <v>4</v>
@@ -4717,10 +4720,10 @@
     </row>
     <row r="242" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A242" s="6">
-        <v>60139</v>
+        <v>60137</v>
       </c>
       <c r="B242" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C242" s="1" t="s">
         <v>4</v>
@@ -4731,10 +4734,10 @@
     </row>
     <row r="243" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A243" s="6">
-        <v>60142</v>
+        <v>60139</v>
       </c>
       <c r="B243" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C243" s="1" t="s">
         <v>4</v>
@@ -4745,10 +4748,10 @@
     </row>
     <row r="244" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A244" s="6">
-        <v>60148</v>
+        <v>60142</v>
       </c>
       <c r="B244" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C244" s="1" t="s">
         <v>4</v>
@@ -4759,10 +4762,10 @@
     </row>
     <row r="245" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A245" s="6">
-        <v>60149</v>
+        <v>60148</v>
       </c>
       <c r="B245" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C245" s="1" t="s">
         <v>4</v>
@@ -4773,10 +4776,10 @@
     </row>
     <row r="246" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A246" s="6">
-        <v>60158</v>
+        <v>60149</v>
       </c>
       <c r="B246" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C246" s="1" t="s">
         <v>4</v>
@@ -4787,10 +4790,10 @@
     </row>
     <row r="247" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A247" s="6">
-        <v>60159</v>
+        <v>60158</v>
       </c>
       <c r="B247" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C247" s="1" t="s">
         <v>4</v>
@@ -4801,24 +4804,24 @@
     </row>
     <row r="248" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A248" s="6">
-        <v>60162</v>
+        <v>60159</v>
       </c>
       <c r="B248" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C248" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D248" s="3" t="s">
-        <v>5</v>
+      <c r="D248" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="249" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A249" s="6">
-        <v>60163</v>
+        <v>60162</v>
       </c>
       <c r="B249" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C249" s="1" t="s">
         <v>4</v>
@@ -4829,24 +4832,24 @@
     </row>
     <row r="250" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A250" s="6">
-        <v>60165</v>
+        <v>60163</v>
       </c>
       <c r="B250" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C250" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D250" s="1" t="s">
-        <v>8</v>
+      <c r="D250" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="251" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A251" s="6">
-        <v>60169</v>
+        <v>60165</v>
       </c>
       <c r="B251" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C251" s="1" t="s">
         <v>4</v>
@@ -4857,10 +4860,10 @@
     </row>
     <row r="252" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A252" s="6">
-        <v>60172</v>
+        <v>60169</v>
       </c>
       <c r="B252" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C252" s="1" t="s">
         <v>4</v>
@@ -4871,24 +4874,24 @@
     </row>
     <row r="253" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A253" s="6">
-        <v>60174</v>
+        <v>60172</v>
       </c>
       <c r="B253" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C253" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D253" s="3" t="s">
-        <v>5</v>
+      <c r="D253" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="254" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A254" s="6">
-        <v>60176</v>
+        <v>60174</v>
       </c>
       <c r="B254" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C254" s="1" t="s">
         <v>4</v>
@@ -4899,24 +4902,24 @@
     </row>
     <row r="255" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A255" s="6">
-        <v>60178</v>
+        <v>60176</v>
       </c>
       <c r="B255" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C255" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D255" s="1" t="s">
-        <v>8</v>
+      <c r="D255" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="256" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A256" s="6">
-        <v>60180</v>
+        <v>60178</v>
       </c>
       <c r="B256" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C256" s="1" t="s">
         <v>4</v>
@@ -4927,10 +4930,10 @@
     </row>
     <row r="257" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A257" s="6">
-        <v>60184</v>
+        <v>60180</v>
       </c>
       <c r="B257" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C257" s="1" t="s">
         <v>4</v>
@@ -4941,10 +4944,10 @@
     </row>
     <row r="258" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A258" s="6">
-        <v>60190</v>
+        <v>60184</v>
       </c>
       <c r="B258" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C258" s="1" t="s">
         <v>4</v>
@@ -4955,10 +4958,10 @@
     </row>
     <row r="259" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A259" s="6">
-        <v>60191</v>
+        <v>60190</v>
       </c>
       <c r="B259" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C259" s="1" t="s">
         <v>4</v>
@@ -4969,10 +4972,10 @@
     </row>
     <row r="260" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A260" s="6">
-        <v>60192</v>
+        <v>60191</v>
       </c>
       <c r="B260" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C260" s="1" t="s">
         <v>4</v>
@@ -4983,10 +4986,10 @@
     </row>
     <row r="261" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A261" s="6">
-        <v>60195</v>
+        <v>60192</v>
       </c>
       <c r="B261" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C261" s="1" t="s">
         <v>4</v>
@@ -4997,10 +5000,10 @@
     </row>
     <row r="262" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A262" s="6">
-        <v>60196</v>
+        <v>60195</v>
       </c>
       <c r="B262" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C262" s="1" t="s">
         <v>4</v>
@@ -5011,10 +5014,10 @@
     </row>
     <row r="263" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A263" s="6">
-        <v>60198</v>
+        <v>60196</v>
       </c>
       <c r="B263" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C263" s="1" t="s">
         <v>4</v>
@@ -5025,10 +5028,10 @@
     </row>
     <row r="264" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A264" s="6">
-        <v>60200</v>
+        <v>60198</v>
       </c>
       <c r="B264" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C264" s="1" t="s">
         <v>4</v>
@@ -5039,52 +5042,52 @@
     </row>
     <row r="265" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A265" s="6">
-        <v>60201</v>
+        <v>60200</v>
       </c>
       <c r="B265" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C265" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D265" t="s">
-        <v>9</v>
+      <c r="D265" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="266" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A266" s="6">
-        <v>60202</v>
+        <v>60201</v>
       </c>
       <c r="B266" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C266" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D266" s="3" t="s">
-        <v>5</v>
+      <c r="D266" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="267" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A267" s="6">
-        <v>60204</v>
+        <v>60202</v>
       </c>
       <c r="B267" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C267" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D267" s="1" t="s">
-        <v>8</v>
+      <c r="D267" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="268" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A268" s="6">
-        <v>60205</v>
+        <v>60204</v>
       </c>
       <c r="B268" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C268" s="1" t="s">
         <v>4</v>
@@ -5095,10 +5098,10 @@
     </row>
     <row r="269" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A269" s="6">
-        <v>60206</v>
+        <v>60205</v>
       </c>
       <c r="B269" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C269" s="1" t="s">
         <v>4</v>
@@ -5109,10 +5112,10 @@
     </row>
     <row r="270" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A270" s="6">
-        <v>60209</v>
+        <v>60206</v>
       </c>
       <c r="B270" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C270" s="1" t="s">
         <v>4</v>
@@ -5123,10 +5126,10 @@
     </row>
     <row r="271" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A271" s="6">
-        <v>60211</v>
+        <v>60209</v>
       </c>
       <c r="B271" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C271" s="1" t="s">
         <v>4</v>
@@ -5137,10 +5140,10 @@
     </row>
     <row r="272" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A272" s="6">
-        <v>60215</v>
+        <v>60211</v>
       </c>
       <c r="B272" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C272" s="1" t="s">
         <v>4</v>
@@ -5151,10 +5154,10 @@
     </row>
     <row r="273" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A273" s="6">
-        <v>60217</v>
+        <v>60215</v>
       </c>
       <c r="B273" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C273" s="1" t="s">
         <v>4</v>
@@ -5165,10 +5168,10 @@
     </row>
     <row r="274" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A274" s="6">
-        <v>60219</v>
+        <v>60217</v>
       </c>
       <c r="B274" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C274" s="1" t="s">
         <v>4</v>
@@ -5179,10 +5182,10 @@
     </row>
     <row r="275" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A275" s="6">
-        <v>60222</v>
+        <v>60219</v>
       </c>
       <c r="B275" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C275" s="1" t="s">
         <v>4</v>
@@ -5193,38 +5196,38 @@
     </row>
     <row r="276" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A276" s="6">
-        <v>60225</v>
+        <v>60222</v>
       </c>
       <c r="B276" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C276" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D276" t="s">
-        <v>9</v>
+      <c r="D276" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="277" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A277" s="6">
-        <v>60230</v>
+        <v>60225</v>
       </c>
       <c r="B277" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C277" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D277" s="1" t="s">
-        <v>8</v>
+      <c r="D277" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="278" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A278" s="6">
-        <v>60234</v>
+        <v>60230</v>
       </c>
       <c r="B278" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C278" s="1" t="s">
         <v>4</v>
@@ -5235,10 +5238,10 @@
     </row>
     <row r="279" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A279" s="6">
-        <v>60253</v>
+        <v>60234</v>
       </c>
       <c r="B279" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C279" s="1" t="s">
         <v>4</v>
@@ -5249,10 +5252,10 @@
     </row>
     <row r="280" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A280" s="6">
-        <v>60254</v>
+        <v>60253</v>
       </c>
       <c r="B280" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C280" s="1" t="s">
         <v>4</v>
@@ -5263,10 +5266,10 @@
     </row>
     <row r="281" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A281" s="6">
-        <v>60257</v>
+        <v>60254</v>
       </c>
       <c r="B281" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C281" s="1" t="s">
         <v>4</v>
@@ -5277,10 +5280,10 @@
     </row>
     <row r="282" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A282" s="6">
-        <v>60258</v>
+        <v>60257</v>
       </c>
       <c r="B282" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C282" s="1" t="s">
         <v>4</v>
@@ -5291,10 +5294,10 @@
     </row>
     <row r="283" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A283" s="6">
-        <v>60269</v>
+        <v>60258</v>
       </c>
       <c r="B283" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C283" s="1" t="s">
         <v>4</v>
@@ -5305,10 +5308,10 @@
     </row>
     <row r="284" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A284" s="6">
-        <v>60270</v>
+        <v>60269</v>
       </c>
       <c r="B284" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C284" s="1" t="s">
         <v>4</v>
@@ -5319,10 +5322,10 @@
     </row>
     <row r="285" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A285" s="6">
-        <v>60272</v>
+        <v>60270</v>
       </c>
       <c r="B285" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C285" s="1" t="s">
         <v>4</v>
@@ -5333,10 +5336,10 @@
     </row>
     <row r="286" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A286" s="6">
-        <v>60275</v>
+        <v>60272</v>
       </c>
       <c r="B286" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C286" s="1" t="s">
         <v>4</v>
@@ -5347,10 +5350,10 @@
     </row>
     <row r="287" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A287" s="6">
-        <v>60276</v>
+        <v>60275</v>
       </c>
       <c r="B287" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C287" s="1" t="s">
         <v>4</v>
@@ -5361,38 +5364,38 @@
     </row>
     <row r="288" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A288" s="6">
-        <v>60278</v>
+        <v>60276</v>
       </c>
       <c r="B288" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C288" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D288" s="3" t="s">
-        <v>5</v>
+      <c r="D288" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="289" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A289" s="6">
-        <v>60279</v>
+        <v>60278</v>
       </c>
       <c r="B289" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C289" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D289" s="1" t="s">
-        <v>8</v>
+      <c r="D289" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="290" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A290" s="6">
-        <v>60280</v>
+        <v>60279</v>
       </c>
       <c r="B290" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C290" s="1" t="s">
         <v>4</v>
@@ -5403,38 +5406,38 @@
     </row>
     <row r="291" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A291" s="6">
-        <v>61004</v>
+        <v>60280</v>
       </c>
       <c r="B291" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C291" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D291" s="3" t="s">
-        <v>5</v>
+      <c r="D291" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="292" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A292" s="6">
-        <v>61009</v>
+        <v>61004</v>
       </c>
       <c r="B292" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C292" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D292" s="1" t="s">
-        <v>8</v>
+      <c r="D292" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="293" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A293" s="6">
-        <v>61012</v>
+        <v>61009</v>
       </c>
       <c r="B293" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C293" s="1" t="s">
         <v>4</v>
@@ -5445,10 +5448,10 @@
     </row>
     <row r="294" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A294" s="6">
-        <v>61018</v>
+        <v>61012</v>
       </c>
       <c r="B294" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C294" s="1" t="s">
         <v>4</v>
@@ -5459,10 +5462,10 @@
     </row>
     <row r="295" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A295" s="6">
-        <v>61102</v>
+        <v>61018</v>
       </c>
       <c r="B295" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C295" s="1" t="s">
         <v>4</v>
@@ -5473,52 +5476,52 @@
     </row>
     <row r="296" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A296" s="6">
-        <v>61205</v>
+        <v>61102</v>
       </c>
       <c r="B296" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C296" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D296" s="3" t="s">
-        <v>5</v>
+      <c r="D296" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="297" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A297" s="6">
-        <v>70100</v>
+        <v>61205</v>
       </c>
       <c r="B297" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C297" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D297" s="1" t="s">
-        <v>8</v>
+      <c r="D297" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="298" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A298" s="6">
-        <v>70101</v>
+        <v>70100</v>
       </c>
       <c r="B298" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C298" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D298" s="3" t="s">
-        <v>5</v>
+      <c r="D298" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="299" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A299" s="6">
-        <v>70102</v>
+        <v>70101</v>
       </c>
       <c r="B299" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C299" s="1" t="s">
         <v>4</v>
@@ -5529,94 +5532,94 @@
     </row>
     <row r="300" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A300" s="6">
-        <v>70103</v>
+        <v>70102</v>
       </c>
       <c r="B300" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C300" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D300" s="1" t="s">
-        <v>8</v>
+      <c r="D300" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="301" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A301" s="6">
-        <v>70106</v>
+        <v>70103</v>
       </c>
       <c r="B301" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C301" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D301" s="3" t="s">
-        <v>5</v>
+      <c r="D301" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="302" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A302" s="6">
-        <v>70109</v>
+        <v>70106</v>
       </c>
       <c r="B302" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C302" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D302" s="1" t="s">
-        <v>8</v>
+      <c r="D302" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="303" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A303" s="6">
-        <v>70113</v>
+        <v>70109</v>
       </c>
       <c r="B303" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C303" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D303" s="3" t="s">
-        <v>5</v>
+      <c r="D303" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="304" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A304" s="6">
-        <v>70114</v>
+        <v>70113</v>
       </c>
       <c r="B304" t="s">
-        <v>327</v>
+        <v>307</v>
       </c>
       <c r="C304" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D304" s="7" t="s">
-        <v>9</v>
+      <c r="D304" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="305" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A305" s="6">
-        <v>70638</v>
+        <v>70114</v>
       </c>
       <c r="B305" t="s">
-        <v>308</v>
+        <v>327</v>
       </c>
       <c r="C305" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D305" s="1" t="s">
-        <v>8</v>
+      <c r="D305" s="7" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="306" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A306" s="6">
-        <v>70639</v>
+        <v>70638</v>
       </c>
       <c r="B306" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C306" s="1" t="s">
         <v>4</v>
@@ -5627,10 +5630,10 @@
     </row>
     <row r="307" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A307" s="6">
-        <v>70640</v>
+        <v>70639</v>
       </c>
       <c r="B307" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C307" s="1" t="s">
         <v>4</v>
@@ -5641,10 +5644,10 @@
     </row>
     <row r="308" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A308" s="6">
-        <v>70642</v>
+        <v>70640</v>
       </c>
       <c r="B308" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C308" s="1" t="s">
         <v>4</v>
@@ -5655,10 +5658,10 @@
     </row>
     <row r="309" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A309" s="6">
-        <v>90504</v>
+        <v>70642</v>
       </c>
       <c r="B309" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C309" s="1" t="s">
         <v>4</v>
@@ -5669,10 +5672,10 @@
     </row>
     <row r="310" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A310" s="6">
-        <v>90509</v>
+        <v>90504</v>
       </c>
       <c r="B310" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C310" s="1" t="s">
         <v>4</v>
@@ -5683,38 +5686,38 @@
     </row>
     <row r="311" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A311" s="6">
-        <v>90602</v>
+        <v>90509</v>
       </c>
       <c r="B311" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C311" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D311" s="3" t="s">
-        <v>5</v>
+      <c r="D311" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="312" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A312" s="6">
-        <v>90621</v>
+        <v>90602</v>
       </c>
       <c r="B312" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C312" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D312" s="1" t="s">
-        <v>8</v>
+      <c r="D312" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="313" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A313" s="6">
-        <v>90658</v>
+        <v>90621</v>
       </c>
       <c r="B313" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C313" s="1" t="s">
         <v>4</v>
@@ -5725,10 +5728,10 @@
     </row>
     <row r="314" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A314" s="6">
-        <v>90660</v>
+        <v>90658</v>
       </c>
       <c r="B314" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C314" s="1" t="s">
         <v>4</v>
@@ -5739,10 +5742,10 @@
     </row>
     <row r="315" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A315" s="6">
-        <v>90668</v>
+        <v>90660</v>
       </c>
       <c r="B315" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C315" s="1" t="s">
         <v>4</v>
@@ -5753,10 +5756,10 @@
     </row>
     <row r="316" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A316" s="6">
-        <v>90671</v>
+        <v>90668</v>
       </c>
       <c r="B316" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C316" s="1" t="s">
         <v>4</v>
@@ -5767,10 +5770,10 @@
     </row>
     <row r="317" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A317" s="6">
-        <v>90679</v>
+        <v>90671</v>
       </c>
       <c r="B317" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C317" s="1" t="s">
         <v>4</v>
@@ -5781,10 +5784,10 @@
     </row>
     <row r="318" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A318" s="6">
-        <v>90683</v>
+        <v>90679</v>
       </c>
       <c r="B318" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C318" s="1" t="s">
         <v>4</v>
@@ -5795,10 +5798,10 @@
     </row>
     <row r="319" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A319" s="6">
-        <v>90705</v>
+        <v>90683</v>
       </c>
       <c r="B319" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C319" s="1" t="s">
         <v>4</v>
@@ -5809,10 +5812,10 @@
     </row>
     <row r="320" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A320" s="6">
-        <v>90706</v>
+        <v>90705</v>
       </c>
       <c r="B320" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C320" s="1" t="s">
         <v>4</v>
@@ -5823,10 +5826,10 @@
     </row>
     <row r="321" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A321" s="6">
-        <v>90708</v>
+        <v>90706</v>
       </c>
       <c r="B321" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C321" s="1" t="s">
         <v>4</v>
@@ -5837,20 +5840,34 @@
     </row>
     <row r="322" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A322" s="6">
+        <v>90708</v>
+      </c>
+      <c r="B322" t="s">
+        <v>324</v>
+      </c>
+      <c r="C322" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D322" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="323" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A323" s="6">
         <v>90709</v>
       </c>
-      <c r="B322" t="s">
+      <c r="B323" t="s">
         <v>325</v>
       </c>
-      <c r="C322" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D322" s="1" t="s">
+      <c r="C323" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D323" s="1" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D322"/>
+  <autoFilter ref="A1:D323"/>
   <conditionalFormatting sqref="B1:B1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>

</xml_diff>

<commit_message>
subi iamgenes de bremen, agregue cta 60109
</commit_message>
<xml_diff>
--- a/excel/CLIENTES_PERMISOS.xlsx
+++ b/excel/CLIENTES_PERMISOS.xlsx
@@ -15,14 +15,14 @@
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Hoja 1'!$A$1:$D$323</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Hoja 1'!$A$1:$D$324</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="970" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="973" uniqueCount="331">
   <si>
     <t>CUENTA</t>
   </si>
@@ -1012,6 +1012,9 @@
   </si>
   <si>
     <t>ENCINA FERRETERIA</t>
+  </si>
+  <si>
+    <t>CERAMICA SANTA MARTA</t>
   </si>
 </sst>
 </file>
@@ -1331,10 +1334,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D323"/>
+  <dimension ref="A1:D324"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A178" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C195" sqref="C195:D195"/>
+    <sheetView tabSelected="1" topLeftCell="A223" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B236" sqref="B236"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4622,24 +4625,24 @@
     </row>
     <row r="235" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A235" s="6">
-        <v>60124</v>
+        <v>60109</v>
       </c>
       <c r="B235" t="s">
-        <v>238</v>
+        <v>330</v>
       </c>
       <c r="C235" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D235" s="3" t="s">
-        <v>5</v>
+      <c r="D235" s="7" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="236" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A236" s="6">
-        <v>60125</v>
+        <v>60124</v>
       </c>
       <c r="B236" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C236" s="1" t="s">
         <v>4</v>
@@ -4650,80 +4653,80 @@
     </row>
     <row r="237" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A237" s="6">
-        <v>60126</v>
+        <v>60125</v>
       </c>
       <c r="B237" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C237" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D237" s="1" t="s">
-        <v>8</v>
+      <c r="D237" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="238" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A238" s="6">
-        <v>60128</v>
+        <v>60126</v>
       </c>
       <c r="B238" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C238" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D238" s="3" t="s">
-        <v>5</v>
+      <c r="D238" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="239" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A239" s="6">
-        <v>60130</v>
+        <v>60128</v>
       </c>
       <c r="B239" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C239" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D239" s="1" t="s">
-        <v>8</v>
+      <c r="D239" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="240" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A240" s="6">
-        <v>60133</v>
+        <v>60130</v>
       </c>
       <c r="B240" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C240" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D240" s="3" t="s">
-        <v>5</v>
+      <c r="D240" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="241" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A241" s="6">
-        <v>60134</v>
+        <v>60133</v>
       </c>
       <c r="B241" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C241" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D241" s="1" t="s">
-        <v>8</v>
+      <c r="D241" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="242" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A242" s="6">
-        <v>60137</v>
+        <v>60134</v>
       </c>
       <c r="B242" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C242" s="1" t="s">
         <v>4</v>
@@ -4734,10 +4737,10 @@
     </row>
     <row r="243" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A243" s="6">
-        <v>60139</v>
+        <v>60137</v>
       </c>
       <c r="B243" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C243" s="1" t="s">
         <v>4</v>
@@ -4748,10 +4751,10 @@
     </row>
     <row r="244" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A244" s="6">
-        <v>60142</v>
+        <v>60139</v>
       </c>
       <c r="B244" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C244" s="1" t="s">
         <v>4</v>
@@ -4762,10 +4765,10 @@
     </row>
     <row r="245" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A245" s="6">
-        <v>60148</v>
+        <v>60142</v>
       </c>
       <c r="B245" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C245" s="1" t="s">
         <v>4</v>
@@ -4776,10 +4779,10 @@
     </row>
     <row r="246" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A246" s="6">
-        <v>60149</v>
+        <v>60148</v>
       </c>
       <c r="B246" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C246" s="1" t="s">
         <v>4</v>
@@ -4790,10 +4793,10 @@
     </row>
     <row r="247" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A247" s="6">
-        <v>60158</v>
+        <v>60149</v>
       </c>
       <c r="B247" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C247" s="1" t="s">
         <v>4</v>
@@ -4804,10 +4807,10 @@
     </row>
     <row r="248" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A248" s="6">
-        <v>60159</v>
+        <v>60158</v>
       </c>
       <c r="B248" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C248" s="1" t="s">
         <v>4</v>
@@ -4818,24 +4821,24 @@
     </row>
     <row r="249" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A249" s="6">
-        <v>60162</v>
+        <v>60159</v>
       </c>
       <c r="B249" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C249" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D249" s="3" t="s">
-        <v>5</v>
+      <c r="D249" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="250" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A250" s="6">
-        <v>60163</v>
+        <v>60162</v>
       </c>
       <c r="B250" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C250" s="1" t="s">
         <v>4</v>
@@ -4846,24 +4849,24 @@
     </row>
     <row r="251" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A251" s="6">
-        <v>60165</v>
+        <v>60163</v>
       </c>
       <c r="B251" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C251" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D251" s="1" t="s">
-        <v>8</v>
+      <c r="D251" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="252" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A252" s="6">
-        <v>60169</v>
+        <v>60165</v>
       </c>
       <c r="B252" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C252" s="1" t="s">
         <v>4</v>
@@ -4874,10 +4877,10 @@
     </row>
     <row r="253" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A253" s="6">
-        <v>60172</v>
+        <v>60169</v>
       </c>
       <c r="B253" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C253" s="1" t="s">
         <v>4</v>
@@ -4888,24 +4891,24 @@
     </row>
     <row r="254" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A254" s="6">
-        <v>60174</v>
+        <v>60172</v>
       </c>
       <c r="B254" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C254" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D254" s="3" t="s">
-        <v>5</v>
+      <c r="D254" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="255" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A255" s="6">
-        <v>60176</v>
+        <v>60174</v>
       </c>
       <c r="B255" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C255" s="1" t="s">
         <v>4</v>
@@ -4916,24 +4919,24 @@
     </row>
     <row r="256" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A256" s="6">
-        <v>60178</v>
+        <v>60176</v>
       </c>
       <c r="B256" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C256" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D256" s="1" t="s">
-        <v>8</v>
+      <c r="D256" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="257" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A257" s="6">
-        <v>60180</v>
+        <v>60178</v>
       </c>
       <c r="B257" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C257" s="1" t="s">
         <v>4</v>
@@ -4944,10 +4947,10 @@
     </row>
     <row r="258" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A258" s="6">
-        <v>60184</v>
+        <v>60180</v>
       </c>
       <c r="B258" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C258" s="1" t="s">
         <v>4</v>
@@ -4958,10 +4961,10 @@
     </row>
     <row r="259" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A259" s="6">
-        <v>60190</v>
+        <v>60184</v>
       </c>
       <c r="B259" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C259" s="1" t="s">
         <v>4</v>
@@ -4972,10 +4975,10 @@
     </row>
     <row r="260" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A260" s="6">
-        <v>60191</v>
+        <v>60190</v>
       </c>
       <c r="B260" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C260" s="1" t="s">
         <v>4</v>
@@ -4986,10 +4989,10 @@
     </row>
     <row r="261" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A261" s="6">
-        <v>60192</v>
+        <v>60191</v>
       </c>
       <c r="B261" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C261" s="1" t="s">
         <v>4</v>
@@ -5000,10 +5003,10 @@
     </row>
     <row r="262" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A262" s="6">
-        <v>60195</v>
+        <v>60192</v>
       </c>
       <c r="B262" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C262" s="1" t="s">
         <v>4</v>
@@ -5014,10 +5017,10 @@
     </row>
     <row r="263" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A263" s="6">
-        <v>60196</v>
+        <v>60195</v>
       </c>
       <c r="B263" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C263" s="1" t="s">
         <v>4</v>
@@ -5028,10 +5031,10 @@
     </row>
     <row r="264" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A264" s="6">
-        <v>60198</v>
+        <v>60196</v>
       </c>
       <c r="B264" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C264" s="1" t="s">
         <v>4</v>
@@ -5042,10 +5045,10 @@
     </row>
     <row r="265" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A265" s="6">
-        <v>60200</v>
+        <v>60198</v>
       </c>
       <c r="B265" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C265" s="1" t="s">
         <v>4</v>
@@ -5056,52 +5059,52 @@
     </row>
     <row r="266" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A266" s="6">
-        <v>60201</v>
+        <v>60200</v>
       </c>
       <c r="B266" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C266" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D266" t="s">
-        <v>9</v>
+      <c r="D266" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="267" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A267" s="6">
-        <v>60202</v>
+        <v>60201</v>
       </c>
       <c r="B267" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C267" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D267" s="3" t="s">
-        <v>5</v>
+      <c r="D267" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="268" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A268" s="6">
-        <v>60204</v>
+        <v>60202</v>
       </c>
       <c r="B268" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C268" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D268" s="1" t="s">
-        <v>8</v>
+      <c r="D268" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="269" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A269" s="6">
-        <v>60205</v>
+        <v>60204</v>
       </c>
       <c r="B269" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C269" s="1" t="s">
         <v>4</v>
@@ -5112,10 +5115,10 @@
     </row>
     <row r="270" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A270" s="6">
-        <v>60206</v>
+        <v>60205</v>
       </c>
       <c r="B270" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C270" s="1" t="s">
         <v>4</v>
@@ -5126,10 +5129,10 @@
     </row>
     <row r="271" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A271" s="6">
-        <v>60209</v>
+        <v>60206</v>
       </c>
       <c r="B271" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C271" s="1" t="s">
         <v>4</v>
@@ -5140,10 +5143,10 @@
     </row>
     <row r="272" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A272" s="6">
-        <v>60211</v>
+        <v>60209</v>
       </c>
       <c r="B272" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C272" s="1" t="s">
         <v>4</v>
@@ -5154,10 +5157,10 @@
     </row>
     <row r="273" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A273" s="6">
-        <v>60215</v>
+        <v>60211</v>
       </c>
       <c r="B273" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C273" s="1" t="s">
         <v>4</v>
@@ -5168,10 +5171,10 @@
     </row>
     <row r="274" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A274" s="6">
-        <v>60217</v>
+        <v>60215</v>
       </c>
       <c r="B274" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C274" s="1" t="s">
         <v>4</v>
@@ -5182,10 +5185,10 @@
     </row>
     <row r="275" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A275" s="6">
-        <v>60219</v>
+        <v>60217</v>
       </c>
       <c r="B275" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C275" s="1" t="s">
         <v>4</v>
@@ -5196,10 +5199,10 @@
     </row>
     <row r="276" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A276" s="6">
-        <v>60222</v>
+        <v>60219</v>
       </c>
       <c r="B276" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C276" s="1" t="s">
         <v>4</v>
@@ -5210,38 +5213,38 @@
     </row>
     <row r="277" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A277" s="6">
-        <v>60225</v>
+        <v>60222</v>
       </c>
       <c r="B277" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C277" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D277" t="s">
-        <v>9</v>
+      <c r="D277" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="278" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A278" s="6">
-        <v>60230</v>
+        <v>60225</v>
       </c>
       <c r="B278" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C278" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D278" s="1" t="s">
-        <v>8</v>
+      <c r="D278" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="279" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A279" s="6">
-        <v>60234</v>
+        <v>60230</v>
       </c>
       <c r="B279" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C279" s="1" t="s">
         <v>4</v>
@@ -5252,10 +5255,10 @@
     </row>
     <row r="280" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A280" s="6">
-        <v>60253</v>
+        <v>60234</v>
       </c>
       <c r="B280" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C280" s="1" t="s">
         <v>4</v>
@@ -5266,10 +5269,10 @@
     </row>
     <row r="281" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A281" s="6">
-        <v>60254</v>
+        <v>60253</v>
       </c>
       <c r="B281" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C281" s="1" t="s">
         <v>4</v>
@@ -5280,10 +5283,10 @@
     </row>
     <row r="282" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A282" s="6">
-        <v>60257</v>
+        <v>60254</v>
       </c>
       <c r="B282" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C282" s="1" t="s">
         <v>4</v>
@@ -5294,10 +5297,10 @@
     </row>
     <row r="283" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A283" s="6">
-        <v>60258</v>
+        <v>60257</v>
       </c>
       <c r="B283" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C283" s="1" t="s">
         <v>4</v>
@@ -5308,10 +5311,10 @@
     </row>
     <row r="284" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A284" s="6">
-        <v>60269</v>
+        <v>60258</v>
       </c>
       <c r="B284" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C284" s="1" t="s">
         <v>4</v>
@@ -5322,10 +5325,10 @@
     </row>
     <row r="285" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A285" s="6">
-        <v>60270</v>
+        <v>60269</v>
       </c>
       <c r="B285" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C285" s="1" t="s">
         <v>4</v>
@@ -5336,10 +5339,10 @@
     </row>
     <row r="286" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A286" s="6">
-        <v>60272</v>
+        <v>60270</v>
       </c>
       <c r="B286" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C286" s="1" t="s">
         <v>4</v>
@@ -5350,10 +5353,10 @@
     </row>
     <row r="287" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A287" s="6">
-        <v>60275</v>
+        <v>60272</v>
       </c>
       <c r="B287" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C287" s="1" t="s">
         <v>4</v>
@@ -5364,10 +5367,10 @@
     </row>
     <row r="288" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A288" s="6">
-        <v>60276</v>
+        <v>60275</v>
       </c>
       <c r="B288" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C288" s="1" t="s">
         <v>4</v>
@@ -5378,38 +5381,38 @@
     </row>
     <row r="289" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A289" s="6">
-        <v>60278</v>
+        <v>60276</v>
       </c>
       <c r="B289" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C289" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D289" s="3" t="s">
-        <v>5</v>
+      <c r="D289" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="290" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A290" s="6">
-        <v>60279</v>
+        <v>60278</v>
       </c>
       <c r="B290" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C290" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D290" s="1" t="s">
-        <v>8</v>
+      <c r="D290" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="291" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A291" s="6">
-        <v>60280</v>
+        <v>60279</v>
       </c>
       <c r="B291" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C291" s="1" t="s">
         <v>4</v>
@@ -5420,38 +5423,38 @@
     </row>
     <row r="292" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A292" s="6">
-        <v>61004</v>
+        <v>60280</v>
       </c>
       <c r="B292" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C292" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D292" s="3" t="s">
-        <v>5</v>
+      <c r="D292" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="293" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A293" s="6">
-        <v>61009</v>
+        <v>61004</v>
       </c>
       <c r="B293" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C293" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D293" s="1" t="s">
-        <v>8</v>
+      <c r="D293" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="294" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A294" s="6">
-        <v>61012</v>
+        <v>61009</v>
       </c>
       <c r="B294" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C294" s="1" t="s">
         <v>4</v>
@@ -5462,10 +5465,10 @@
     </row>
     <row r="295" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A295" s="6">
-        <v>61018</v>
+        <v>61012</v>
       </c>
       <c r="B295" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C295" s="1" t="s">
         <v>4</v>
@@ -5476,10 +5479,10 @@
     </row>
     <row r="296" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A296" s="6">
-        <v>61102</v>
+        <v>61018</v>
       </c>
       <c r="B296" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C296" s="1" t="s">
         <v>4</v>
@@ -5490,52 +5493,52 @@
     </row>
     <row r="297" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A297" s="6">
-        <v>61205</v>
+        <v>61102</v>
       </c>
       <c r="B297" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C297" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D297" s="3" t="s">
-        <v>5</v>
+      <c r="D297" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="298" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A298" s="6">
-        <v>70100</v>
+        <v>61205</v>
       </c>
       <c r="B298" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C298" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D298" s="1" t="s">
-        <v>8</v>
+      <c r="D298" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="299" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A299" s="6">
-        <v>70101</v>
+        <v>70100</v>
       </c>
       <c r="B299" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C299" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D299" s="3" t="s">
-        <v>5</v>
+      <c r="D299" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="300" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A300" s="6">
-        <v>70102</v>
+        <v>70101</v>
       </c>
       <c r="B300" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C300" s="1" t="s">
         <v>4</v>
@@ -5546,94 +5549,94 @@
     </row>
     <row r="301" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A301" s="6">
-        <v>70103</v>
+        <v>70102</v>
       </c>
       <c r="B301" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C301" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D301" s="1" t="s">
-        <v>8</v>
+      <c r="D301" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="302" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A302" s="6">
-        <v>70106</v>
+        <v>70103</v>
       </c>
       <c r="B302" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C302" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D302" s="3" t="s">
-        <v>5</v>
+      <c r="D302" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="303" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A303" s="6">
-        <v>70109</v>
+        <v>70106</v>
       </c>
       <c r="B303" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C303" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D303" s="1" t="s">
-        <v>8</v>
+      <c r="D303" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="304" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A304" s="6">
-        <v>70113</v>
+        <v>70109</v>
       </c>
       <c r="B304" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C304" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D304" s="3" t="s">
-        <v>5</v>
+      <c r="D304" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="305" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A305" s="6">
-        <v>70114</v>
+        <v>70113</v>
       </c>
       <c r="B305" t="s">
-        <v>327</v>
+        <v>307</v>
       </c>
       <c r="C305" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D305" s="7" t="s">
-        <v>9</v>
+      <c r="D305" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="306" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A306" s="6">
-        <v>70638</v>
+        <v>70114</v>
       </c>
       <c r="B306" t="s">
-        <v>308</v>
+        <v>327</v>
       </c>
       <c r="C306" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D306" s="1" t="s">
-        <v>8</v>
+      <c r="D306" s="7" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="307" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A307" s="6">
-        <v>70639</v>
+        <v>70638</v>
       </c>
       <c r="B307" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C307" s="1" t="s">
         <v>4</v>
@@ -5644,10 +5647,10 @@
     </row>
     <row r="308" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A308" s="6">
-        <v>70640</v>
+        <v>70639</v>
       </c>
       <c r="B308" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C308" s="1" t="s">
         <v>4</v>
@@ -5658,10 +5661,10 @@
     </row>
     <row r="309" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A309" s="6">
-        <v>70642</v>
+        <v>70640</v>
       </c>
       <c r="B309" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C309" s="1" t="s">
         <v>4</v>
@@ -5672,10 +5675,10 @@
     </row>
     <row r="310" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A310" s="6">
-        <v>90504</v>
+        <v>70642</v>
       </c>
       <c r="B310" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C310" s="1" t="s">
         <v>4</v>
@@ -5686,10 +5689,10 @@
     </row>
     <row r="311" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A311" s="6">
-        <v>90509</v>
+        <v>90504</v>
       </c>
       <c r="B311" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C311" s="1" t="s">
         <v>4</v>
@@ -5700,38 +5703,38 @@
     </row>
     <row r="312" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A312" s="6">
-        <v>90602</v>
+        <v>90509</v>
       </c>
       <c r="B312" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C312" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D312" s="3" t="s">
-        <v>5</v>
+      <c r="D312" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="313" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A313" s="6">
-        <v>90621</v>
+        <v>90602</v>
       </c>
       <c r="B313" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C313" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D313" s="1" t="s">
-        <v>8</v>
+      <c r="D313" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="314" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A314" s="6">
-        <v>90658</v>
+        <v>90621</v>
       </c>
       <c r="B314" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C314" s="1" t="s">
         <v>4</v>
@@ -5742,10 +5745,10 @@
     </row>
     <row r="315" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A315" s="6">
-        <v>90660</v>
+        <v>90658</v>
       </c>
       <c r="B315" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C315" s="1" t="s">
         <v>4</v>
@@ -5756,10 +5759,10 @@
     </row>
     <row r="316" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A316" s="6">
-        <v>90668</v>
+        <v>90660</v>
       </c>
       <c r="B316" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C316" s="1" t="s">
         <v>4</v>
@@ -5770,10 +5773,10 @@
     </row>
     <row r="317" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A317" s="6">
-        <v>90671</v>
+        <v>90668</v>
       </c>
       <c r="B317" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C317" s="1" t="s">
         <v>4</v>
@@ -5784,10 +5787,10 @@
     </row>
     <row r="318" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A318" s="6">
-        <v>90679</v>
+        <v>90671</v>
       </c>
       <c r="B318" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C318" s="1" t="s">
         <v>4</v>
@@ -5798,10 +5801,10 @@
     </row>
     <row r="319" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A319" s="6">
-        <v>90683</v>
+        <v>90679</v>
       </c>
       <c r="B319" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C319" s="1" t="s">
         <v>4</v>
@@ -5812,10 +5815,10 @@
     </row>
     <row r="320" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A320" s="6">
-        <v>90705</v>
+        <v>90683</v>
       </c>
       <c r="B320" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C320" s="1" t="s">
         <v>4</v>
@@ -5826,10 +5829,10 @@
     </row>
     <row r="321" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A321" s="6">
-        <v>90706</v>
+        <v>90705</v>
       </c>
       <c r="B321" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C321" s="1" t="s">
         <v>4</v>
@@ -5840,10 +5843,10 @@
     </row>
     <row r="322" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A322" s="6">
-        <v>90708</v>
+        <v>90706</v>
       </c>
       <c r="B322" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C322" s="1" t="s">
         <v>4</v>
@@ -5854,20 +5857,34 @@
     </row>
     <row r="323" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A323" s="6">
+        <v>90708</v>
+      </c>
+      <c r="B323" t="s">
+        <v>324</v>
+      </c>
+      <c r="C323" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D323" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="324" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A324" s="6">
         <v>90709</v>
       </c>
-      <c r="B323" t="s">
+      <c r="B324" t="s">
         <v>325</v>
       </c>
-      <c r="C323" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D323" s="1" t="s">
+      <c r="C324" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D324" s="1" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D323"/>
+  <autoFilter ref="A1:D324"/>
   <conditionalFormatting sqref="B1:B1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>

</xml_diff>

<commit_message>
agregue las ctas 20189, 70115, 20396
</commit_message>
<xml_diff>
--- a/excel/CLIENTES_PERMISOS.xlsx
+++ b/excel/CLIENTES_PERMISOS.xlsx
@@ -15,14 +15,14 @@
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Hoja 1'!$A$1:$D$324</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Hoja 1'!$A$1:$D$327</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="973" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="982" uniqueCount="334">
   <si>
     <t>CUENTA</t>
   </si>
@@ -1015,6 +1015,15 @@
   </si>
   <si>
     <t>CERAMICA SANTA MARTA</t>
+  </si>
+  <si>
+    <t>PINTURERIA NINA</t>
+  </si>
+  <si>
+    <t>FERRETERIA JUJUY</t>
+  </si>
+  <si>
+    <t>FERRETERIA ROSITA</t>
   </si>
 </sst>
 </file>
@@ -1334,10 +1343,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D324"/>
+  <dimension ref="A1:D327"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D77" sqref="D77"/>
+    <sheetView tabSelected="1" topLeftCell="A297" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D309" sqref="D309"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2903,24 +2912,24 @@
     </row>
     <row r="112" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="6">
-        <v>20200</v>
+        <v>20189</v>
       </c>
       <c r="B112" t="s">
-        <v>83</v>
+        <v>331</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D112" s="3" t="s">
-        <v>5</v>
+      <c r="D112" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="113" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A113" s="6">
-        <v>20201</v>
+        <v>20200</v>
       </c>
       <c r="B113" t="s">
-        <v>145</v>
+        <v>83</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>4</v>
@@ -2931,52 +2940,52 @@
     </row>
     <row r="114" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A114" s="6">
-        <v>20204</v>
+        <v>20201</v>
       </c>
       <c r="B114" t="s">
-        <v>57</v>
+        <v>145</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D114" s="1" t="s">
-        <v>8</v>
+      <c r="D114" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="115" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" s="6">
-        <v>20205</v>
+        <v>20204</v>
       </c>
       <c r="B115" t="s">
-        <v>206</v>
+        <v>57</v>
       </c>
       <c r="C115" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="116" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" s="6">
-        <v>20211</v>
+        <v>20205</v>
       </c>
       <c r="B116" t="s">
-        <v>190</v>
+        <v>206</v>
       </c>
       <c r="C116" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="117" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A117" s="6">
-        <v>20224</v>
+        <v>20211</v>
       </c>
       <c r="B117" t="s">
-        <v>85</v>
+        <v>190</v>
       </c>
       <c r="C117" s="1" t="s">
         <v>4</v>
@@ -2987,10 +2996,10 @@
     </row>
     <row r="118" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A118" s="6">
-        <v>20227</v>
+        <v>20224</v>
       </c>
       <c r="B118" t="s">
-        <v>192</v>
+        <v>85</v>
       </c>
       <c r="C118" s="1" t="s">
         <v>4</v>
@@ -3001,52 +3010,52 @@
     </row>
     <row r="119" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A119" s="6">
-        <v>20228</v>
+        <v>20227</v>
       </c>
       <c r="B119" t="s">
-        <v>91</v>
+        <v>192</v>
       </c>
       <c r="C119" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D119" s="3" t="s">
-        <v>5</v>
+      <c r="D119" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="120" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A120" s="6">
-        <v>20230</v>
+        <v>20228</v>
       </c>
       <c r="B120" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C120" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D120" s="1" t="s">
-        <v>8</v>
+      <c r="D120" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="121" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A121" s="6">
-        <v>20234</v>
+        <v>20230</v>
       </c>
       <c r="B121" t="s">
-        <v>29</v>
+        <v>89</v>
       </c>
       <c r="C121" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D121" s="3" t="s">
-        <v>5</v>
+      <c r="D121" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="122" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A122" s="6">
-        <v>20236</v>
+        <v>20234</v>
       </c>
       <c r="B122" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C122" s="1" t="s">
         <v>4</v>
@@ -3057,10 +3066,10 @@
     </row>
     <row r="123" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A123" s="6">
-        <v>20238</v>
+        <v>20236</v>
       </c>
       <c r="B123" t="s">
-        <v>139</v>
+        <v>31</v>
       </c>
       <c r="C123" s="1" t="s">
         <v>4</v>
@@ -3071,10 +3080,10 @@
     </row>
     <row r="124" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" s="6">
-        <v>20241</v>
+        <v>20238</v>
       </c>
       <c r="B124" t="s">
-        <v>22</v>
+        <v>139</v>
       </c>
       <c r="C124" s="1" t="s">
         <v>4</v>
@@ -3085,24 +3094,24 @@
     </row>
     <row r="125" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A125" s="6">
-        <v>20242</v>
+        <v>20241</v>
       </c>
       <c r="B125" t="s">
-        <v>216</v>
+        <v>22</v>
       </c>
       <c r="C125" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D125" s="1" t="s">
-        <v>8</v>
+      <c r="D125" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="126" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A126" s="6">
-        <v>20244</v>
+        <v>20242</v>
       </c>
       <c r="B126" t="s">
-        <v>124</v>
+        <v>216</v>
       </c>
       <c r="C126" s="1" t="s">
         <v>4</v>
@@ -3113,38 +3122,38 @@
     </row>
     <row r="127" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A127" s="6">
-        <v>20246</v>
+        <v>20244</v>
       </c>
       <c r="B127" t="s">
-        <v>14</v>
+        <v>124</v>
       </c>
       <c r="C127" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D127" s="3" t="s">
-        <v>5</v>
+      <c r="D127" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="128" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A128" s="6">
-        <v>20249</v>
+        <v>20246</v>
       </c>
       <c r="B128" t="s">
-        <v>72</v>
+        <v>14</v>
       </c>
       <c r="C128" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D128" s="1" t="s">
-        <v>8</v>
+      <c r="D128" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="129" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A129" s="6">
-        <v>20256</v>
+        <v>20249</v>
       </c>
       <c r="B129" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="C129" s="1" t="s">
         <v>4</v>
@@ -3155,66 +3164,66 @@
     </row>
     <row r="130" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A130" s="6">
-        <v>20257</v>
+        <v>20256</v>
       </c>
       <c r="B130" t="s">
-        <v>150</v>
+        <v>50</v>
       </c>
       <c r="C130" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D130" t="s">
-        <v>9</v>
+      <c r="D130" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="131" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A131" s="6">
-        <v>20258</v>
+        <v>20257</v>
       </c>
       <c r="B131" t="s">
-        <v>199</v>
+        <v>150</v>
       </c>
       <c r="C131" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D131" s="1" t="s">
-        <v>8</v>
+      <c r="D131" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="132" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A132" s="6">
-        <v>20260</v>
+        <v>20258</v>
       </c>
       <c r="B132" t="s">
-        <v>68</v>
+        <v>199</v>
       </c>
       <c r="C132" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D132" s="3" t="s">
-        <v>5</v>
+      <c r="D132" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="133" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A133" s="6">
-        <v>20261</v>
+        <v>20260</v>
       </c>
       <c r="B133" t="s">
-        <v>207</v>
+        <v>68</v>
       </c>
       <c r="C133" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D133" s="1" t="s">
-        <v>8</v>
+      <c r="D133" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="134" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A134" s="6">
-        <v>20262</v>
+        <v>20261</v>
       </c>
       <c r="B134" t="s">
-        <v>92</v>
+        <v>207</v>
       </c>
       <c r="C134" s="1" t="s">
         <v>4</v>
@@ -3225,10 +3234,10 @@
     </row>
     <row r="135" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A135" s="6">
-        <v>20268</v>
+        <v>20262</v>
       </c>
       <c r="B135" t="s">
-        <v>201</v>
+        <v>92</v>
       </c>
       <c r="C135" s="1" t="s">
         <v>4</v>
@@ -3239,150 +3248,150 @@
     </row>
     <row r="136" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A136" s="6">
-        <v>20271</v>
+        <v>20268</v>
       </c>
       <c r="B136" t="s">
-        <v>34</v>
+        <v>201</v>
       </c>
       <c r="C136" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D136" s="3" t="s">
-        <v>5</v>
+      <c r="D136" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="137" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A137" s="6">
-        <v>20272</v>
+        <v>20271</v>
       </c>
       <c r="B137" t="s">
-        <v>178</v>
+        <v>34</v>
       </c>
       <c r="C137" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D137" s="1" t="s">
-        <v>8</v>
+      <c r="D137" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="138" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A138" s="6">
-        <v>20275</v>
+        <v>20272</v>
       </c>
       <c r="B138" t="s">
-        <v>166</v>
+        <v>178</v>
       </c>
       <c r="C138" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D138" s="3" t="s">
-        <v>5</v>
+      <c r="D138" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="139" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A139" s="6">
-        <v>20277</v>
+        <v>20275</v>
       </c>
       <c r="B139" t="s">
-        <v>154</v>
+        <v>166</v>
       </c>
       <c r="C139" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D139" s="1" t="s">
-        <v>8</v>
+      <c r="D139" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="140" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A140" s="6">
-        <v>20281</v>
+        <v>20277</v>
       </c>
       <c r="B140" t="s">
-        <v>105</v>
+        <v>154</v>
       </c>
       <c r="C140" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D140" s="3" t="s">
-        <v>5</v>
+      <c r="D140" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="141" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A141" s="6">
-        <v>20282</v>
+        <v>20281</v>
       </c>
       <c r="B141" t="s">
-        <v>141</v>
+        <v>105</v>
       </c>
       <c r="C141" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D141" s="1" t="s">
-        <v>9</v>
+      <c r="D141" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="142" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A142" s="6">
-        <v>20284</v>
+        <v>20282</v>
       </c>
       <c r="B142" t="s">
-        <v>17</v>
+        <v>141</v>
       </c>
       <c r="C142" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D142" t="s">
+      <c r="D142" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="143" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A143" s="6">
-        <v>20285</v>
+        <v>20284</v>
       </c>
       <c r="B143" t="s">
-        <v>146</v>
+        <v>17</v>
       </c>
       <c r="C143" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D143" s="1" t="s">
-        <v>8</v>
+      <c r="D143" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="144" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A144" s="6">
-        <v>20289</v>
+        <v>20285</v>
       </c>
       <c r="B144" t="s">
-        <v>52</v>
+        <v>146</v>
       </c>
       <c r="C144" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D144" s="3" t="s">
-        <v>5</v>
+      <c r="D144" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="145" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A145" s="6">
-        <v>20290</v>
+        <v>20289</v>
       </c>
       <c r="B145" t="s">
-        <v>103</v>
+        <v>52</v>
       </c>
       <c r="C145" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D145" s="1" t="s">
-        <v>8</v>
+      <c r="D145" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="146" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A146" s="6">
-        <v>20291</v>
+        <v>20290</v>
       </c>
       <c r="B146" t="s">
-        <v>187</v>
+        <v>103</v>
       </c>
       <c r="C146" s="1" t="s">
         <v>4</v>
@@ -3393,24 +3402,24 @@
     </row>
     <row r="147" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A147" s="6">
-        <v>20292</v>
+        <v>20291</v>
       </c>
       <c r="B147" t="s">
-        <v>32</v>
+        <v>187</v>
       </c>
       <c r="C147" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D147" s="3" t="s">
-        <v>5</v>
+      <c r="D147" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="148" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A148" s="6">
-        <v>20293</v>
+        <v>20292</v>
       </c>
       <c r="B148" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="C148" s="1" t="s">
         <v>4</v>
@@ -3421,52 +3430,52 @@
     </row>
     <row r="149" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A149" s="6">
-        <v>20294</v>
+        <v>20293</v>
       </c>
       <c r="B149" t="s">
-        <v>202</v>
+        <v>43</v>
       </c>
       <c r="C149" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D149" s="1" t="s">
-        <v>8</v>
+      <c r="D149" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="150" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A150" s="6">
-        <v>20296</v>
+        <v>20294</v>
       </c>
       <c r="B150" t="s">
-        <v>144</v>
+        <v>202</v>
       </c>
       <c r="C150" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D150" s="3" t="s">
-        <v>5</v>
+      <c r="D150" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="151" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A151" s="6">
-        <v>20298</v>
+        <v>20296</v>
       </c>
       <c r="B151" t="s">
-        <v>169</v>
+        <v>144</v>
       </c>
       <c r="C151" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D151" s="1" t="s">
-        <v>8</v>
+      <c r="D151" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="152" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A152" s="6">
-        <v>20299</v>
+        <v>20298</v>
       </c>
       <c r="B152" t="s">
-        <v>58</v>
+        <v>169</v>
       </c>
       <c r="C152" s="1" t="s">
         <v>4</v>
@@ -3477,10 +3486,10 @@
     </row>
     <row r="153" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A153" s="6">
-        <v>20301</v>
+        <v>20299</v>
       </c>
       <c r="B153" t="s">
-        <v>134</v>
+        <v>58</v>
       </c>
       <c r="C153" s="1" t="s">
         <v>4</v>
@@ -3491,10 +3500,10 @@
     </row>
     <row r="154" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A154" s="6">
-        <v>20303</v>
+        <v>20301</v>
       </c>
       <c r="B154" t="s">
-        <v>37</v>
+        <v>134</v>
       </c>
       <c r="C154" s="1" t="s">
         <v>4</v>
@@ -3505,24 +3514,24 @@
     </row>
     <row r="155" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A155" s="6">
-        <v>20309</v>
+        <v>20303</v>
       </c>
       <c r="B155" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="C155" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D155" s="3" t="s">
-        <v>5</v>
+      <c r="D155" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="156" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A156" s="6">
-        <v>20310</v>
+        <v>20309</v>
       </c>
       <c r="B156" t="s">
-        <v>59</v>
+        <v>28</v>
       </c>
       <c r="C156" s="1" t="s">
         <v>4</v>
@@ -3533,24 +3542,24 @@
     </row>
     <row r="157" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A157" s="6">
-        <v>20318</v>
+        <v>20310</v>
       </c>
       <c r="B157" t="s">
-        <v>209</v>
+        <v>59</v>
       </c>
       <c r="C157" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D157" s="1" t="s">
-        <v>8</v>
+      <c r="D157" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="158" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A158" s="6">
-        <v>20319</v>
+        <v>20318</v>
       </c>
       <c r="B158" t="s">
-        <v>101</v>
+        <v>209</v>
       </c>
       <c r="C158" s="1" t="s">
         <v>4</v>
@@ -3561,10 +3570,10 @@
     </row>
     <row r="159" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A159" s="6">
-        <v>20320</v>
+        <v>20319</v>
       </c>
       <c r="B159" t="s">
-        <v>130</v>
+        <v>101</v>
       </c>
       <c r="C159" s="1" t="s">
         <v>4</v>
@@ -3575,10 +3584,10 @@
     </row>
     <row r="160" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A160" s="6">
-        <v>20324</v>
+        <v>20320</v>
       </c>
       <c r="B160" t="s">
-        <v>210</v>
+        <v>130</v>
       </c>
       <c r="C160" s="1" t="s">
         <v>4</v>
@@ -3589,10 +3598,10 @@
     </row>
     <row r="161" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A161" s="6">
-        <v>20331</v>
+        <v>20324</v>
       </c>
       <c r="B161" t="s">
-        <v>51</v>
+        <v>210</v>
       </c>
       <c r="C161" s="1" t="s">
         <v>4</v>
@@ -3603,38 +3612,38 @@
     </row>
     <row r="162" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A162" s="6">
-        <v>20333</v>
+        <v>20331</v>
       </c>
       <c r="B162" t="s">
-        <v>136</v>
+        <v>51</v>
       </c>
       <c r="C162" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D162" s="3" t="s">
-        <v>5</v>
+      <c r="D162" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="163" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A163" s="6">
-        <v>20337</v>
+        <v>20333</v>
       </c>
       <c r="B163" t="s">
-        <v>104</v>
+        <v>136</v>
       </c>
       <c r="C163" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D163" s="1" t="s">
-        <v>8</v>
+      <c r="D163" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="164" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A164" s="6">
-        <v>20343</v>
+        <v>20337</v>
       </c>
       <c r="B164" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="C164" s="1" t="s">
         <v>4</v>
@@ -3645,10 +3654,10 @@
     </row>
     <row r="165" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A165" s="6">
-        <v>20344</v>
+        <v>20343</v>
       </c>
       <c r="B165" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="C165" s="1" t="s">
         <v>4</v>
@@ -3659,66 +3668,66 @@
     </row>
     <row r="166" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A166" s="6">
-        <v>20351</v>
+        <v>20344</v>
       </c>
       <c r="B166" t="s">
-        <v>26</v>
+        <v>127</v>
       </c>
       <c r="C166" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D166" s="3" t="s">
-        <v>5</v>
+      <c r="D166" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="167" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A167" s="6">
-        <v>20357</v>
+        <v>20351</v>
       </c>
       <c r="B167" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="C167" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D167" s="1" t="s">
-        <v>8</v>
+      <c r="D167" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="168" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A168" s="6">
-        <v>20361</v>
+        <v>20357</v>
       </c>
       <c r="B168" t="s">
-        <v>164</v>
+        <v>56</v>
       </c>
       <c r="C168" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D168" s="3" t="s">
-        <v>5</v>
+      <c r="D168" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="169" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A169" s="6">
-        <v>20362</v>
+        <v>20361</v>
       </c>
       <c r="B169" t="s">
-        <v>45</v>
+        <v>164</v>
       </c>
       <c r="C169" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D169" s="1" t="s">
-        <v>8</v>
+      <c r="D169" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="170" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A170" s="6">
-        <v>20363</v>
+        <v>20362</v>
       </c>
       <c r="B170" t="s">
-        <v>213</v>
+        <v>45</v>
       </c>
       <c r="C170" s="1" t="s">
         <v>4</v>
@@ -3729,38 +3738,38 @@
     </row>
     <row r="171" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A171" s="6">
-        <v>20364</v>
+        <v>20363</v>
       </c>
       <c r="B171" t="s">
-        <v>196</v>
+        <v>213</v>
       </c>
       <c r="C171" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D171" s="3" t="s">
-        <v>5</v>
+      <c r="D171" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="172" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A172" s="6">
-        <v>20366</v>
+        <v>20364</v>
       </c>
       <c r="B172" t="s">
-        <v>220</v>
+        <v>196</v>
       </c>
       <c r="C172" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D172" s="1" t="s">
-        <v>8</v>
+      <c r="D172" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="173" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A173" s="6">
-        <v>20367</v>
+        <v>20366</v>
       </c>
       <c r="B173" t="s">
-        <v>47</v>
+        <v>220</v>
       </c>
       <c r="C173" s="1" t="s">
         <v>4</v>
@@ -3771,10 +3780,10 @@
     </row>
     <row r="174" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A174" s="6">
-        <v>20369</v>
+        <v>20367</v>
       </c>
       <c r="B174" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="C174" s="1" t="s">
         <v>4</v>
@@ -3785,10 +3794,10 @@
     </row>
     <row r="175" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A175" s="6">
-        <v>20371</v>
+        <v>20369</v>
       </c>
       <c r="B175" t="s">
-        <v>223</v>
+        <v>63</v>
       </c>
       <c r="C175" s="1" t="s">
         <v>4</v>
@@ -3799,10 +3808,10 @@
     </row>
     <row r="176" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A176" s="6">
-        <v>20372</v>
+        <v>20371</v>
       </c>
       <c r="B176" t="s">
-        <v>70</v>
+        <v>223</v>
       </c>
       <c r="C176" s="1" t="s">
         <v>4</v>
@@ -3813,10 +3822,10 @@
     </row>
     <row r="177" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A177" s="6">
-        <v>20374</v>
+        <v>20372</v>
       </c>
       <c r="B177" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="C177" s="1" t="s">
         <v>4</v>
@@ -3827,10 +3836,10 @@
     </row>
     <row r="178" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A178" s="6">
-        <v>20377</v>
+        <v>20374</v>
       </c>
       <c r="B178" t="s">
-        <v>225</v>
+        <v>61</v>
       </c>
       <c r="C178" s="1" t="s">
         <v>4</v>
@@ -3841,10 +3850,10 @@
     </row>
     <row r="179" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A179" s="6">
-        <v>20379</v>
+        <v>20377</v>
       </c>
       <c r="B179" t="s">
-        <v>49</v>
+        <v>225</v>
       </c>
       <c r="C179" s="1" t="s">
         <v>4</v>
@@ -3855,38 +3864,38 @@
     </row>
     <row r="180" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A180" s="6">
-        <v>20380</v>
+        <v>20379</v>
       </c>
       <c r="B180" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="C180" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D180" s="3" t="s">
-        <v>5</v>
+      <c r="D180" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="181" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A181" s="6">
-        <v>20381</v>
+        <v>20380</v>
       </c>
       <c r="B181" t="s">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="C181" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D181" s="1" t="s">
-        <v>8</v>
+      <c r="D181" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="182" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A182" s="6">
-        <v>20384</v>
+        <v>20381</v>
       </c>
       <c r="B182" t="s">
-        <v>181</v>
+        <v>60</v>
       </c>
       <c r="C182" s="1" t="s">
         <v>4</v>
@@ -3897,10 +3906,10 @@
     </row>
     <row r="183" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A183" s="6">
-        <v>20385</v>
+        <v>20384</v>
       </c>
       <c r="B183" t="s">
-        <v>36</v>
+        <v>181</v>
       </c>
       <c r="C183" s="1" t="s">
         <v>4</v>
@@ -3911,10 +3920,10 @@
     </row>
     <row r="184" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A184" s="6">
-        <v>20386</v>
+        <v>20385</v>
       </c>
       <c r="B184" t="s">
-        <v>119</v>
+        <v>36</v>
       </c>
       <c r="C184" s="1" t="s">
         <v>4</v>
@@ -3925,10 +3934,10 @@
     </row>
     <row r="185" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A185" s="6">
-        <v>20388</v>
+        <v>20386</v>
       </c>
       <c r="B185" t="s">
-        <v>100</v>
+        <v>119</v>
       </c>
       <c r="C185" s="1" t="s">
         <v>4</v>
@@ -3939,10 +3948,10 @@
     </row>
     <row r="186" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A186" s="6">
-        <v>20391</v>
+        <v>20388</v>
       </c>
       <c r="B186" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C186" s="1" t="s">
         <v>4</v>
@@ -3953,10 +3962,10 @@
     </row>
     <row r="187" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A187" s="6">
-        <v>20394</v>
+        <v>20391</v>
       </c>
       <c r="B187" t="s">
-        <v>173</v>
+        <v>106</v>
       </c>
       <c r="C187" s="1" t="s">
         <v>4</v>
@@ -3967,10 +3976,10 @@
     </row>
     <row r="188" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A188" s="6">
-        <v>20395</v>
+        <v>20394</v>
       </c>
       <c r="B188" t="s">
-        <v>161</v>
+        <v>173</v>
       </c>
       <c r="C188" s="1" t="s">
         <v>4</v>
@@ -3981,10 +3990,10 @@
     </row>
     <row r="189" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A189" s="6">
-        <v>30101</v>
+        <v>20395</v>
       </c>
       <c r="B189" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="C189" s="1" t="s">
         <v>4</v>
@@ -3995,66 +4004,66 @@
     </row>
     <row r="190" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A190" s="6">
-        <v>40124</v>
+        <v>20396</v>
       </c>
       <c r="B190" t="s">
-        <v>24</v>
+        <v>332</v>
       </c>
       <c r="C190" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D190" s="3" t="s">
-        <v>5</v>
+      <c r="D190" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="191" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A191" s="6">
-        <v>40125</v>
+        <v>30101</v>
       </c>
       <c r="B191" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="C191" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D191" s="3" t="s">
-        <v>5</v>
+      <c r="D191" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="192" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A192" s="6">
-        <v>40127</v>
+        <v>40124</v>
       </c>
       <c r="B192" t="s">
-        <v>163</v>
+        <v>24</v>
       </c>
       <c r="C192" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D192" s="1" t="s">
-        <v>8</v>
+      <c r="D192" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="193" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A193" s="6">
-        <v>40129</v>
+        <v>40125</v>
       </c>
       <c r="B193" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="C193" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D193" s="1" t="s">
-        <v>8</v>
+      <c r="D193" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="194" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A194" s="6">
-        <v>40137</v>
+        <v>40127</v>
       </c>
       <c r="B194" t="s">
-        <v>121</v>
+        <v>163</v>
       </c>
       <c r="C194" s="1" t="s">
         <v>4</v>
@@ -4065,10 +4074,10 @@
     </row>
     <row r="195" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A195" s="6">
-        <v>40139</v>
+        <v>40129</v>
       </c>
       <c r="B195" t="s">
-        <v>329</v>
+        <v>138</v>
       </c>
       <c r="C195" s="1" t="s">
         <v>4</v>
@@ -4079,10 +4088,10 @@
     </row>
     <row r="196" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A196" s="6">
-        <v>40140</v>
+        <v>40137</v>
       </c>
       <c r="B196" t="s">
-        <v>170</v>
+        <v>121</v>
       </c>
       <c r="C196" s="1" t="s">
         <v>4</v>
@@ -4093,24 +4102,24 @@
     </row>
     <row r="197" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A197" s="6">
-        <v>40141</v>
+        <v>40139</v>
       </c>
       <c r="B197" t="s">
-        <v>111</v>
+        <v>329</v>
       </c>
       <c r="C197" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D197" s="3" t="s">
-        <v>5</v>
+      <c r="D197" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="198" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A198" s="6">
-        <v>40143</v>
+        <v>40140</v>
       </c>
       <c r="B198" t="s">
-        <v>94</v>
+        <v>170</v>
       </c>
       <c r="C198" s="1" t="s">
         <v>4</v>
@@ -4121,10 +4130,10 @@
     </row>
     <row r="199" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A199" s="6">
-        <v>40144</v>
+        <v>40141</v>
       </c>
       <c r="B199" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C199" s="1" t="s">
         <v>4</v>
@@ -4135,66 +4144,66 @@
     </row>
     <row r="200" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A200" s="6">
-        <v>40145</v>
+        <v>40143</v>
       </c>
       <c r="B200" t="s">
-        <v>165</v>
+        <v>94</v>
       </c>
       <c r="C200" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D200" s="3" t="s">
-        <v>5</v>
+      <c r="D200" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="201" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A201" s="6">
-        <v>40150</v>
+        <v>40144</v>
       </c>
       <c r="B201" t="s">
-        <v>221</v>
+        <v>107</v>
       </c>
       <c r="C201" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D201" s="1" t="s">
-        <v>8</v>
+      <c r="D201" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="202" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A202" s="6">
-        <v>40151</v>
+        <v>40145</v>
       </c>
       <c r="B202" t="s">
-        <v>54</v>
+        <v>165</v>
       </c>
       <c r="C202" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D202" s="1" t="s">
-        <v>8</v>
+      <c r="D202" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="203" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A203" s="6">
-        <v>50102</v>
+        <v>40150</v>
       </c>
       <c r="B203" t="s">
-        <v>67</v>
+        <v>221</v>
       </c>
       <c r="C203" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D203" s="3" t="s">
-        <v>5</v>
+      <c r="D203" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="204" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A204" s="6">
-        <v>50222</v>
+        <v>40151</v>
       </c>
       <c r="B204" t="s">
-        <v>215</v>
+        <v>54</v>
       </c>
       <c r="C204" s="1" t="s">
         <v>4</v>
@@ -4205,38 +4214,38 @@
     </row>
     <row r="205" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A205" s="6">
-        <v>50223</v>
+        <v>50102</v>
       </c>
       <c r="B205" t="s">
-        <v>194</v>
+        <v>67</v>
       </c>
       <c r="C205" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D205" s="1" t="s">
-        <v>8</v>
+      <c r="D205" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="206" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A206" s="6">
-        <v>50224</v>
+        <v>50222</v>
       </c>
       <c r="B206" t="s">
-        <v>42</v>
+        <v>215</v>
       </c>
       <c r="C206" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D206" s="3" t="s">
-        <v>5</v>
+      <c r="D206" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="207" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A207" s="6">
-        <v>50444</v>
+        <v>50223</v>
       </c>
       <c r="B207" t="s">
-        <v>116</v>
+        <v>194</v>
       </c>
       <c r="C207" s="1" t="s">
         <v>4</v>
@@ -4247,10 +4256,10 @@
     </row>
     <row r="208" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A208" s="6">
-        <v>50607</v>
+        <v>50224</v>
       </c>
       <c r="B208" t="s">
-        <v>76</v>
+        <v>42</v>
       </c>
       <c r="C208" s="1" t="s">
         <v>4</v>
@@ -4261,10 +4270,10 @@
     </row>
     <row r="209" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A209" s="6">
-        <v>50608</v>
+        <v>50444</v>
       </c>
       <c r="B209" t="s">
-        <v>177</v>
+        <v>116</v>
       </c>
       <c r="C209" s="1" t="s">
         <v>4</v>
@@ -4275,24 +4284,24 @@
     </row>
     <row r="210" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A210" s="6">
-        <v>50622</v>
+        <v>50607</v>
       </c>
       <c r="B210" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="C210" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D210" s="1" t="s">
-        <v>8</v>
+      <c r="D210" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="211" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A211" s="6">
-        <v>50623</v>
+        <v>50608</v>
       </c>
       <c r="B211" t="s">
-        <v>110</v>
+        <v>177</v>
       </c>
       <c r="C211" s="1" t="s">
         <v>4</v>
@@ -4303,10 +4312,10 @@
     </row>
     <row r="212" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A212" s="6">
-        <v>50625</v>
+        <v>50622</v>
       </c>
       <c r="B212" t="s">
-        <v>204</v>
+        <v>95</v>
       </c>
       <c r="C212" s="1" t="s">
         <v>4</v>
@@ -4317,10 +4326,10 @@
     </row>
     <row r="213" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A213" s="6">
-        <v>50629</v>
+        <v>50623</v>
       </c>
       <c r="B213" t="s">
-        <v>188</v>
+        <v>110</v>
       </c>
       <c r="C213" s="1" t="s">
         <v>4</v>
@@ -4331,10 +4340,10 @@
     </row>
     <row r="214" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A214" s="6">
-        <v>50803</v>
+        <v>50625</v>
       </c>
       <c r="B214" t="s">
-        <v>82</v>
+        <v>204</v>
       </c>
       <c r="C214" s="1" t="s">
         <v>4</v>
@@ -4345,10 +4354,10 @@
     </row>
     <row r="215" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A215" s="6">
-        <v>50805</v>
+        <v>50629</v>
       </c>
       <c r="B215" t="s">
-        <v>135</v>
+        <v>188</v>
       </c>
       <c r="C215" s="1" t="s">
         <v>4</v>
@@ -4359,10 +4368,10 @@
     </row>
     <row r="216" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A216" s="6">
-        <v>50806</v>
+        <v>50803</v>
       </c>
       <c r="B216" t="s">
-        <v>156</v>
+        <v>82</v>
       </c>
       <c r="C216" s="1" t="s">
         <v>4</v>
@@ -4373,80 +4382,80 @@
     </row>
     <row r="217" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A217" s="6">
-        <v>50808</v>
+        <v>50805</v>
       </c>
       <c r="B217" t="s">
-        <v>16</v>
+        <v>135</v>
       </c>
       <c r="C217" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D217" s="3" t="s">
-        <v>5</v>
+      <c r="D217" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="218" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A218" s="6">
-        <v>50809</v>
+        <v>50806</v>
       </c>
       <c r="B218" t="s">
-        <v>98</v>
+        <v>156</v>
       </c>
       <c r="C218" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D218" s="3" t="s">
-        <v>5</v>
+      <c r="D218" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="219" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A219" s="6">
-        <v>50810</v>
+        <v>50808</v>
       </c>
       <c r="B219" t="s">
-        <v>175</v>
+        <v>16</v>
       </c>
       <c r="C219" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D219" s="1" t="s">
-        <v>8</v>
+      <c r="D219" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="220" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A220" s="6">
-        <v>50812</v>
+        <v>50809</v>
       </c>
       <c r="B220" t="s">
-        <v>184</v>
+        <v>98</v>
       </c>
       <c r="C220" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D220" s="1" t="s">
-        <v>8</v>
+      <c r="D220" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="221" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A221" s="6">
-        <v>50813</v>
+        <v>50810</v>
       </c>
       <c r="B221" t="s">
-        <v>71</v>
+        <v>175</v>
       </c>
       <c r="C221" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D221" t="s">
-        <v>9</v>
+      <c r="D221" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="222" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A222" s="6">
-        <v>50815</v>
+        <v>50812</v>
       </c>
       <c r="B222" t="s">
-        <v>114</v>
+        <v>184</v>
       </c>
       <c r="C222" s="1" t="s">
         <v>4</v>
@@ -4457,38 +4466,38 @@
     </row>
     <row r="223" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A223" s="6">
-        <v>50816</v>
+        <v>50813</v>
       </c>
       <c r="B223" t="s">
-        <v>205</v>
+        <v>71</v>
       </c>
       <c r="C223" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D223" s="1" t="s">
-        <v>8</v>
+      <c r="D223" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="224" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A224" s="6">
-        <v>50818</v>
+        <v>50815</v>
       </c>
       <c r="B224" t="s">
-        <v>227</v>
+        <v>114</v>
       </c>
       <c r="C224" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D224" s="3" t="s">
-        <v>5</v>
+      <c r="D224" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="225" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A225" s="6">
-        <v>50819</v>
+        <v>50816</v>
       </c>
       <c r="B225" t="s">
-        <v>228</v>
+        <v>205</v>
       </c>
       <c r="C225" s="1" t="s">
         <v>4</v>
@@ -4499,24 +4508,24 @@
     </row>
     <row r="226" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A226" s="6">
-        <v>50820</v>
+        <v>50818</v>
       </c>
       <c r="B226" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C226" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D226" s="1" t="s">
-        <v>8</v>
+      <c r="D226" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="227" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A227" s="6">
-        <v>50821</v>
+        <v>50819</v>
       </c>
       <c r="B227" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C227" s="1" t="s">
         <v>4</v>
@@ -4527,66 +4536,66 @@
     </row>
     <row r="228" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A228" s="6">
-        <v>50823</v>
+        <v>50820</v>
       </c>
       <c r="B228" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C228" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D228" t="s">
-        <v>9</v>
+      <c r="D228" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="229" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A229" s="6">
-        <v>50824</v>
+        <v>50821</v>
       </c>
       <c r="B229" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C229" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D229" s="3" t="s">
-        <v>5</v>
+      <c r="D229" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="230" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A230" s="6">
-        <v>50825</v>
+        <v>50823</v>
       </c>
       <c r="B230" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C230" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D230" s="1" t="s">
-        <v>8</v>
+      <c r="D230" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="231" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A231" s="6">
-        <v>50826</v>
+        <v>50824</v>
       </c>
       <c r="B231" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C231" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D231" s="1" t="s">
-        <v>8</v>
+      <c r="D231" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="232" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A232" s="6">
-        <v>50827</v>
+        <v>50825</v>
       </c>
       <c r="B232" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C232" s="1" t="s">
         <v>4</v>
@@ -4597,10 +4606,10 @@
     </row>
     <row r="233" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A233" s="6">
-        <v>50829</v>
+        <v>50826</v>
       </c>
       <c r="B233" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C233" s="1" t="s">
         <v>4</v>
@@ -4611,38 +4620,38 @@
     </row>
     <row r="234" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A234" s="6">
-        <v>60103</v>
+        <v>50827</v>
       </c>
       <c r="B234" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C234" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D234" s="3" t="s">
-        <v>5</v>
+      <c r="D234" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="235" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A235" s="6">
-        <v>60109</v>
+        <v>50829</v>
       </c>
       <c r="B235" t="s">
-        <v>330</v>
+        <v>236</v>
       </c>
       <c r="C235" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D235" s="7" t="s">
-        <v>9</v>
+      <c r="D235" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="236" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A236" s="6">
-        <v>60124</v>
+        <v>60103</v>
       </c>
       <c r="B236" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C236" s="1" t="s">
         <v>4</v>
@@ -4653,38 +4662,38 @@
     </row>
     <row r="237" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A237" s="6">
-        <v>60125</v>
+        <v>60109</v>
       </c>
       <c r="B237" t="s">
-        <v>239</v>
+        <v>330</v>
       </c>
       <c r="C237" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D237" s="3" t="s">
-        <v>5</v>
+      <c r="D237" s="7" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="238" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A238" s="6">
-        <v>60126</v>
+        <v>60124</v>
       </c>
       <c r="B238" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C238" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D238" s="1" t="s">
-        <v>8</v>
+      <c r="D238" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="239" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A239" s="6">
-        <v>60128</v>
+        <v>60125</v>
       </c>
       <c r="B239" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C239" s="1" t="s">
         <v>4</v>
@@ -4695,10 +4704,10 @@
     </row>
     <row r="240" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A240" s="6">
-        <v>60130</v>
+        <v>60126</v>
       </c>
       <c r="B240" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C240" s="1" t="s">
         <v>4</v>
@@ -4709,10 +4718,10 @@
     </row>
     <row r="241" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A241" s="6">
-        <v>60133</v>
+        <v>60128</v>
       </c>
       <c r="B241" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C241" s="1" t="s">
         <v>4</v>
@@ -4723,10 +4732,10 @@
     </row>
     <row r="242" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A242" s="6">
-        <v>60134</v>
+        <v>60130</v>
       </c>
       <c r="B242" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C242" s="1" t="s">
         <v>4</v>
@@ -4737,24 +4746,24 @@
     </row>
     <row r="243" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A243" s="6">
-        <v>60137</v>
+        <v>60133</v>
       </c>
       <c r="B243" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C243" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D243" s="1" t="s">
-        <v>8</v>
+      <c r="D243" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="244" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A244" s="6">
-        <v>60139</v>
+        <v>60134</v>
       </c>
       <c r="B244" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C244" s="1" t="s">
         <v>4</v>
@@ -4765,10 +4774,10 @@
     </row>
     <row r="245" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A245" s="6">
-        <v>60142</v>
+        <v>60137</v>
       </c>
       <c r="B245" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C245" s="1" t="s">
         <v>4</v>
@@ -4779,10 +4788,10 @@
     </row>
     <row r="246" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A246" s="6">
-        <v>60148</v>
+        <v>60139</v>
       </c>
       <c r="B246" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C246" s="1" t="s">
         <v>4</v>
@@ -4793,10 +4802,10 @@
     </row>
     <row r="247" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A247" s="6">
-        <v>60149</v>
+        <v>60142</v>
       </c>
       <c r="B247" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C247" s="1" t="s">
         <v>4</v>
@@ -4807,10 +4816,10 @@
     </row>
     <row r="248" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A248" s="6">
-        <v>60158</v>
+        <v>60148</v>
       </c>
       <c r="B248" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C248" s="1" t="s">
         <v>4</v>
@@ -4821,10 +4830,10 @@
     </row>
     <row r="249" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A249" s="6">
-        <v>60159</v>
+        <v>60149</v>
       </c>
       <c r="B249" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C249" s="1" t="s">
         <v>4</v>
@@ -4835,66 +4844,66 @@
     </row>
     <row r="250" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A250" s="6">
-        <v>60162</v>
+        <v>60158</v>
       </c>
       <c r="B250" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C250" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D250" s="3" t="s">
-        <v>5</v>
+      <c r="D250" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="251" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A251" s="6">
-        <v>60163</v>
+        <v>60159</v>
       </c>
       <c r="B251" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C251" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D251" s="3" t="s">
-        <v>5</v>
+      <c r="D251" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="252" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A252" s="6">
-        <v>60165</v>
+        <v>60162</v>
       </c>
       <c r="B252" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C252" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D252" s="1" t="s">
-        <v>8</v>
+      <c r="D252" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="253" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A253" s="6">
-        <v>60169</v>
+        <v>60163</v>
       </c>
       <c r="B253" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C253" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D253" s="1" t="s">
-        <v>8</v>
+      <c r="D253" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="254" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A254" s="6">
-        <v>60172</v>
+        <v>60165</v>
       </c>
       <c r="B254" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C254" s="1" t="s">
         <v>4</v>
@@ -4905,66 +4914,66 @@
     </row>
     <row r="255" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A255" s="6">
-        <v>60174</v>
+        <v>60169</v>
       </c>
       <c r="B255" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C255" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D255" s="3" t="s">
-        <v>5</v>
+      <c r="D255" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="256" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A256" s="6">
-        <v>60176</v>
+        <v>60172</v>
       </c>
       <c r="B256" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C256" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D256" s="3" t="s">
-        <v>5</v>
+      <c r="D256" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="257" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A257" s="6">
-        <v>60178</v>
+        <v>60174</v>
       </c>
       <c r="B257" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C257" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D257" s="1" t="s">
-        <v>8</v>
+      <c r="D257" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="258" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A258" s="6">
-        <v>60180</v>
+        <v>60176</v>
       </c>
       <c r="B258" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C258" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D258" s="1" t="s">
-        <v>8</v>
+      <c r="D258" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="259" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A259" s="6">
-        <v>60184</v>
+        <v>60178</v>
       </c>
       <c r="B259" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C259" s="1" t="s">
         <v>4</v>
@@ -4975,10 +4984,10 @@
     </row>
     <row r="260" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A260" s="6">
-        <v>60190</v>
+        <v>60180</v>
       </c>
       <c r="B260" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C260" s="1" t="s">
         <v>4</v>
@@ -4989,10 +4998,10 @@
     </row>
     <row r="261" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A261" s="6">
-        <v>60191</v>
+        <v>60184</v>
       </c>
       <c r="B261" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C261" s="1" t="s">
         <v>4</v>
@@ -5003,10 +5012,10 @@
     </row>
     <row r="262" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A262" s="6">
-        <v>60192</v>
+        <v>60190</v>
       </c>
       <c r="B262" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C262" s="1" t="s">
         <v>4</v>
@@ -5017,10 +5026,10 @@
     </row>
     <row r="263" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A263" s="6">
-        <v>60195</v>
+        <v>60191</v>
       </c>
       <c r="B263" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C263" s="1" t="s">
         <v>4</v>
@@ -5031,10 +5040,10 @@
     </row>
     <row r="264" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A264" s="6">
-        <v>60196</v>
+        <v>60192</v>
       </c>
       <c r="B264" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C264" s="1" t="s">
         <v>4</v>
@@ -5045,10 +5054,10 @@
     </row>
     <row r="265" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A265" s="6">
-        <v>60198</v>
+        <v>60195</v>
       </c>
       <c r="B265" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C265" s="1" t="s">
         <v>4</v>
@@ -5059,10 +5068,10 @@
     </row>
     <row r="266" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A266" s="6">
-        <v>60200</v>
+        <v>60196</v>
       </c>
       <c r="B266" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C266" s="1" t="s">
         <v>4</v>
@@ -5073,66 +5082,66 @@
     </row>
     <row r="267" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A267" s="6">
-        <v>60201</v>
+        <v>60198</v>
       </c>
       <c r="B267" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C267" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D267" t="s">
-        <v>9</v>
+      <c r="D267" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="268" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A268" s="6">
-        <v>60202</v>
+        <v>60200</v>
       </c>
       <c r="B268" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C268" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D268" s="3" t="s">
-        <v>5</v>
+      <c r="D268" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="269" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A269" s="6">
-        <v>60204</v>
+        <v>60201</v>
       </c>
       <c r="B269" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C269" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D269" s="1" t="s">
-        <v>8</v>
+      <c r="D269" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="270" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A270" s="6">
-        <v>60205</v>
+        <v>60202</v>
       </c>
       <c r="B270" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C270" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D270" s="1" t="s">
-        <v>8</v>
+      <c r="D270" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="271" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A271" s="6">
-        <v>60206</v>
+        <v>60204</v>
       </c>
       <c r="B271" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C271" s="1" t="s">
         <v>4</v>
@@ -5143,10 +5152,10 @@
     </row>
     <row r="272" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A272" s="6">
-        <v>60209</v>
+        <v>60205</v>
       </c>
       <c r="B272" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C272" s="1" t="s">
         <v>4</v>
@@ -5157,10 +5166,10 @@
     </row>
     <row r="273" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A273" s="6">
-        <v>60211</v>
+        <v>60206</v>
       </c>
       <c r="B273" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C273" s="1" t="s">
         <v>4</v>
@@ -5171,10 +5180,10 @@
     </row>
     <row r="274" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A274" s="6">
-        <v>60215</v>
+        <v>60209</v>
       </c>
       <c r="B274" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C274" s="1" t="s">
         <v>4</v>
@@ -5185,10 +5194,10 @@
     </row>
     <row r="275" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A275" s="6">
-        <v>60217</v>
+        <v>60211</v>
       </c>
       <c r="B275" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C275" s="1" t="s">
         <v>4</v>
@@ -5199,10 +5208,10 @@
     </row>
     <row r="276" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A276" s="6">
-        <v>60219</v>
+        <v>60215</v>
       </c>
       <c r="B276" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C276" s="1" t="s">
         <v>4</v>
@@ -5213,10 +5222,10 @@
     </row>
     <row r="277" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A277" s="6">
-        <v>60222</v>
+        <v>60217</v>
       </c>
       <c r="B277" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C277" s="1" t="s">
         <v>4</v>
@@ -5227,24 +5236,24 @@
     </row>
     <row r="278" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A278" s="6">
-        <v>60225</v>
+        <v>60219</v>
       </c>
       <c r="B278" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C278" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D278" t="s">
-        <v>9</v>
+      <c r="D278" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="279" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A279" s="6">
-        <v>60230</v>
+        <v>60222</v>
       </c>
       <c r="B279" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C279" s="1" t="s">
         <v>4</v>
@@ -5255,24 +5264,24 @@
     </row>
     <row r="280" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A280" s="6">
-        <v>60234</v>
+        <v>60225</v>
       </c>
       <c r="B280" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C280" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D280" s="1" t="s">
-        <v>8</v>
+      <c r="D280" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="281" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A281" s="6">
-        <v>60253</v>
+        <v>60230</v>
       </c>
       <c r="B281" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C281" s="1" t="s">
         <v>4</v>
@@ -5283,10 +5292,10 @@
     </row>
     <row r="282" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A282" s="6">
-        <v>60254</v>
+        <v>60234</v>
       </c>
       <c r="B282" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C282" s="1" t="s">
         <v>4</v>
@@ -5297,10 +5306,10 @@
     </row>
     <row r="283" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A283" s="6">
-        <v>60257</v>
+        <v>60253</v>
       </c>
       <c r="B283" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C283" s="1" t="s">
         <v>4</v>
@@ -5311,10 +5320,10 @@
     </row>
     <row r="284" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A284" s="6">
-        <v>60258</v>
+        <v>60254</v>
       </c>
       <c r="B284" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C284" s="1" t="s">
         <v>4</v>
@@ -5325,10 +5334,10 @@
     </row>
     <row r="285" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A285" s="6">
-        <v>60269</v>
+        <v>60257</v>
       </c>
       <c r="B285" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C285" s="1" t="s">
         <v>4</v>
@@ -5339,10 +5348,10 @@
     </row>
     <row r="286" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A286" s="6">
-        <v>60270</v>
+        <v>60258</v>
       </c>
       <c r="B286" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C286" s="1" t="s">
         <v>4</v>
@@ -5353,10 +5362,10 @@
     </row>
     <row r="287" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A287" s="6">
-        <v>60272</v>
+        <v>60269</v>
       </c>
       <c r="B287" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C287" s="1" t="s">
         <v>4</v>
@@ -5367,10 +5376,10 @@
     </row>
     <row r="288" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A288" s="6">
-        <v>60275</v>
+        <v>60270</v>
       </c>
       <c r="B288" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C288" s="1" t="s">
         <v>4</v>
@@ -5381,10 +5390,10 @@
     </row>
     <row r="289" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A289" s="6">
-        <v>60276</v>
+        <v>60272</v>
       </c>
       <c r="B289" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C289" s="1" t="s">
         <v>4</v>
@@ -5395,24 +5404,24 @@
     </row>
     <row r="290" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A290" s="6">
-        <v>60278</v>
+        <v>60275</v>
       </c>
       <c r="B290" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C290" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D290" s="3" t="s">
-        <v>5</v>
+      <c r="D290" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="291" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A291" s="6">
-        <v>60279</v>
+        <v>60276</v>
       </c>
       <c r="B291" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C291" s="1" t="s">
         <v>4</v>
@@ -5423,38 +5432,38 @@
     </row>
     <row r="292" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A292" s="6">
-        <v>60280</v>
+        <v>60278</v>
       </c>
       <c r="B292" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C292" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D292" s="1" t="s">
-        <v>8</v>
+      <c r="D292" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="293" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A293" s="6">
-        <v>61004</v>
+        <v>60279</v>
       </c>
       <c r="B293" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C293" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D293" s="3" t="s">
-        <v>5</v>
+      <c r="D293" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="294" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A294" s="6">
-        <v>61009</v>
+        <v>60280</v>
       </c>
       <c r="B294" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C294" s="1" t="s">
         <v>4</v>
@@ -5465,24 +5474,24 @@
     </row>
     <row r="295" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A295" s="6">
-        <v>61012</v>
+        <v>61004</v>
       </c>
       <c r="B295" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C295" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D295" s="1" t="s">
-        <v>8</v>
+      <c r="D295" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="296" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A296" s="6">
-        <v>61018</v>
+        <v>61009</v>
       </c>
       <c r="B296" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C296" s="1" t="s">
         <v>4</v>
@@ -5493,10 +5502,10 @@
     </row>
     <row r="297" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A297" s="6">
-        <v>61102</v>
+        <v>61012</v>
       </c>
       <c r="B297" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C297" s="1" t="s">
         <v>4</v>
@@ -5507,24 +5516,24 @@
     </row>
     <row r="298" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A298" s="6">
-        <v>61205</v>
+        <v>61018</v>
       </c>
       <c r="B298" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C298" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D298" s="3" t="s">
-        <v>5</v>
+      <c r="D298" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="299" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A299" s="6">
-        <v>70100</v>
+        <v>61102</v>
       </c>
       <c r="B299" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C299" s="1" t="s">
         <v>4</v>
@@ -5535,10 +5544,10 @@
     </row>
     <row r="300" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A300" s="6">
-        <v>70101</v>
+        <v>61205</v>
       </c>
       <c r="B300" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C300" s="1" t="s">
         <v>4</v>
@@ -5549,38 +5558,38 @@
     </row>
     <row r="301" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A301" s="6">
-        <v>70102</v>
+        <v>70100</v>
       </c>
       <c r="B301" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C301" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D301" s="3" t="s">
-        <v>5</v>
+      <c r="D301" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="302" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A302" s="6">
-        <v>70103</v>
+        <v>70101</v>
       </c>
       <c r="B302" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C302" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D302" s="1" t="s">
-        <v>8</v>
+      <c r="D302" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="303" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A303" s="6">
-        <v>70106</v>
+        <v>70102</v>
       </c>
       <c r="B303" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C303" s="1" t="s">
         <v>4</v>
@@ -5591,10 +5600,10 @@
     </row>
     <row r="304" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A304" s="6">
-        <v>70109</v>
+        <v>70103</v>
       </c>
       <c r="B304" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C304" s="1" t="s">
         <v>4</v>
@@ -5605,10 +5614,10 @@
     </row>
     <row r="305" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A305" s="6">
-        <v>70113</v>
+        <v>70106</v>
       </c>
       <c r="B305" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C305" s="1" t="s">
         <v>4</v>
@@ -5619,66 +5628,66 @@
     </row>
     <row r="306" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A306" s="6">
-        <v>70114</v>
+        <v>70109</v>
       </c>
       <c r="B306" t="s">
-        <v>327</v>
+        <v>306</v>
       </c>
       <c r="C306" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D306" s="7" t="s">
-        <v>9</v>
+      <c r="D306" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="307" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A307" s="6">
-        <v>70638</v>
+        <v>70113</v>
       </c>
       <c r="B307" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C307" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D307" s="1" t="s">
-        <v>8</v>
+      <c r="D307" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="308" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A308" s="6">
-        <v>70639</v>
+        <v>70114</v>
       </c>
       <c r="B308" t="s">
-        <v>309</v>
+        <v>327</v>
       </c>
       <c r="C308" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D308" s="1" t="s">
-        <v>8</v>
+      <c r="D308" s="7" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="309" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A309" s="6">
-        <v>70640</v>
+        <v>70115</v>
       </c>
       <c r="B309" t="s">
-        <v>310</v>
+        <v>333</v>
       </c>
       <c r="C309" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D309" s="1" t="s">
-        <v>8</v>
+      <c r="D309" s="7" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="310" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A310" s="6">
-        <v>70642</v>
+        <v>70638</v>
       </c>
       <c r="B310" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="C310" s="1" t="s">
         <v>4</v>
@@ -5689,10 +5698,10 @@
     </row>
     <row r="311" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A311" s="6">
-        <v>90504</v>
+        <v>70639</v>
       </c>
       <c r="B311" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="C311" s="1" t="s">
         <v>4</v>
@@ -5703,10 +5712,10 @@
     </row>
     <row r="312" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A312" s="6">
-        <v>90509</v>
+        <v>70640</v>
       </c>
       <c r="B312" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="C312" s="1" t="s">
         <v>4</v>
@@ -5717,24 +5726,24 @@
     </row>
     <row r="313" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A313" s="6">
-        <v>90602</v>
+        <v>70642</v>
       </c>
       <c r="B313" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="C313" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D313" s="3" t="s">
-        <v>5</v>
+      <c r="D313" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="314" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A314" s="6">
-        <v>90621</v>
+        <v>90504</v>
       </c>
       <c r="B314" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="C314" s="1" t="s">
         <v>4</v>
@@ -5745,10 +5754,10 @@
     </row>
     <row r="315" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A315" s="6">
-        <v>90658</v>
+        <v>90509</v>
       </c>
       <c r="B315" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="C315" s="1" t="s">
         <v>4</v>
@@ -5759,24 +5768,24 @@
     </row>
     <row r="316" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A316" s="6">
-        <v>90660</v>
+        <v>90602</v>
       </c>
       <c r="B316" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="C316" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D316" s="1" t="s">
-        <v>8</v>
+      <c r="D316" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="317" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A317" s="6">
-        <v>90668</v>
+        <v>90621</v>
       </c>
       <c r="B317" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="C317" s="1" t="s">
         <v>4</v>
@@ -5787,10 +5796,10 @@
     </row>
     <row r="318" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A318" s="6">
-        <v>90671</v>
+        <v>90658</v>
       </c>
       <c r="B318" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="C318" s="1" t="s">
         <v>4</v>
@@ -5801,10 +5810,10 @@
     </row>
     <row r="319" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A319" s="6">
-        <v>90679</v>
+        <v>90660</v>
       </c>
       <c r="B319" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="C319" s="1" t="s">
         <v>4</v>
@@ -5815,10 +5824,10 @@
     </row>
     <row r="320" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A320" s="6">
-        <v>90683</v>
+        <v>90668</v>
       </c>
       <c r="B320" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="C320" s="1" t="s">
         <v>4</v>
@@ -5829,10 +5838,10 @@
     </row>
     <row r="321" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A321" s="6">
-        <v>90705</v>
+        <v>90671</v>
       </c>
       <c r="B321" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="C321" s="1" t="s">
         <v>4</v>
@@ -5843,10 +5852,10 @@
     </row>
     <row r="322" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A322" s="6">
-        <v>90706</v>
+        <v>90679</v>
       </c>
       <c r="B322" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="C322" s="1" t="s">
         <v>4</v>
@@ -5857,10 +5866,10 @@
     </row>
     <row r="323" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A323" s="6">
-        <v>90708</v>
+        <v>90683</v>
       </c>
       <c r="B323" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C323" s="1" t="s">
         <v>4</v>
@@ -5871,20 +5880,62 @@
     </row>
     <row r="324" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A324" s="6">
+        <v>90705</v>
+      </c>
+      <c r="B324" t="s">
+        <v>322</v>
+      </c>
+      <c r="C324" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D324" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="325" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A325" s="6">
+        <v>90706</v>
+      </c>
+      <c r="B325" t="s">
+        <v>323</v>
+      </c>
+      <c r="C325" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D325" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="326" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A326" s="6">
+        <v>90708</v>
+      </c>
+      <c r="B326" t="s">
+        <v>324</v>
+      </c>
+      <c r="C326" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D326" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="327" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A327" s="6">
         <v>90709</v>
       </c>
-      <c r="B324" t="s">
+      <c r="B327" t="s">
         <v>325</v>
       </c>
-      <c r="C324" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D324" s="1" t="s">
+      <c r="C327" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D327" s="1" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D324"/>
+  <autoFilter ref="A1:D327"/>
   <conditionalFormatting sqref="B1:B1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>

</xml_diff>

<commit_message>
agregue cuenta 60150 f. alvarez
</commit_message>
<xml_diff>
--- a/excel/CLIENTES_PERMISOS.xlsx
+++ b/excel/CLIENTES_PERMISOS.xlsx
@@ -15,14 +15,14 @@
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Hoja 1'!$A$1:$D$327</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Hoja 1'!$A$1:$D$328</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="982" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="985" uniqueCount="335">
   <si>
     <t>CUENTA</t>
   </si>
@@ -1024,6 +1024,9 @@
   </si>
   <si>
     <t>FERRETERIA ROSITA</t>
+  </si>
+  <si>
+    <t>FERRETERIA ALVAREZ</t>
   </si>
 </sst>
 </file>
@@ -1343,10 +1346,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D327"/>
+  <dimension ref="A1:D328"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A297" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D309" sqref="D309"/>
+    <sheetView tabSelected="1" topLeftCell="A241" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G248" sqref="G248"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4844,24 +4847,24 @@
     </row>
     <row r="250" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A250" s="6">
-        <v>60158</v>
+        <v>60150</v>
       </c>
       <c r="B250" t="s">
-        <v>250</v>
+        <v>334</v>
       </c>
       <c r="C250" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D250" s="1" t="s">
-        <v>8</v>
+      <c r="D250" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="251" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A251" s="6">
-        <v>60159</v>
+        <v>60158</v>
       </c>
       <c r="B251" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C251" s="1" t="s">
         <v>4</v>
@@ -4872,24 +4875,24 @@
     </row>
     <row r="252" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A252" s="6">
-        <v>60162</v>
+        <v>60159</v>
       </c>
       <c r="B252" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C252" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D252" s="3" t="s">
-        <v>5</v>
+      <c r="D252" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="253" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A253" s="6">
-        <v>60163</v>
+        <v>60162</v>
       </c>
       <c r="B253" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C253" s="1" t="s">
         <v>4</v>
@@ -4900,24 +4903,24 @@
     </row>
     <row r="254" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A254" s="6">
-        <v>60165</v>
+        <v>60163</v>
       </c>
       <c r="B254" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C254" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D254" s="1" t="s">
-        <v>8</v>
+      <c r="D254" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="255" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A255" s="6">
-        <v>60169</v>
+        <v>60165</v>
       </c>
       <c r="B255" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C255" s="1" t="s">
         <v>4</v>
@@ -4928,10 +4931,10 @@
     </row>
     <row r="256" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A256" s="6">
-        <v>60172</v>
+        <v>60169</v>
       </c>
       <c r="B256" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C256" s="1" t="s">
         <v>4</v>
@@ -4942,24 +4945,24 @@
     </row>
     <row r="257" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A257" s="6">
-        <v>60174</v>
+        <v>60172</v>
       </c>
       <c r="B257" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C257" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D257" s="3" t="s">
-        <v>5</v>
+      <c r="D257" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="258" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A258" s="6">
-        <v>60176</v>
+        <v>60174</v>
       </c>
       <c r="B258" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C258" s="1" t="s">
         <v>4</v>
@@ -4970,24 +4973,24 @@
     </row>
     <row r="259" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A259" s="6">
-        <v>60178</v>
+        <v>60176</v>
       </c>
       <c r="B259" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C259" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D259" s="1" t="s">
-        <v>8</v>
+      <c r="D259" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="260" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A260" s="6">
-        <v>60180</v>
+        <v>60178</v>
       </c>
       <c r="B260" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C260" s="1" t="s">
         <v>4</v>
@@ -4998,10 +5001,10 @@
     </row>
     <row r="261" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A261" s="6">
-        <v>60184</v>
+        <v>60180</v>
       </c>
       <c r="B261" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C261" s="1" t="s">
         <v>4</v>
@@ -5012,10 +5015,10 @@
     </row>
     <row r="262" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A262" s="6">
-        <v>60190</v>
+        <v>60184</v>
       </c>
       <c r="B262" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C262" s="1" t="s">
         <v>4</v>
@@ -5026,10 +5029,10 @@
     </row>
     <row r="263" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A263" s="6">
-        <v>60191</v>
+        <v>60190</v>
       </c>
       <c r="B263" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C263" s="1" t="s">
         <v>4</v>
@@ -5040,10 +5043,10 @@
     </row>
     <row r="264" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A264" s="6">
-        <v>60192</v>
+        <v>60191</v>
       </c>
       <c r="B264" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C264" s="1" t="s">
         <v>4</v>
@@ -5054,10 +5057,10 @@
     </row>
     <row r="265" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A265" s="6">
-        <v>60195</v>
+        <v>60192</v>
       </c>
       <c r="B265" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C265" s="1" t="s">
         <v>4</v>
@@ -5068,10 +5071,10 @@
     </row>
     <row r="266" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A266" s="6">
-        <v>60196</v>
+        <v>60195</v>
       </c>
       <c r="B266" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C266" s="1" t="s">
         <v>4</v>
@@ -5082,10 +5085,10 @@
     </row>
     <row r="267" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A267" s="6">
-        <v>60198</v>
+        <v>60196</v>
       </c>
       <c r="B267" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C267" s="1" t="s">
         <v>4</v>
@@ -5096,10 +5099,10 @@
     </row>
     <row r="268" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A268" s="6">
-        <v>60200</v>
+        <v>60198</v>
       </c>
       <c r="B268" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C268" s="1" t="s">
         <v>4</v>
@@ -5110,52 +5113,52 @@
     </row>
     <row r="269" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A269" s="6">
-        <v>60201</v>
+        <v>60200</v>
       </c>
       <c r="B269" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C269" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D269" t="s">
-        <v>9</v>
+      <c r="D269" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="270" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A270" s="6">
-        <v>60202</v>
+        <v>60201</v>
       </c>
       <c r="B270" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C270" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D270" s="3" t="s">
-        <v>5</v>
+      <c r="D270" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="271" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A271" s="6">
-        <v>60204</v>
+        <v>60202</v>
       </c>
       <c r="B271" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C271" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D271" s="1" t="s">
-        <v>8</v>
+      <c r="D271" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="272" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A272" s="6">
-        <v>60205</v>
+        <v>60204</v>
       </c>
       <c r="B272" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C272" s="1" t="s">
         <v>4</v>
@@ -5166,10 +5169,10 @@
     </row>
     <row r="273" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A273" s="6">
-        <v>60206</v>
+        <v>60205</v>
       </c>
       <c r="B273" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C273" s="1" t="s">
         <v>4</v>
@@ -5180,10 +5183,10 @@
     </row>
     <row r="274" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A274" s="6">
-        <v>60209</v>
+        <v>60206</v>
       </c>
       <c r="B274" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C274" s="1" t="s">
         <v>4</v>
@@ -5194,10 +5197,10 @@
     </row>
     <row r="275" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A275" s="6">
-        <v>60211</v>
+        <v>60209</v>
       </c>
       <c r="B275" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C275" s="1" t="s">
         <v>4</v>
@@ -5208,10 +5211,10 @@
     </row>
     <row r="276" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A276" s="6">
-        <v>60215</v>
+        <v>60211</v>
       </c>
       <c r="B276" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C276" s="1" t="s">
         <v>4</v>
@@ -5222,10 +5225,10 @@
     </row>
     <row r="277" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A277" s="6">
-        <v>60217</v>
+        <v>60215</v>
       </c>
       <c r="B277" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C277" s="1" t="s">
         <v>4</v>
@@ -5236,10 +5239,10 @@
     </row>
     <row r="278" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A278" s="6">
-        <v>60219</v>
+        <v>60217</v>
       </c>
       <c r="B278" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C278" s="1" t="s">
         <v>4</v>
@@ -5250,10 +5253,10 @@
     </row>
     <row r="279" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A279" s="6">
-        <v>60222</v>
+        <v>60219</v>
       </c>
       <c r="B279" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C279" s="1" t="s">
         <v>4</v>
@@ -5264,38 +5267,38 @@
     </row>
     <row r="280" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A280" s="6">
-        <v>60225</v>
+        <v>60222</v>
       </c>
       <c r="B280" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C280" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D280" t="s">
-        <v>9</v>
+      <c r="D280" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="281" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A281" s="6">
-        <v>60230</v>
+        <v>60225</v>
       </c>
       <c r="B281" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C281" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D281" s="1" t="s">
-        <v>8</v>
+      <c r="D281" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="282" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A282" s="6">
-        <v>60234</v>
+        <v>60230</v>
       </c>
       <c r="B282" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C282" s="1" t="s">
         <v>4</v>
@@ -5306,10 +5309,10 @@
     </row>
     <row r="283" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A283" s="6">
-        <v>60253</v>
+        <v>60234</v>
       </c>
       <c r="B283" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C283" s="1" t="s">
         <v>4</v>
@@ -5320,10 +5323,10 @@
     </row>
     <row r="284" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A284" s="6">
-        <v>60254</v>
+        <v>60253</v>
       </c>
       <c r="B284" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C284" s="1" t="s">
         <v>4</v>
@@ -5334,10 +5337,10 @@
     </row>
     <row r="285" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A285" s="6">
-        <v>60257</v>
+        <v>60254</v>
       </c>
       <c r="B285" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C285" s="1" t="s">
         <v>4</v>
@@ -5348,10 +5351,10 @@
     </row>
     <row r="286" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A286" s="6">
-        <v>60258</v>
+        <v>60257</v>
       </c>
       <c r="B286" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C286" s="1" t="s">
         <v>4</v>
@@ -5362,10 +5365,10 @@
     </row>
     <row r="287" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A287" s="6">
-        <v>60269</v>
+        <v>60258</v>
       </c>
       <c r="B287" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C287" s="1" t="s">
         <v>4</v>
@@ -5376,10 +5379,10 @@
     </row>
     <row r="288" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A288" s="6">
-        <v>60270</v>
+        <v>60269</v>
       </c>
       <c r="B288" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C288" s="1" t="s">
         <v>4</v>
@@ -5390,10 +5393,10 @@
     </row>
     <row r="289" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A289" s="6">
-        <v>60272</v>
+        <v>60270</v>
       </c>
       <c r="B289" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C289" s="1" t="s">
         <v>4</v>
@@ -5404,10 +5407,10 @@
     </row>
     <row r="290" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A290" s="6">
-        <v>60275</v>
+        <v>60272</v>
       </c>
       <c r="B290" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C290" s="1" t="s">
         <v>4</v>
@@ -5418,10 +5421,10 @@
     </row>
     <row r="291" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A291" s="6">
-        <v>60276</v>
+        <v>60275</v>
       </c>
       <c r="B291" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C291" s="1" t="s">
         <v>4</v>
@@ -5432,38 +5435,38 @@
     </row>
     <row r="292" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A292" s="6">
-        <v>60278</v>
+        <v>60276</v>
       </c>
       <c r="B292" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C292" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D292" s="3" t="s">
-        <v>5</v>
+      <c r="D292" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="293" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A293" s="6">
-        <v>60279</v>
+        <v>60278</v>
       </c>
       <c r="B293" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C293" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D293" s="1" t="s">
-        <v>8</v>
+      <c r="D293" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="294" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A294" s="6">
-        <v>60280</v>
+        <v>60279</v>
       </c>
       <c r="B294" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C294" s="1" t="s">
         <v>4</v>
@@ -5474,38 +5477,38 @@
     </row>
     <row r="295" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A295" s="6">
-        <v>61004</v>
+        <v>60280</v>
       </c>
       <c r="B295" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C295" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D295" s="3" t="s">
-        <v>5</v>
+      <c r="D295" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="296" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A296" s="6">
-        <v>61009</v>
+        <v>61004</v>
       </c>
       <c r="B296" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C296" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D296" s="1" t="s">
-        <v>8</v>
+      <c r="D296" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="297" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A297" s="6">
-        <v>61012</v>
+        <v>61009</v>
       </c>
       <c r="B297" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C297" s="1" t="s">
         <v>4</v>
@@ -5516,10 +5519,10 @@
     </row>
     <row r="298" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A298" s="6">
-        <v>61018</v>
+        <v>61012</v>
       </c>
       <c r="B298" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C298" s="1" t="s">
         <v>4</v>
@@ -5530,10 +5533,10 @@
     </row>
     <row r="299" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A299" s="6">
-        <v>61102</v>
+        <v>61018</v>
       </c>
       <c r="B299" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C299" s="1" t="s">
         <v>4</v>
@@ -5544,52 +5547,52 @@
     </row>
     <row r="300" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A300" s="6">
-        <v>61205</v>
+        <v>61102</v>
       </c>
       <c r="B300" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C300" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D300" s="3" t="s">
-        <v>5</v>
+      <c r="D300" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="301" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A301" s="6">
-        <v>70100</v>
+        <v>61205</v>
       </c>
       <c r="B301" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C301" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D301" s="1" t="s">
-        <v>8</v>
+      <c r="D301" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="302" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A302" s="6">
-        <v>70101</v>
+        <v>70100</v>
       </c>
       <c r="B302" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C302" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D302" s="3" t="s">
-        <v>5</v>
+      <c r="D302" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="303" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A303" s="6">
-        <v>70102</v>
+        <v>70101</v>
       </c>
       <c r="B303" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C303" s="1" t="s">
         <v>4</v>
@@ -5600,80 +5603,80 @@
     </row>
     <row r="304" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A304" s="6">
-        <v>70103</v>
+        <v>70102</v>
       </c>
       <c r="B304" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C304" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D304" s="1" t="s">
-        <v>8</v>
+      <c r="D304" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="305" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A305" s="6">
-        <v>70106</v>
+        <v>70103</v>
       </c>
       <c r="B305" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C305" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D305" s="3" t="s">
-        <v>5</v>
+      <c r="D305" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="306" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A306" s="6">
-        <v>70109</v>
+        <v>70106</v>
       </c>
       <c r="B306" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C306" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D306" s="1" t="s">
-        <v>8</v>
+      <c r="D306" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="307" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A307" s="6">
-        <v>70113</v>
+        <v>70109</v>
       </c>
       <c r="B307" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C307" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D307" s="3" t="s">
-        <v>5</v>
+      <c r="D307" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="308" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A308" s="6">
-        <v>70114</v>
+        <v>70113</v>
       </c>
       <c r="B308" t="s">
-        <v>327</v>
+        <v>307</v>
       </c>
       <c r="C308" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D308" s="7" t="s">
-        <v>9</v>
+      <c r="D308" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="309" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A309" s="6">
-        <v>70115</v>
+        <v>70114</v>
       </c>
       <c r="B309" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="C309" s="1" t="s">
         <v>4</v>
@@ -5684,24 +5687,24 @@
     </row>
     <row r="310" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A310" s="6">
-        <v>70638</v>
+        <v>70115</v>
       </c>
       <c r="B310" t="s">
-        <v>308</v>
+        <v>333</v>
       </c>
       <c r="C310" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D310" s="1" t="s">
-        <v>8</v>
+      <c r="D310" s="7" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="311" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A311" s="6">
-        <v>70639</v>
+        <v>70638</v>
       </c>
       <c r="B311" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C311" s="1" t="s">
         <v>4</v>
@@ -5712,10 +5715,10 @@
     </row>
     <row r="312" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A312" s="6">
-        <v>70640</v>
+        <v>70639</v>
       </c>
       <c r="B312" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C312" s="1" t="s">
         <v>4</v>
@@ -5726,10 +5729,10 @@
     </row>
     <row r="313" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A313" s="6">
-        <v>70642</v>
+        <v>70640</v>
       </c>
       <c r="B313" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C313" s="1" t="s">
         <v>4</v>
@@ -5740,10 +5743,10 @@
     </row>
     <row r="314" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A314" s="6">
-        <v>90504</v>
+        <v>70642</v>
       </c>
       <c r="B314" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C314" s="1" t="s">
         <v>4</v>
@@ -5754,10 +5757,10 @@
     </row>
     <row r="315" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A315" s="6">
-        <v>90509</v>
+        <v>90504</v>
       </c>
       <c r="B315" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C315" s="1" t="s">
         <v>4</v>
@@ -5768,38 +5771,38 @@
     </row>
     <row r="316" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A316" s="6">
-        <v>90602</v>
+        <v>90509</v>
       </c>
       <c r="B316" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C316" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D316" s="3" t="s">
-        <v>5</v>
+      <c r="D316" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="317" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A317" s="6">
-        <v>90621</v>
+        <v>90602</v>
       </c>
       <c r="B317" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C317" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D317" s="1" t="s">
-        <v>8</v>
+      <c r="D317" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="318" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A318" s="6">
-        <v>90658</v>
+        <v>90621</v>
       </c>
       <c r="B318" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C318" s="1" t="s">
         <v>4</v>
@@ -5810,10 +5813,10 @@
     </row>
     <row r="319" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A319" s="6">
-        <v>90660</v>
+        <v>90658</v>
       </c>
       <c r="B319" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C319" s="1" t="s">
         <v>4</v>
@@ -5824,10 +5827,10 @@
     </row>
     <row r="320" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A320" s="6">
-        <v>90668</v>
+        <v>90660</v>
       </c>
       <c r="B320" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C320" s="1" t="s">
         <v>4</v>
@@ -5838,10 +5841,10 @@
     </row>
     <row r="321" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A321" s="6">
-        <v>90671</v>
+        <v>90668</v>
       </c>
       <c r="B321" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C321" s="1" t="s">
         <v>4</v>
@@ -5852,10 +5855,10 @@
     </row>
     <row r="322" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A322" s="6">
-        <v>90679</v>
+        <v>90671</v>
       </c>
       <c r="B322" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C322" s="1" t="s">
         <v>4</v>
@@ -5866,10 +5869,10 @@
     </row>
     <row r="323" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A323" s="6">
-        <v>90683</v>
+        <v>90679</v>
       </c>
       <c r="B323" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C323" s="1" t="s">
         <v>4</v>
@@ -5880,10 +5883,10 @@
     </row>
     <row r="324" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A324" s="6">
-        <v>90705</v>
+        <v>90683</v>
       </c>
       <c r="B324" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C324" s="1" t="s">
         <v>4</v>
@@ -5894,10 +5897,10 @@
     </row>
     <row r="325" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A325" s="6">
-        <v>90706</v>
+        <v>90705</v>
       </c>
       <c r="B325" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C325" s="1" t="s">
         <v>4</v>
@@ -5908,10 +5911,10 @@
     </row>
     <row r="326" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A326" s="6">
-        <v>90708</v>
+        <v>90706</v>
       </c>
       <c r="B326" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C326" s="1" t="s">
         <v>4</v>
@@ -5922,20 +5925,34 @@
     </row>
     <row r="327" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A327" s="6">
+        <v>90708</v>
+      </c>
+      <c r="B327" t="s">
+        <v>324</v>
+      </c>
+      <c r="C327" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D327" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="328" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A328" s="6">
         <v>90709</v>
       </c>
-      <c r="B327" t="s">
+      <c r="B328" t="s">
         <v>325</v>
       </c>
-      <c r="C327" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D327" s="1" t="s">
+      <c r="C328" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D328" s="1" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D327"/>
+  <autoFilter ref="A1:D328"/>
   <conditionalFormatting sqref="B1:B1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>

</xml_diff>

<commit_message>
agregue las cuentas de los nuevos clientes 13-10-25
</commit_message>
<xml_diff>
--- a/excel/CLIENTES_PERMISOS.xlsx
+++ b/excel/CLIENTES_PERMISOS.xlsx
@@ -15,14 +15,14 @@
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Hoja 1'!$A$1:$D$328</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Hoja 1'!$A$1:$D$326</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="985" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1105" uniqueCount="375">
   <si>
     <t>CUENTA</t>
   </si>
@@ -828,9 +828,6 @@
     <t>MATERIALES EL CHILENO</t>
   </si>
   <si>
-    <t>MEGAFER FERRETERIA</t>
-  </si>
-  <si>
     <t>BULONERA WORO</t>
   </si>
   <si>
@@ -870,9 +867,6 @@
     <t>CORRALON BETO</t>
   </si>
   <si>
-    <t>CORRALON M y M</t>
-  </si>
-  <si>
     <t>FERRETERIA EMILIANO LOS 4 HERM</t>
   </si>
   <si>
@@ -1027,6 +1021,132 @@
   </si>
   <si>
     <t>FERRETERIA ALVAREZ</t>
+  </si>
+  <si>
+    <t>EL PANTER</t>
+  </si>
+  <si>
+    <t>FERRETERIA CASERES</t>
+  </si>
+  <si>
+    <t>FERRETERIA LA FLECHA</t>
+  </si>
+  <si>
+    <t>CASA MAXIMO</t>
+  </si>
+  <si>
+    <t>CORRALON OASIS</t>
+  </si>
+  <si>
+    <t>FERRETERIA LA LUZ</t>
+  </si>
+  <si>
+    <t>SANITARIOS RZ</t>
+  </si>
+  <si>
+    <t>FERRETERIA JMK</t>
+  </si>
+  <si>
+    <t>FERRETERIA DOBLE C</t>
+  </si>
+  <si>
+    <t>FERRETERIA NALDO</t>
+  </si>
+  <si>
+    <t>FERRETERIA EL PUENTE</t>
+  </si>
+  <si>
+    <t>FERRETERIA CACHO</t>
+  </si>
+  <si>
+    <t>CORRALON SAN JORGE</t>
+  </si>
+  <si>
+    <t>FERRETERIA TORRENT</t>
+  </si>
+  <si>
+    <t>TRENTIN ALEJANDRO</t>
+  </si>
+  <si>
+    <t>FERRETERIA HORACIO</t>
+  </si>
+  <si>
+    <t>FERRETERIA LA HORMIGUITA</t>
+  </si>
+  <si>
+    <t>LAS 3 HERMANAS</t>
+  </si>
+  <si>
+    <t>FERRETERIA MATEO</t>
+  </si>
+  <si>
+    <t>FERRETERIA MYM</t>
+  </si>
+  <si>
+    <t>FERRETERIA LOCK</t>
+  </si>
+  <si>
+    <t>FERRETERIA ML 2</t>
+  </si>
+  <si>
+    <t>FERRETERIA ALAN</t>
+  </si>
+  <si>
+    <t>ARIDOS MOSCONI</t>
+  </si>
+  <si>
+    <t>FERRETERIA CONTRERAS</t>
+  </si>
+  <si>
+    <t>FERRETERIA FERREMIX</t>
+  </si>
+  <si>
+    <t>FERRETERIA ALBERTO</t>
+  </si>
+  <si>
+    <t>FERRETERIA LA BROCA</t>
+  </si>
+  <si>
+    <t>FERRETERIA BENJAMIN</t>
+  </si>
+  <si>
+    <t>FERRETERIA MP</t>
+  </si>
+  <si>
+    <t>FERRETERIA LAS CHICAS</t>
+  </si>
+  <si>
+    <t>FERRETERIA GARAY</t>
+  </si>
+  <si>
+    <t>MADERERA SERGIO</t>
+  </si>
+  <si>
+    <t>ELECTRO CHIQUI</t>
+  </si>
+  <si>
+    <t>BULL MAQ FERRETERIA</t>
+  </si>
+  <si>
+    <t>FERRETERIA GERMAN</t>
+  </si>
+  <si>
+    <t>FERRETERIA BRADAMEL</t>
+  </si>
+  <si>
+    <t>FERRETERIA MELANI</t>
+  </si>
+  <si>
+    <t>CORRALON COLODRERO</t>
+  </si>
+  <si>
+    <t>FERRETERIA PERICO</t>
+  </si>
+  <si>
+    <t>FERRETERIA ORION</t>
+  </si>
+  <si>
+    <t>FERRETERIA LUIS VARELA</t>
   </si>
 </sst>
 </file>
@@ -1062,7 +1182,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -1094,11 +1214,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1115,6 +1246,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1346,10 +1481,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D328"/>
+  <dimension ref="A1:D368"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A241" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G248" sqref="G248"/>
+    <sheetView tabSelected="1" topLeftCell="A351" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C326" sqref="C326:C368"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1378,7 +1513,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>4</v>
@@ -2638,7 +2773,7 @@
         <v>20129</v>
       </c>
       <c r="B92" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>4</v>
@@ -2918,7 +3053,7 @@
         <v>20189</v>
       </c>
       <c r="B112" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>4</v>
@@ -4010,7 +4145,7 @@
         <v>20396</v>
       </c>
       <c r="B190" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C190" s="1" t="s">
         <v>4</v>
@@ -4108,7 +4243,7 @@
         <v>40139</v>
       </c>
       <c r="B197" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C197" s="1" t="s">
         <v>4</v>
@@ -4668,7 +4803,7 @@
         <v>60109</v>
       </c>
       <c r="B237" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C237" s="1" t="s">
         <v>4</v>
@@ -4850,7 +4985,7 @@
         <v>60150</v>
       </c>
       <c r="B250" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C250" s="1" t="s">
         <v>4</v>
@@ -5113,7 +5248,7 @@
     </row>
     <row r="269" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A269" s="6">
-        <v>60200</v>
+        <v>60201</v>
       </c>
       <c r="B269" t="s">
         <v>268</v>
@@ -5121,13 +5256,13 @@
       <c r="C269" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D269" s="1" t="s">
-        <v>8</v>
+      <c r="D269" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="270" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A270" s="6">
-        <v>60201</v>
+        <v>60202</v>
       </c>
       <c r="B270" t="s">
         <v>269</v>
@@ -5135,13 +5270,13 @@
       <c r="C270" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D270" t="s">
-        <v>9</v>
+      <c r="D270" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="271" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A271" s="6">
-        <v>60202</v>
+        <v>60204</v>
       </c>
       <c r="B271" t="s">
         <v>270</v>
@@ -5149,13 +5284,13 @@
       <c r="C271" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D271" s="3" t="s">
-        <v>5</v>
+      <c r="D271" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="272" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A272" s="6">
-        <v>60204</v>
+        <v>60205</v>
       </c>
       <c r="B272" t="s">
         <v>271</v>
@@ -5169,7 +5304,7 @@
     </row>
     <row r="273" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A273" s="6">
-        <v>60205</v>
+        <v>60206</v>
       </c>
       <c r="B273" t="s">
         <v>272</v>
@@ -5183,7 +5318,7 @@
     </row>
     <row r="274" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A274" s="6">
-        <v>60206</v>
+        <v>60209</v>
       </c>
       <c r="B274" t="s">
         <v>273</v>
@@ -5197,7 +5332,7 @@
     </row>
     <row r="275" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A275" s="6">
-        <v>60209</v>
+        <v>60211</v>
       </c>
       <c r="B275" t="s">
         <v>274</v>
@@ -5211,7 +5346,7 @@
     </row>
     <row r="276" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A276" s="6">
-        <v>60211</v>
+        <v>60215</v>
       </c>
       <c r="B276" t="s">
         <v>275</v>
@@ -5225,7 +5360,7 @@
     </row>
     <row r="277" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A277" s="6">
-        <v>60215</v>
+        <v>60217</v>
       </c>
       <c r="B277" t="s">
         <v>276</v>
@@ -5239,7 +5374,7 @@
     </row>
     <row r="278" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A278" s="6">
-        <v>60217</v>
+        <v>60219</v>
       </c>
       <c r="B278" t="s">
         <v>277</v>
@@ -5253,7 +5388,7 @@
     </row>
     <row r="279" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A279" s="6">
-        <v>60219</v>
+        <v>60222</v>
       </c>
       <c r="B279" t="s">
         <v>278</v>
@@ -5267,7 +5402,7 @@
     </row>
     <row r="280" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A280" s="6">
-        <v>60222</v>
+        <v>60225</v>
       </c>
       <c r="B280" t="s">
         <v>279</v>
@@ -5275,13 +5410,13 @@
       <c r="C280" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D280" s="1" t="s">
-        <v>8</v>
+      <c r="D280" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="281" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A281" s="6">
-        <v>60225</v>
+        <v>60230</v>
       </c>
       <c r="B281" t="s">
         <v>280</v>
@@ -5289,13 +5424,13 @@
       <c r="C281" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D281" t="s">
-        <v>9</v>
+      <c r="D281" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="282" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A282" s="6">
-        <v>60230</v>
+        <v>60253</v>
       </c>
       <c r="B282" t="s">
         <v>281</v>
@@ -5309,7 +5444,7 @@
     </row>
     <row r="283" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A283" s="6">
-        <v>60234</v>
+        <v>60254</v>
       </c>
       <c r="B283" t="s">
         <v>282</v>
@@ -5323,7 +5458,7 @@
     </row>
     <row r="284" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A284" s="6">
-        <v>60253</v>
+        <v>60257</v>
       </c>
       <c r="B284" t="s">
         <v>283</v>
@@ -5337,7 +5472,7 @@
     </row>
     <row r="285" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A285" s="6">
-        <v>60254</v>
+        <v>60258</v>
       </c>
       <c r="B285" t="s">
         <v>284</v>
@@ -5351,7 +5486,7 @@
     </row>
     <row r="286" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A286" s="6">
-        <v>60257</v>
+        <v>60269</v>
       </c>
       <c r="B286" t="s">
         <v>285</v>
@@ -5365,7 +5500,7 @@
     </row>
     <row r="287" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A287" s="6">
-        <v>60258</v>
+        <v>60270</v>
       </c>
       <c r="B287" t="s">
         <v>286</v>
@@ -5379,7 +5514,7 @@
     </row>
     <row r="288" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A288" s="6">
-        <v>60269</v>
+        <v>60272</v>
       </c>
       <c r="B288" t="s">
         <v>287</v>
@@ -5393,7 +5528,7 @@
     </row>
     <row r="289" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A289" s="6">
-        <v>60270</v>
+        <v>60275</v>
       </c>
       <c r="B289" t="s">
         <v>288</v>
@@ -5407,7 +5542,7 @@
     </row>
     <row r="290" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A290" s="6">
-        <v>60272</v>
+        <v>60276</v>
       </c>
       <c r="B290" t="s">
         <v>289</v>
@@ -5421,7 +5556,7 @@
     </row>
     <row r="291" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A291" s="6">
-        <v>60275</v>
+        <v>60278</v>
       </c>
       <c r="B291" t="s">
         <v>290</v>
@@ -5429,13 +5564,13 @@
       <c r="C291" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D291" s="1" t="s">
-        <v>8</v>
+      <c r="D291" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="292" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A292" s="6">
-        <v>60276</v>
+        <v>60279</v>
       </c>
       <c r="B292" t="s">
         <v>291</v>
@@ -5449,7 +5584,7 @@
     </row>
     <row r="293" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A293" s="6">
-        <v>60278</v>
+        <v>60280</v>
       </c>
       <c r="B293" t="s">
         <v>292</v>
@@ -5457,13 +5592,13 @@
       <c r="C293" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D293" s="3" t="s">
-        <v>5</v>
+      <c r="D293" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="294" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A294" s="6">
-        <v>60279</v>
+        <v>61004</v>
       </c>
       <c r="B294" t="s">
         <v>293</v>
@@ -5471,13 +5606,13 @@
       <c r="C294" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D294" s="1" t="s">
-        <v>8</v>
+      <c r="D294" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="295" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A295" s="6">
-        <v>60280</v>
+        <v>61009</v>
       </c>
       <c r="B295" t="s">
         <v>294</v>
@@ -5491,7 +5626,7 @@
     </row>
     <row r="296" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A296" s="6">
-        <v>61004</v>
+        <v>61012</v>
       </c>
       <c r="B296" t="s">
         <v>295</v>
@@ -5499,13 +5634,13 @@
       <c r="C296" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D296" s="3" t="s">
-        <v>5</v>
+      <c r="D296" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="297" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A297" s="6">
-        <v>61009</v>
+        <v>61018</v>
       </c>
       <c r="B297" t="s">
         <v>296</v>
@@ -5519,7 +5654,7 @@
     </row>
     <row r="298" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A298" s="6">
-        <v>61012</v>
+        <v>61102</v>
       </c>
       <c r="B298" t="s">
         <v>297</v>
@@ -5533,7 +5668,7 @@
     </row>
     <row r="299" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A299" s="6">
-        <v>61018</v>
+        <v>61205</v>
       </c>
       <c r="B299" t="s">
         <v>298</v>
@@ -5541,13 +5676,13 @@
       <c r="C299" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D299" s="1" t="s">
-        <v>8</v>
+      <c r="D299" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="300" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A300" s="6">
-        <v>61102</v>
+        <v>70100</v>
       </c>
       <c r="B300" t="s">
         <v>299</v>
@@ -5561,7 +5696,7 @@
     </row>
     <row r="301" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A301" s="6">
-        <v>61205</v>
+        <v>70101</v>
       </c>
       <c r="B301" t="s">
         <v>300</v>
@@ -5575,7 +5710,7 @@
     </row>
     <row r="302" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A302" s="6">
-        <v>70100</v>
+        <v>70102</v>
       </c>
       <c r="B302" t="s">
         <v>301</v>
@@ -5583,13 +5718,13 @@
       <c r="C302" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D302" s="1" t="s">
-        <v>8</v>
+      <c r="D302" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="303" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A303" s="6">
-        <v>70101</v>
+        <v>70103</v>
       </c>
       <c r="B303" t="s">
         <v>302</v>
@@ -5597,13 +5732,13 @@
       <c r="C303" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D303" s="3" t="s">
-        <v>5</v>
+      <c r="D303" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="304" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A304" s="6">
-        <v>70102</v>
+        <v>70106</v>
       </c>
       <c r="B304" t="s">
         <v>303</v>
@@ -5617,7 +5752,7 @@
     </row>
     <row r="305" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A305" s="6">
-        <v>70103</v>
+        <v>70109</v>
       </c>
       <c r="B305" t="s">
         <v>304</v>
@@ -5631,7 +5766,7 @@
     </row>
     <row r="306" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A306" s="6">
-        <v>70106</v>
+        <v>70113</v>
       </c>
       <c r="B306" t="s">
         <v>305</v>
@@ -5645,63 +5780,63 @@
     </row>
     <row r="307" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A307" s="6">
-        <v>70109</v>
+        <v>70114</v>
       </c>
       <c r="B307" t="s">
-        <v>306</v>
+        <v>325</v>
       </c>
       <c r="C307" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D307" s="1" t="s">
-        <v>8</v>
+      <c r="D307" s="7" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="308" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A308" s="6">
-        <v>70113</v>
+        <v>70115</v>
       </c>
       <c r="B308" t="s">
-        <v>307</v>
+        <v>331</v>
       </c>
       <c r="C308" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D308" s="3" t="s">
-        <v>5</v>
+      <c r="D308" s="7" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="309" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A309" s="6">
-        <v>70114</v>
+        <v>70638</v>
       </c>
       <c r="B309" t="s">
-        <v>327</v>
+        <v>306</v>
       </c>
       <c r="C309" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D309" s="7" t="s">
-        <v>9</v>
+      <c r="D309" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="310" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A310" s="6">
-        <v>70115</v>
+        <v>70639</v>
       </c>
       <c r="B310" t="s">
-        <v>333</v>
+        <v>307</v>
       </c>
       <c r="C310" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D310" s="7" t="s">
-        <v>9</v>
+      <c r="D310" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="311" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A311" s="6">
-        <v>70638</v>
+        <v>70640</v>
       </c>
       <c r="B311" t="s">
         <v>308</v>
@@ -5715,7 +5850,7 @@
     </row>
     <row r="312" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A312" s="6">
-        <v>70639</v>
+        <v>70642</v>
       </c>
       <c r="B312" t="s">
         <v>309</v>
@@ -5729,7 +5864,7 @@
     </row>
     <row r="313" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A313" s="6">
-        <v>70640</v>
+        <v>90504</v>
       </c>
       <c r="B313" t="s">
         <v>310</v>
@@ -5743,7 +5878,7 @@
     </row>
     <row r="314" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A314" s="6">
-        <v>70642</v>
+        <v>90509</v>
       </c>
       <c r="B314" t="s">
         <v>311</v>
@@ -5757,7 +5892,7 @@
     </row>
     <row r="315" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A315" s="6">
-        <v>90504</v>
+        <v>90602</v>
       </c>
       <c r="B315" t="s">
         <v>312</v>
@@ -5765,13 +5900,13 @@
       <c r="C315" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D315" s="1" t="s">
-        <v>8</v>
+      <c r="D315" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="316" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A316" s="6">
-        <v>90509</v>
+        <v>90621</v>
       </c>
       <c r="B316" t="s">
         <v>313</v>
@@ -5785,7 +5920,7 @@
     </row>
     <row r="317" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A317" s="6">
-        <v>90602</v>
+        <v>90658</v>
       </c>
       <c r="B317" t="s">
         <v>314</v>
@@ -5793,13 +5928,13 @@
       <c r="C317" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D317" s="3" t="s">
-        <v>5</v>
+      <c r="D317" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="318" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A318" s="6">
-        <v>90621</v>
+        <v>90660</v>
       </c>
       <c r="B318" t="s">
         <v>315</v>
@@ -5813,7 +5948,7 @@
     </row>
     <row r="319" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A319" s="6">
-        <v>90658</v>
+        <v>90668</v>
       </c>
       <c r="B319" t="s">
         <v>316</v>
@@ -5827,7 +5962,7 @@
     </row>
     <row r="320" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A320" s="6">
-        <v>90660</v>
+        <v>90671</v>
       </c>
       <c r="B320" t="s">
         <v>317</v>
@@ -5841,7 +5976,7 @@
     </row>
     <row r="321" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A321" s="6">
-        <v>90668</v>
+        <v>90679</v>
       </c>
       <c r="B321" t="s">
         <v>318</v>
@@ -5855,7 +5990,7 @@
     </row>
     <row r="322" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A322" s="6">
-        <v>90671</v>
+        <v>90683</v>
       </c>
       <c r="B322" t="s">
         <v>319</v>
@@ -5869,7 +6004,7 @@
     </row>
     <row r="323" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A323" s="6">
-        <v>90679</v>
+        <v>90705</v>
       </c>
       <c r="B323" t="s">
         <v>320</v>
@@ -5883,7 +6018,7 @@
     </row>
     <row r="324" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A324" s="6">
-        <v>90683</v>
+        <v>90706</v>
       </c>
       <c r="B324" t="s">
         <v>321</v>
@@ -5897,7 +6032,7 @@
     </row>
     <row r="325" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A325" s="6">
-        <v>90705</v>
+        <v>90708</v>
       </c>
       <c r="B325" t="s">
         <v>322</v>
@@ -5911,7 +6046,7 @@
     </row>
     <row r="326" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A326" s="6">
-        <v>90706</v>
+        <v>90709</v>
       </c>
       <c r="B326" t="s">
         <v>323</v>
@@ -5925,34 +6060,594 @@
     </row>
     <row r="327" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A327" s="6">
-        <v>90708</v>
+        <v>90622</v>
       </c>
       <c r="B327" t="s">
-        <v>324</v>
+        <v>333</v>
       </c>
       <c r="C327" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D327" s="1" t="s">
-        <v>8</v>
+      <c r="D327" s="9" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="328" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A328" s="6">
-        <v>90709</v>
-      </c>
-      <c r="B328" t="s">
-        <v>325</v>
+        <v>60286</v>
+      </c>
+      <c r="B328" s="8" t="s">
+        <v>334</v>
       </c>
       <c r="C328" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D328" s="1" t="s">
+      <c r="D328" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="329" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A329" s="6">
+        <v>60284</v>
+      </c>
+      <c r="B329" s="8" t="s">
+        <v>335</v>
+      </c>
+      <c r="C329" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D329" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="330" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A330" s="6">
+        <v>60281</v>
+      </c>
+      <c r="B330" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="C330" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D330" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="331" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A331" s="6">
+        <v>60170</v>
+      </c>
+      <c r="B331" s="8" t="s">
+        <v>337</v>
+      </c>
+      <c r="C331" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D331" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="332" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A332" s="6">
+        <v>60241</v>
+      </c>
+      <c r="B332" s="8" t="s">
+        <v>338</v>
+      </c>
+      <c r="C332" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D332" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="333" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A333" s="6">
+        <v>60250</v>
+      </c>
+      <c r="B333" s="8" t="s">
+        <v>339</v>
+      </c>
+      <c r="C333" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D333" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="334" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A334" s="6">
+        <v>60282</v>
+      </c>
+      <c r="B334" s="8" t="s">
+        <v>340</v>
+      </c>
+      <c r="C334" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D334" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="335" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A335" s="6">
+        <v>60242</v>
+      </c>
+      <c r="B335" s="8" t="s">
+        <v>341</v>
+      </c>
+      <c r="C335" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D335" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="336" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A336" s="6">
+        <v>90631</v>
+      </c>
+      <c r="B336" s="8" t="s">
+        <v>342</v>
+      </c>
+      <c r="C336" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D336" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="337" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A337" s="6">
+        <v>60266</v>
+      </c>
+      <c r="B337" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="C337" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D337" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="338" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A338" s="6">
+        <v>60283</v>
+      </c>
+      <c r="B338" s="8" t="s">
+        <v>344</v>
+      </c>
+      <c r="C338" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D338" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="339" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A339" s="6">
+        <v>20397</v>
+      </c>
+      <c r="B339" s="8" t="s">
+        <v>345</v>
+      </c>
+      <c r="C339" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D339" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="340" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A340" s="6">
+        <v>1035</v>
+      </c>
+      <c r="B340" s="8" t="s">
+        <v>346</v>
+      </c>
+      <c r="C340" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D340" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="341" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A341" s="6">
+        <v>1031</v>
+      </c>
+      <c r="B341" s="8" t="s">
+        <v>347</v>
+      </c>
+      <c r="C341" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D341" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="342" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A342" s="6">
+        <v>50611</v>
+      </c>
+      <c r="B342" s="8" t="s">
+        <v>348</v>
+      </c>
+      <c r="C342" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D342" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="343" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A343" s="6">
+        <v>10166</v>
+      </c>
+      <c r="B343" s="8" t="s">
+        <v>349</v>
+      </c>
+      <c r="C343" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D343" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="344" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A344" s="6">
+        <v>1034</v>
+      </c>
+      <c r="B344" s="8" t="s">
+        <v>374</v>
+      </c>
+      <c r="C344" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D344" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="345" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A345" s="6">
+        <v>50832</v>
+      </c>
+      <c r="B345" s="8" t="s">
+        <v>350</v>
+      </c>
+      <c r="C345" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D345" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="346" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A346" s="6">
+        <v>60285</v>
+      </c>
+      <c r="B346" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="C346" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D346" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="347" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A347" s="6">
+        <v>50831</v>
+      </c>
+      <c r="B347" t="s">
+        <v>352</v>
+      </c>
+      <c r="C347" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D347" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="348" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A348" s="6">
+        <v>1038</v>
+      </c>
+      <c r="B348" t="s">
+        <v>353</v>
+      </c>
+      <c r="C348" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D348" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="349" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A349" s="6">
+        <v>1037</v>
+      </c>
+      <c r="B349" t="s">
+        <v>354</v>
+      </c>
+      <c r="C349" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D349" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="350" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A350" s="6">
+        <v>50445</v>
+      </c>
+      <c r="B350" t="s">
+        <v>355</v>
+      </c>
+      <c r="C350" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D350" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="351" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A351" s="6">
+        <v>1023</v>
+      </c>
+      <c r="B351" t="s">
+        <v>356</v>
+      </c>
+      <c r="C351" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D351" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="352" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A352" s="6">
+        <v>1030</v>
+      </c>
+      <c r="B352" t="s">
+        <v>357</v>
+      </c>
+      <c r="C352" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D352" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="353" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A353" s="6">
+        <v>1033</v>
+      </c>
+      <c r="B353" t="s">
+        <v>358</v>
+      </c>
+      <c r="C353" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D353" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="354" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A354" s="6">
+        <v>1036</v>
+      </c>
+      <c r="B354" t="s">
+        <v>359</v>
+      </c>
+      <c r="C354" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D354" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="355" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A355" s="6">
+        <v>1029</v>
+      </c>
+      <c r="B355" t="s">
+        <v>360</v>
+      </c>
+      <c r="C355" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D355" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="356" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A356" s="6">
+        <v>50630</v>
+      </c>
+      <c r="B356" t="s">
+        <v>361</v>
+      </c>
+      <c r="C356" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D356" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="357" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A357" s="6">
+        <v>1024</v>
+      </c>
+      <c r="B357" t="s">
+        <v>362</v>
+      </c>
+      <c r="C357" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D357" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="358" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A358" s="6">
+        <v>1020</v>
+      </c>
+      <c r="B358" t="s">
+        <v>363</v>
+      </c>
+      <c r="C358" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D358" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="359" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A359" s="6">
+        <v>1027</v>
+      </c>
+      <c r="B359" t="s">
+        <v>364</v>
+      </c>
+      <c r="C359" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D359" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="360" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A360" s="6">
+        <v>1025</v>
+      </c>
+      <c r="B360" t="s">
+        <v>365</v>
+      </c>
+      <c r="C360" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D360" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="361" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A361" s="6">
+        <v>1028</v>
+      </c>
+      <c r="B361" t="s">
+        <v>366</v>
+      </c>
+      <c r="C361" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D361" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="362" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A362" s="6">
+        <v>50830</v>
+      </c>
+      <c r="B362" t="s">
+        <v>367</v>
+      </c>
+      <c r="C362" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D362" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="363" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A363" s="6">
+        <v>1021</v>
+      </c>
+      <c r="B363" t="s">
+        <v>368</v>
+      </c>
+      <c r="C363" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D363" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="364" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A364" s="6">
+        <v>1026</v>
+      </c>
+      <c r="B364" t="s">
+        <v>369</v>
+      </c>
+      <c r="C364" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D364" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="365" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A365" s="6">
+        <v>1032</v>
+      </c>
+      <c r="B365" t="s">
+        <v>370</v>
+      </c>
+      <c r="C365" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D365" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="366" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A366" s="6">
+        <v>20183</v>
+      </c>
+      <c r="B366" t="s">
+        <v>371</v>
+      </c>
+      <c r="C366" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D366" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="367" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A367" s="6">
+        <v>1039</v>
+      </c>
+      <c r="B367" t="s">
+        <v>372</v>
+      </c>
+      <c r="C367" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D367" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="368" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A368" s="6">
+        <v>1040</v>
+      </c>
+      <c r="B368" t="s">
+        <v>373</v>
+      </c>
+      <c r="C368" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D368" s="9" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D328"/>
+  <autoFilter ref="A1:D326"/>
   <conditionalFormatting sqref="B1:B1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>

</xml_diff>

<commit_message>
actualice lista de precios, cambie la letra lista precios cliente 60278
</commit_message>
<xml_diff>
--- a/excel/CLIENTES_PERMISOS.xlsx
+++ b/excel/CLIENTES_PERMISOS.xlsx
@@ -1516,8 +1516,8 @@
   </sheetPr>
   <dimension ref="A1:D373"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A254" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D266" sqref="D266"/>
+    <sheetView tabSelected="1" topLeftCell="A317" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D327" sqref="D327"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6088,7 +6088,7 @@
         <v>4</v>
       </c>
       <c r="D326" s="13" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="327" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
subi imagenes de egeo 12-11-25
</commit_message>
<xml_diff>
--- a/excel/CLIENTES_PERMISOS.xlsx
+++ b/excel/CLIENTES_PERMISOS.xlsx
@@ -1517,7 +1517,7 @@
   <dimension ref="A1:D373"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A317" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D327" sqref="D327"/>
+      <selection activeCell="D329" sqref="D329"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6116,7 +6116,7 @@
         <v>4</v>
       </c>
       <c r="D328" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="329" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
actualice lista de precios 21-11-25, agregue cuenta 60274
</commit_message>
<xml_diff>
--- a/excel/CLIENTES_PERMISOS.xlsx
+++ b/excel/CLIENTES_PERMISOS.xlsx
@@ -15,14 +15,14 @@
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Hoja 1'!$A$1:$D$331</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Hoja 1'!$A$1:$D$332</definedName>
   </definedNames>
-  <calcPr calcId="162913" iterateDelta="1E-4"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1120" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1123" uniqueCount="381">
   <si>
     <t>CUENTA</t>
   </si>
@@ -1162,6 +1162,9 @@
   </si>
   <si>
     <t>FERRETERIA LOS VASCOS</t>
+  </si>
+  <si>
+    <t>ELECTRICA LOLY</t>
   </si>
 </sst>
 </file>
@@ -1514,10 +1517,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D373"/>
+  <dimension ref="A1:D374"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A317" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D329" sqref="D329"/>
+      <selection activeCell="C324" sqref="C324:D324"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6051,10 +6054,10 @@
     </row>
     <row r="324" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A324" s="6">
-        <v>60275</v>
+        <v>60274</v>
       </c>
       <c r="B324" t="s">
-        <v>288</v>
+        <v>380</v>
       </c>
       <c r="C324" s="1" t="s">
         <v>4</v>
@@ -6065,10 +6068,10 @@
     </row>
     <row r="325" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A325" s="6">
-        <v>60276</v>
+        <v>60275</v>
       </c>
       <c r="B325" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C325" s="1" t="s">
         <v>4</v>
@@ -6079,108 +6082,108 @@
     </row>
     <row r="326" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A326" s="6">
-        <v>60278</v>
+        <v>60276</v>
       </c>
       <c r="B326" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C326" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D326" s="13" t="s">
-        <v>9</v>
+      <c r="D326" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="327" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A327" s="6">
-        <v>60279</v>
+        <v>60278</v>
       </c>
       <c r="B327" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C327" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D327" s="1" t="s">
-        <v>8</v>
+      <c r="D327" s="13" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="328" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A328" s="6">
-        <v>60280</v>
+        <v>60279</v>
       </c>
       <c r="B328" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C328" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D328" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="329" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A329" s="6">
-        <v>60281</v>
-      </c>
-      <c r="B329" s="8" t="s">
-        <v>336</v>
+        <v>60280</v>
+      </c>
+      <c r="B329" t="s">
+        <v>292</v>
       </c>
       <c r="C329" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D329" s="11" t="s">
-        <v>9</v>
+      <c r="D329" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="330" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A330" s="6">
-        <v>60282</v>
+        <v>60281</v>
       </c>
       <c r="B330" s="8" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="C330" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D330" s="11" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="331" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A331" s="6">
-        <v>60283</v>
-      </c>
-      <c r="B331" t="s">
-        <v>378</v>
+        <v>60282</v>
+      </c>
+      <c r="B331" s="8" t="s">
+        <v>340</v>
       </c>
       <c r="C331" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D331" s="1" t="s">
-        <v>8</v>
+      <c r="D331" s="11" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="332" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A332" s="6">
-        <v>60284</v>
-      </c>
-      <c r="B332" s="8" t="s">
-        <v>335</v>
+        <v>60283</v>
+      </c>
+      <c r="B332" t="s">
+        <v>378</v>
       </c>
       <c r="C332" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D332" s="9" t="s">
-        <v>5</v>
+      <c r="D332" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="333" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A333" s="6">
-        <v>60285</v>
+        <v>60284</v>
       </c>
       <c r="B333" s="8" t="s">
-        <v>350</v>
+        <v>335</v>
       </c>
       <c r="C333" s="1" t="s">
         <v>4</v>
@@ -6191,10 +6194,10 @@
     </row>
     <row r="334" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A334" s="6">
-        <v>60286</v>
+        <v>60285</v>
       </c>
       <c r="B334" s="8" t="s">
-        <v>334</v>
+        <v>350</v>
       </c>
       <c r="C334" s="1" t="s">
         <v>4</v>
@@ -6205,38 +6208,38 @@
     </row>
     <row r="335" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A335" s="6">
-        <v>60287</v>
-      </c>
-      <c r="B335" t="s">
-        <v>377</v>
+        <v>60286</v>
+      </c>
+      <c r="B335" s="8" t="s">
+        <v>334</v>
       </c>
       <c r="C335" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D335" s="12" t="s">
+      <c r="D335" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="336" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A336" s="6">
-        <v>60289</v>
+        <v>60287</v>
       </c>
       <c r="B336" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="C336" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D336" s="12" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="337" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A337" s="6">
-        <v>60290</v>
+        <v>60289</v>
       </c>
       <c r="B337" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C337" s="1" t="s">
         <v>4</v>
@@ -6247,52 +6250,52 @@
     </row>
     <row r="338" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A338" s="6">
-        <v>60291</v>
+        <v>60290</v>
       </c>
       <c r="B338" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C338" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D338" s="12" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="339" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A339" s="6">
-        <v>61004</v>
+        <v>60291</v>
       </c>
       <c r="B339" t="s">
-        <v>293</v>
+        <v>376</v>
       </c>
       <c r="C339" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D339" s="15" t="s">
+      <c r="D339" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="340" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A340" s="6">
-        <v>61009</v>
+        <v>61004</v>
       </c>
       <c r="B340" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C340" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D340" s="12" t="s">
-        <v>8</v>
+      <c r="D340" s="15" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="341" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A341" s="6">
-        <v>61012</v>
+        <v>61009</v>
       </c>
       <c r="B341" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C341" s="1" t="s">
         <v>4</v>
@@ -6303,10 +6306,10 @@
     </row>
     <row r="342" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A342" s="6">
-        <v>61018</v>
+        <v>61012</v>
       </c>
       <c r="B342" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C342" s="1" t="s">
         <v>4</v>
@@ -6317,10 +6320,10 @@
     </row>
     <row r="343" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A343" s="6">
-        <v>61102</v>
+        <v>61018</v>
       </c>
       <c r="B343" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C343" s="1" t="s">
         <v>4</v>
@@ -6331,52 +6334,52 @@
     </row>
     <row r="344" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A344" s="6">
-        <v>61205</v>
+        <v>61102</v>
       </c>
       <c r="B344" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C344" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D344" s="15" t="s">
-        <v>5</v>
+      <c r="D344" s="12" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="345" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A345" s="6">
-        <v>70100</v>
+        <v>61205</v>
       </c>
       <c r="B345" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C345" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D345" s="12" t="s">
-        <v>8</v>
+      <c r="D345" s="15" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="346" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A346" s="6">
-        <v>70101</v>
+        <v>70100</v>
       </c>
       <c r="B346" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C346" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D346" s="15" t="s">
-        <v>5</v>
+      <c r="D346" s="12" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="347" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A347" s="6">
-        <v>70102</v>
+        <v>70101</v>
       </c>
       <c r="B347" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C347" s="1" t="s">
         <v>4</v>
@@ -6387,80 +6390,80 @@
     </row>
     <row r="348" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A348" s="6">
-        <v>70103</v>
+        <v>70102</v>
       </c>
       <c r="B348" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C348" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D348" s="12" t="s">
-        <v>8</v>
+      <c r="D348" s="15" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="349" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A349" s="6">
-        <v>70106</v>
+        <v>70103</v>
       </c>
       <c r="B349" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C349" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D349" s="15" t="s">
-        <v>5</v>
+      <c r="D349" s="12" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="350" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A350" s="6">
-        <v>70109</v>
+        <v>70106</v>
       </c>
       <c r="B350" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C350" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D350" s="12" t="s">
-        <v>8</v>
+      <c r="D350" s="15" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="351" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A351" s="6">
-        <v>70113</v>
+        <v>70109</v>
       </c>
       <c r="B351" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C351" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D351" s="15" t="s">
-        <v>5</v>
+      <c r="D351" s="12" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="352" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A352" s="6">
-        <v>70114</v>
+        <v>70113</v>
       </c>
       <c r="B352" t="s">
-        <v>325</v>
+        <v>305</v>
       </c>
       <c r="C352" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D352" s="9" t="s">
-        <v>9</v>
+      <c r="D352" s="15" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="353" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A353" s="6">
-        <v>70115</v>
+        <v>70114</v>
       </c>
       <c r="B353" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="C353" s="1" t="s">
         <v>4</v>
@@ -6471,24 +6474,24 @@
     </row>
     <row r="354" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A354" s="6">
-        <v>70638</v>
+        <v>70115</v>
       </c>
       <c r="B354" t="s">
-        <v>306</v>
+        <v>331</v>
       </c>
       <c r="C354" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D354" s="12" t="s">
-        <v>8</v>
+      <c r="D354" s="9" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="355" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A355" s="6">
-        <v>70639</v>
+        <v>70638</v>
       </c>
       <c r="B355" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C355" s="1" t="s">
         <v>4</v>
@@ -6499,10 +6502,10 @@
     </row>
     <row r="356" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A356" s="6">
-        <v>70640</v>
+        <v>70639</v>
       </c>
       <c r="B356" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C356" s="1" t="s">
         <v>4</v>
@@ -6513,10 +6516,10 @@
     </row>
     <row r="357" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A357" s="6">
-        <v>70642</v>
+        <v>70640</v>
       </c>
       <c r="B357" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C357" s="1" t="s">
         <v>4</v>
@@ -6527,10 +6530,10 @@
     </row>
     <row r="358" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A358" s="6">
-        <v>90504</v>
+        <v>70642</v>
       </c>
       <c r="B358" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C358" s="1" t="s">
         <v>4</v>
@@ -6541,10 +6544,10 @@
     </row>
     <row r="359" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A359" s="6">
-        <v>90509</v>
+        <v>90504</v>
       </c>
       <c r="B359" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C359" s="1" t="s">
         <v>4</v>
@@ -6555,52 +6558,52 @@
     </row>
     <row r="360" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A360" s="6">
-        <v>90602</v>
+        <v>90509</v>
       </c>
       <c r="B360" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C360" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D360" s="15" t="s">
-        <v>5</v>
+      <c r="D360" s="12" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="361" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A361" s="6">
-        <v>90621</v>
+        <v>90602</v>
       </c>
       <c r="B361" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C361" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D361" s="12" t="s">
-        <v>8</v>
+      <c r="D361" s="15" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="362" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A362" s="6">
-        <v>90622</v>
+        <v>90621</v>
       </c>
       <c r="B362" t="s">
-        <v>333</v>
+        <v>313</v>
       </c>
       <c r="C362" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D362" s="9" t="s">
-        <v>5</v>
+      <c r="D362" s="12" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="363" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A363" s="6">
-        <v>90631</v>
-      </c>
-      <c r="B363" s="8" t="s">
-        <v>342</v>
+        <v>90622</v>
+      </c>
+      <c r="B363" t="s">
+        <v>333</v>
       </c>
       <c r="C363" s="1" t="s">
         <v>4</v>
@@ -6611,24 +6614,24 @@
     </row>
     <row r="364" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A364" s="6">
-        <v>90658</v>
-      </c>
-      <c r="B364" t="s">
-        <v>314</v>
+        <v>90631</v>
+      </c>
+      <c r="B364" s="8" t="s">
+        <v>342</v>
       </c>
       <c r="C364" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D364" s="12" t="s">
-        <v>8</v>
+      <c r="D364" s="9" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="365" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A365" s="6">
-        <v>90660</v>
+        <v>90658</v>
       </c>
       <c r="B365" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C365" s="1" t="s">
         <v>4</v>
@@ -6639,10 +6642,10 @@
     </row>
     <row r="366" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A366" s="6">
-        <v>90668</v>
+        <v>90660</v>
       </c>
       <c r="B366" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C366" s="1" t="s">
         <v>4</v>
@@ -6653,10 +6656,10 @@
     </row>
     <row r="367" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A367" s="6">
-        <v>90671</v>
+        <v>90668</v>
       </c>
       <c r="B367" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C367" s="1" t="s">
         <v>4</v>
@@ -6667,10 +6670,10 @@
     </row>
     <row r="368" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A368" s="6">
-        <v>90679</v>
+        <v>90671</v>
       </c>
       <c r="B368" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C368" s="1" t="s">
         <v>4</v>
@@ -6681,10 +6684,10 @@
     </row>
     <row r="369" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A369" s="6">
-        <v>90683</v>
+        <v>90679</v>
       </c>
       <c r="B369" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C369" s="1" t="s">
         <v>4</v>
@@ -6695,10 +6698,10 @@
     </row>
     <row r="370" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A370" s="6">
-        <v>90705</v>
+        <v>90683</v>
       </c>
       <c r="B370" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C370" s="1" t="s">
         <v>4</v>
@@ -6709,10 +6712,10 @@
     </row>
     <row r="371" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A371" s="6">
-        <v>90706</v>
+        <v>90705</v>
       </c>
       <c r="B371" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C371" s="1" t="s">
         <v>4</v>
@@ -6723,10 +6726,10 @@
     </row>
     <row r="372" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A372" s="6">
-        <v>90708</v>
+        <v>90706</v>
       </c>
       <c r="B372" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C372" s="1" t="s">
         <v>4</v>
@@ -6737,20 +6740,34 @@
     </row>
     <row r="373" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A373" s="6">
+        <v>90708</v>
+      </c>
+      <c r="B373" t="s">
+        <v>322</v>
+      </c>
+      <c r="C373" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D373" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="374" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A374" s="6">
         <v>90709</v>
       </c>
-      <c r="B373" t="s">
+      <c r="B374" t="s">
         <v>323</v>
       </c>
-      <c r="C373" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D373" s="12" t="s">
+      <c r="C374" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D374" s="12" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D331"/>
+  <autoFilter ref="A1:D332"/>
   <sortState ref="A2:D374">
     <sortCondition ref="A277"/>
   </sortState>

</xml_diff>

<commit_message>
agregue cuenta MANOLO 60216 PRECIO F
</commit_message>
<xml_diff>
--- a/excel/CLIENTES_PERMISOS.xlsx
+++ b/excel/CLIENTES_PERMISOS.xlsx
@@ -15,14 +15,14 @@
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Hoja 1'!$A$1:$D$332</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Hoja 1'!$A$1:$D$333</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1123" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1126" uniqueCount="382">
   <si>
     <t>CUENTA</t>
   </si>
@@ -1165,6 +1165,9 @@
   </si>
   <si>
     <t>ELECTRICA LOLY</t>
+  </si>
+  <si>
+    <t>MANOLO FERRETERIA</t>
   </si>
 </sst>
 </file>
@@ -1517,10 +1520,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D374"/>
+  <dimension ref="A1:D375"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A317" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C324" sqref="C324:D324"/>
+    <sheetView tabSelected="1" topLeftCell="A305" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G308" sqref="G308"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5830,136 +5833,136 @@
     </row>
     <row r="308" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A308" s="6">
-        <v>60217</v>
+        <v>60216</v>
       </c>
       <c r="B308" t="s">
-        <v>276</v>
+        <v>381</v>
       </c>
       <c r="C308" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D308" s="10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="309" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A309" s="6">
-        <v>60219</v>
+        <v>60217</v>
       </c>
       <c r="B309" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C309" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D309" s="1" t="s">
+      <c r="D309" s="10" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="310" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A310" s="6">
-        <v>60222</v>
+        <v>60219</v>
       </c>
       <c r="B310" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C310" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D310" s="10" t="s">
+      <c r="D310" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="311" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A311" s="6">
-        <v>60225</v>
+        <v>60222</v>
       </c>
       <c r="B311" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C311" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D311" s="17" t="s">
-        <v>9</v>
+      <c r="D311" s="10" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="312" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A312" s="6">
-        <v>60230</v>
+        <v>60225</v>
       </c>
       <c r="B312" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C312" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D312" s="10" t="s">
-        <v>8</v>
+      <c r="D312" s="17" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="313" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A313" s="6">
-        <v>60241</v>
-      </c>
-      <c r="B313" s="8" t="s">
-        <v>338</v>
+        <v>60230</v>
+      </c>
+      <c r="B313" t="s">
+        <v>280</v>
       </c>
       <c r="C313" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D313" s="7" t="s">
-        <v>9</v>
+      <c r="D313" s="10" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="314" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A314" s="6">
-        <v>60242</v>
+        <v>60241</v>
       </c>
       <c r="B314" s="8" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="C314" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D314" s="7" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="315" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A315" s="6">
-        <v>60250</v>
+        <v>60242</v>
       </c>
       <c r="B315" s="8" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="C315" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D315" s="11" t="s">
-        <v>8</v>
+      <c r="D315" s="7" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="316" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A316" s="6">
-        <v>60253</v>
-      </c>
-      <c r="B316" t="s">
-        <v>281</v>
+        <v>60250</v>
+      </c>
+      <c r="B316" s="8" t="s">
+        <v>339</v>
       </c>
       <c r="C316" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D316" s="1" t="s">
+      <c r="D316" s="11" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="317" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A317" s="6">
-        <v>60254</v>
+        <v>60253</v>
       </c>
       <c r="B317" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C317" s="1" t="s">
         <v>4</v>
@@ -5970,10 +5973,10 @@
     </row>
     <row r="318" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A318" s="6">
-        <v>60257</v>
+        <v>60254</v>
       </c>
       <c r="B318" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C318" s="1" t="s">
         <v>4</v>
@@ -5984,10 +5987,10 @@
     </row>
     <row r="319" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A319" s="6">
-        <v>60258</v>
+        <v>60257</v>
       </c>
       <c r="B319" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C319" s="1" t="s">
         <v>4</v>
@@ -5998,52 +6001,52 @@
     </row>
     <row r="320" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A320" s="6">
-        <v>60266</v>
-      </c>
-      <c r="B320" s="8" t="s">
-        <v>343</v>
+        <v>60258</v>
+      </c>
+      <c r="B320" t="s">
+        <v>284</v>
       </c>
       <c r="C320" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D320" s="11" t="s">
+      <c r="D320" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="321" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A321" s="6">
-        <v>60269</v>
-      </c>
-      <c r="B321" t="s">
-        <v>285</v>
+        <v>60266</v>
+      </c>
+      <c r="B321" s="8" t="s">
+        <v>343</v>
       </c>
       <c r="C321" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D321" s="10" t="s">
+      <c r="D321" s="11" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="322" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A322" s="6">
-        <v>60270</v>
+        <v>60269</v>
       </c>
       <c r="B322" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C322" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D322" s="1" t="s">
+      <c r="D322" s="10" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="323" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A323" s="6">
-        <v>60272</v>
+        <v>60270</v>
       </c>
       <c r="B323" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C323" s="1" t="s">
         <v>4</v>
@@ -6054,10 +6057,10 @@
     </row>
     <row r="324" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A324" s="6">
-        <v>60274</v>
+        <v>60272</v>
       </c>
       <c r="B324" t="s">
-        <v>380</v>
+        <v>287</v>
       </c>
       <c r="C324" s="1" t="s">
         <v>4</v>
@@ -6068,10 +6071,10 @@
     </row>
     <row r="325" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A325" s="6">
-        <v>60275</v>
+        <v>60274</v>
       </c>
       <c r="B325" t="s">
-        <v>288</v>
+        <v>380</v>
       </c>
       <c r="C325" s="1" t="s">
         <v>4</v>
@@ -6082,10 +6085,10 @@
     </row>
     <row r="326" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A326" s="6">
-        <v>60276</v>
+        <v>60275</v>
       </c>
       <c r="B326" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C326" s="1" t="s">
         <v>4</v>
@@ -6096,108 +6099,108 @@
     </row>
     <row r="327" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A327" s="6">
-        <v>60278</v>
+        <v>60276</v>
       </c>
       <c r="B327" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C327" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D327" s="13" t="s">
-        <v>9</v>
+      <c r="D327" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="328" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A328" s="6">
-        <v>60279</v>
+        <v>60278</v>
       </c>
       <c r="B328" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C328" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D328" s="1" t="s">
-        <v>8</v>
+      <c r="D328" s="13" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="329" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A329" s="6">
-        <v>60280</v>
+        <v>60279</v>
       </c>
       <c r="B329" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C329" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D329" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="330" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A330" s="6">
-        <v>60281</v>
-      </c>
-      <c r="B330" s="8" t="s">
-        <v>336</v>
+        <v>60280</v>
+      </c>
+      <c r="B330" t="s">
+        <v>292</v>
       </c>
       <c r="C330" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D330" s="11" t="s">
-        <v>9</v>
+      <c r="D330" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="331" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A331" s="6">
-        <v>60282</v>
+        <v>60281</v>
       </c>
       <c r="B331" s="8" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="C331" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D331" s="11" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="332" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A332" s="6">
-        <v>60283</v>
-      </c>
-      <c r="B332" t="s">
-        <v>378</v>
+        <v>60282</v>
+      </c>
+      <c r="B332" s="8" t="s">
+        <v>340</v>
       </c>
       <c r="C332" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D332" s="1" t="s">
-        <v>8</v>
+      <c r="D332" s="11" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="333" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A333" s="6">
-        <v>60284</v>
-      </c>
-      <c r="B333" s="8" t="s">
-        <v>335</v>
+        <v>60283</v>
+      </c>
+      <c r="B333" t="s">
+        <v>378</v>
       </c>
       <c r="C333" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D333" s="9" t="s">
-        <v>5</v>
+      <c r="D333" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="334" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A334" s="6">
-        <v>60285</v>
+        <v>60284</v>
       </c>
       <c r="B334" s="8" t="s">
-        <v>350</v>
+        <v>335</v>
       </c>
       <c r="C334" s="1" t="s">
         <v>4</v>
@@ -6208,10 +6211,10 @@
     </row>
     <row r="335" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A335" s="6">
-        <v>60286</v>
+        <v>60285</v>
       </c>
       <c r="B335" s="8" t="s">
-        <v>334</v>
+        <v>350</v>
       </c>
       <c r="C335" s="1" t="s">
         <v>4</v>
@@ -6222,38 +6225,38 @@
     </row>
     <row r="336" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A336" s="6">
-        <v>60287</v>
-      </c>
-      <c r="B336" t="s">
-        <v>377</v>
+        <v>60286</v>
+      </c>
+      <c r="B336" s="8" t="s">
+        <v>334</v>
       </c>
       <c r="C336" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D336" s="12" t="s">
+      <c r="D336" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="337" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A337" s="6">
-        <v>60289</v>
+        <v>60287</v>
       </c>
       <c r="B337" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="C337" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D337" s="12" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="338" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A338" s="6">
-        <v>60290</v>
+        <v>60289</v>
       </c>
       <c r="B338" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C338" s="1" t="s">
         <v>4</v>
@@ -6264,52 +6267,52 @@
     </row>
     <row r="339" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A339" s="6">
-        <v>60291</v>
+        <v>60290</v>
       </c>
       <c r="B339" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C339" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D339" s="12" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="340" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A340" s="6">
-        <v>61004</v>
+        <v>60291</v>
       </c>
       <c r="B340" t="s">
-        <v>293</v>
+        <v>376</v>
       </c>
       <c r="C340" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D340" s="15" t="s">
+      <c r="D340" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="341" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A341" s="6">
-        <v>61009</v>
+        <v>61004</v>
       </c>
       <c r="B341" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C341" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D341" s="12" t="s">
-        <v>8</v>
+      <c r="D341" s="15" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="342" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A342" s="6">
-        <v>61012</v>
+        <v>61009</v>
       </c>
       <c r="B342" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C342" s="1" t="s">
         <v>4</v>
@@ -6320,10 +6323,10 @@
     </row>
     <row r="343" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A343" s="6">
-        <v>61018</v>
+        <v>61012</v>
       </c>
       <c r="B343" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C343" s="1" t="s">
         <v>4</v>
@@ -6334,10 +6337,10 @@
     </row>
     <row r="344" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A344" s="6">
-        <v>61102</v>
+        <v>61018</v>
       </c>
       <c r="B344" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C344" s="1" t="s">
         <v>4</v>
@@ -6348,52 +6351,52 @@
     </row>
     <row r="345" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A345" s="6">
-        <v>61205</v>
+        <v>61102</v>
       </c>
       <c r="B345" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C345" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D345" s="15" t="s">
-        <v>5</v>
+      <c r="D345" s="12" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="346" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A346" s="6">
-        <v>70100</v>
+        <v>61205</v>
       </c>
       <c r="B346" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C346" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D346" s="12" t="s">
-        <v>8</v>
+      <c r="D346" s="15" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="347" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A347" s="6">
-        <v>70101</v>
+        <v>70100</v>
       </c>
       <c r="B347" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C347" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D347" s="15" t="s">
-        <v>5</v>
+      <c r="D347" s="12" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="348" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A348" s="6">
-        <v>70102</v>
+        <v>70101</v>
       </c>
       <c r="B348" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C348" s="1" t="s">
         <v>4</v>
@@ -6404,80 +6407,80 @@
     </row>
     <row r="349" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A349" s="6">
-        <v>70103</v>
+        <v>70102</v>
       </c>
       <c r="B349" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C349" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D349" s="12" t="s">
-        <v>8</v>
+      <c r="D349" s="15" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="350" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A350" s="6">
-        <v>70106</v>
+        <v>70103</v>
       </c>
       <c r="B350" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C350" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D350" s="15" t="s">
-        <v>5</v>
+      <c r="D350" s="12" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="351" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A351" s="6">
-        <v>70109</v>
+        <v>70106</v>
       </c>
       <c r="B351" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C351" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D351" s="12" t="s">
-        <v>8</v>
+      <c r="D351" s="15" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="352" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A352" s="6">
-        <v>70113</v>
+        <v>70109</v>
       </c>
       <c r="B352" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C352" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D352" s="15" t="s">
-        <v>5</v>
+      <c r="D352" s="12" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="353" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A353" s="6">
-        <v>70114</v>
+        <v>70113</v>
       </c>
       <c r="B353" t="s">
-        <v>325</v>
+        <v>305</v>
       </c>
       <c r="C353" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D353" s="9" t="s">
-        <v>9</v>
+      <c r="D353" s="15" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="354" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A354" s="6">
-        <v>70115</v>
+        <v>70114</v>
       </c>
       <c r="B354" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="C354" s="1" t="s">
         <v>4</v>
@@ -6488,24 +6491,24 @@
     </row>
     <row r="355" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A355" s="6">
-        <v>70638</v>
+        <v>70115</v>
       </c>
       <c r="B355" t="s">
-        <v>306</v>
+        <v>331</v>
       </c>
       <c r="C355" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D355" s="12" t="s">
-        <v>8</v>
+      <c r="D355" s="9" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="356" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A356" s="6">
-        <v>70639</v>
+        <v>70638</v>
       </c>
       <c r="B356" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C356" s="1" t="s">
         <v>4</v>
@@ -6516,10 +6519,10 @@
     </row>
     <row r="357" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A357" s="6">
-        <v>70640</v>
+        <v>70639</v>
       </c>
       <c r="B357" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C357" s="1" t="s">
         <v>4</v>
@@ -6530,10 +6533,10 @@
     </row>
     <row r="358" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A358" s="6">
-        <v>70642</v>
+        <v>70640</v>
       </c>
       <c r="B358" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C358" s="1" t="s">
         <v>4</v>
@@ -6544,10 +6547,10 @@
     </row>
     <row r="359" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A359" s="6">
-        <v>90504</v>
+        <v>70642</v>
       </c>
       <c r="B359" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C359" s="1" t="s">
         <v>4</v>
@@ -6558,10 +6561,10 @@
     </row>
     <row r="360" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A360" s="6">
-        <v>90509</v>
+        <v>90504</v>
       </c>
       <c r="B360" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C360" s="1" t="s">
         <v>4</v>
@@ -6572,52 +6575,52 @@
     </row>
     <row r="361" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A361" s="6">
-        <v>90602</v>
+        <v>90509</v>
       </c>
       <c r="B361" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C361" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D361" s="15" t="s">
-        <v>5</v>
+      <c r="D361" s="12" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="362" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A362" s="6">
-        <v>90621</v>
+        <v>90602</v>
       </c>
       <c r="B362" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C362" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D362" s="12" t="s">
-        <v>8</v>
+      <c r="D362" s="15" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="363" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A363" s="6">
-        <v>90622</v>
+        <v>90621</v>
       </c>
       <c r="B363" t="s">
-        <v>333</v>
+        <v>313</v>
       </c>
       <c r="C363" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D363" s="9" t="s">
-        <v>5</v>
+      <c r="D363" s="12" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="364" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A364" s="6">
-        <v>90631</v>
-      </c>
-      <c r="B364" s="8" t="s">
-        <v>342</v>
+        <v>90622</v>
+      </c>
+      <c r="B364" t="s">
+        <v>333</v>
       </c>
       <c r="C364" s="1" t="s">
         <v>4</v>
@@ -6628,24 +6631,24 @@
     </row>
     <row r="365" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A365" s="6">
-        <v>90658</v>
-      </c>
-      <c r="B365" t="s">
-        <v>314</v>
+        <v>90631</v>
+      </c>
+      <c r="B365" s="8" t="s">
+        <v>342</v>
       </c>
       <c r="C365" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D365" s="12" t="s">
-        <v>8</v>
+      <c r="D365" s="9" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="366" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A366" s="6">
-        <v>90660</v>
+        <v>90658</v>
       </c>
       <c r="B366" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C366" s="1" t="s">
         <v>4</v>
@@ -6656,10 +6659,10 @@
     </row>
     <row r="367" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A367" s="6">
-        <v>90668</v>
+        <v>90660</v>
       </c>
       <c r="B367" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C367" s="1" t="s">
         <v>4</v>
@@ -6670,10 +6673,10 @@
     </row>
     <row r="368" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A368" s="6">
-        <v>90671</v>
+        <v>90668</v>
       </c>
       <c r="B368" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C368" s="1" t="s">
         <v>4</v>
@@ -6684,10 +6687,10 @@
     </row>
     <row r="369" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A369" s="6">
-        <v>90679</v>
+        <v>90671</v>
       </c>
       <c r="B369" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C369" s="1" t="s">
         <v>4</v>
@@ -6698,10 +6701,10 @@
     </row>
     <row r="370" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A370" s="6">
-        <v>90683</v>
+        <v>90679</v>
       </c>
       <c r="B370" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C370" s="1" t="s">
         <v>4</v>
@@ -6712,10 +6715,10 @@
     </row>
     <row r="371" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A371" s="6">
-        <v>90705</v>
+        <v>90683</v>
       </c>
       <c r="B371" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C371" s="1" t="s">
         <v>4</v>
@@ -6726,10 +6729,10 @@
     </row>
     <row r="372" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A372" s="6">
-        <v>90706</v>
+        <v>90705</v>
       </c>
       <c r="B372" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C372" s="1" t="s">
         <v>4</v>
@@ -6740,10 +6743,10 @@
     </row>
     <row r="373" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A373" s="6">
-        <v>90708</v>
+        <v>90706</v>
       </c>
       <c r="B373" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C373" s="1" t="s">
         <v>4</v>
@@ -6754,20 +6757,34 @@
     </row>
     <row r="374" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A374" s="6">
+        <v>90708</v>
+      </c>
+      <c r="B374" t="s">
+        <v>322</v>
+      </c>
+      <c r="C374" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D374" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="375" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A375" s="6">
         <v>90709</v>
       </c>
-      <c r="B374" t="s">
+      <c r="B375" t="s">
         <v>323</v>
       </c>
-      <c r="C374" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D374" s="12" t="s">
+      <c r="C375" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D375" s="12" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D332"/>
+  <autoFilter ref="A1:D333"/>
   <sortState ref="A2:D374">
     <sortCondition ref="A277"/>
   </sortState>

</xml_diff>

<commit_message>
actualice lista de precios 23-1-26
</commit_message>
<xml_diff>
--- a/excel/CLIENTES_PERMISOS.xlsx
+++ b/excel/CLIENTES_PERMISOS.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1126" uniqueCount="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1135" uniqueCount="385">
   <si>
     <t>CUENTA</t>
   </si>
@@ -1168,6 +1168,15 @@
   </si>
   <si>
     <t>MANOLO FERRETERIA</t>
+  </si>
+  <si>
+    <t>ROBERTO FERRIN</t>
+  </si>
+  <si>
+    <t>JAIME GONZALEZ</t>
+  </si>
+  <si>
+    <t>CHRISTIAN SEQUEIRA</t>
   </si>
 </sst>
 </file>
@@ -1520,10 +1529,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D375"/>
+  <dimension ref="A1:D378"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A305" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G308" sqref="G308"/>
+    <sheetView tabSelected="1" topLeftCell="A365" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C376" sqref="C376:D378"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6783,6 +6792,48 @@
         <v>8</v>
       </c>
     </row>
+    <row r="376" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A376" s="6">
+        <v>1218</v>
+      </c>
+      <c r="B376" t="s">
+        <v>382</v>
+      </c>
+      <c r="C376" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D376" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="377" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A377" s="6">
+        <v>1959</v>
+      </c>
+      <c r="B377" s="8" t="s">
+        <v>383</v>
+      </c>
+      <c r="C377" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D377" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="378" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A378" s="6">
+        <v>5625</v>
+      </c>
+      <c r="B378" s="8" t="s">
+        <v>384</v>
+      </c>
+      <c r="C378" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D378" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:D333"/>
   <sortState ref="A2:D374">

</xml_diff>

<commit_message>
Actualizar permisos de clientes, grupos y configuración de márgenes
</commit_message>
<xml_diff>
--- a/excel/CLIENTES_PERMISOS.xlsx
+++ b/excel/CLIENTES_PERMISOS.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1135" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1141" uniqueCount="387">
   <si>
     <t>CUENTA</t>
   </si>
@@ -1177,6 +1177,12 @@
   </si>
   <si>
     <t>CHRISTIAN SEQUEIRA</t>
+  </si>
+  <si>
+    <t>FERRETERIA FERREMAR</t>
+  </si>
+  <si>
+    <t>FERRETERIA MARTINS</t>
   </si>
 </sst>
 </file>
@@ -1529,10 +1535,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D378"/>
+  <dimension ref="A1:D380"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A365" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C376" sqref="C376:D378"/>
+      <selection activeCell="D380" sqref="D380"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6834,6 +6840,34 @@
         <v>8</v>
       </c>
     </row>
+    <row r="379" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A379" s="6">
+        <v>60295</v>
+      </c>
+      <c r="B379" s="8" t="s">
+        <v>385</v>
+      </c>
+      <c r="C379" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D379" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="380" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A380" s="6">
+        <v>1045</v>
+      </c>
+      <c r="B380" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="C380" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D380" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:D333"/>
   <sortState ref="A2:D374">

</xml_diff>

<commit_message>
actualice lista precios, cambie formula a ctas juan fer, doble c, f general. 6-2-26
</commit_message>
<xml_diff>
--- a/excel/CLIENTES_PERMISOS.xlsx
+++ b/excel/CLIENTES_PERMISOS.xlsx
@@ -15,14 +15,14 @@
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Hoja 1'!$A$1:$D$333</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Hoja 1'!$A$1:$D$334</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1141" uniqueCount="387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1147" uniqueCount="389">
   <si>
     <t>CUENTA</t>
   </si>
@@ -1183,6 +1183,12 @@
   </si>
   <si>
     <t>FERRETERIA MARTINS</t>
+  </si>
+  <si>
+    <t>FERRETERIA GENERAL</t>
+  </si>
+  <si>
+    <t>QUIMICA</t>
   </si>
 </sst>
 </file>
@@ -1535,10 +1541,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D380"/>
+  <dimension ref="A1:D382"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A365" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D380" sqref="D380"/>
+    <sheetView tabSelected="1" topLeftCell="A333" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B343" sqref="B343"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5960,38 +5966,38 @@
     </row>
     <row r="316" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A316" s="6">
-        <v>60250</v>
+        <v>60245</v>
       </c>
       <c r="B316" s="8" t="s">
-        <v>339</v>
+        <v>387</v>
       </c>
       <c r="C316" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D316" s="11" t="s">
-        <v>8</v>
+      <c r="D316" s="7" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="317" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A317" s="6">
-        <v>60253</v>
-      </c>
-      <c r="B317" t="s">
-        <v>281</v>
+        <v>60250</v>
+      </c>
+      <c r="B317" s="8" t="s">
+        <v>339</v>
       </c>
       <c r="C317" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D317" s="1" t="s">
+      <c r="D317" s="11" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="318" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A318" s="6">
-        <v>60254</v>
+        <v>60253</v>
       </c>
       <c r="B318" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C318" s="1" t="s">
         <v>4</v>
@@ -6002,10 +6008,10 @@
     </row>
     <row r="319" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A319" s="6">
-        <v>60257</v>
+        <v>60254</v>
       </c>
       <c r="B319" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C319" s="1" t="s">
         <v>4</v>
@@ -6016,10 +6022,10 @@
     </row>
     <row r="320" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A320" s="6">
-        <v>60258</v>
+        <v>60257</v>
       </c>
       <c r="B320" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C320" s="1" t="s">
         <v>4</v>
@@ -6030,52 +6036,52 @@
     </row>
     <row r="321" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A321" s="6">
-        <v>60266</v>
-      </c>
-      <c r="B321" s="8" t="s">
-        <v>343</v>
+        <v>60258</v>
+      </c>
+      <c r="B321" t="s">
+        <v>284</v>
       </c>
       <c r="C321" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D321" s="11" t="s">
+      <c r="D321" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="322" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A322" s="6">
-        <v>60269</v>
-      </c>
-      <c r="B322" t="s">
-        <v>285</v>
+        <v>60266</v>
+      </c>
+      <c r="B322" s="8" t="s">
+        <v>343</v>
       </c>
       <c r="C322" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D322" s="10" t="s">
+      <c r="D322" s="11" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="323" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A323" s="6">
-        <v>60270</v>
+        <v>60269</v>
       </c>
       <c r="B323" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C323" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D323" s="1" t="s">
+      <c r="D323" s="10" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="324" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A324" s="6">
-        <v>60272</v>
+        <v>60270</v>
       </c>
       <c r="B324" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C324" s="1" t="s">
         <v>4</v>
@@ -6086,10 +6092,10 @@
     </row>
     <row r="325" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A325" s="6">
-        <v>60274</v>
+        <v>60272</v>
       </c>
       <c r="B325" t="s">
-        <v>380</v>
+        <v>287</v>
       </c>
       <c r="C325" s="1" t="s">
         <v>4</v>
@@ -6100,10 +6106,10 @@
     </row>
     <row r="326" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A326" s="6">
-        <v>60275</v>
+        <v>60274</v>
       </c>
       <c r="B326" t="s">
-        <v>288</v>
+        <v>380</v>
       </c>
       <c r="C326" s="1" t="s">
         <v>4</v>
@@ -6114,10 +6120,10 @@
     </row>
     <row r="327" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A327" s="6">
-        <v>60276</v>
+        <v>60275</v>
       </c>
       <c r="B327" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C327" s="1" t="s">
         <v>4</v>
@@ -6128,108 +6134,108 @@
     </row>
     <row r="328" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A328" s="6">
-        <v>60278</v>
+        <v>60276</v>
       </c>
       <c r="B328" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C328" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D328" s="13" t="s">
-        <v>9</v>
+      <c r="D328" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="329" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A329" s="6">
-        <v>60279</v>
+        <v>60278</v>
       </c>
       <c r="B329" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C329" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D329" s="1" t="s">
-        <v>8</v>
+      <c r="D329" s="13" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="330" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A330" s="6">
-        <v>60280</v>
+        <v>60279</v>
       </c>
       <c r="B330" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C330" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D330" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="331" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A331" s="6">
-        <v>60281</v>
-      </c>
-      <c r="B331" s="8" t="s">
-        <v>336</v>
+        <v>60280</v>
+      </c>
+      <c r="B331" t="s">
+        <v>292</v>
       </c>
       <c r="C331" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D331" s="11" t="s">
-        <v>9</v>
+      <c r="D331" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="332" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A332" s="6">
-        <v>60282</v>
+        <v>60281</v>
       </c>
       <c r="B332" s="8" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="C332" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D332" s="11" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="333" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A333" s="6">
-        <v>60283</v>
-      </c>
-      <c r="B333" t="s">
-        <v>378</v>
+        <v>60282</v>
+      </c>
+      <c r="B333" s="8" t="s">
+        <v>340</v>
       </c>
       <c r="C333" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D333" s="1" t="s">
-        <v>8</v>
+      <c r="D333" s="11" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="334" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A334" s="6">
-        <v>60284</v>
-      </c>
-      <c r="B334" s="8" t="s">
-        <v>335</v>
+        <v>60283</v>
+      </c>
+      <c r="B334" t="s">
+        <v>378</v>
       </c>
       <c r="C334" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D334" s="9" t="s">
-        <v>5</v>
+      <c r="D334" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="335" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A335" s="6">
-        <v>60285</v>
+        <v>60284</v>
       </c>
       <c r="B335" s="8" t="s">
-        <v>350</v>
+        <v>335</v>
       </c>
       <c r="C335" s="1" t="s">
         <v>4</v>
@@ -6240,10 +6246,10 @@
     </row>
     <row r="336" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A336" s="6">
-        <v>60286</v>
+        <v>60285</v>
       </c>
       <c r="B336" s="8" t="s">
-        <v>334</v>
+        <v>350</v>
       </c>
       <c r="C336" s="1" t="s">
         <v>4</v>
@@ -6254,38 +6260,38 @@
     </row>
     <row r="337" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A337" s="6">
-        <v>60287</v>
-      </c>
-      <c r="B337" t="s">
-        <v>377</v>
+        <v>60286</v>
+      </c>
+      <c r="B337" s="8" t="s">
+        <v>334</v>
       </c>
       <c r="C337" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D337" s="12" t="s">
+      <c r="D337" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="338" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A338" s="6">
-        <v>60289</v>
+        <v>60287</v>
       </c>
       <c r="B338" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="C338" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D338" s="12" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="339" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A339" s="6">
-        <v>60290</v>
+        <v>60289</v>
       </c>
       <c r="B339" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C339" s="1" t="s">
         <v>4</v>
@@ -6296,10 +6302,10 @@
     </row>
     <row r="340" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A340" s="6">
-        <v>60291</v>
+        <v>60290</v>
       </c>
       <c r="B340" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C340" s="1" t="s">
         <v>4</v>
@@ -6310,52 +6316,52 @@
     </row>
     <row r="341" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A341" s="6">
-        <v>61004</v>
+        <v>60291</v>
       </c>
       <c r="B341" t="s">
-        <v>293</v>
+        <v>376</v>
       </c>
       <c r="C341" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D341" s="15" t="s">
+      <c r="D341" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="342" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A342" s="6">
-        <v>61009</v>
+        <v>60299</v>
       </c>
       <c r="B342" t="s">
-        <v>294</v>
+        <v>388</v>
       </c>
       <c r="C342" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D342" s="12" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="343" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A343" s="6">
-        <v>61012</v>
+        <v>61004</v>
       </c>
       <c r="B343" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C343" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D343" s="12" t="s">
-        <v>8</v>
+      <c r="D343" s="15" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="344" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A344" s="6">
-        <v>61018</v>
+        <v>61009</v>
       </c>
       <c r="B344" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C344" s="1" t="s">
         <v>4</v>
@@ -6366,10 +6372,10 @@
     </row>
     <row r="345" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A345" s="6">
-        <v>61102</v>
+        <v>61012</v>
       </c>
       <c r="B345" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C345" s="1" t="s">
         <v>4</v>
@@ -6380,24 +6386,24 @@
     </row>
     <row r="346" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A346" s="6">
-        <v>61205</v>
+        <v>61018</v>
       </c>
       <c r="B346" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C346" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D346" s="15" t="s">
-        <v>5</v>
+      <c r="D346" s="12" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="347" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A347" s="6">
-        <v>70100</v>
+        <v>61102</v>
       </c>
       <c r="B347" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C347" s="1" t="s">
         <v>4</v>
@@ -6408,10 +6414,10 @@
     </row>
     <row r="348" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A348" s="6">
-        <v>70101</v>
+        <v>61205</v>
       </c>
       <c r="B348" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C348" s="1" t="s">
         <v>4</v>
@@ -6422,38 +6428,38 @@
     </row>
     <row r="349" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A349" s="6">
-        <v>70102</v>
+        <v>70100</v>
       </c>
       <c r="B349" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C349" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D349" s="15" t="s">
-        <v>5</v>
+      <c r="D349" s="12" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="350" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A350" s="6">
-        <v>70103</v>
+        <v>70101</v>
       </c>
       <c r="B350" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C350" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D350" s="12" t="s">
-        <v>8</v>
+      <c r="D350" s="15" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="351" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A351" s="6">
-        <v>70106</v>
+        <v>70102</v>
       </c>
       <c r="B351" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C351" s="1" t="s">
         <v>4</v>
@@ -6464,10 +6470,10 @@
     </row>
     <row r="352" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A352" s="6">
-        <v>70109</v>
+        <v>70103</v>
       </c>
       <c r="B352" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C352" s="1" t="s">
         <v>4</v>
@@ -6478,10 +6484,10 @@
     </row>
     <row r="353" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A353" s="6">
-        <v>70113</v>
+        <v>70106</v>
       </c>
       <c r="B353" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C353" s="1" t="s">
         <v>4</v>
@@ -6492,66 +6498,66 @@
     </row>
     <row r="354" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A354" s="6">
-        <v>70114</v>
+        <v>70109</v>
       </c>
       <c r="B354" t="s">
-        <v>325</v>
+        <v>304</v>
       </c>
       <c r="C354" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D354" s="9" t="s">
-        <v>9</v>
+      <c r="D354" s="12" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="355" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A355" s="6">
-        <v>70115</v>
+        <v>70113</v>
       </c>
       <c r="B355" t="s">
-        <v>331</v>
+        <v>305</v>
       </c>
       <c r="C355" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D355" s="9" t="s">
-        <v>9</v>
+      <c r="D355" s="15" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="356" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A356" s="6">
-        <v>70638</v>
+        <v>70114</v>
       </c>
       <c r="B356" t="s">
-        <v>306</v>
+        <v>325</v>
       </c>
       <c r="C356" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D356" s="12" t="s">
-        <v>8</v>
+      <c r="D356" s="9" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="357" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A357" s="6">
-        <v>70639</v>
+        <v>70115</v>
       </c>
       <c r="B357" t="s">
-        <v>307</v>
+        <v>331</v>
       </c>
       <c r="C357" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D357" s="12" t="s">
-        <v>8</v>
+      <c r="D357" s="9" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="358" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A358" s="6">
-        <v>70640</v>
+        <v>70638</v>
       </c>
       <c r="B358" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C358" s="1" t="s">
         <v>4</v>
@@ -6562,10 +6568,10 @@
     </row>
     <row r="359" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A359" s="6">
-        <v>70642</v>
+        <v>70639</v>
       </c>
       <c r="B359" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C359" s="1" t="s">
         <v>4</v>
@@ -6576,10 +6582,10 @@
     </row>
     <row r="360" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A360" s="6">
-        <v>90504</v>
+        <v>70640</v>
       </c>
       <c r="B360" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C360" s="1" t="s">
         <v>4</v>
@@ -6590,10 +6596,10 @@
     </row>
     <row r="361" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A361" s="6">
-        <v>90509</v>
+        <v>70642</v>
       </c>
       <c r="B361" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C361" s="1" t="s">
         <v>4</v>
@@ -6604,24 +6610,24 @@
     </row>
     <row r="362" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A362" s="6">
-        <v>90602</v>
+        <v>90504</v>
       </c>
       <c r="B362" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C362" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D362" s="15" t="s">
-        <v>5</v>
+      <c r="D362" s="12" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="363" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A363" s="6">
-        <v>90621</v>
+        <v>90509</v>
       </c>
       <c r="B363" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C363" s="1" t="s">
         <v>4</v>
@@ -6632,66 +6638,66 @@
     </row>
     <row r="364" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A364" s="6">
-        <v>90622</v>
+        <v>90602</v>
       </c>
       <c r="B364" t="s">
-        <v>333</v>
+        <v>312</v>
       </c>
       <c r="C364" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D364" s="9" t="s">
+      <c r="D364" s="15" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="365" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A365" s="6">
-        <v>90631</v>
-      </c>
-      <c r="B365" s="8" t="s">
-        <v>342</v>
+        <v>90621</v>
+      </c>
+      <c r="B365" t="s">
+        <v>313</v>
       </c>
       <c r="C365" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D365" s="9" t="s">
-        <v>5</v>
+      <c r="D365" s="12" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="366" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A366" s="6">
-        <v>90658</v>
+        <v>90622</v>
       </c>
       <c r="B366" t="s">
-        <v>314</v>
+        <v>333</v>
       </c>
       <c r="C366" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D366" s="12" t="s">
-        <v>8</v>
+      <c r="D366" s="9" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="367" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A367" s="6">
-        <v>90660</v>
-      </c>
-      <c r="B367" t="s">
-        <v>315</v>
+        <v>90631</v>
+      </c>
+      <c r="B367" s="8" t="s">
+        <v>342</v>
       </c>
       <c r="C367" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D367" s="12" t="s">
-        <v>8</v>
+      <c r="D367" s="9" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="368" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A368" s="6">
-        <v>90668</v>
+        <v>90658</v>
       </c>
       <c r="B368" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C368" s="1" t="s">
         <v>4</v>
@@ -6702,10 +6708,10 @@
     </row>
     <row r="369" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A369" s="6">
-        <v>90671</v>
+        <v>90660</v>
       </c>
       <c r="B369" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C369" s="1" t="s">
         <v>4</v>
@@ -6716,10 +6722,10 @@
     </row>
     <row r="370" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A370" s="6">
-        <v>90679</v>
+        <v>90668</v>
       </c>
       <c r="B370" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C370" s="1" t="s">
         <v>4</v>
@@ -6730,10 +6736,10 @@
     </row>
     <row r="371" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A371" s="6">
-        <v>90683</v>
+        <v>90671</v>
       </c>
       <c r="B371" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C371" s="1" t="s">
         <v>4</v>
@@ -6744,10 +6750,10 @@
     </row>
     <row r="372" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A372" s="6">
-        <v>90705</v>
+        <v>90679</v>
       </c>
       <c r="B372" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C372" s="1" t="s">
         <v>4</v>
@@ -6758,10 +6764,10 @@
     </row>
     <row r="373" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A373" s="6">
-        <v>90706</v>
+        <v>90683</v>
       </c>
       <c r="B373" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C373" s="1" t="s">
         <v>4</v>
@@ -6772,10 +6778,10 @@
     </row>
     <row r="374" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A374" s="6">
-        <v>90708</v>
+        <v>90705</v>
       </c>
       <c r="B374" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C374" s="1" t="s">
         <v>4</v>
@@ -6786,10 +6792,10 @@
     </row>
     <row r="375" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A375" s="6">
-        <v>90709</v>
+        <v>90706</v>
       </c>
       <c r="B375" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C375" s="1" t="s">
         <v>4</v>
@@ -6800,10 +6806,10 @@
     </row>
     <row r="376" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A376" s="6">
-        <v>1218</v>
+        <v>90708</v>
       </c>
       <c r="B376" t="s">
-        <v>382</v>
+        <v>322</v>
       </c>
       <c r="C376" s="1" t="s">
         <v>4</v>
@@ -6814,10 +6820,10 @@
     </row>
     <row r="377" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A377" s="6">
-        <v>1959</v>
-      </c>
-      <c r="B377" s="8" t="s">
-        <v>383</v>
+        <v>90709</v>
+      </c>
+      <c r="B377" t="s">
+        <v>323</v>
       </c>
       <c r="C377" s="1" t="s">
         <v>4</v>
@@ -6828,10 +6834,10 @@
     </row>
     <row r="378" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A378" s="6">
-        <v>5625</v>
-      </c>
-      <c r="B378" s="8" t="s">
-        <v>384</v>
+        <v>1218</v>
+      </c>
+      <c r="B378" t="s">
+        <v>382</v>
       </c>
       <c r="C378" s="1" t="s">
         <v>4</v>
@@ -6842,34 +6848,62 @@
     </row>
     <row r="379" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A379" s="6">
-        <v>60295</v>
+        <v>1959</v>
       </c>
       <c r="B379" s="8" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C379" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D379" s="9" t="s">
+      <c r="D379" s="12" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="380" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A380" s="6">
+        <v>5625</v>
+      </c>
+      <c r="B380" s="8" t="s">
+        <v>384</v>
+      </c>
+      <c r="C380" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D380" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="381" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A381" s="6">
+        <v>60295</v>
+      </c>
+      <c r="B381" s="8" t="s">
+        <v>385</v>
+      </c>
+      <c r="C381" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D381" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="382" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A382" s="6">
         <v>1045</v>
       </c>
-      <c r="B380" s="8" t="s">
+      <c r="B382" s="8" t="s">
         <v>386</v>
       </c>
-      <c r="C380" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D380" s="9" t="s">
+      <c r="C382" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D382" s="9" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D333"/>
+  <autoFilter ref="A1:D334"/>
   <sortState ref="A2:D374">
     <sortCondition ref="A277"/>
   </sortState>

</xml_diff>